<commit_message>
perubahan table da spec order booking
</commit_message>
<xml_diff>
--- a/document/spec.xlsx
+++ b/document/spec.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="174">
   <si>
     <t>Agent Register</t>
   </si>
@@ -304,6 +304,240 @@
   </si>
   <si>
     <t>selain itu Pending</t>
+  </si>
+  <si>
+    <t>trx011.check_in_date</t>
+  </si>
+  <si>
+    <t>trx011.check_out_date</t>
+  </si>
+  <si>
+    <t>trx011.day</t>
+  </si>
+  <si>
+    <t>trx011.type_room</t>
+  </si>
+  <si>
+    <t>trx011.type</t>
+  </si>
+  <si>
+    <t>pantek idr</t>
+  </si>
+  <si>
+    <t>trx011.gross_value_day</t>
+  </si>
+  <si>
+    <t>trx011.tot_value</t>
+  </si>
+  <si>
+    <t>trx011.guest_first_name</t>
+  </si>
+  <si>
+    <t>trx011.guest_last_name</t>
+  </si>
+  <si>
+    <t>trx011.title</t>
+  </si>
+  <si>
+    <t>mr/mrs</t>
+  </si>
+  <si>
+    <t>trx011.interconnetion_flag</t>
+  </si>
+  <si>
+    <t>trx011.early_check_in_flag</t>
+  </si>
+  <si>
+    <t>trx011.late_check_in_flag</t>
+  </si>
+  <si>
+    <t>trx011.high_floor_flag</t>
+  </si>
+  <si>
+    <t>trx011.low_floor_flag</t>
+  </si>
+  <si>
+    <t>trx011.twin_flag</t>
+  </si>
+  <si>
+    <t>trx011.non_smoking_flag</t>
+  </si>
+  <si>
+    <t>trx011.note</t>
+  </si>
+  <si>
+    <t>trx011.cancel_policy</t>
+  </si>
+  <si>
+    <t>trx011.photo</t>
+  </si>
+  <si>
+    <t>spesifikasi</t>
+  </si>
+  <si>
+    <t>data diambil dari table temp table api (menyusul)</t>
+  </si>
+  <si>
+    <t>waktu payment isi ke table trx010,trx011</t>
+  </si>
+  <si>
+    <t>trx010</t>
+  </si>
+  <si>
+    <t>order_no</t>
+  </si>
+  <si>
+    <t>generate otomatis tgl+counter</t>
+  </si>
+  <si>
+    <t>oder_yrmo</t>
+  </si>
+  <si>
+    <t>thn bln sysdate</t>
+  </si>
+  <si>
+    <t>order_date</t>
+  </si>
+  <si>
+    <t>sysdate</t>
+  </si>
+  <si>
+    <t>tot_base_value</t>
+  </si>
+  <si>
+    <t>tot_gross_value</t>
+  </si>
+  <si>
+    <t>disc_value</t>
+  </si>
+  <si>
+    <t>tot_dpp_value</t>
+  </si>
+  <si>
+    <t>ppn_value</t>
+  </si>
+  <si>
+    <t>tot_nett_value</t>
+  </si>
+  <si>
+    <t>status_flg</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>dari total trx011.base_value</t>
+  </si>
+  <si>
+    <t>dari total trx011.disc_value</t>
+  </si>
+  <si>
+    <t>dari total trx011.gross_value</t>
+  </si>
+  <si>
+    <t>dari total trx011.ppn_value</t>
+  </si>
+  <si>
+    <t>dari total trx011.tot_value</t>
+  </si>
+  <si>
+    <t>dari total trx011.dpp_value</t>
+  </si>
+  <si>
+    <t>trx011</t>
+  </si>
+  <si>
+    <t>trx011.hotel_name</t>
+  </si>
+  <si>
+    <t>trx011.star</t>
+  </si>
+  <si>
+    <t>base_value</t>
+  </si>
+  <si>
+    <t>gross_value</t>
+  </si>
+  <si>
+    <t>dpp_value</t>
+  </si>
+  <si>
+    <t>dari api</t>
+  </si>
+  <si>
+    <t>gross_value_day * day</t>
+  </si>
+  <si>
+    <t>sementara 0</t>
+  </si>
+  <si>
+    <t>gross_value - disc_value</t>
+  </si>
+  <si>
+    <t>tot_value</t>
+  </si>
+  <si>
+    <t>dpp_value+ppn_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grosss_value_day </t>
+  </si>
+  <si>
+    <t>(10% X base_value)+base_value</t>
+  </si>
+  <si>
+    <t>confirm isi ke table trx012</t>
+  </si>
+  <si>
+    <t>payment_method</t>
+  </si>
+  <si>
+    <t>tergantung check apa</t>
+  </si>
+  <si>
+    <t>Deposit/Transfer/Card</t>
+  </si>
+  <si>
+    <t>tanya jonse mau diisi apa</t>
+  </si>
+  <si>
+    <t>card_type</t>
+  </si>
+  <si>
+    <t>jika car tipe bayarnya maka diisi</t>
+  </si>
+  <si>
+    <t>visa/master, selain tu kosong</t>
+  </si>
+  <si>
+    <t>card_number</t>
+  </si>
+  <si>
+    <t>card_name</t>
+  </si>
+  <si>
+    <t>ccv</t>
+  </si>
+  <si>
+    <t>jika card tipe bayarnya maka diisi</t>
+  </si>
+  <si>
+    <t>jika di check muncul</t>
+  </si>
+  <si>
+    <t>Card Number</t>
+  </si>
+  <si>
+    <t>card Name</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>expired date</t>
   </si>
 </sst>
 </file>
@@ -2928,10 +3162,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AG77"/>
+  <dimension ref="B2:AM80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="AG58" sqref="AG58"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="Q68" sqref="Q68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2939,7 +3173,7 @@
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C2" s="18" t="s">
         <v>53</v>
       </c>
@@ -2969,8 +3203,11 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
       <c r="AC2" s="6"/>
-    </row>
-    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -2998,8 +3235,14 @@
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
       <c r="AC3" s="9"/>
-    </row>
-    <row r="4" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C4" s="7"/>
       <c r="D4" s="18" t="s">
         <v>29</v>
@@ -3029,12 +3272,20 @@
       <c r="AA4" s="8"/>
       <c r="AB4" s="8"/>
       <c r="AC4" s="9"/>
-    </row>
-    <row r="5" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD4">
+        <v>2</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -3059,8 +3310,11 @@
       <c r="AA5" s="8"/>
       <c r="AB5" s="8"/>
       <c r="AC5" s="9"/>
-    </row>
-    <row r="6" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -3074,7 +3328,9 @@
         <v>30</v>
       </c>
       <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
+      <c r="K6" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
@@ -3084,7 +3340,9 @@
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
+      <c r="U6" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="V6" s="8"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
@@ -3093,8 +3351,17 @@
       <c r="AA6" s="8"/>
       <c r="AB6" s="8"/>
       <c r="AC6" s="9"/>
-    </row>
-    <row r="7" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -3123,8 +3390,17 @@
       <c r="AA7" s="8"/>
       <c r="AB7" s="8"/>
       <c r="AC7" s="9"/>
-    </row>
-    <row r="8" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE7" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -3141,7 +3417,9 @@
         <v>42325</v>
       </c>
       <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="L8" s="8" t="s">
+        <v>96</v>
+      </c>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -3159,8 +3437,17 @@
       <c r="AA8" s="8"/>
       <c r="AB8" s="8"/>
       <c r="AC8" s="9"/>
-    </row>
-    <row r="9" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE8" t="s">
+        <v>126</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -3177,7 +3464,9 @@
         <v>42326</v>
       </c>
       <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="L9" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
@@ -3197,8 +3486,17 @@
       <c r="AA9" s="8"/>
       <c r="AB9" s="8"/>
       <c r="AC9" s="9"/>
-    </row>
-    <row r="10" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE9" t="s">
+        <v>128</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -3215,7 +3513,9 @@
         <v>1</v>
       </c>
       <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="L10" s="8" t="s">
+        <v>98</v>
+      </c>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -3233,8 +3533,17 @@
       <c r="AA10" s="8"/>
       <c r="AB10" s="8"/>
       <c r="AC10" s="9"/>
-    </row>
-    <row r="11" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE10" t="s">
+        <v>129</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -3263,8 +3572,17 @@
       <c r="AA11" s="8"/>
       <c r="AB11" s="8"/>
       <c r="AC11" s="9"/>
-    </row>
-    <row r="12" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE11" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -3283,7 +3601,9 @@
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
+      <c r="N12" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
@@ -3299,8 +3619,17 @@
       <c r="AA12" s="8"/>
       <c r="AB12" s="8"/>
       <c r="AC12" s="9"/>
-    </row>
-    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE12" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -3329,8 +3658,17 @@
       <c r="AA13" s="8"/>
       <c r="AB13" s="8"/>
       <c r="AC13" s="9"/>
-    </row>
-    <row r="14" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE13" t="s">
+        <v>132</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -3349,7 +3687,9 @@
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
+      <c r="N14" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
@@ -3365,8 +3705,17 @@
       <c r="AA14" s="8"/>
       <c r="AB14" s="8"/>
       <c r="AC14" s="9"/>
-    </row>
-    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE14" t="s">
+        <v>133</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -3395,8 +3744,17 @@
       <c r="AA15" s="8"/>
       <c r="AB15" s="8"/>
       <c r="AC15" s="9"/>
-    </row>
-    <row r="16" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE15" t="s">
+        <v>134</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B16" s="8"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -3415,7 +3773,9 @@
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
+      <c r="N16" s="8" t="s">
+        <v>101</v>
+      </c>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="8"/>
@@ -3432,7 +3792,7 @@
       <c r="AB16" s="8"/>
       <c r="AC16" s="9"/>
     </row>
-    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -3451,7 +3811,9 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
+      <c r="N17" s="19" t="s">
+        <v>102</v>
+      </c>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
@@ -3467,8 +3829,11 @@
       <c r="AA17" s="8"/>
       <c r="AB17" s="8"/>
       <c r="AC17" s="9"/>
-    </row>
-    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -3487,7 +3852,9 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
+      <c r="N18" s="19" t="s">
+        <v>103</v>
+      </c>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
@@ -3503,8 +3870,17 @@
       <c r="AA18" s="8"/>
       <c r="AB18" s="8"/>
       <c r="AC18" s="9"/>
-    </row>
-    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE18" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
       <c r="C19" s="7"/>
       <c r="D19" s="10"/>
@@ -3533,8 +3909,17 @@
       <c r="AA19" s="8"/>
       <c r="AB19" s="8"/>
       <c r="AC19" s="9"/>
-    </row>
-    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE19" t="s">
+        <v>146</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B20" s="8"/>
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
@@ -3563,8 +3948,17 @@
       <c r="AA20" s="8"/>
       <c r="AB20" s="8"/>
       <c r="AC20" s="9"/>
-    </row>
-    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE20" t="s">
+        <v>130</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>
       <c r="C21" s="7"/>
       <c r="D21" s="18" t="s">
@@ -3595,8 +3989,17 @@
       <c r="AA21" s="8"/>
       <c r="AB21" s="8"/>
       <c r="AC21" s="9"/>
-    </row>
-    <row r="22" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE21" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -3604,7 +4007,9 @@
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
+      <c r="I22" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
@@ -3625,8 +4030,17 @@
       <c r="AA22" s="8"/>
       <c r="AB22" s="8"/>
       <c r="AC22" s="9"/>
-    </row>
-    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE22" t="s">
+        <v>132</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -3636,9 +4050,13 @@
       </c>
       <c r="G23" s="8"/>
       <c r="I23" s="21"/>
-      <c r="J23" s="8"/>
+      <c r="J23" s="8" t="s">
+        <v>83</v>
+      </c>
       <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
+      <c r="L23" s="8" t="s">
+        <v>106</v>
+      </c>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
@@ -3656,8 +4074,17 @@
       <c r="AA23" s="8"/>
       <c r="AB23" s="8"/>
       <c r="AC23" s="9"/>
-    </row>
-    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE23" t="s">
+        <v>152</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -3670,7 +4097,9 @@
       <c r="I24" s="1"/>
       <c r="J24" s="3"/>
       <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
+      <c r="L24" s="8" t="s">
+        <v>104</v>
+      </c>
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
@@ -3688,8 +4117,17 @@
       <c r="AA24" s="8"/>
       <c r="AB24" s="8"/>
       <c r="AC24" s="9"/>
-    </row>
-    <row r="25" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AE24" t="s">
+        <v>154</v>
+      </c>
+      <c r="AJ24" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -3702,7 +4140,9 @@
       <c r="I25" s="1"/>
       <c r="J25" s="3"/>
       <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
+      <c r="L25" s="8" t="s">
+        <v>105</v>
+      </c>
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
@@ -3721,7 +4161,7 @@
       <c r="AB25" s="8"/>
       <c r="AC25" s="9"/>
     </row>
-    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
       <c r="C26" s="7"/>
       <c r="D26" s="10"/>
@@ -3751,7 +4191,7 @@
       <c r="AB26" s="8"/>
       <c r="AC26" s="9"/>
     </row>
-    <row r="27" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
@@ -3781,7 +4221,7 @@
       <c r="AB27" s="8"/>
       <c r="AC27" s="9"/>
     </row>
-    <row r="28" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B28" s="8"/>
       <c r="C28" s="7"/>
       <c r="D28" s="15" t="s">
@@ -3813,7 +4253,7 @@
       <c r="AB28" s="8"/>
       <c r="AC28" s="9"/>
     </row>
-    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B29" s="8"/>
       <c r="C29" s="7"/>
       <c r="D29" s="8"/>
@@ -3843,8 +4283,10 @@
       <c r="AB29" s="8"/>
       <c r="AC29" s="9"/>
     </row>
-    <row r="30" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
+    <row r="30" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>108</v>
+      </c>
       <c r="C30" s="7"/>
       <c r="D30" s="8"/>
       <c r="E30" s="13"/>
@@ -3861,7 +4303,9 @@
       </c>
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
+      <c r="O30" s="8" t="s">
+        <v>111</v>
+      </c>
       <c r="P30" s="8"/>
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
@@ -3877,8 +4321,10 @@
       <c r="AB30" s="8"/>
       <c r="AC30" s="9"/>
     </row>
-    <row r="31" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
+    <row r="31" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>114</v>
+      </c>
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
       <c r="E31" s="13"/>
@@ -3895,7 +4341,9 @@
       </c>
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
+      <c r="O31" s="8" t="s">
+        <v>112</v>
+      </c>
       <c r="P31" s="8"/>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
@@ -3911,8 +4359,10 @@
       <c r="AB31" s="8"/>
       <c r="AC31" s="9"/>
     </row>
-    <row r="32" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
+    <row r="32" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>109</v>
+      </c>
       <c r="C32" s="7"/>
       <c r="D32" s="8"/>
       <c r="E32" s="13"/>
@@ -3932,7 +4382,9 @@
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
       <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
+      <c r="R32" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="S32" s="8"/>
       <c r="T32" s="8"/>
       <c r="U32" s="8"/>
@@ -3982,7 +4434,9 @@
       <c r="C34" s="7"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
+      <c r="F34" s="19" t="s">
+        <v>110</v>
+      </c>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
@@ -4110,7 +4564,9 @@
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
+      <c r="L38" s="8" t="s">
+        <v>115</v>
+      </c>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
       <c r="O38" s="8"/>
@@ -4226,7 +4682,9 @@
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
+      <c r="J42" s="8" t="s">
+        <v>116</v>
+      </c>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
@@ -4425,7 +4883,7 @@
       <c r="AB48" s="8"/>
       <c r="AC48" s="9"/>
     </row>
-    <row r="49" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:39" x14ac:dyDescent="0.25">
       <c r="C49" s="10"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
@@ -4454,7 +4912,7 @@
       <c r="AB49" s="11"/>
       <c r="AC49" s="12"/>
     </row>
-    <row r="51" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B51" s="18" t="s">
         <v>52</v>
       </c>
@@ -4490,7 +4948,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
       <c r="C52" s="15" t="s">
         <v>57</v>
@@ -4529,7 +4987,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B53" s="7"/>
       <c r="C53" s="1"/>
       <c r="D53" s="2"/>
@@ -4575,7 +5033,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="8"/>
@@ -4612,7 +5070,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="8"/>
@@ -4649,7 +5107,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="8"/>
@@ -4686,7 +5144,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="8"/>
@@ -4720,7 +5178,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="8"/>
@@ -4750,8 +5208,14 @@
       <c r="AB58" s="8"/>
       <c r="AC58" s="9"/>
       <c r="AD58" s="9"/>
-    </row>
-    <row r="59" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AF58">
+        <v>5</v>
+      </c>
+      <c r="AG58" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="59" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
       <c r="C59" s="10"/>
       <c r="D59" s="11"/>
@@ -4781,8 +5245,17 @@
       <c r="AB59" s="11"/>
       <c r="AC59" s="12"/>
       <c r="AD59" s="9"/>
-    </row>
-    <row r="60" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AG59" t="s">
+        <v>157</v>
+      </c>
+      <c r="AL59" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM59" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="60" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
@@ -4812,8 +5285,11 @@
       <c r="AB60" s="8"/>
       <c r="AC60" s="8"/>
       <c r="AD60" s="9"/>
-    </row>
-    <row r="61" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AM60" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="61" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
@@ -4843,8 +5319,20 @@
       <c r="AB61" s="8"/>
       <c r="AC61" s="8"/>
       <c r="AD61" s="9"/>
-    </row>
-    <row r="62" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AF61">
+        <v>6</v>
+      </c>
+      <c r="AG61" t="s">
+        <v>161</v>
+      </c>
+      <c r="AJ61" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK61" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B62" s="7"/>
       <c r="C62" s="8" t="s">
         <v>65</v>
@@ -4880,8 +5368,11 @@
       <c r="AB62" s="8"/>
       <c r="AC62" s="8"/>
       <c r="AD62" s="9"/>
-    </row>
-    <row r="63" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AK62" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="63" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
@@ -4911,8 +5402,20 @@
       <c r="AB63" s="8"/>
       <c r="AC63" s="8"/>
       <c r="AD63" s="9"/>
-    </row>
-    <row r="64" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AF63">
+        <v>7</v>
+      </c>
+      <c r="AG63" t="s">
+        <v>164</v>
+      </c>
+      <c r="AK63" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL63" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="64" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B64" s="7"/>
       <c r="C64" s="8"/>
       <c r="D64" s="13"/>
@@ -4947,7 +5450,7 @@
       <c r="AC64" s="8"/>
       <c r="AD64" s="9"/>
     </row>
-    <row r="65" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B65" s="7"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
@@ -4977,8 +5480,20 @@
       <c r="AB65" s="8"/>
       <c r="AC65" s="8"/>
       <c r="AD65" s="9"/>
-    </row>
-    <row r="66" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AF65">
+        <v>8</v>
+      </c>
+      <c r="AG65" t="s">
+        <v>165</v>
+      </c>
+      <c r="AK65" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL65" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="66" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B66" s="7"/>
       <c r="C66" s="8"/>
       <c r="D66" s="13"/>
@@ -5011,7 +5526,7 @@
       <c r="AC66" s="8"/>
       <c r="AD66" s="9"/>
     </row>
-    <row r="67" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B67" s="7"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
@@ -5043,13 +5558,27 @@
       <c r="AB67" s="8"/>
       <c r="AC67" s="8"/>
       <c r="AD67" s="9"/>
-    </row>
-    <row r="68" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AF67">
+        <v>9</v>
+      </c>
+      <c r="AG67" t="s">
+        <v>166</v>
+      </c>
+      <c r="AK67" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL67" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="68" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B68" s="7"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
       <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
+      <c r="F68" s="19" t="s">
+        <v>160</v>
+      </c>
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
@@ -5075,7 +5604,7 @@
       <c r="AC68" s="8"/>
       <c r="AD68" s="9"/>
     </row>
-    <row r="69" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B69" s="7"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
@@ -5106,7 +5635,7 @@
       <c r="AC69" s="8"/>
       <c r="AD69" s="9"/>
     </row>
-    <row r="70" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B70" s="7"/>
       <c r="C70" s="8"/>
       <c r="D70" s="13"/>
@@ -5139,12 +5668,14 @@
       <c r="AC70" s="8"/>
       <c r="AD70" s="9"/>
     </row>
-    <row r="71" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B71" s="7"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
       <c r="E71" s="8"/>
-      <c r="F71" s="8"/>
+      <c r="F71" s="19" t="s">
+        <v>168</v>
+      </c>
       <c r="G71" s="8"/>
       <c r="H71" s="8"/>
       <c r="I71" s="8"/>
@@ -5170,29 +5701,19 @@
       <c r="AC71" s="8"/>
       <c r="AD71" s="9"/>
     </row>
-    <row r="72" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B72" s="7"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
       <c r="E72" s="8"/>
-      <c r="F72" s="8"/>
-      <c r="G72" s="8"/>
-      <c r="H72" s="8"/>
-      <c r="I72" s="8"/>
-      <c r="J72" s="8"/>
-      <c r="K72" s="8"/>
-      <c r="L72" s="8"/>
-      <c r="M72" s="8"/>
-      <c r="N72" s="8"/>
-      <c r="O72" s="8"/>
-      <c r="P72" s="8"/>
-      <c r="Q72" s="8"/>
-      <c r="R72" s="8"/>
-      <c r="S72" s="8"/>
-      <c r="T72" s="8"/>
-      <c r="U72" s="8"/>
-      <c r="V72" s="8"/>
-      <c r="W72" s="8"/>
+      <c r="G72" s="13"/>
+      <c r="H72" t="s">
+        <v>171</v>
+      </c>
+      <c r="K72" s="13"/>
+      <c r="L72" t="s">
+        <v>172</v>
+      </c>
       <c r="X72" s="8"/>
       <c r="Y72" s="8"/>
       <c r="Z72" s="8"/>
@@ -5201,12 +5722,12 @@
       <c r="AC72" s="8"/>
       <c r="AD72" s="9"/>
     </row>
-    <row r="73" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B73" s="7"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
-      <c r="F73" s="8"/>
+      <c r="F73" s="19"/>
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
       <c r="I73" s="8"/>
@@ -5232,31 +5753,33 @@
       <c r="AC73" s="8"/>
       <c r="AD73" s="9"/>
     </row>
-    <row r="74" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B74" s="7"/>
       <c r="C74" s="8"/>
-      <c r="D74" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E74" s="2"/>
-      <c r="F74" s="3"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="19" t="s">
+        <v>169</v>
+      </c>
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
-      <c r="J74" s="8"/>
-      <c r="K74" s="8"/>
-      <c r="L74" s="8"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="3"/>
       <c r="M74" s="8"/>
       <c r="N74" s="8"/>
-      <c r="O74" s="8"/>
+      <c r="O74" s="8" t="s">
+        <v>170</v>
+      </c>
       <c r="P74" s="8"/>
       <c r="Q74" s="8"/>
       <c r="R74" s="8"/>
-      <c r="S74" s="8"/>
-      <c r="T74" s="8"/>
-      <c r="U74" s="8"/>
-      <c r="V74" s="8"/>
-      <c r="W74" s="8"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="2"/>
+      <c r="U74" s="2"/>
+      <c r="V74" s="2"/>
+      <c r="W74" s="3"/>
       <c r="X74" s="8"/>
       <c r="Y74" s="8"/>
       <c r="Z74" s="8"/>
@@ -5265,26 +5788,30 @@
       <c r="AC74" s="8"/>
       <c r="AD74" s="9"/>
     </row>
-    <row r="75" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B75" s="7"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
       <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
+      <c r="F75" s="19" t="s">
+        <v>166</v>
+      </c>
       <c r="G75" s="8"/>
       <c r="H75" s="8"/>
       <c r="I75" s="8"/>
-      <c r="J75" s="8"/>
+      <c r="J75" s="13"/>
       <c r="K75" s="8"/>
       <c r="L75" s="8"/>
       <c r="M75" s="8"/>
       <c r="N75" s="8"/>
-      <c r="O75" s="8"/>
+      <c r="O75" s="8" t="s">
+        <v>173</v>
+      </c>
       <c r="P75" s="8"/>
       <c r="Q75" s="8"/>
       <c r="R75" s="8"/>
-      <c r="S75" s="8"/>
-      <c r="T75" s="8"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="3"/>
       <c r="U75" s="8"/>
       <c r="V75" s="8"/>
       <c r="W75" s="8"/>
@@ -5296,7 +5823,7 @@
       <c r="AC75" s="8"/>
       <c r="AD75" s="9"/>
     </row>
-    <row r="76" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B76" s="7"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
@@ -5327,36 +5854,131 @@
       <c r="AC76" s="8"/>
       <c r="AD76" s="9"/>
     </row>
-    <row r="77" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B77" s="10"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="11"/>
-      <c r="J77" s="11"/>
-      <c r="K77" s="11"/>
-      <c r="L77" s="11"/>
-      <c r="M77" s="11"/>
-      <c r="N77" s="11"/>
-      <c r="O77" s="11"/>
-      <c r="P77" s="11"/>
-      <c r="Q77" s="11"/>
-      <c r="R77" s="11"/>
-      <c r="S77" s="11"/>
-      <c r="T77" s="11"/>
-      <c r="U77" s="11"/>
-      <c r="V77" s="11"/>
-      <c r="W77" s="11"/>
-      <c r="X77" s="11"/>
-      <c r="Y77" s="11"/>
-      <c r="Z77" s="11"/>
-      <c r="AA77" s="11"/>
-      <c r="AB77" s="11"/>
-      <c r="AC77" s="11"/>
-      <c r="AD77" s="12"/>
+    <row r="77" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B77" s="7"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E77" s="2"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
+      <c r="I77" s="8"/>
+      <c r="J77" s="8"/>
+      <c r="K77" s="8"/>
+      <c r="L77" s="8"/>
+      <c r="M77" s="8"/>
+      <c r="N77" s="8"/>
+      <c r="O77" s="8"/>
+      <c r="P77" s="8"/>
+      <c r="Q77" s="8"/>
+      <c r="R77" s="8"/>
+      <c r="S77" s="8"/>
+      <c r="T77" s="8"/>
+      <c r="U77" s="8"/>
+      <c r="V77" s="8"/>
+      <c r="W77" s="8"/>
+      <c r="X77" s="8"/>
+      <c r="Y77" s="8"/>
+      <c r="Z77" s="8"/>
+      <c r="AA77" s="8"/>
+      <c r="AB77" s="8"/>
+      <c r="AC77" s="8"/>
+      <c r="AD77" s="9"/>
+    </row>
+    <row r="78" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B78" s="7"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="8"/>
+      <c r="K78" s="8"/>
+      <c r="L78" s="8"/>
+      <c r="M78" s="8"/>
+      <c r="N78" s="8"/>
+      <c r="O78" s="8"/>
+      <c r="P78" s="8"/>
+      <c r="Q78" s="8"/>
+      <c r="R78" s="8"/>
+      <c r="S78" s="8"/>
+      <c r="T78" s="8"/>
+      <c r="U78" s="8"/>
+      <c r="V78" s="8"/>
+      <c r="W78" s="8"/>
+      <c r="X78" s="8"/>
+      <c r="Y78" s="8"/>
+      <c r="Z78" s="8"/>
+      <c r="AA78" s="8"/>
+      <c r="AB78" s="8"/>
+      <c r="AC78" s="8"/>
+      <c r="AD78" s="9"/>
+    </row>
+    <row r="79" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B79" s="7"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="8"/>
+      <c r="K79" s="8"/>
+      <c r="L79" s="8"/>
+      <c r="M79" s="8"/>
+      <c r="N79" s="8"/>
+      <c r="O79" s="8"/>
+      <c r="P79" s="8"/>
+      <c r="Q79" s="8"/>
+      <c r="R79" s="8"/>
+      <c r="S79" s="8"/>
+      <c r="T79" s="8"/>
+      <c r="U79" s="8"/>
+      <c r="V79" s="8"/>
+      <c r="W79" s="8"/>
+      <c r="X79" s="8"/>
+      <c r="Y79" s="8"/>
+      <c r="Z79" s="8"/>
+      <c r="AA79" s="8"/>
+      <c r="AB79" s="8"/>
+      <c r="AC79" s="8"/>
+      <c r="AD79" s="9"/>
+    </row>
+    <row r="80" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B80" s="10"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="11"/>
+      <c r="J80" s="11"/>
+      <c r="K80" s="11"/>
+      <c r="L80" s="11"/>
+      <c r="M80" s="11"/>
+      <c r="N80" s="11"/>
+      <c r="O80" s="11"/>
+      <c r="P80" s="11"/>
+      <c r="Q80" s="11"/>
+      <c r="R80" s="11"/>
+      <c r="S80" s="11"/>
+      <c r="T80" s="11"/>
+      <c r="U80" s="11"/>
+      <c r="V80" s="11"/>
+      <c r="W80" s="11"/>
+      <c r="X80" s="11"/>
+      <c r="Y80" s="11"/>
+      <c r="Z80" s="11"/>
+      <c r="AA80" s="11"/>
+      <c r="AB80" s="11"/>
+      <c r="AC80" s="11"/>
+      <c r="AD80" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
perubahan pada browse payment
</commit_message>
<xml_diff>
--- a/document/spec.xlsx
+++ b/document/spec.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="7500" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="7500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Agent Register" sheetId="2" r:id="rId1"/>
     <sheet name="Confirmation Payment" sheetId="3" r:id="rId2"/>
     <sheet name="order hotel" sheetId="4" r:id="rId3"/>
+    <sheet name="Cancel Booking" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="176">
   <si>
     <t>Agent Register</t>
   </si>
@@ -276,9 +277,6 @@
     <t>Save</t>
   </si>
   <si>
-    <t>Search dari trx001</t>
-  </si>
-  <si>
     <t>Browse Payment</t>
   </si>
   <si>
@@ -538,6 +536,15 @@
   </si>
   <si>
     <t>expired date</t>
+  </si>
+  <si>
+    <t>Search dari trx001 yang statusnya pending dan cancel</t>
+  </si>
+  <si>
+    <t>Ubah Status payment</t>
+  </si>
+  <si>
+    <t>hanya bisa ubah dari pending or cancel ke done</t>
   </si>
 </sst>
 </file>
@@ -759,7 +766,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -784,6 +791,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1088,7 +1096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AA28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="AB33" sqref="AB33"/>
     </sheetView>
   </sheetViews>
@@ -1894,10 +1902,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AA49"/>
+  <dimension ref="B2:AA50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA34" sqref="AA34"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,7 +2331,7 @@
       <c r="X16" s="8"/>
       <c r="Y16" s="9"/>
     </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -2349,7 +2357,7 @@
       <c r="X17" s="8"/>
       <c r="Y17" s="9"/>
     </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8" t="s">
@@ -2377,7 +2385,7 @@
       <c r="X18" s="8"/>
       <c r="Y18" s="9"/>
     </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2403,7 +2411,7 @@
       <c r="X19" s="8"/>
       <c r="Y19" s="9"/>
     </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
@@ -2431,7 +2439,7 @@
       <c r="X20" s="8"/>
       <c r="Y20" s="9"/>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2457,7 +2465,7 @@
       <c r="X21" s="8"/>
       <c r="Y21" s="9"/>
     </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
@@ -2485,7 +2493,7 @@
       <c r="X22" s="8"/>
       <c r="Y22" s="9"/>
     </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2511,7 +2519,7 @@
       <c r="X23" s="8"/>
       <c r="Y23" s="9"/>
     </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -2537,7 +2545,7 @@
       <c r="X24" s="8"/>
       <c r="Y24" s="9"/>
     </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -2563,7 +2571,7 @@
       <c r="X25" s="8"/>
       <c r="Y25" s="9"/>
     </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
       <c r="D26" s="4"/>
@@ -2589,7 +2597,7 @@
       <c r="X26" s="8"/>
       <c r="Y26" s="9"/>
     </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
       <c r="D27" s="17" t="s">
@@ -2617,7 +2625,7 @@
       <c r="X27" s="8"/>
       <c r="Y27" s="9"/>
     </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
       <c r="D28" s="10"/>
@@ -2643,7 +2651,7 @@
       <c r="X28" s="8"/>
       <c r="Y28" s="9"/>
     </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
@@ -2669,79 +2677,54 @@
       <c r="X29" s="11"/>
       <c r="Y29" s="12"/>
     </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B32" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
-      <c r="W32" s="5"/>
-      <c r="X32" s="6"/>
-      <c r="AA32" t="s">
+    <row r="32" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B32" s="24" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B33" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="6"/>
+      <c r="AA33" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="9"/>
-      <c r="AA33" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="34" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
-      <c r="D34" s="8" t="s">
-        <v>75</v>
-      </c>
+      <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="3"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
       <c r="N34" s="8"/>
       <c r="O34" s="8"/>
       <c r="P34" s="8"/>
@@ -2754,22 +2737,24 @@
       <c r="W34" s="8"/>
       <c r="X34" s="9"/>
       <c r="AA34" t="s">
-        <v>88</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
+      <c r="D35" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="3"/>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
@@ -2781,55 +2766,61 @@
       <c r="V35" s="8"/>
       <c r="W35" s="8"/>
       <c r="X35" s="9"/>
+      <c r="AA35" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="36" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="O36" s="1"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="3"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
       <c r="T36" s="8"/>
       <c r="U36" s="8"/>
       <c r="V36" s="8"/>
       <c r="W36" s="8"/>
       <c r="X36" s="9"/>
+      <c r="AA36" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="37" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
+      <c r="D37" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="O37" s="1"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="3"/>
       <c r="T37" s="8"/>
       <c r="U37" s="8"/>
       <c r="V37" s="8"/>
@@ -2839,10 +2830,8 @@
     <row r="38" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="E38" s="3"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
@@ -2866,8 +2855,10 @@
     <row r="39" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
+      <c r="D39" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="3"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
@@ -2890,98 +2881,96 @@
     </row>
     <row r="40" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="K40" s="5"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="6"/>
-      <c r="T40" s="4"/>
-      <c r="U40" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="V40" s="5"/>
-      <c r="W40" s="6"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
+      <c r="V40" s="8"/>
+      <c r="W40" s="8"/>
       <c r="X40" s="9"/>
     </row>
     <row r="41" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="H41" s="11"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="12"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="12"/>
-      <c r="T41" s="10"/>
-      <c r="U41" s="11"/>
-      <c r="V41" s="11"/>
-      <c r="W41" s="12"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="K41" s="5"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="V41" s="5"/>
+      <c r="W41" s="6"/>
       <c r="X41" s="9"/>
     </row>
     <row r="42" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
-      <c r="C42" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="8"/>
-      <c r="S42" s="9"/>
-      <c r="T42" s="7"/>
-      <c r="U42" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="V42" s="3"/>
-      <c r="W42" s="9"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H42" s="11"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="12"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="11"/>
+      <c r="V42" s="11"/>
+      <c r="W42" s="12"/>
       <c r="X42" s="9"/>
     </row>
     <row r="43" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
-      <c r="C43" s="22"/>
+      <c r="C43" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="D43" s="7"/>
       <c r="E43" s="8"/>
       <c r="F43" s="9"/>
@@ -2999,8 +2988,10 @@
       <c r="R43" s="8"/>
       <c r="S43" s="9"/>
       <c r="T43" s="7"/>
-      <c r="U43" s="8"/>
-      <c r="V43" s="8"/>
+      <c r="U43" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V43" s="3"/>
       <c r="W43" s="9"/>
       <c r="X43" s="9"/>
     </row>
@@ -3056,52 +3047,52 @@
     </row>
     <row r="46" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B46" s="7"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="11"/>
-      <c r="L46" s="12"/>
-      <c r="M46" s="10"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="11"/>
-      <c r="S46" s="12"/>
-      <c r="T46" s="10"/>
-      <c r="U46" s="11"/>
-      <c r="V46" s="11"/>
-      <c r="W46" s="12"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="9"/>
+      <c r="T46" s="7"/>
+      <c r="U46" s="8"/>
+      <c r="V46" s="8"/>
+      <c r="W46" s="9"/>
       <c r="X46" s="9"/>
     </row>
     <row r="47" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B47" s="7"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="8"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="8"/>
-      <c r="Q47" s="8"/>
-      <c r="R47" s="8"/>
-      <c r="S47" s="8"/>
-      <c r="T47" s="8"/>
-      <c r="U47" s="8"/>
-      <c r="V47" s="8"/>
-      <c r="W47" s="8"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="10"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="12"/>
+      <c r="T47" s="10"/>
+      <c r="U47" s="11"/>
+      <c r="V47" s="11"/>
+      <c r="W47" s="12"/>
       <c r="X47" s="9"/>
     </row>
     <row r="48" spans="2:27" x14ac:dyDescent="0.25">
@@ -3130,29 +3121,54 @@
       <c r="X48" s="9"/>
     </row>
     <row r="49" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B49" s="10"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-      <c r="S49" s="11"/>
-      <c r="T49" s="11"/>
-      <c r="U49" s="11"/>
-      <c r="V49" s="11"/>
-      <c r="W49" s="11"/>
-      <c r="X49" s="12"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="8"/>
+      <c r="S49" s="8"/>
+      <c r="T49" s="8"/>
+      <c r="U49" s="8"/>
+      <c r="V49" s="8"/>
+      <c r="W49" s="8"/>
+      <c r="X49" s="9"/>
+    </row>
+    <row r="50" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B50" s="10"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="T50" s="11"/>
+      <c r="U50" s="11"/>
+      <c r="V50" s="11"/>
+      <c r="W50" s="11"/>
+      <c r="X50" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3164,8 +3180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AM80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="Q68" sqref="Q68"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3204,7 +3220,7 @@
       <c r="AB2" s="5"/>
       <c r="AC2" s="6"/>
       <c r="AD2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="2:36" x14ac:dyDescent="0.25">
@@ -3239,7 +3255,7 @@
         <v>1</v>
       </c>
       <c r="AE3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="2:36" x14ac:dyDescent="0.25">
@@ -3276,7 +3292,7 @@
         <v>2</v>
       </c>
       <c r="AE4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="2:36" x14ac:dyDescent="0.25">
@@ -3284,7 +3300,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -3311,7 +3327,7 @@
       <c r="AB5" s="8"/>
       <c r="AC5" s="9"/>
       <c r="AE5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="2:36" x14ac:dyDescent="0.25">
@@ -3329,7 +3345,7 @@
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
@@ -3341,7 +3357,7 @@
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V6" s="8"/>
       <c r="W6" s="8"/>
@@ -3352,13 +3368,13 @@
       <c r="AB6" s="8"/>
       <c r="AC6" s="9"/>
       <c r="AE6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AI6" t="s">
         <v>35</v>
       </c>
       <c r="AJ6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="2:36" x14ac:dyDescent="0.25">
@@ -3391,13 +3407,13 @@
       <c r="AB7" s="8"/>
       <c r="AC7" s="9"/>
       <c r="AE7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AI7" t="s">
         <v>35</v>
       </c>
       <c r="AJ7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="2:36" x14ac:dyDescent="0.25">
@@ -3418,7 +3434,7 @@
       </c>
       <c r="K8" s="8"/>
       <c r="L8" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
@@ -3438,13 +3454,13 @@
       <c r="AB8" s="8"/>
       <c r="AC8" s="9"/>
       <c r="AE8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI8" t="s">
         <v>35</v>
       </c>
       <c r="AJ8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="2:36" x14ac:dyDescent="0.25">
@@ -3465,7 +3481,7 @@
       </c>
       <c r="K9" s="8"/>
       <c r="L9" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
@@ -3487,13 +3503,13 @@
       <c r="AB9" s="8"/>
       <c r="AC9" s="9"/>
       <c r="AE9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AI9" t="s">
         <v>35</v>
       </c>
       <c r="AJ9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="2:36" x14ac:dyDescent="0.25">
@@ -3514,7 +3530,7 @@
       </c>
       <c r="K10" s="8"/>
       <c r="L10" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
@@ -3534,13 +3550,13 @@
       <c r="AB10" s="8"/>
       <c r="AC10" s="9"/>
       <c r="AE10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AI10" t="s">
         <v>35</v>
       </c>
       <c r="AJ10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="2:36" x14ac:dyDescent="0.25">
@@ -3573,13 +3589,13 @@
       <c r="AB11" s="8"/>
       <c r="AC11" s="9"/>
       <c r="AE11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AI11" t="s">
         <v>35</v>
       </c>
       <c r="AJ11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="2:36" x14ac:dyDescent="0.25">
@@ -3602,7 +3618,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
@@ -3620,13 +3636,13 @@
       <c r="AB12" s="8"/>
       <c r="AC12" s="9"/>
       <c r="AE12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI12" t="s">
         <v>35</v>
       </c>
       <c r="AJ12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="2:36" x14ac:dyDescent="0.25">
@@ -3659,13 +3675,13 @@
       <c r="AB13" s="8"/>
       <c r="AC13" s="9"/>
       <c r="AE13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AI13" t="s">
         <v>35</v>
       </c>
       <c r="AJ13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="2:36" x14ac:dyDescent="0.25">
@@ -3688,7 +3704,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
@@ -3706,13 +3722,13 @@
       <c r="AB14" s="8"/>
       <c r="AC14" s="9"/>
       <c r="AE14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AI14" t="s">
         <v>35</v>
       </c>
       <c r="AJ14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="2:36" x14ac:dyDescent="0.25">
@@ -3745,13 +3761,13 @@
       <c r="AB15" s="8"/>
       <c r="AC15" s="9"/>
       <c r="AE15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AI15" t="s">
         <v>35</v>
       </c>
       <c r="AJ15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="2:36" x14ac:dyDescent="0.25">
@@ -3774,7 +3790,7 @@
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
@@ -3812,7 +3828,7 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
@@ -3830,7 +3846,7 @@
       <c r="AB17" s="8"/>
       <c r="AC17" s="9"/>
       <c r="AE17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="2:37" x14ac:dyDescent="0.25">
@@ -3853,7 +3869,7 @@
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -3871,13 +3887,13 @@
       <c r="AB18" s="8"/>
       <c r="AC18" s="9"/>
       <c r="AE18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AH18" t="s">
         <v>35</v>
       </c>
       <c r="AI18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="2:37" x14ac:dyDescent="0.25">
@@ -3910,13 +3926,13 @@
       <c r="AB19" s="8"/>
       <c r="AC19" s="9"/>
       <c r="AE19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AH19" t="s">
         <v>35</v>
       </c>
       <c r="AI19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="2:37" x14ac:dyDescent="0.25">
@@ -3949,13 +3965,13 @@
       <c r="AB20" s="8"/>
       <c r="AC20" s="9"/>
       <c r="AE20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AH20" t="s">
         <v>35</v>
       </c>
       <c r="AI20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="2:37" x14ac:dyDescent="0.25">
@@ -3990,13 +4006,13 @@
       <c r="AB21" s="8"/>
       <c r="AC21" s="9"/>
       <c r="AE21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AH21" t="s">
         <v>35</v>
       </c>
       <c r="AI21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="2:37" x14ac:dyDescent="0.25">
@@ -4008,7 +4024,7 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -4031,13 +4047,13 @@
       <c r="AB22" s="8"/>
       <c r="AC22" s="9"/>
       <c r="AE22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AH22" t="s">
         <v>35</v>
       </c>
       <c r="AI22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="2:37" x14ac:dyDescent="0.25">
@@ -4055,7 +4071,7 @@
       </c>
       <c r="K23" s="8"/>
       <c r="L23" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
@@ -4075,13 +4091,13 @@
       <c r="AB23" s="8"/>
       <c r="AC23" s="9"/>
       <c r="AE23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AH23" t="s">
         <v>35</v>
       </c>
       <c r="AI23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="2:37" x14ac:dyDescent="0.25">
@@ -4098,7 +4114,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
@@ -4118,13 +4134,13 @@
       <c r="AB24" s="8"/>
       <c r="AC24" s="9"/>
       <c r="AE24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AJ24" t="s">
         <v>35</v>
       </c>
       <c r="AK24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="2:37" x14ac:dyDescent="0.25">
@@ -4141,7 +4157,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
@@ -4285,7 +4301,7 @@
     </row>
     <row r="30" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="8"/>
@@ -4304,7 +4320,7 @@
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
       <c r="O30" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P30" s="8"/>
       <c r="Q30" s="8"/>
@@ -4323,7 +4339,7 @@
     </row>
     <row r="31" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
@@ -4342,7 +4358,7 @@
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
       <c r="O31" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P31" s="8"/>
       <c r="Q31" s="8"/>
@@ -4361,7 +4377,7 @@
     </row>
     <row r="32" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="8"/>
@@ -4383,7 +4399,7 @@
       <c r="P32" s="8"/>
       <c r="Q32" s="8"/>
       <c r="R32" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S32" s="8"/>
       <c r="T32" s="8"/>
@@ -4435,7 +4451,7 @@
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
@@ -4565,7 +4581,7 @@
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
@@ -4683,7 +4699,7 @@
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
       <c r="J42" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
@@ -4945,7 +4961,7 @@
       <c r="AC51" s="5"/>
       <c r="AD51" s="6"/>
       <c r="AF51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="2:39" x14ac:dyDescent="0.25">
@@ -4984,7 +5000,7 @@
         <v>1</v>
       </c>
       <c r="AG52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="2:39" x14ac:dyDescent="0.25">
@@ -5030,7 +5046,7 @@
       <c r="AC53" s="3"/>
       <c r="AD53" s="9"/>
       <c r="AG53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="2:39" x14ac:dyDescent="0.25">
@@ -5067,7 +5083,7 @@
         <v>2</v>
       </c>
       <c r="AG54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="2:39" x14ac:dyDescent="0.25">
@@ -5104,7 +5120,7 @@
         <v>3</v>
       </c>
       <c r="AG55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="2:39" x14ac:dyDescent="0.25">
@@ -5141,7 +5157,7 @@
         <v>4</v>
       </c>
       <c r="AG56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="2:39" x14ac:dyDescent="0.25">
@@ -5175,7 +5191,7 @@
       <c r="AC57" s="9"/>
       <c r="AD57" s="9"/>
       <c r="AG57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="2:39" x14ac:dyDescent="0.25">
@@ -5212,7 +5228,7 @@
         <v>5</v>
       </c>
       <c r="AG58" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="2:39" x14ac:dyDescent="0.25">
@@ -5246,13 +5262,13 @@
       <c r="AC59" s="12"/>
       <c r="AD59" s="9"/>
       <c r="AG59" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AL59" t="s">
         <v>35</v>
       </c>
       <c r="AM59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="2:39" x14ac:dyDescent="0.25">
@@ -5286,7 +5302,7 @@
       <c r="AC60" s="8"/>
       <c r="AD60" s="9"/>
       <c r="AM60" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="2:39" x14ac:dyDescent="0.25">
@@ -5323,13 +5339,13 @@
         <v>6</v>
       </c>
       <c r="AG61" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AJ61" t="s">
         <v>35</v>
       </c>
       <c r="AK61" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="2:39" x14ac:dyDescent="0.25">
@@ -5369,7 +5385,7 @@
       <c r="AC62" s="8"/>
       <c r="AD62" s="9"/>
       <c r="AK62" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="63" spans="2:39" x14ac:dyDescent="0.25">
@@ -5406,13 +5422,13 @@
         <v>7</v>
       </c>
       <c r="AG63" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AK63" t="s">
         <v>35</v>
       </c>
       <c r="AL63" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="2:39" x14ac:dyDescent="0.25">
@@ -5484,13 +5500,13 @@
         <v>8</v>
       </c>
       <c r="AG65" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AK65" t="s">
         <v>35</v>
       </c>
       <c r="AL65" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="2:38" x14ac:dyDescent="0.25">
@@ -5562,13 +5578,13 @@
         <v>9</v>
       </c>
       <c r="AG67" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AK67" t="s">
         <v>35</v>
       </c>
       <c r="AL67" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="2:38" x14ac:dyDescent="0.25">
@@ -5577,7 +5593,7 @@
       <c r="D68" s="8"/>
       <c r="E68" s="8"/>
       <c r="F68" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
@@ -5674,7 +5690,7 @@
       <c r="D71" s="8"/>
       <c r="E71" s="8"/>
       <c r="F71" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G71" s="8"/>
       <c r="H71" s="8"/>
@@ -5708,11 +5724,11 @@
       <c r="E72" s="8"/>
       <c r="G72" s="13"/>
       <c r="H72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K72" s="13"/>
       <c r="L72" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X72" s="8"/>
       <c r="Y72" s="8"/>
@@ -5759,7 +5775,7 @@
       <c r="D74" s="8"/>
       <c r="E74" s="8"/>
       <c r="F74" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
@@ -5770,7 +5786,7 @@
       <c r="M74" s="8"/>
       <c r="N74" s="8"/>
       <c r="O74" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P74" s="8"/>
       <c r="Q74" s="8"/>
@@ -5794,7 +5810,7 @@
       <c r="D75" s="8"/>
       <c r="E75" s="8"/>
       <c r="F75" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G75" s="8"/>
       <c r="H75" s="8"/>
@@ -5805,7 +5821,7 @@
       <c r="M75" s="8"/>
       <c r="N75" s="8"/>
       <c r="O75" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P75" s="8"/>
       <c r="Q75" s="8"/>
@@ -5983,4 +5999,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
penambahan master kamar hotel
</commit_message>
<xml_diff>
--- a/document/spec.xlsx
+++ b/document/spec.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="291">
   <si>
     <t>Agent Register</t>
   </si>
@@ -711,6 +711,186 @@
   </si>
   <si>
     <t>market = all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotel Name </t>
+  </si>
+  <si>
+    <t>Periode</t>
+  </si>
+  <si>
+    <t>S/d</t>
+  </si>
+  <si>
+    <t>Periode*</t>
+  </si>
+  <si>
+    <t>Room Name*</t>
+  </si>
+  <si>
+    <t>Number Adults*</t>
+  </si>
+  <si>
+    <t>Number Children*</t>
+  </si>
+  <si>
+    <t>Daily Price</t>
+  </si>
+  <si>
+    <t>Daily Price*</t>
+  </si>
+  <si>
+    <t>Rp</t>
+  </si>
+  <si>
+    <t>Bed Type*</t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
+    <t>queen/king/</t>
+  </si>
+  <si>
+    <t>Internet Fee</t>
+  </si>
+  <si>
+    <t>enable jika internet = yes</t>
+  </si>
+  <si>
+    <t>cut off</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Allotment</t>
+  </si>
+  <si>
+    <t>Breakfast</t>
+  </si>
+  <si>
+    <t>pax</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>nett/commision</t>
+  </si>
+  <si>
+    <t>jika type =  commision maka ini baru</t>
+  </si>
+  <si>
+    <t>Type Commision</t>
+  </si>
+  <si>
+    <t>%/value</t>
+  </si>
+  <si>
+    <t>% commision</t>
+  </si>
+  <si>
+    <t>Commision Value</t>
+  </si>
+  <si>
+    <t>kalau tipe komisi =% baru visible</t>
+  </si>
+  <si>
+    <t>visible</t>
+  </si>
+  <si>
+    <t>kalau tipe komisi &lt;&gt;% baru visible</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>Detail Room Type</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Room Name</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Browse</t>
+  </si>
+  <si>
+    <t>Foto setelah di upload</t>
+  </si>
+  <si>
+    <t>MST022</t>
+  </si>
+  <si>
+    <t>from_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>room_name</t>
+  </si>
+  <si>
+    <t>num_adults</t>
+  </si>
+  <si>
+    <t>num_child</t>
+  </si>
+  <si>
+    <t>num_breakfast</t>
+  </si>
+  <si>
+    <t>cut_off</t>
+  </si>
+  <si>
+    <t>allotment</t>
+  </si>
+  <si>
+    <t>net_fee</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>room_desc</t>
+  </si>
+  <si>
+    <t>bet_type</t>
+  </si>
+  <si>
+    <t>net</t>
+  </si>
+  <si>
+    <t>rate_type</t>
+  </si>
+  <si>
+    <t>daily_price</t>
+  </si>
+  <si>
+    <t>comm_pct</t>
+  </si>
+  <si>
+    <t>comm_value</t>
+  </si>
+  <si>
+    <t>comm_type</t>
   </si>
 </sst>
 </file>
@@ -940,7 +1120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -972,6 +1152,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8584,10 +8767,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AB57"/>
+  <dimension ref="B2:BC99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" topLeftCell="F75" workbookViewId="0">
+      <selection activeCell="AR87" sqref="AR87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9871,7 +10054,7 @@
       <c r="AA48" s="8"/>
       <c r="AB48" s="9"/>
     </row>
-    <row r="49" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
       <c r="C49" s="8"/>
       <c r="D49" s="1"/>
@@ -9902,7 +10085,7 @@
       <c r="AA49" s="8"/>
       <c r="AB49" s="9"/>
     </row>
-    <row r="50" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
@@ -9931,7 +10114,7 @@
       <c r="AA50" s="8"/>
       <c r="AB50" s="9"/>
     </row>
-    <row r="51" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B51" s="7"/>
       <c r="C51" s="8"/>
       <c r="D51" s="14" t="s">
@@ -9962,7 +10145,7 @@
       <c r="AA51" s="8"/>
       <c r="AB51" s="9"/>
     </row>
-    <row r="52" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -9991,7 +10174,7 @@
       <c r="AA52" s="8"/>
       <c r="AB52" s="9"/>
     </row>
-    <row r="53" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B53" s="7"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
@@ -10020,7 +10203,7 @@
       <c r="AA53" s="8"/>
       <c r="AB53" s="9"/>
     </row>
-    <row r="54" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B54" s="10"/>
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
@@ -10049,7 +10232,63 @@
       <c r="AA54" s="11"/>
       <c r="AB54" s="12"/>
     </row>
-    <row r="57" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="AE55" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="AF55" s="5"/>
+      <c r="AG55" s="5"/>
+      <c r="AH55" s="5"/>
+      <c r="AI55" s="5"/>
+      <c r="AJ55" s="5"/>
+      <c r="AK55" s="5"/>
+      <c r="AL55" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="AM55" s="5"/>
+      <c r="AN55" s="5"/>
+      <c r="AO55" s="5"/>
+      <c r="AP55" s="5"/>
+      <c r="AQ55" s="5"/>
+      <c r="AR55" s="5"/>
+      <c r="AS55" s="5"/>
+      <c r="AT55" s="5"/>
+      <c r="AU55" s="5"/>
+      <c r="AV55" s="5"/>
+      <c r="AW55" s="5"/>
+      <c r="AX55" s="5"/>
+      <c r="AY55" s="5"/>
+      <c r="AZ55" s="5"/>
+      <c r="BA55" s="5"/>
+      <c r="BB55" s="6"/>
+    </row>
+    <row r="56" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="AE56" s="7"/>
+      <c r="AF56" s="8"/>
+      <c r="AG56" s="8"/>
+      <c r="AH56" s="8"/>
+      <c r="AI56" s="8"/>
+      <c r="AJ56" s="8"/>
+      <c r="AK56" s="8"/>
+      <c r="AL56" s="8"/>
+      <c r="AM56" s="8"/>
+      <c r="AN56" s="8"/>
+      <c r="AO56" s="8"/>
+      <c r="AP56" s="8"/>
+      <c r="AQ56" s="8"/>
+      <c r="AR56" s="8"/>
+      <c r="AS56" s="8"/>
+      <c r="AT56" s="4"/>
+      <c r="AU56" s="5"/>
+      <c r="AV56" s="5"/>
+      <c r="AW56" s="5"/>
+      <c r="AX56" s="6"/>
+      <c r="AY56" s="8"/>
+      <c r="AZ56" s="8"/>
+      <c r="BA56" s="8"/>
+      <c r="BB56" s="9"/>
+    </row>
+    <row r="57" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="28" t="s">
         <v>204</v>
@@ -10083,8 +10322,2406 @@
       <c r="Z57" s="5"/>
       <c r="AA57" s="5"/>
       <c r="AB57" s="6"/>
+      <c r="AE57" s="7"/>
+      <c r="AF57" s="8"/>
+      <c r="AG57" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="AH57" s="2"/>
+      <c r="AI57" s="2"/>
+      <c r="AJ57" s="2"/>
+      <c r="AK57" s="3"/>
+      <c r="AL57" s="8"/>
+      <c r="AM57" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="AN57" s="8"/>
+      <c r="AO57" s="8"/>
+      <c r="AP57" s="8"/>
+      <c r="AQ57" s="8"/>
+      <c r="AR57" s="8"/>
+      <c r="AS57" s="8"/>
+      <c r="AT57" s="7"/>
+      <c r="AU57" s="8"/>
+      <c r="AV57" s="8"/>
+      <c r="AW57" s="8"/>
+      <c r="AX57" s="9"/>
+      <c r="AY57" s="8"/>
+      <c r="AZ57" s="8"/>
+      <c r="BA57" s="8"/>
+      <c r="BB57" s="9"/>
+    </row>
+    <row r="58" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B58" s="7"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="8"/>
+      <c r="Q58" s="8"/>
+      <c r="R58" s="8"/>
+      <c r="S58" s="8"/>
+      <c r="T58" s="8"/>
+      <c r="U58" s="8"/>
+      <c r="V58" s="8"/>
+      <c r="W58" s="8"/>
+      <c r="X58" s="8"/>
+      <c r="Y58" s="8"/>
+      <c r="Z58" s="8"/>
+      <c r="AA58" s="8"/>
+      <c r="AB58" s="9"/>
+      <c r="AE58" s="7"/>
+      <c r="AF58" s="8"/>
+      <c r="AG58" s="8"/>
+      <c r="AH58" s="8"/>
+      <c r="AI58" s="8"/>
+      <c r="AJ58" s="8"/>
+      <c r="AK58" s="8"/>
+      <c r="AL58" s="8"/>
+      <c r="AM58" s="8"/>
+      <c r="AN58" s="8"/>
+      <c r="AO58" s="8"/>
+      <c r="AP58" s="8"/>
+      <c r="AQ58" s="8"/>
+      <c r="AR58" s="8"/>
+      <c r="AS58" s="8"/>
+      <c r="AT58" s="7"/>
+      <c r="AU58" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="AV58" s="8"/>
+      <c r="AW58" s="8"/>
+      <c r="AX58" s="9"/>
+      <c r="AY58" s="8"/>
+      <c r="AZ58" s="8"/>
+      <c r="BA58" s="8"/>
+      <c r="BB58" s="9"/>
+    </row>
+    <row r="59" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B59" s="7"/>
+      <c r="C59" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
+      <c r="K59" s="8"/>
+      <c r="L59" s="8"/>
+      <c r="M59" s="8"/>
+      <c r="N59" s="8"/>
+      <c r="O59" s="8"/>
+      <c r="P59" s="8"/>
+      <c r="Q59" s="8"/>
+      <c r="R59" s="8"/>
+      <c r="S59" s="8"/>
+      <c r="T59" s="8"/>
+      <c r="U59" s="8"/>
+      <c r="V59" s="8"/>
+      <c r="W59" s="8"/>
+      <c r="X59" s="8"/>
+      <c r="Y59" s="8"/>
+      <c r="Z59" s="8"/>
+      <c r="AA59" s="8"/>
+      <c r="AB59" s="9"/>
+      <c r="AE59" s="7"/>
+      <c r="AF59" s="8"/>
+      <c r="AG59" s="8"/>
+      <c r="AH59" s="8"/>
+      <c r="AI59" s="8"/>
+      <c r="AJ59" s="8"/>
+      <c r="AK59" s="8"/>
+      <c r="AL59" s="8"/>
+      <c r="AM59" s="8"/>
+      <c r="AN59" s="8"/>
+      <c r="AO59" s="8"/>
+      <c r="AP59" s="8"/>
+      <c r="AQ59" s="8"/>
+      <c r="AR59" s="8"/>
+      <c r="AS59" s="8"/>
+      <c r="AT59" s="7"/>
+      <c r="AU59" s="8"/>
+      <c r="AV59" s="8"/>
+      <c r="AW59" s="8"/>
+      <c r="AX59" s="9"/>
+      <c r="AY59" s="8"/>
+      <c r="AZ59" s="8"/>
+      <c r="BA59" s="8"/>
+      <c r="BB59" s="9"/>
+      <c r="BC59" s="8"/>
+    </row>
+    <row r="60" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B60" s="7"/>
+      <c r="C60" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E60" s="3"/>
+      <c r="F60" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="K60" s="2"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="8"/>
+      <c r="S60" s="8"/>
+      <c r="T60" s="8"/>
+      <c r="U60" s="8"/>
+      <c r="V60" s="8"/>
+      <c r="W60" s="8"/>
+      <c r="X60" s="8"/>
+      <c r="Y60" s="8"/>
+      <c r="Z60" s="8"/>
+      <c r="AA60" s="8"/>
+      <c r="AB60" s="9"/>
+      <c r="AE60" s="7"/>
+      <c r="AF60" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="AG60" s="8"/>
+      <c r="AH60" s="8"/>
+      <c r="AI60" s="8"/>
+      <c r="AJ60" s="8"/>
+      <c r="AK60" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AL60" s="2"/>
+      <c r="AM60" s="2"/>
+      <c r="AN60" s="2"/>
+      <c r="AO60" s="2"/>
+      <c r="AP60" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ60" s="8"/>
+      <c r="AR60" s="8"/>
+      <c r="AS60" s="8"/>
+      <c r="AT60" s="10"/>
+      <c r="AU60" s="11"/>
+      <c r="AV60" s="11"/>
+      <c r="AW60" s="11"/>
+      <c r="AX60" s="12"/>
+      <c r="AY60" s="8"/>
+      <c r="AZ60" s="8"/>
+      <c r="BA60" s="8"/>
+      <c r="BB60" s="9"/>
+      <c r="BC60" s="8"/>
+    </row>
+    <row r="61" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B61" s="7"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="9"/>
+      <c r="M61" s="8"/>
+      <c r="N61" s="8"/>
+      <c r="O61" s="8"/>
+      <c r="P61" s="8"/>
+      <c r="Q61" s="9"/>
+      <c r="R61" s="8"/>
+      <c r="S61" s="8"/>
+      <c r="T61" s="8"/>
+      <c r="U61" s="8"/>
+      <c r="V61" s="8"/>
+      <c r="W61" s="8"/>
+      <c r="X61" s="8"/>
+      <c r="Y61" s="8"/>
+      <c r="Z61" s="8"/>
+      <c r="AA61" s="8"/>
+      <c r="AB61" s="9"/>
+      <c r="AE61" s="7"/>
+      <c r="AF61" s="8"/>
+      <c r="AG61" s="8"/>
+      <c r="AH61" s="8"/>
+      <c r="AI61" s="8"/>
+      <c r="AJ61" s="8"/>
+      <c r="AK61" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="AL61" s="8"/>
+      <c r="AM61" s="8"/>
+      <c r="AN61" s="8"/>
+      <c r="AO61" s="8"/>
+      <c r="AP61" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="AQ61" s="8"/>
+      <c r="AR61" s="8"/>
+      <c r="AS61" s="8"/>
+      <c r="AT61" s="8"/>
+      <c r="AU61" s="8"/>
+      <c r="AV61" s="8"/>
+      <c r="AW61" s="8"/>
+      <c r="AX61" s="8"/>
+      <c r="AY61" s="8"/>
+      <c r="AZ61" s="8"/>
+      <c r="BA61" s="8"/>
+      <c r="BB61" s="9"/>
+      <c r="BC61" s="8"/>
+    </row>
+    <row r="62" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B62" s="7"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="7"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="9"/>
+      <c r="M62" s="8"/>
+      <c r="N62" s="8"/>
+      <c r="O62" s="8"/>
+      <c r="P62" s="8"/>
+      <c r="Q62" s="9"/>
+      <c r="R62" s="8"/>
+      <c r="S62" s="8"/>
+      <c r="T62" s="8"/>
+      <c r="U62" s="8"/>
+      <c r="V62" s="8"/>
+      <c r="W62" s="8"/>
+      <c r="X62" s="8"/>
+      <c r="Y62" s="8"/>
+      <c r="Z62" s="8"/>
+      <c r="AA62" s="8"/>
+      <c r="AB62" s="9"/>
+      <c r="AE62" s="7"/>
+      <c r="AF62" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG62" s="8"/>
+      <c r="AH62" s="8"/>
+      <c r="AI62" s="8"/>
+      <c r="AJ62" s="8"/>
+      <c r="AK62" s="1"/>
+      <c r="AL62" s="13"/>
+      <c r="AM62" s="1"/>
+      <c r="AN62" s="3"/>
+      <c r="AO62" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="AP62" s="1"/>
+      <c r="AQ62" s="13"/>
+      <c r="AR62" s="1"/>
+      <c r="AS62" s="3"/>
+      <c r="AT62" s="8"/>
+      <c r="AU62" s="8"/>
+      <c r="AV62" s="8"/>
+      <c r="AW62" s="8"/>
+      <c r="AX62" s="8"/>
+      <c r="AY62" s="8"/>
+      <c r="AZ62" s="8"/>
+      <c r="BA62" s="8"/>
+      <c r="BB62" s="9"/>
+      <c r="BC62" s="8"/>
+    </row>
+    <row r="63" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B63" s="7"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="8"/>
+      <c r="L63" s="9"/>
+      <c r="M63" s="8"/>
+      <c r="N63" s="8"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="9"/>
+      <c r="R63" s="8"/>
+      <c r="S63" s="8"/>
+      <c r="T63" s="8"/>
+      <c r="U63" s="8"/>
+      <c r="V63" s="8"/>
+      <c r="W63" s="8"/>
+      <c r="X63" s="8"/>
+      <c r="Y63" s="8"/>
+      <c r="Z63" s="8"/>
+      <c r="AA63" s="8"/>
+      <c r="AB63" s="9"/>
+      <c r="AE63" s="7"/>
+      <c r="AF63" s="8"/>
+      <c r="AG63" s="8"/>
+      <c r="AH63" s="8"/>
+      <c r="AI63" s="8"/>
+      <c r="AJ63" s="8"/>
+      <c r="AK63" s="8"/>
+      <c r="AL63" s="8"/>
+      <c r="AM63" s="8"/>
+      <c r="AN63" s="8"/>
+      <c r="AO63" s="8"/>
+      <c r="AP63" s="8"/>
+      <c r="AQ63" s="8"/>
+      <c r="AR63" s="8"/>
+      <c r="AS63" s="8"/>
+      <c r="AT63" s="8"/>
+      <c r="AU63" s="8"/>
+      <c r="AV63" s="8"/>
+      <c r="AW63" s="8"/>
+      <c r="AX63" s="8"/>
+      <c r="AY63" s="8"/>
+      <c r="AZ63" s="8"/>
+      <c r="BA63" s="8"/>
+      <c r="BB63" s="9"/>
+      <c r="BC63" s="8"/>
+    </row>
+    <row r="64" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B64" s="7"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="8"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="8"/>
+      <c r="N64" s="8"/>
+      <c r="O64" s="8"/>
+      <c r="P64" s="8"/>
+      <c r="Q64" s="9"/>
+      <c r="R64" s="8"/>
+      <c r="S64" s="8"/>
+      <c r="T64" s="8"/>
+      <c r="U64" s="8"/>
+      <c r="V64" s="8"/>
+      <c r="W64" s="8"/>
+      <c r="X64" s="8"/>
+      <c r="Y64" s="8"/>
+      <c r="Z64" s="8"/>
+      <c r="AA64" s="8"/>
+      <c r="AB64" s="9"/>
+      <c r="AE64" s="7"/>
+      <c r="AF64" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="AG64" s="8"/>
+      <c r="AH64" s="8"/>
+      <c r="AI64" s="8"/>
+      <c r="AJ64" s="8"/>
+      <c r="AK64" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="AL64" s="2"/>
+      <c r="AM64" s="2"/>
+      <c r="AN64" s="2"/>
+      <c r="AO64" s="3"/>
+      <c r="AP64" s="8"/>
+      <c r="AQ64" s="8"/>
+      <c r="AR64" s="8"/>
+      <c r="AS64" s="8"/>
+      <c r="AT64" s="8"/>
+      <c r="AU64" s="8"/>
+      <c r="AV64" s="8"/>
+      <c r="AW64" s="8"/>
+      <c r="AX64" s="8"/>
+      <c r="AY64" s="8"/>
+      <c r="AZ64" s="8"/>
+      <c r="BA64" s="8"/>
+      <c r="BB64" s="9"/>
+      <c r="BC64" s="8"/>
+    </row>
+    <row r="65" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B65" s="7"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="8"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="8"/>
+      <c r="N65" s="8"/>
+      <c r="O65" s="8"/>
+      <c r="P65" s="8"/>
+      <c r="Q65" s="9"/>
+      <c r="R65" s="8"/>
+      <c r="S65" s="8"/>
+      <c r="T65" s="8"/>
+      <c r="U65" s="8"/>
+      <c r="V65" s="8"/>
+      <c r="W65" s="8"/>
+      <c r="X65" s="8"/>
+      <c r="Y65" s="8"/>
+      <c r="Z65" s="8"/>
+      <c r="AA65" s="8"/>
+      <c r="AB65" s="9"/>
+      <c r="AE65" s="7"/>
+      <c r="AF65" s="8"/>
+      <c r="AG65" s="8"/>
+      <c r="AH65" s="8"/>
+      <c r="AI65" s="8"/>
+      <c r="AJ65" s="8"/>
+      <c r="AK65" s="8"/>
+      <c r="AL65" s="8"/>
+      <c r="AM65" s="8"/>
+      <c r="AN65" s="8"/>
+      <c r="AO65" s="8"/>
+      <c r="AP65" s="8"/>
+      <c r="AQ65" s="8"/>
+      <c r="AR65" s="8"/>
+      <c r="AS65" s="8"/>
+      <c r="AT65" s="8"/>
+      <c r="AU65" s="8"/>
+      <c r="AV65" s="8"/>
+      <c r="AW65" s="8"/>
+      <c r="AX65" s="8"/>
+      <c r="AY65" s="8"/>
+      <c r="AZ65" s="8"/>
+      <c r="BA65" s="8"/>
+      <c r="BB65" s="9"/>
+      <c r="BC65" s="8"/>
+    </row>
+    <row r="66" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B66" s="7"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="11"/>
+      <c r="L66" s="12"/>
+      <c r="M66" s="11"/>
+      <c r="N66" s="11"/>
+      <c r="O66" s="11"/>
+      <c r="P66" s="11"/>
+      <c r="Q66" s="12"/>
+      <c r="R66" s="8"/>
+      <c r="S66" s="8"/>
+      <c r="T66" s="8"/>
+      <c r="U66" s="31"/>
+      <c r="V66" s="8"/>
+      <c r="W66" s="8"/>
+      <c r="X66" s="8"/>
+      <c r="Y66" s="8"/>
+      <c r="Z66" s="8"/>
+      <c r="AA66" s="8"/>
+      <c r="AB66" s="9"/>
+      <c r="AE66" s="7"/>
+      <c r="AF66" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="AG66" s="8"/>
+      <c r="AH66" s="8"/>
+      <c r="AI66" s="8"/>
+      <c r="AJ66" s="8"/>
+      <c r="AK66" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="AL66" s="3"/>
+      <c r="AM66" s="8"/>
+      <c r="AN66" s="8"/>
+      <c r="AO66" s="8"/>
+      <c r="AP66" s="8"/>
+      <c r="AQ66" s="8"/>
+      <c r="AR66" s="8"/>
+      <c r="AS66" s="8"/>
+      <c r="AT66" s="8"/>
+      <c r="AU66" s="8"/>
+      <c r="AV66" s="8"/>
+      <c r="AW66" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AX66" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="AY66" s="3"/>
+      <c r="AZ66" s="8"/>
+      <c r="BA66" s="8"/>
+      <c r="BB66" s="9"/>
+      <c r="BC66" s="8"/>
+    </row>
+    <row r="67" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B67" s="7"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="8"/>
+      <c r="K67" s="8"/>
+      <c r="L67" s="8"/>
+      <c r="M67" s="8"/>
+      <c r="N67" s="8"/>
+      <c r="O67" s="8"/>
+      <c r="P67" s="8"/>
+      <c r="Q67" s="8"/>
+      <c r="R67" s="8"/>
+      <c r="S67" s="8"/>
+      <c r="T67" s="8"/>
+      <c r="U67" s="8"/>
+      <c r="V67" s="8"/>
+      <c r="W67" s="8"/>
+      <c r="X67" s="8"/>
+      <c r="Y67" s="8"/>
+      <c r="Z67" s="8"/>
+      <c r="AA67" s="8"/>
+      <c r="AB67" s="9"/>
+      <c r="AE67" s="7"/>
+      <c r="AF67" s="8"/>
+      <c r="AG67" s="8"/>
+      <c r="AH67" s="8"/>
+      <c r="AI67" s="8"/>
+      <c r="AJ67" s="8"/>
+      <c r="AK67" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="AL67" s="8"/>
+      <c r="AM67" s="8"/>
+      <c r="AN67" s="8"/>
+      <c r="AO67" s="8"/>
+      <c r="AP67" s="8"/>
+      <c r="AQ67" s="8"/>
+      <c r="AR67" s="8"/>
+      <c r="AS67" s="8"/>
+      <c r="AT67" s="8"/>
+      <c r="AU67" s="8"/>
+      <c r="AV67" s="8"/>
+      <c r="AW67" s="8"/>
+      <c r="AX67" s="8"/>
+      <c r="AY67" s="8"/>
+      <c r="AZ67" s="8"/>
+      <c r="BA67" s="8"/>
+      <c r="BB67" s="9"/>
+      <c r="BC67" s="8"/>
+    </row>
+    <row r="68" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B68" s="7"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+      <c r="K68" s="8"/>
+      <c r="L68" s="8"/>
+      <c r="M68" s="8"/>
+      <c r="N68" s="8"/>
+      <c r="O68" s="8"/>
+      <c r="P68" s="8"/>
+      <c r="Q68" s="8"/>
+      <c r="R68" s="8"/>
+      <c r="S68" s="8"/>
+      <c r="T68" s="8"/>
+      <c r="U68" s="31"/>
+      <c r="V68" s="8"/>
+      <c r="W68" s="8"/>
+      <c r="X68" s="8"/>
+      <c r="Y68" s="8"/>
+      <c r="Z68" s="8"/>
+      <c r="AA68" s="8"/>
+      <c r="AB68" s="9"/>
+      <c r="AE68" s="7"/>
+      <c r="AF68" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="AG68" s="8"/>
+      <c r="AH68" s="8"/>
+      <c r="AI68" s="8"/>
+      <c r="AJ68" s="8"/>
+      <c r="AK68" s="1"/>
+      <c r="AL68" s="2"/>
+      <c r="AM68" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN68" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="AO68" s="8"/>
+      <c r="AP68" s="8"/>
+      <c r="AQ68" s="8"/>
+      <c r="AR68" s="8"/>
+      <c r="AS68" s="8"/>
+      <c r="AT68" s="8"/>
+      <c r="AU68" s="8"/>
+      <c r="AV68" s="8"/>
+      <c r="AW68" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="AX68" s="1"/>
+      <c r="AY68" s="3"/>
+      <c r="AZ68" s="8"/>
+      <c r="BA68" s="8"/>
+      <c r="BB68" s="9"/>
+      <c r="BC68" s="8"/>
+    </row>
+    <row r="69" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B69" s="10"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="11"/>
+      <c r="L69" s="11"/>
+      <c r="M69" s="11"/>
+      <c r="N69" s="11"/>
+      <c r="O69" s="11"/>
+      <c r="P69" s="11"/>
+      <c r="Q69" s="11"/>
+      <c r="R69" s="11"/>
+      <c r="S69" s="11"/>
+      <c r="T69" s="11"/>
+      <c r="U69" s="11"/>
+      <c r="V69" s="11"/>
+      <c r="W69" s="11"/>
+      <c r="X69" s="11"/>
+      <c r="Y69" s="11"/>
+      <c r="Z69" s="11"/>
+      <c r="AA69" s="11"/>
+      <c r="AB69" s="12"/>
+      <c r="AE69" s="7"/>
+      <c r="AF69" s="8"/>
+      <c r="AG69" s="8"/>
+      <c r="AH69" s="8"/>
+      <c r="AI69" s="8"/>
+      <c r="AJ69" s="8"/>
+      <c r="AK69" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="AL69" s="8"/>
+      <c r="AM69" s="8"/>
+      <c r="AN69" s="8"/>
+      <c r="AO69" s="8"/>
+      <c r="AP69" s="8"/>
+      <c r="AQ69" s="8"/>
+      <c r="AR69" s="8"/>
+      <c r="AS69" s="8"/>
+      <c r="AT69" s="8"/>
+      <c r="AU69" s="8"/>
+      <c r="AV69" s="8"/>
+      <c r="AW69" s="8"/>
+      <c r="AX69" s="8"/>
+      <c r="AY69" s="8"/>
+      <c r="AZ69" s="8"/>
+      <c r="BA69" s="8"/>
+      <c r="BB69" s="9"/>
+      <c r="BC69" s="8"/>
+    </row>
+    <row r="70" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
+      <c r="J70" s="8"/>
+      <c r="K70" s="8"/>
+      <c r="L70" s="8"/>
+      <c r="M70" s="8"/>
+      <c r="N70" s="8"/>
+      <c r="O70" s="8"/>
+      <c r="P70" s="8"/>
+      <c r="Q70" s="8"/>
+      <c r="R70" s="8"/>
+      <c r="S70" s="8"/>
+      <c r="T70" s="8"/>
+      <c r="U70" s="8"/>
+      <c r="V70" s="8"/>
+      <c r="W70" s="8"/>
+      <c r="X70" s="8"/>
+      <c r="Y70" s="8"/>
+      <c r="Z70" s="8"/>
+      <c r="AA70" s="8"/>
+      <c r="AB70" s="8"/>
+      <c r="AE70" s="7"/>
+      <c r="AF70" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="AG70" s="8"/>
+      <c r="AH70" s="8"/>
+      <c r="AI70" s="8"/>
+      <c r="AJ70" s="8"/>
+      <c r="AK70" s="1"/>
+      <c r="AL70" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM70" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="AN70" s="8"/>
+      <c r="AO70" s="8"/>
+      <c r="AP70" s="8"/>
+      <c r="AQ70" s="8"/>
+      <c r="AR70" s="8"/>
+      <c r="AS70" s="8"/>
+      <c r="AT70" s="8"/>
+      <c r="AU70" s="8"/>
+      <c r="AV70" s="8"/>
+      <c r="AW70" s="8"/>
+      <c r="AX70" s="8"/>
+      <c r="AY70" s="8"/>
+      <c r="AZ70" s="8"/>
+      <c r="BA70" s="8"/>
+      <c r="BB70" s="9"/>
+      <c r="BC70" s="8"/>
+    </row>
+    <row r="71" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="8"/>
+      <c r="K71" s="8"/>
+      <c r="L71" s="8"/>
+      <c r="M71" s="8"/>
+      <c r="N71" s="8"/>
+      <c r="O71" s="8"/>
+      <c r="P71" s="8"/>
+      <c r="Q71" s="8"/>
+      <c r="R71" s="8"/>
+      <c r="S71" s="8"/>
+      <c r="T71" s="8"/>
+      <c r="U71" s="8"/>
+      <c r="V71" s="8"/>
+      <c r="W71" s="8"/>
+      <c r="X71" s="8"/>
+      <c r="Y71" s="8"/>
+      <c r="Z71" s="8"/>
+      <c r="AA71" s="8"/>
+      <c r="AB71" s="8"/>
+      <c r="AE71" s="7"/>
+      <c r="AF71" s="8"/>
+      <c r="AG71" s="8"/>
+      <c r="AH71" s="8"/>
+      <c r="AI71" s="8"/>
+      <c r="AJ71" s="8"/>
+      <c r="AK71" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL71" s="8"/>
+      <c r="AM71" s="8"/>
+      <c r="AN71" s="8"/>
+      <c r="AO71" s="8"/>
+      <c r="AP71" s="8"/>
+      <c r="AQ71" s="8"/>
+      <c r="AR71" s="8"/>
+      <c r="AS71" s="8"/>
+      <c r="AT71" s="8"/>
+      <c r="AU71" s="8"/>
+      <c r="AV71" s="8"/>
+      <c r="AW71" s="8"/>
+      <c r="AX71" s="8"/>
+      <c r="AY71" s="8"/>
+      <c r="AZ71" s="8"/>
+      <c r="BA71" s="8"/>
+      <c r="BB71" s="9"/>
+      <c r="BC71" s="8"/>
+    </row>
+    <row r="72" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="8"/>
+      <c r="K72" s="8"/>
+      <c r="L72" s="8"/>
+      <c r="M72" s="8"/>
+      <c r="N72" s="8"/>
+      <c r="O72" s="8"/>
+      <c r="P72" s="8"/>
+      <c r="Q72" s="8"/>
+      <c r="R72" s="8"/>
+      <c r="S72" s="8"/>
+      <c r="T72" s="8"/>
+      <c r="U72" s="8"/>
+      <c r="V72" s="8"/>
+      <c r="W72" s="8"/>
+      <c r="X72" s="8"/>
+      <c r="Y72" s="8"/>
+      <c r="Z72" s="8"/>
+      <c r="AA72" s="8"/>
+      <c r="AB72" s="8"/>
+      <c r="AE72" s="7"/>
+      <c r="AF72" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="AG72" s="8"/>
+      <c r="AH72" s="8"/>
+      <c r="AI72" s="8"/>
+      <c r="AJ72" s="8"/>
+      <c r="AK72" s="1"/>
+      <c r="AL72" s="2"/>
+      <c r="AM72" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN72" s="8"/>
+      <c r="AO72" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="AP72" s="8"/>
+      <c r="AQ72" s="8"/>
+      <c r="AR72" s="8"/>
+      <c r="AS72" s="8"/>
+      <c r="AT72" s="8"/>
+      <c r="AU72" s="8"/>
+      <c r="AV72" s="8"/>
+      <c r="AW72" s="8"/>
+      <c r="AX72" s="8"/>
+      <c r="AY72" s="8"/>
+      <c r="AZ72" s="8"/>
+      <c r="BA72" s="8"/>
+      <c r="BB72" s="9"/>
+      <c r="BC72" s="8"/>
+    </row>
+    <row r="73" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="8"/>
+      <c r="K73" s="8"/>
+      <c r="L73" s="8"/>
+      <c r="M73" s="8"/>
+      <c r="N73" s="8"/>
+      <c r="O73" s="8"/>
+      <c r="P73" s="8"/>
+      <c r="Q73" s="8"/>
+      <c r="R73" s="8"/>
+      <c r="S73" s="8"/>
+      <c r="T73" s="8"/>
+      <c r="U73" s="8"/>
+      <c r="V73" s="8"/>
+      <c r="W73" s="8"/>
+      <c r="X73" s="8"/>
+      <c r="Y73" s="8"/>
+      <c r="Z73" s="8"/>
+      <c r="AA73" s="8"/>
+      <c r="AB73" s="8"/>
+      <c r="AE73" s="7"/>
+      <c r="AF73" s="8"/>
+      <c r="AG73" s="8"/>
+      <c r="AH73" s="8"/>
+      <c r="AI73" s="8"/>
+      <c r="AJ73" s="8"/>
+      <c r="AK73" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="AL73" s="8"/>
+      <c r="AM73" s="8"/>
+      <c r="AN73" s="8"/>
+      <c r="AO73" s="8"/>
+      <c r="AP73" s="8"/>
+      <c r="AQ73" s="8"/>
+      <c r="AR73" s="8"/>
+      <c r="AS73" s="8"/>
+      <c r="AT73" s="8"/>
+      <c r="AU73" s="8"/>
+      <c r="AV73" s="8"/>
+      <c r="AW73" s="8"/>
+      <c r="AX73" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="AY73" s="8"/>
+      <c r="AZ73" s="8"/>
+      <c r="BA73" s="8"/>
+      <c r="BB73" s="9"/>
+      <c r="BC73" s="8"/>
+    </row>
+    <row r="74" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="8"/>
+      <c r="K74" s="8"/>
+      <c r="L74" s="8"/>
+      <c r="M74" s="8"/>
+      <c r="N74" s="8"/>
+      <c r="O74" s="8"/>
+      <c r="P74" s="8"/>
+      <c r="Q74" s="8"/>
+      <c r="R74" s="8"/>
+      <c r="S74" s="8"/>
+      <c r="T74" s="8"/>
+      <c r="U74" s="31"/>
+      <c r="V74" s="8"/>
+      <c r="W74" s="8"/>
+      <c r="X74" s="8"/>
+      <c r="Y74" s="8"/>
+      <c r="Z74" s="8"/>
+      <c r="AA74" s="8"/>
+      <c r="AB74" s="8"/>
+      <c r="AE74" s="7"/>
+      <c r="AF74" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="AG74" s="8"/>
+      <c r="AH74" s="8"/>
+      <c r="AI74" s="8"/>
+      <c r="AJ74" s="8"/>
+      <c r="AK74" s="1"/>
+      <c r="AL74" s="3"/>
+      <c r="AM74" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="AN74" s="8"/>
+      <c r="AO74" s="8"/>
+      <c r="AP74" s="8"/>
+      <c r="AQ74" s="8"/>
+      <c r="AR74" s="8"/>
+      <c r="AS74" s="8"/>
+      <c r="AT74" s="8"/>
+      <c r="AU74" s="8"/>
+      <c r="AV74" s="8"/>
+      <c r="AW74" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="AX74" s="1"/>
+      <c r="AY74" s="3"/>
+      <c r="AZ74" s="8"/>
+      <c r="BA74" s="8"/>
+      <c r="BB74" s="9"/>
+      <c r="BC74" s="8"/>
+    </row>
+    <row r="75" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="8"/>
+      <c r="K75" s="8"/>
+      <c r="L75" s="8"/>
+      <c r="M75" s="8"/>
+      <c r="N75" s="8"/>
+      <c r="O75" s="8"/>
+      <c r="P75" s="8"/>
+      <c r="Q75" s="8"/>
+      <c r="R75" s="8"/>
+      <c r="S75" s="8"/>
+      <c r="T75" s="8"/>
+      <c r="U75" s="8"/>
+      <c r="V75" s="8"/>
+      <c r="W75" s="8"/>
+      <c r="X75" s="8"/>
+      <c r="Y75" s="8"/>
+      <c r="Z75" s="8"/>
+      <c r="AA75" s="8"/>
+      <c r="AB75" s="8"/>
+      <c r="AE75" s="7"/>
+      <c r="AF75" s="8"/>
+      <c r="AG75" s="8"/>
+      <c r="AH75" s="8"/>
+      <c r="AI75" s="8"/>
+      <c r="AJ75" s="8"/>
+      <c r="AK75" s="8"/>
+      <c r="AL75" s="8"/>
+      <c r="AM75" s="8"/>
+      <c r="AN75" s="8"/>
+      <c r="AO75" s="8"/>
+      <c r="AP75" s="8"/>
+      <c r="AQ75" s="8"/>
+      <c r="AR75" s="8"/>
+      <c r="AS75" s="8"/>
+      <c r="AT75" s="8"/>
+      <c r="AU75" s="8"/>
+      <c r="AV75" s="8"/>
+      <c r="AW75" s="8"/>
+      <c r="AX75" s="8"/>
+      <c r="AY75" s="8"/>
+      <c r="AZ75" s="8"/>
+      <c r="BA75" s="8"/>
+      <c r="BB75" s="9"/>
+      <c r="BC75" s="8"/>
+    </row>
+    <row r="76" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
+      <c r="I76" s="8"/>
+      <c r="J76" s="8"/>
+      <c r="K76" s="8"/>
+      <c r="L76" s="8"/>
+      <c r="M76" s="8"/>
+      <c r="N76" s="8"/>
+      <c r="O76" s="8"/>
+      <c r="P76" s="8"/>
+      <c r="Q76" s="8"/>
+      <c r="R76" s="8"/>
+      <c r="S76" s="8"/>
+      <c r="T76" s="8"/>
+      <c r="U76" s="8"/>
+      <c r="V76" s="8"/>
+      <c r="W76" s="8"/>
+      <c r="X76" s="8"/>
+      <c r="Y76" s="8"/>
+      <c r="Z76" s="8"/>
+      <c r="AA76" s="8"/>
+      <c r="AB76" s="8"/>
+      <c r="AE76" s="7"/>
+      <c r="AF76" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG76" s="8"/>
+      <c r="AH76" s="8"/>
+      <c r="AI76" s="8"/>
+      <c r="AJ76" s="8"/>
+      <c r="AK76" s="1"/>
+      <c r="AL76" s="3"/>
+      <c r="AM76" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="AN76" s="8"/>
+      <c r="AO76" s="8"/>
+      <c r="AP76" s="8"/>
+      <c r="AQ76" s="8"/>
+      <c r="AR76" s="8"/>
+      <c r="AS76" s="8"/>
+      <c r="AT76" s="8"/>
+      <c r="AU76" s="8"/>
+      <c r="AV76" s="8"/>
+      <c r="AW76" s="8"/>
+      <c r="AX76" s="8"/>
+      <c r="AY76" s="8"/>
+      <c r="AZ76" s="8"/>
+      <c r="BA76" s="8"/>
+      <c r="BB76" s="9"/>
+      <c r="BC76" s="8"/>
+    </row>
+    <row r="77" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
+      <c r="I77" s="8"/>
+      <c r="J77" s="8"/>
+      <c r="K77" s="8"/>
+      <c r="L77" s="8"/>
+      <c r="M77" s="8"/>
+      <c r="N77" s="8"/>
+      <c r="O77" s="8"/>
+      <c r="P77" s="8"/>
+      <c r="Q77" s="8"/>
+      <c r="R77" s="8"/>
+      <c r="S77" s="8"/>
+      <c r="T77" s="8"/>
+      <c r="U77" s="8"/>
+      <c r="V77" s="8"/>
+      <c r="W77" s="8"/>
+      <c r="X77" s="8"/>
+      <c r="Y77" s="8"/>
+      <c r="Z77" s="8"/>
+      <c r="AA77" s="8"/>
+      <c r="AB77" s="8"/>
+      <c r="AE77" s="7"/>
+      <c r="AF77" s="8"/>
+      <c r="AG77" s="8"/>
+      <c r="AH77" s="8"/>
+      <c r="AI77" s="8"/>
+      <c r="AJ77" s="8"/>
+      <c r="AK77" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="AL77" s="8"/>
+      <c r="AM77" s="8"/>
+      <c r="AN77" s="8"/>
+      <c r="AO77" s="8"/>
+      <c r="AP77" s="8"/>
+      <c r="AQ77" s="8"/>
+      <c r="AR77" s="8"/>
+      <c r="AS77" s="8"/>
+      <c r="AT77" s="8"/>
+      <c r="AU77" s="8"/>
+      <c r="AV77" s="8"/>
+      <c r="AW77" s="8"/>
+      <c r="AX77" s="8"/>
+      <c r="AY77" s="8"/>
+      <c r="AZ77" s="8"/>
+      <c r="BA77" s="8"/>
+      <c r="BB77" s="9"/>
+      <c r="BC77" s="8"/>
+    </row>
+    <row r="78" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="8"/>
+      <c r="K78" s="8"/>
+      <c r="L78" s="8"/>
+      <c r="M78" s="8"/>
+      <c r="N78" s="8"/>
+      <c r="O78" s="8"/>
+      <c r="P78" s="8"/>
+      <c r="Q78" s="8"/>
+      <c r="R78" s="8"/>
+      <c r="S78" s="8"/>
+      <c r="T78" s="8"/>
+      <c r="U78" s="8"/>
+      <c r="V78" s="8"/>
+      <c r="W78" s="8"/>
+      <c r="X78" s="8"/>
+      <c r="Y78" s="8"/>
+      <c r="Z78" s="8"/>
+      <c r="AA78" s="8"/>
+      <c r="AB78" s="8"/>
+      <c r="AE78" s="7"/>
+      <c r="AF78" s="8"/>
+      <c r="AG78" s="8"/>
+      <c r="AH78" s="8"/>
+      <c r="AI78" s="8"/>
+      <c r="AJ78" s="8"/>
+      <c r="AK78" s="8"/>
+      <c r="AL78" s="8"/>
+      <c r="AM78" s="8"/>
+      <c r="AN78" s="8"/>
+      <c r="AO78" s="8"/>
+      <c r="AP78" s="8"/>
+      <c r="AQ78" s="8"/>
+      <c r="AR78" s="8"/>
+      <c r="AS78" s="8"/>
+      <c r="AT78" s="8"/>
+      <c r="AU78" s="8"/>
+      <c r="AV78" s="8"/>
+      <c r="AW78" s="8"/>
+      <c r="AX78" s="8"/>
+      <c r="AY78" s="8"/>
+      <c r="AZ78" s="8"/>
+      <c r="BA78" s="8"/>
+      <c r="BB78" s="9"/>
+      <c r="BC78" s="8"/>
+    </row>
+    <row r="79" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="8"/>
+      <c r="K79" s="8"/>
+      <c r="L79" s="8"/>
+      <c r="M79" s="8"/>
+      <c r="N79" s="8"/>
+      <c r="O79" s="8"/>
+      <c r="P79" s="8"/>
+      <c r="Q79" s="8"/>
+      <c r="R79" s="8"/>
+      <c r="S79" s="8"/>
+      <c r="T79" s="8"/>
+      <c r="U79" s="8"/>
+      <c r="V79" s="8"/>
+      <c r="W79" s="8"/>
+      <c r="X79" s="8"/>
+      <c r="Y79" s="8"/>
+      <c r="Z79" s="8"/>
+      <c r="AA79" s="8"/>
+      <c r="AB79" s="8"/>
+      <c r="AE79" s="7"/>
+      <c r="AF79" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="AG79" s="8"/>
+      <c r="AH79" s="8"/>
+      <c r="AI79" s="8"/>
+      <c r="AJ79" s="8"/>
+      <c r="AK79" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="AL79" s="5"/>
+      <c r="AM79" s="5"/>
+      <c r="AN79" s="5"/>
+      <c r="AO79" s="5"/>
+      <c r="AP79" s="5"/>
+      <c r="AQ79" s="5"/>
+      <c r="AR79" s="5"/>
+      <c r="AS79" s="5"/>
+      <c r="AT79" s="5"/>
+      <c r="AU79" s="5"/>
+      <c r="AV79" s="5"/>
+      <c r="AW79" s="6"/>
+      <c r="AX79" s="8"/>
+      <c r="AY79" s="8"/>
+      <c r="AZ79" s="8"/>
+      <c r="BA79" s="8"/>
+      <c r="BB79" s="9"/>
+      <c r="BC79" s="8"/>
+    </row>
+    <row r="80" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8"/>
+      <c r="I80" s="8"/>
+      <c r="J80" s="8"/>
+      <c r="K80" s="8"/>
+      <c r="L80" s="8"/>
+      <c r="M80" s="8"/>
+      <c r="N80" s="8"/>
+      <c r="O80" s="8"/>
+      <c r="P80" s="8"/>
+      <c r="Q80" s="8"/>
+      <c r="R80" s="8"/>
+      <c r="S80" s="8"/>
+      <c r="T80" s="8"/>
+      <c r="U80" s="8"/>
+      <c r="V80" s="8"/>
+      <c r="W80" s="8"/>
+      <c r="X80" s="8"/>
+      <c r="Y80" s="8"/>
+      <c r="Z80" s="8"/>
+      <c r="AA80" s="8"/>
+      <c r="AB80" s="8"/>
+      <c r="AE80" s="7"/>
+      <c r="AF80" s="8"/>
+      <c r="AG80" s="8"/>
+      <c r="AH80" s="8"/>
+      <c r="AI80" s="8"/>
+      <c r="AJ80" s="8"/>
+      <c r="AK80" s="7"/>
+      <c r="AL80" s="8"/>
+      <c r="AM80" s="8"/>
+      <c r="AN80" s="8"/>
+      <c r="AO80" s="8"/>
+      <c r="AP80" s="8"/>
+      <c r="AQ80" s="8"/>
+      <c r="AR80" s="8"/>
+      <c r="AS80" s="8"/>
+      <c r="AT80" s="8"/>
+      <c r="AU80" s="8"/>
+      <c r="AV80" s="8"/>
+      <c r="AW80" s="9"/>
+      <c r="AX80" s="8"/>
+      <c r="AY80" s="8"/>
+      <c r="AZ80" s="8"/>
+      <c r="BA80" s="8"/>
+      <c r="BB80" s="9"/>
+      <c r="BC80" s="8"/>
+    </row>
+    <row r="81" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B81" s="8"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="8"/>
+      <c r="G81" s="8"/>
+      <c r="H81" s="8"/>
+      <c r="I81" s="8"/>
+      <c r="J81" s="8"/>
+      <c r="K81" s="8"/>
+      <c r="L81" s="8"/>
+      <c r="M81" s="8"/>
+      <c r="N81" s="8"/>
+      <c r="O81" s="8"/>
+      <c r="P81" s="8"/>
+      <c r="Q81" s="8"/>
+      <c r="R81" s="8"/>
+      <c r="S81" s="8"/>
+      <c r="T81" s="8"/>
+      <c r="U81" s="8"/>
+      <c r="V81" s="8"/>
+      <c r="W81" s="8"/>
+      <c r="X81" s="8"/>
+      <c r="Y81" s="8"/>
+      <c r="Z81" s="8"/>
+      <c r="AA81" s="8"/>
+      <c r="AB81" s="8"/>
+      <c r="AE81" s="7"/>
+      <c r="AF81" s="8"/>
+      <c r="AG81" s="8"/>
+      <c r="AH81" s="8"/>
+      <c r="AI81" s="8"/>
+      <c r="AJ81" s="8"/>
+      <c r="AK81" s="10"/>
+      <c r="AL81" s="11"/>
+      <c r="AM81" s="11"/>
+      <c r="AN81" s="11"/>
+      <c r="AO81" s="11"/>
+      <c r="AP81" s="11"/>
+      <c r="AQ81" s="11"/>
+      <c r="AR81" s="11"/>
+      <c r="AS81" s="11"/>
+      <c r="AT81" s="11"/>
+      <c r="AU81" s="11"/>
+      <c r="AV81" s="11"/>
+      <c r="AW81" s="12"/>
+      <c r="AX81" s="8"/>
+      <c r="AY81" s="8"/>
+      <c r="AZ81" s="8"/>
+      <c r="BA81" s="8"/>
+      <c r="BB81" s="9"/>
+      <c r="BC81" s="8"/>
+    </row>
+    <row r="82" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="8"/>
+      <c r="I82" s="8"/>
+      <c r="J82" s="8"/>
+      <c r="K82" s="8"/>
+      <c r="L82" s="8"/>
+      <c r="M82" s="8"/>
+      <c r="N82" s="8"/>
+      <c r="O82" s="8"/>
+      <c r="P82" s="8"/>
+      <c r="Q82" s="8"/>
+      <c r="R82" s="8"/>
+      <c r="S82" s="8"/>
+      <c r="T82" s="8"/>
+      <c r="U82" s="8"/>
+      <c r="V82" s="8"/>
+      <c r="W82" s="8"/>
+      <c r="X82" s="8"/>
+      <c r="Y82" s="8"/>
+      <c r="Z82" s="8"/>
+      <c r="AA82" s="8"/>
+      <c r="AB82" s="8"/>
+      <c r="AE82" s="7"/>
+      <c r="AF82" s="8"/>
+      <c r="AG82" s="8"/>
+      <c r="AH82" s="8"/>
+      <c r="AI82" s="8"/>
+      <c r="AJ82" s="8"/>
+      <c r="AK82" s="8"/>
+      <c r="AL82" s="8"/>
+      <c r="AM82" s="8"/>
+      <c r="AN82" s="8"/>
+      <c r="AO82" s="8"/>
+      <c r="AP82" s="8"/>
+      <c r="AQ82" s="8"/>
+      <c r="AR82" s="8"/>
+      <c r="AS82" s="8"/>
+      <c r="AT82" s="8"/>
+      <c r="AU82" s="8"/>
+      <c r="AV82" s="8"/>
+      <c r="AW82" s="8"/>
+      <c r="AX82" s="8"/>
+      <c r="AY82" s="8"/>
+      <c r="AZ82" s="8"/>
+      <c r="BA82" s="8"/>
+      <c r="BB82" s="9"/>
+      <c r="BC82" s="8"/>
+    </row>
+    <row r="83" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+      <c r="G83" s="8"/>
+      <c r="H83" s="8"/>
+      <c r="I83" s="8"/>
+      <c r="J83" s="8"/>
+      <c r="K83" s="8"/>
+      <c r="L83" s="8"/>
+      <c r="M83" s="8"/>
+      <c r="N83" s="8"/>
+      <c r="O83" s="8"/>
+      <c r="P83" s="8"/>
+      <c r="Q83" s="8"/>
+      <c r="R83" s="8"/>
+      <c r="S83" s="8"/>
+      <c r="T83" s="8"/>
+      <c r="U83" s="8"/>
+      <c r="V83" s="8"/>
+      <c r="W83" s="8"/>
+      <c r="X83" s="8"/>
+      <c r="Y83" s="8"/>
+      <c r="Z83" s="8"/>
+      <c r="AA83" s="8"/>
+      <c r="AB83" s="8"/>
+      <c r="AE83" s="7"/>
+      <c r="AF83" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="AG83" s="5"/>
+      <c r="AH83" s="5"/>
+      <c r="AI83" s="5"/>
+      <c r="AJ83" s="5"/>
+      <c r="AK83" s="5"/>
+      <c r="AL83" s="5"/>
+      <c r="AM83" s="5"/>
+      <c r="AN83" s="5"/>
+      <c r="AO83" s="5"/>
+      <c r="AP83" s="5"/>
+      <c r="AQ83" s="5"/>
+      <c r="AR83" s="5"/>
+      <c r="AS83" s="5"/>
+      <c r="AT83" s="5"/>
+      <c r="AU83" s="5"/>
+      <c r="AV83" s="5"/>
+      <c r="AW83" s="5"/>
+      <c r="AX83" s="5"/>
+      <c r="AY83" s="5"/>
+      <c r="AZ83" s="6"/>
+      <c r="BA83" s="8"/>
+      <c r="BB83" s="9"/>
+      <c r="BC83" s="8"/>
+    </row>
+    <row r="84" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="8"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
+      <c r="I84" s="8"/>
+      <c r="J84" s="8"/>
+      <c r="K84" s="8"/>
+      <c r="L84" s="8"/>
+      <c r="M84" s="8"/>
+      <c r="N84" s="8"/>
+      <c r="O84" s="8"/>
+      <c r="P84" s="8"/>
+      <c r="Q84" s="8"/>
+      <c r="R84" s="8"/>
+      <c r="S84" s="8"/>
+      <c r="T84" s="8"/>
+      <c r="U84" s="8"/>
+      <c r="V84" s="8"/>
+      <c r="W84" s="8"/>
+      <c r="X84" s="8"/>
+      <c r="Y84" s="8"/>
+      <c r="Z84" s="8"/>
+      <c r="AA84" s="8"/>
+      <c r="AB84" s="8"/>
+      <c r="AE84" s="7"/>
+      <c r="AF84" s="7"/>
+      <c r="AG84" s="8"/>
+      <c r="AH84" s="8"/>
+      <c r="AI84" s="8"/>
+      <c r="AJ84" s="8"/>
+      <c r="AK84" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="AL84" s="8"/>
+      <c r="AM84" s="8"/>
+      <c r="AN84" s="8"/>
+      <c r="AO84" s="8"/>
+      <c r="AP84" s="8"/>
+      <c r="AQ84" s="8"/>
+      <c r="AR84" s="8"/>
+      <c r="AS84" s="8"/>
+      <c r="AT84" s="8"/>
+      <c r="AU84" s="8"/>
+      <c r="AV84" s="8"/>
+      <c r="AW84" s="8"/>
+      <c r="AX84" s="8"/>
+      <c r="AY84" s="8"/>
+      <c r="AZ84" s="9"/>
+      <c r="BA84" s="8"/>
+      <c r="BB84" s="9"/>
+      <c r="BC84" s="8"/>
+    </row>
+    <row r="85" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="8"/>
+      <c r="J85" s="8"/>
+      <c r="K85" s="8"/>
+      <c r="L85" s="8"/>
+      <c r="M85" s="8"/>
+      <c r="N85" s="8"/>
+      <c r="O85" s="8"/>
+      <c r="P85" s="8"/>
+      <c r="Q85" s="8"/>
+      <c r="R85" s="8"/>
+      <c r="S85" s="8"/>
+      <c r="T85" s="8"/>
+      <c r="U85" s="8"/>
+      <c r="V85" s="8"/>
+      <c r="W85" s="8"/>
+      <c r="X85" s="8"/>
+      <c r="Y85" s="8"/>
+      <c r="Z85" s="8"/>
+      <c r="AA85" s="8"/>
+      <c r="AB85" s="8"/>
+      <c r="AE85" s="7"/>
+      <c r="AF85" s="7"/>
+      <c r="AG85" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH85" s="8"/>
+      <c r="AI85" s="8"/>
+      <c r="AJ85" s="8"/>
+      <c r="AK85" s="1"/>
+      <c r="AL85" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM85" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN85" s="8"/>
+      <c r="AO85" s="8"/>
+      <c r="AP85" s="8"/>
+      <c r="AQ85" s="8"/>
+      <c r="AR85" s="8"/>
+      <c r="AS85" s="8"/>
+      <c r="AT85" s="8"/>
+      <c r="AU85" s="8"/>
+      <c r="AV85" s="8"/>
+      <c r="AW85" s="8"/>
+      <c r="AX85" s="8"/>
+      <c r="AY85" s="8"/>
+      <c r="AZ85" s="9"/>
+      <c r="BA85" s="8"/>
+      <c r="BB85" s="9"/>
+      <c r="BC85" s="8"/>
+    </row>
+    <row r="86" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="8"/>
+      <c r="I86" s="8"/>
+      <c r="J86" s="8"/>
+      <c r="K86" s="8"/>
+      <c r="L86" s="8"/>
+      <c r="M86" s="8"/>
+      <c r="N86" s="8"/>
+      <c r="O86" s="8"/>
+      <c r="P86" s="8"/>
+      <c r="Q86" s="8"/>
+      <c r="R86" s="8"/>
+      <c r="S86" s="8"/>
+      <c r="T86" s="8"/>
+      <c r="U86" s="8"/>
+      <c r="V86" s="8"/>
+      <c r="W86" s="8"/>
+      <c r="X86" s="8"/>
+      <c r="Y86" s="8"/>
+      <c r="Z86" s="8"/>
+      <c r="AA86" s="8"/>
+      <c r="AB86" s="8"/>
+      <c r="AE86" s="7"/>
+      <c r="AF86" s="7"/>
+      <c r="AG86" s="8"/>
+      <c r="AH86" s="8"/>
+      <c r="AI86" s="8"/>
+      <c r="AJ86" s="8"/>
+      <c r="AK86" s="8"/>
+      <c r="AL86" s="8"/>
+      <c r="AM86" s="8"/>
+      <c r="AN86" s="8"/>
+      <c r="AO86" s="8"/>
+      <c r="AP86" s="8"/>
+      <c r="AQ86" s="8"/>
+      <c r="AR86" s="8"/>
+      <c r="AS86" s="8"/>
+      <c r="AT86" s="8"/>
+      <c r="AU86" s="8"/>
+      <c r="AV86" s="8"/>
+      <c r="AW86" s="8"/>
+      <c r="AX86" s="8"/>
+      <c r="AY86" s="8"/>
+      <c r="AZ86" s="9"/>
+      <c r="BA86" s="8"/>
+      <c r="BB86" s="9"/>
+      <c r="BC86" s="8"/>
+    </row>
+    <row r="87" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B87" s="8"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="8"/>
+      <c r="G87" s="8"/>
+      <c r="H87" s="8"/>
+      <c r="I87" s="8"/>
+      <c r="J87" s="8"/>
+      <c r="K87" s="8"/>
+      <c r="L87" s="8"/>
+      <c r="M87" s="8"/>
+      <c r="N87" s="8"/>
+      <c r="O87" s="8"/>
+      <c r="P87" s="8"/>
+      <c r="Q87" s="8"/>
+      <c r="R87" s="8"/>
+      <c r="S87" s="8"/>
+      <c r="T87" s="8"/>
+      <c r="U87" s="8"/>
+      <c r="V87" s="8"/>
+      <c r="W87" s="8"/>
+      <c r="X87" s="8"/>
+      <c r="Y87" s="8"/>
+      <c r="Z87" s="8"/>
+      <c r="AA87" s="8"/>
+      <c r="AB87" s="8"/>
+      <c r="AE87" s="7"/>
+      <c r="AF87" s="7"/>
+      <c r="AG87" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="AH87" s="8"/>
+      <c r="AI87" s="8"/>
+      <c r="AJ87" s="8"/>
+      <c r="AK87" s="8"/>
+      <c r="AL87" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="AM87" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="AN87" s="2"/>
+      <c r="AO87" s="2"/>
+      <c r="AP87" s="3"/>
+      <c r="AQ87" s="8"/>
+      <c r="AR87" s="8"/>
+      <c r="AS87" s="8"/>
+      <c r="AT87" s="8"/>
+      <c r="AU87" s="8"/>
+      <c r="AV87" s="8"/>
+      <c r="AW87" s="8"/>
+      <c r="AX87" s="8"/>
+      <c r="AY87" s="8"/>
+      <c r="AZ87" s="9"/>
+      <c r="BA87" s="8"/>
+      <c r="BB87" s="9"/>
+      <c r="BC87" s="8"/>
+    </row>
+    <row r="88" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8"/>
+      <c r="H88" s="8"/>
+      <c r="I88" s="8"/>
+      <c r="J88" s="8"/>
+      <c r="K88" s="8"/>
+      <c r="L88" s="8"/>
+      <c r="M88" s="8"/>
+      <c r="N88" s="8"/>
+      <c r="O88" s="8"/>
+      <c r="P88" s="8"/>
+      <c r="Q88" s="8"/>
+      <c r="R88" s="8"/>
+      <c r="S88" s="8"/>
+      <c r="T88" s="8"/>
+      <c r="U88" s="8"/>
+      <c r="V88" s="8"/>
+      <c r="W88" s="8"/>
+      <c r="X88" s="8"/>
+      <c r="Y88" s="8"/>
+      <c r="Z88" s="8"/>
+      <c r="AA88" s="8"/>
+      <c r="AB88" s="8"/>
+      <c r="AE88" s="7"/>
+      <c r="AF88" s="7"/>
+      <c r="AG88" s="8"/>
+      <c r="AH88" s="8"/>
+      <c r="AI88" s="8"/>
+      <c r="AJ88" s="8"/>
+      <c r="AK88" s="8"/>
+      <c r="AL88" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="AM88" s="8"/>
+      <c r="AN88" s="8"/>
+      <c r="AO88" s="8"/>
+      <c r="AP88" s="8"/>
+      <c r="AQ88" s="8"/>
+      <c r="AR88" s="8"/>
+      <c r="AS88" s="8"/>
+      <c r="AT88" s="8"/>
+      <c r="AU88" s="8"/>
+      <c r="AV88" s="8"/>
+      <c r="AW88" s="8"/>
+      <c r="AX88" s="8"/>
+      <c r="AY88" s="8"/>
+      <c r="AZ88" s="9"/>
+      <c r="BA88" s="8"/>
+      <c r="BB88" s="9"/>
+      <c r="BC88" s="8"/>
+    </row>
+    <row r="89" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="8"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="8"/>
+      <c r="K89" s="8"/>
+      <c r="L89" s="8"/>
+      <c r="M89" s="8"/>
+      <c r="N89" s="8"/>
+      <c r="O89" s="8"/>
+      <c r="P89" s="8"/>
+      <c r="Q89" s="8"/>
+      <c r="R89" s="8"/>
+      <c r="S89" s="8"/>
+      <c r="T89" s="8"/>
+      <c r="U89" s="8"/>
+      <c r="V89" s="8"/>
+      <c r="W89" s="8"/>
+      <c r="X89" s="8"/>
+      <c r="Y89" s="8"/>
+      <c r="Z89" s="8"/>
+      <c r="AA89" s="8"/>
+      <c r="AB89" s="8"/>
+      <c r="AE89" s="7"/>
+      <c r="AF89" s="7"/>
+      <c r="AG89" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="AH89" s="8"/>
+      <c r="AI89" s="8"/>
+      <c r="AJ89" s="8"/>
+      <c r="AK89" s="8"/>
+      <c r="AL89" s="1"/>
+      <c r="AM89" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN89" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="AO89" s="8"/>
+      <c r="AP89" s="8"/>
+      <c r="AQ89" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR89" s="8"/>
+      <c r="AS89" s="8"/>
+      <c r="AT89" s="8"/>
+      <c r="AU89" s="8"/>
+      <c r="AV89" s="8"/>
+      <c r="AW89" s="8"/>
+      <c r="AX89" s="8"/>
+      <c r="AY89" s="8"/>
+      <c r="AZ89" s="9"/>
+      <c r="BA89" s="8"/>
+      <c r="BB89" s="9"/>
+      <c r="BC89" s="8"/>
+    </row>
+    <row r="90" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="8"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="8"/>
+      <c r="I90" s="8"/>
+      <c r="J90" s="8"/>
+      <c r="K90" s="8"/>
+      <c r="L90" s="8"/>
+      <c r="M90" s="8"/>
+      <c r="N90" s="8"/>
+      <c r="O90" s="8"/>
+      <c r="P90" s="8"/>
+      <c r="Q90" s="8"/>
+      <c r="R90" s="8"/>
+      <c r="S90" s="8"/>
+      <c r="T90" s="8"/>
+      <c r="U90" s="8"/>
+      <c r="V90" s="8"/>
+      <c r="W90" s="8"/>
+      <c r="X90" s="8"/>
+      <c r="Y90" s="8"/>
+      <c r="Z90" s="8"/>
+      <c r="AA90" s="8"/>
+      <c r="AB90" s="8"/>
+      <c r="AE90" s="7"/>
+      <c r="AF90" s="7"/>
+      <c r="AG90" s="8"/>
+      <c r="AH90" s="8"/>
+      <c r="AI90" s="8"/>
+      <c r="AJ90" s="8"/>
+      <c r="AK90" s="8"/>
+      <c r="AL90" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="AM90" s="8"/>
+      <c r="AN90" s="8"/>
+      <c r="AO90" s="8"/>
+      <c r="AP90" s="8"/>
+      <c r="AQ90" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="AR90" s="8"/>
+      <c r="AS90" s="8"/>
+      <c r="AT90" s="8"/>
+      <c r="AU90" s="8"/>
+      <c r="AV90" s="8"/>
+      <c r="AW90" s="8"/>
+      <c r="AX90" s="8"/>
+      <c r="AY90" s="8"/>
+      <c r="AZ90" s="9"/>
+      <c r="BA90" s="8"/>
+      <c r="BB90" s="9"/>
+      <c r="BC90" s="8"/>
+    </row>
+    <row r="91" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="8"/>
+      <c r="G91" s="8"/>
+      <c r="H91" s="8"/>
+      <c r="I91" s="8"/>
+      <c r="J91" s="8"/>
+      <c r="K91" s="8"/>
+      <c r="L91" s="8"/>
+      <c r="M91" s="8"/>
+      <c r="N91" s="8"/>
+      <c r="O91" s="8"/>
+      <c r="P91" s="8"/>
+      <c r="Q91" s="8"/>
+      <c r="R91" s="8"/>
+      <c r="S91" s="8"/>
+      <c r="T91" s="8"/>
+      <c r="U91" s="8"/>
+      <c r="V91" s="8"/>
+      <c r="W91" s="8"/>
+      <c r="X91" s="8"/>
+      <c r="Y91" s="8"/>
+      <c r="Z91" s="8"/>
+      <c r="AA91" s="8"/>
+      <c r="AB91" s="8"/>
+      <c r="AE91" s="7"/>
+      <c r="AF91" s="7"/>
+      <c r="AG91" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="AH91" s="8"/>
+      <c r="AI91" s="8"/>
+      <c r="AJ91" s="8"/>
+      <c r="AK91" s="8"/>
+      <c r="AL91" s="1"/>
+      <c r="AM91" s="3"/>
+      <c r="AN91" s="8"/>
+      <c r="AO91" s="8"/>
+      <c r="AP91" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="AQ91" s="8"/>
+      <c r="AR91" s="8"/>
+      <c r="AS91" s="8"/>
+      <c r="AT91" s="8"/>
+      <c r="AU91" s="8"/>
+      <c r="AV91" s="8"/>
+      <c r="AW91" s="8"/>
+      <c r="AX91" s="8"/>
+      <c r="AY91" s="8"/>
+      <c r="AZ91" s="9"/>
+      <c r="BA91" s="8"/>
+      <c r="BB91" s="9"/>
+      <c r="BC91" s="8"/>
+    </row>
+    <row r="92" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="8"/>
+      <c r="G92" s="8"/>
+      <c r="H92" s="8"/>
+      <c r="I92" s="8"/>
+      <c r="J92" s="8"/>
+      <c r="K92" s="8"/>
+      <c r="L92" s="8"/>
+      <c r="M92" s="8"/>
+      <c r="N92" s="8"/>
+      <c r="O92" s="8"/>
+      <c r="P92" s="8"/>
+      <c r="Q92" s="8"/>
+      <c r="R92" s="8"/>
+      <c r="S92" s="8"/>
+      <c r="T92" s="8"/>
+      <c r="U92" s="8"/>
+      <c r="V92" s="8"/>
+      <c r="W92" s="8"/>
+      <c r="X92" s="8"/>
+      <c r="Y92" s="8"/>
+      <c r="Z92" s="8"/>
+      <c r="AA92" s="8"/>
+      <c r="AB92" s="8"/>
+      <c r="AE92" s="7"/>
+      <c r="AF92" s="7"/>
+      <c r="AG92" s="8"/>
+      <c r="AH92" s="8"/>
+      <c r="AI92" s="8"/>
+      <c r="AJ92" s="8"/>
+      <c r="AK92" s="8"/>
+      <c r="AL92" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="AM92" s="8"/>
+      <c r="AN92" s="8"/>
+      <c r="AO92" s="8"/>
+      <c r="AP92" s="8"/>
+      <c r="AQ92" s="8"/>
+      <c r="AR92" s="8"/>
+      <c r="AS92" s="8"/>
+      <c r="AT92" s="8"/>
+      <c r="AU92" s="8"/>
+      <c r="AV92" s="8"/>
+      <c r="AW92" s="8"/>
+      <c r="AX92" s="8"/>
+      <c r="AY92" s="8"/>
+      <c r="AZ92" s="9"/>
+      <c r="BA92" s="8"/>
+      <c r="BB92" s="9"/>
+      <c r="BC92" s="8"/>
+    </row>
+    <row r="93" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="8"/>
+      <c r="I93" s="8"/>
+      <c r="J93" s="8"/>
+      <c r="K93" s="8"/>
+      <c r="L93" s="8"/>
+      <c r="M93" s="8"/>
+      <c r="N93" s="8"/>
+      <c r="O93" s="8"/>
+      <c r="P93" s="8"/>
+      <c r="Q93" s="8"/>
+      <c r="R93" s="8"/>
+      <c r="S93" s="8"/>
+      <c r="T93" s="8"/>
+      <c r="U93" s="8"/>
+      <c r="V93" s="8"/>
+      <c r="W93" s="8"/>
+      <c r="X93" s="8"/>
+      <c r="Y93" s="8"/>
+      <c r="Z93" s="8"/>
+      <c r="AA93" s="8"/>
+      <c r="AB93" s="8"/>
+      <c r="AE93" s="7"/>
+      <c r="AF93" s="7"/>
+      <c r="AG93" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="AH93" s="8"/>
+      <c r="AI93" s="8"/>
+      <c r="AJ93" s="8"/>
+      <c r="AK93" s="8"/>
+      <c r="AL93" s="1"/>
+      <c r="AM93" s="3"/>
+      <c r="AN93" s="8"/>
+      <c r="AO93" s="8"/>
+      <c r="AP93" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="AQ93" s="8"/>
+      <c r="AR93" s="8"/>
+      <c r="AS93" s="8"/>
+      <c r="AT93" s="8"/>
+      <c r="AU93" s="8"/>
+      <c r="AV93" s="8"/>
+      <c r="AW93" s="8"/>
+      <c r="AX93" s="8"/>
+      <c r="AY93" s="8"/>
+      <c r="AZ93" s="9"/>
+      <c r="BA93" s="8"/>
+      <c r="BB93" s="9"/>
+      <c r="BC93" s="8"/>
+    </row>
+    <row r="94" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="8"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="8"/>
+      <c r="I94" s="8"/>
+      <c r="J94" s="8"/>
+      <c r="K94" s="8"/>
+      <c r="L94" s="8"/>
+      <c r="M94" s="8"/>
+      <c r="N94" s="8"/>
+      <c r="O94" s="8"/>
+      <c r="P94" s="8"/>
+      <c r="Q94" s="8"/>
+      <c r="R94" s="8"/>
+      <c r="S94" s="8"/>
+      <c r="T94" s="8"/>
+      <c r="U94" s="8"/>
+      <c r="V94" s="8"/>
+      <c r="W94" s="8"/>
+      <c r="X94" s="8"/>
+      <c r="Y94" s="8"/>
+      <c r="Z94" s="8"/>
+      <c r="AA94" s="8"/>
+      <c r="AB94" s="8"/>
+      <c r="AE94" s="7"/>
+      <c r="AF94" s="7"/>
+      <c r="AG94" s="8"/>
+      <c r="AH94" s="8"/>
+      <c r="AI94" s="8"/>
+      <c r="AJ94" s="8"/>
+      <c r="AK94" s="8"/>
+      <c r="AL94" s="8"/>
+      <c r="AM94" s="8"/>
+      <c r="AN94" s="8"/>
+      <c r="AO94" s="8"/>
+      <c r="AP94" s="8"/>
+      <c r="AQ94" s="8"/>
+      <c r="AR94" s="8"/>
+      <c r="AS94" s="8"/>
+      <c r="AT94" s="8"/>
+      <c r="AU94" s="8"/>
+      <c r="AV94" s="8"/>
+      <c r="AW94" s="8"/>
+      <c r="AX94" s="8"/>
+      <c r="AY94" s="8"/>
+      <c r="AZ94" s="9"/>
+      <c r="BA94" s="8"/>
+      <c r="BB94" s="9"/>
+      <c r="BC94" s="8"/>
+    </row>
+    <row r="95" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B95" s="8"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="8"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="8"/>
+      <c r="G95" s="8"/>
+      <c r="H95" s="8"/>
+      <c r="I95" s="8"/>
+      <c r="J95" s="8"/>
+      <c r="K95" s="8"/>
+      <c r="L95" s="8"/>
+      <c r="M95" s="8"/>
+      <c r="N95" s="8"/>
+      <c r="O95" s="8"/>
+      <c r="P95" s="8"/>
+      <c r="Q95" s="8"/>
+      <c r="R95" s="8"/>
+      <c r="S95" s="8"/>
+      <c r="T95" s="8"/>
+      <c r="U95" s="8"/>
+      <c r="V95" s="8"/>
+      <c r="W95" s="8"/>
+      <c r="X95" s="8"/>
+      <c r="Y95" s="8"/>
+      <c r="Z95" s="8"/>
+      <c r="AA95" s="8"/>
+      <c r="AB95" s="8"/>
+      <c r="AE95" s="7"/>
+      <c r="AF95" s="10"/>
+      <c r="AG95" s="11"/>
+      <c r="AH95" s="11"/>
+      <c r="AI95" s="11"/>
+      <c r="AJ95" s="11"/>
+      <c r="AK95" s="11"/>
+      <c r="AL95" s="11"/>
+      <c r="AM95" s="11"/>
+      <c r="AN95" s="11"/>
+      <c r="AO95" s="11"/>
+      <c r="AP95" s="11"/>
+      <c r="AQ95" s="11"/>
+      <c r="AR95" s="11"/>
+      <c r="AS95" s="11"/>
+      <c r="AT95" s="11"/>
+      <c r="AU95" s="11"/>
+      <c r="AV95" s="11"/>
+      <c r="AW95" s="11"/>
+      <c r="AX95" s="11"/>
+      <c r="AY95" s="11"/>
+      <c r="AZ95" s="12"/>
+      <c r="BA95" s="8"/>
+      <c r="BB95" s="9"/>
+      <c r="BC95" s="8"/>
+    </row>
+    <row r="96" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B96" s="8"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
+      <c r="F96" s="8"/>
+      <c r="G96" s="8"/>
+      <c r="H96" s="8"/>
+      <c r="I96" s="8"/>
+      <c r="J96" s="8"/>
+      <c r="K96" s="8"/>
+      <c r="L96" s="8"/>
+      <c r="M96" s="8"/>
+      <c r="N96" s="8"/>
+      <c r="O96" s="8"/>
+      <c r="P96" s="8"/>
+      <c r="Q96" s="8"/>
+      <c r="R96" s="8"/>
+      <c r="S96" s="8"/>
+      <c r="T96" s="8"/>
+      <c r="U96" s="8"/>
+      <c r="V96" s="8"/>
+      <c r="W96" s="8"/>
+      <c r="X96" s="8"/>
+      <c r="Y96" s="8"/>
+      <c r="Z96" s="8"/>
+      <c r="AA96" s="8"/>
+      <c r="AB96" s="8"/>
+      <c r="AE96" s="7"/>
+      <c r="AF96" s="8"/>
+      <c r="AG96" s="8"/>
+      <c r="AH96" s="8"/>
+      <c r="AI96" s="8"/>
+      <c r="AJ96" s="8"/>
+      <c r="AK96" s="8"/>
+      <c r="AL96" s="8"/>
+      <c r="AM96" s="8"/>
+      <c r="AN96" s="8"/>
+      <c r="AO96" s="8"/>
+      <c r="AP96" s="8"/>
+      <c r="AQ96" s="8"/>
+      <c r="AR96" s="8"/>
+      <c r="AS96" s="8"/>
+      <c r="AT96" s="8"/>
+      <c r="AU96" s="8"/>
+      <c r="AV96" s="8"/>
+      <c r="AW96" s="8"/>
+      <c r="AX96" s="8"/>
+      <c r="AY96" s="8"/>
+      <c r="AZ96" s="8"/>
+      <c r="BA96" s="8"/>
+      <c r="BB96" s="9"/>
+      <c r="BC96" s="8"/>
+    </row>
+    <row r="97" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B97" s="8"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="8"/>
+      <c r="E97" s="8"/>
+      <c r="F97" s="8"/>
+      <c r="G97" s="8"/>
+      <c r="H97" s="8"/>
+      <c r="I97" s="8"/>
+      <c r="J97" s="8"/>
+      <c r="K97" s="8"/>
+      <c r="L97" s="8"/>
+      <c r="M97" s="8"/>
+      <c r="N97" s="8"/>
+      <c r="O97" s="8"/>
+      <c r="P97" s="8"/>
+      <c r="Q97" s="8"/>
+      <c r="R97" s="8"/>
+      <c r="S97" s="8"/>
+      <c r="T97" s="8"/>
+      <c r="U97" s="8"/>
+      <c r="V97" s="8"/>
+      <c r="W97" s="8"/>
+      <c r="X97" s="8"/>
+      <c r="Y97" s="8"/>
+      <c r="Z97" s="8"/>
+      <c r="AA97" s="8"/>
+      <c r="AB97" s="8"/>
+      <c r="AE97" s="7"/>
+      <c r="AF97" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="AG97" s="3"/>
+      <c r="AH97" s="8"/>
+      <c r="AI97" s="8"/>
+      <c r="AJ97" s="8"/>
+      <c r="AK97" s="8"/>
+      <c r="AL97" s="8"/>
+      <c r="AM97" s="8"/>
+      <c r="AN97" s="8"/>
+      <c r="AO97" s="8"/>
+      <c r="AP97" s="8"/>
+      <c r="AQ97" s="8"/>
+      <c r="AR97" s="8"/>
+      <c r="AS97" s="8"/>
+      <c r="AT97" s="8"/>
+      <c r="AU97" s="8"/>
+      <c r="AV97" s="8"/>
+      <c r="AW97" s="8"/>
+      <c r="AX97" s="8"/>
+      <c r="AY97" s="8"/>
+      <c r="AZ97" s="8"/>
+      <c r="BA97" s="8"/>
+      <c r="BB97" s="9"/>
+      <c r="BC97" s="8"/>
+    </row>
+    <row r="98" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B98" s="8"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="8"/>
+      <c r="F98" s="8"/>
+      <c r="G98" s="8"/>
+      <c r="H98" s="8"/>
+      <c r="I98" s="8"/>
+      <c r="J98" s="8"/>
+      <c r="K98" s="8"/>
+      <c r="L98" s="8"/>
+      <c r="M98" s="8"/>
+      <c r="N98" s="8"/>
+      <c r="O98" s="8"/>
+      <c r="P98" s="8"/>
+      <c r="Q98" s="8"/>
+      <c r="R98" s="8"/>
+      <c r="S98" s="8"/>
+      <c r="T98" s="8"/>
+      <c r="U98" s="8"/>
+      <c r="V98" s="8"/>
+      <c r="W98" s="8"/>
+      <c r="X98" s="8"/>
+      <c r="Y98" s="8"/>
+      <c r="Z98" s="8"/>
+      <c r="AA98" s="8"/>
+      <c r="AB98" s="8"/>
+      <c r="AE98" s="10"/>
+      <c r="AF98" s="11"/>
+      <c r="AG98" s="11"/>
+      <c r="AH98" s="11"/>
+      <c r="AI98" s="11"/>
+      <c r="AJ98" s="11"/>
+      <c r="AK98" s="11"/>
+      <c r="AL98" s="11"/>
+      <c r="AM98" s="11"/>
+      <c r="AN98" s="11"/>
+      <c r="AO98" s="11"/>
+      <c r="AP98" s="11"/>
+      <c r="AQ98" s="11"/>
+      <c r="AR98" s="11"/>
+      <c r="AS98" s="11"/>
+      <c r="AT98" s="11"/>
+      <c r="AU98" s="11"/>
+      <c r="AV98" s="11"/>
+      <c r="AW98" s="11"/>
+      <c r="AX98" s="11"/>
+      <c r="AY98" s="11"/>
+      <c r="AZ98" s="11"/>
+      <c r="BA98" s="11"/>
+      <c r="BB98" s="12"/>
+    </row>
+    <row r="99" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="8"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="8"/>
+      <c r="I99" s="8"/>
+      <c r="J99" s="8"/>
+      <c r="K99" s="8"/>
+      <c r="L99" s="8"/>
+      <c r="M99" s="8"/>
+      <c r="N99" s="8"/>
+      <c r="O99" s="8"/>
+      <c r="P99" s="8"/>
+      <c r="Q99" s="8"/>
+      <c r="R99" s="8"/>
+      <c r="S99" s="8"/>
+      <c r="T99" s="8"/>
+      <c r="U99" s="8"/>
+      <c r="V99" s="8"/>
+      <c r="W99" s="8"/>
+      <c r="X99" s="8"/>
+      <c r="Y99" s="8"/>
+      <c r="Z99" s="8"/>
+      <c r="AA99" s="8"/>
+      <c r="AB99" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
query list hotel dan detail hotel
</commit_message>
<xml_diff>
--- a/document/spec.xlsx
+++ b/document/spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="7500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="7500" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Agent Register" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="401">
   <si>
     <t>Agent Register</t>
   </si>
@@ -1058,48 +1058,12 @@
     <t>querynya:</t>
   </si>
   <si>
-    <t xml:space="preserve">select </t>
-  </si>
-  <si>
-    <t>from mst020 a</t>
-  </si>
-  <si>
-    <t>inner join mst022 c on c.mst020_id = a.id</t>
-  </si>
-  <si>
-    <t>where a.mst002_id = countryid</t>
-  </si>
-  <si>
-    <t>and a.mst003_id = cityid</t>
-  </si>
-  <si>
-    <t>and  b.num_adult &gt;= adult</t>
-  </si>
-  <si>
-    <t>and b.allotment &gt;= room</t>
-  </si>
-  <si>
     <t>isi ke table blnc001-blnc003</t>
   </si>
   <si>
     <t>sama persis ma transaksinya cm beda ada stts_flg di table blnc001</t>
   </si>
   <si>
-    <t xml:space="preserve">                   and b.line_number =1</t>
-  </si>
-  <si>
-    <t>and  c.from_date &gt;= checkindate</t>
-  </si>
-  <si>
-    <t>and c.end_date &gt;= checkoutDate</t>
-  </si>
-  <si>
-    <t>left join (select e.pict as pict from mst021 e where e.line_number = (select max(f.line_number) from mst021 f where f.mst020_id = a.id)</t>
-  </si>
-  <si>
-    <t>and e.mst020_id = a.id) j</t>
-  </si>
-  <si>
     <t>Nama Hotel</t>
   </si>
   <si>
@@ -1248,6 +1212,18 @@
   </si>
   <si>
     <t>used_allotment</t>
+  </si>
+  <si>
+    <t>Lihat detail query di file searchListHotel.sql</t>
+  </si>
+  <si>
+    <t>combo room tu muncul sesuai jumlah allotment dari query tp ada maxnya</t>
+  </si>
+  <si>
+    <t>klo jumlah allotmentnya &gt; 10 yg muncul di combo 10</t>
+  </si>
+  <si>
+    <t>bs ga gini?</t>
   </si>
 </sst>
 </file>
@@ -1483,7 +1459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1547,6 +1523,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3596,7 +3573,7 @@
       <c r="W34" s="8"/>
       <c r="X34" s="9"/>
       <c r="AA34" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="35" spans="2:27" x14ac:dyDescent="0.25">
@@ -5473,7 +5450,7 @@
       <c r="AB37" s="8"/>
       <c r="AC37" s="9"/>
       <c r="AE37" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="38" spans="2:40" x14ac:dyDescent="0.25">
@@ -5508,7 +5485,7 @@
       <c r="AB38" s="8"/>
       <c r="AC38" s="9"/>
       <c r="AE38" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="39" spans="2:40" x14ac:dyDescent="0.25">
@@ -6784,7 +6761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC92"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C28" sqref="C28:Z54"/>
     </sheetView>
   </sheetViews>
@@ -9185,7 +9162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BE138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="S92" sqref="S92:S93"/>
     </sheetView>
   </sheetViews>
@@ -9220,7 +9197,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="1" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="3"/>
@@ -9254,7 +9231,7 @@
       <c r="AS2" s="44"/>
       <c r="AT2" s="43"/>
       <c r="AU2" s="52" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="AV2" s="44"/>
       <c r="AW2" s="43"/>
@@ -9300,7 +9277,7 @@
       <c r="AI3" s="39"/>
       <c r="AJ3" s="39"/>
       <c r="AK3" s="39" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="AL3" s="39"/>
       <c r="AM3" s="39"/>
@@ -9351,7 +9328,7 @@
       <c r="Z4" s="8"/>
       <c r="AE4" s="38"/>
       <c r="AF4" s="39" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="AG4" s="39"/>
       <c r="AH4" s="39"/>
@@ -9413,11 +9390,11 @@
         <v>247</v>
       </c>
       <c r="AG5" s="42" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="AH5" s="43"/>
       <c r="AI5" s="42" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="AJ5" s="44"/>
       <c r="AK5" s="44"/>
@@ -9473,7 +9450,7 @@
       <c r="AH6" s="40"/>
       <c r="AI6" s="55"/>
       <c r="AJ6" s="53" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="AK6" s="53"/>
       <c r="AL6" s="53"/>
@@ -10423,7 +10400,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="1" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="S34" s="2"/>
       <c r="T34" s="3"/>
@@ -11114,7 +11091,7 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="3"/>
       <c r="R57" s="1" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="S57" s="2"/>
       <c r="T57" s="3"/>
@@ -13515,7 +13492,7 @@
         <v>3</v>
       </c>
       <c r="C98" s="39" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="D98" s="39"/>
       <c r="E98" s="39"/>
@@ -13573,7 +13550,7 @@
     <row r="99" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B99" s="39"/>
       <c r="C99" s="39" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="D99" s="39"/>
       <c r="E99" s="39"/>
@@ -13629,7 +13606,7 @@
     <row r="100" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B100" s="39"/>
       <c r="C100" s="39" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="D100" s="39"/>
       <c r="E100" s="39"/>
@@ -13687,7 +13664,7 @@
     <row r="101" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B101" s="39"/>
       <c r="C101" s="39" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="D101" s="39"/>
       <c r="E101" s="39"/>
@@ -13744,7 +13721,7 @@
         <v>4</v>
       </c>
       <c r="C102" s="39" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="D102" s="39"/>
       <c r="E102" s="39"/>
@@ -14865,18 +14842,18 @@
     <row r="131" spans="31:54" x14ac:dyDescent="0.25">
       <c r="AE131" s="38"/>
       <c r="AF131" s="39" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="AG131" s="39"/>
       <c r="AH131" s="39"/>
       <c r="AI131" s="39" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="AJ131" s="39"/>
       <c r="AK131" s="39"/>
       <c r="AL131" s="39"/>
       <c r="AM131" s="39" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="AN131" s="39"/>
       <c r="AO131" s="39"/>
@@ -14904,7 +14881,7 @@
       </c>
       <c r="AH132" s="43"/>
       <c r="AI132" s="44" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="AJ132" s="44"/>
       <c r="AK132" s="44"/>
@@ -14932,7 +14909,7 @@
       <c r="AG133" s="38"/>
       <c r="AH133" s="40"/>
       <c r="AI133" s="39" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="AJ133" s="39"/>
       <c r="AK133" s="39"/>
@@ -15096,13 +15073,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AP45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AO12" sqref="AO12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AI7" sqref="AI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
         <v>82</v>
@@ -15134,7 +15111,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="3" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -15161,10 +15138,10 @@
       <c r="Y3" s="8"/>
       <c r="Z3" s="9"/>
       <c r="AC3" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="4" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
         <v>3</v>
@@ -15198,11 +15175,8 @@
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
       <c r="Z4" s="9"/>
-      <c r="AC4" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -15228,11 +15202,8 @@
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
       <c r="Z5" s="9"/>
-      <c r="AC5" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>330</v>
@@ -15264,11 +15235,8 @@
       <c r="X6" s="3"/>
       <c r="Y6" s="8"/>
       <c r="Z6" s="9"/>
-      <c r="AC6" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -15294,14 +15262,8 @@
       <c r="X7" s="8"/>
       <c r="Y7" s="8"/>
       <c r="Z7" s="9"/>
-      <c r="AC7" t="s">
-        <v>354</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="8" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="s">
         <v>331</v>
@@ -15334,11 +15296,8 @@
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
       <c r="Z8" s="9"/>
-      <c r="AC8" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -15367,11 +15326,8 @@
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
       <c r="Z9" s="9"/>
-      <c r="AC9" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="8" t="s">
         <v>187</v>
@@ -15403,7 +15359,7 @@
       <c r="Y10" s="8"/>
       <c r="Z10" s="9"/>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -15429,11 +15385,8 @@
       <c r="X11" s="8"/>
       <c r="Y11" s="8"/>
       <c r="Z11" s="9"/>
-      <c r="AC11" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="C12" s="1" t="s">
         <v>82</v>
@@ -15462,7 +15415,7 @@
       <c r="Y12" s="8"/>
       <c r="Z12" s="9"/>
     </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -15488,24 +15441,13 @@
       <c r="X13" s="11"/>
       <c r="Y13" s="11"/>
       <c r="Z13" s="12"/>
-      <c r="AC13" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="14" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="AC14" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="15" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>336</v>
       </c>
-      <c r="AC15" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -16466,18 +16408,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BB71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AF47" sqref="AF47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="AI37" sqref="AI37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="F2" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3" spans="2:54" x14ac:dyDescent="0.25">
@@ -16821,7 +16763,7 @@
       <c r="P12" s="8"/>
       <c r="Q12" s="9"/>
       <c r="AD12" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="AG12" s="8"/>
       <c r="AH12" s="8"/>
@@ -16913,7 +16855,7 @@
       <c r="V14" s="9"/>
       <c r="X14" s="7"/>
       <c r="Y14" s="8" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="Z14" s="8"/>
       <c r="AA14" s="9"/>
@@ -17005,7 +16947,7 @@
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -17013,12 +16955,12 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -17043,7 +16985,7 @@
       <c r="AM17" s="8"/>
       <c r="AN17" s="8"/>
       <c r="AO17" s="8" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="AP17" s="8"/>
       <c r="AQ17" s="8"/>
@@ -17087,7 +17029,7 @@
       <c r="AA18" s="9"/>
       <c r="AI18" s="7"/>
       <c r="AJ18" s="8" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="AK18" s="8"/>
       <c r="AL18" s="8"/>
@@ -17490,7 +17432,7 @@
     </row>
     <row r="28" spans="1:53" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.25">
@@ -17523,6 +17465,26 @@
       <c r="AA29" s="5"/>
       <c r="AB29" s="5"/>
       <c r="AC29" s="6"/>
+      <c r="AE29" s="59" t="s">
+        <v>398</v>
+      </c>
+      <c r="AF29" s="59"/>
+      <c r="AG29" s="59"/>
+      <c r="AH29" s="59"/>
+      <c r="AI29" s="59"/>
+      <c r="AJ29" s="59"/>
+      <c r="AK29" s="59"/>
+      <c r="AL29" s="59"/>
+      <c r="AM29" s="59"/>
+      <c r="AN29" s="59"/>
+      <c r="AO29" s="59"/>
+      <c r="AP29" s="59"/>
+      <c r="AQ29" s="59"/>
+      <c r="AR29" s="59"/>
+      <c r="AS29" s="59"/>
+      <c r="AT29" s="59"/>
+      <c r="AU29" s="59"/>
+      <c r="AV29" s="59"/>
     </row>
     <row r="30" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
@@ -17532,18 +17494,18 @@
       <c r="E30" s="6"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
       <c r="N30" s="8" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="O30" s="8"/>
       <c r="P30" s="8"/>
@@ -17560,6 +17522,26 @@
       <c r="AA30" s="8"/>
       <c r="AB30" s="8"/>
       <c r="AC30" s="9"/>
+      <c r="AE30" s="59" t="s">
+        <v>399</v>
+      </c>
+      <c r="AF30" s="59"/>
+      <c r="AG30" s="59"/>
+      <c r="AH30" s="59"/>
+      <c r="AI30" s="59"/>
+      <c r="AJ30" s="59"/>
+      <c r="AK30" s="59"/>
+      <c r="AL30" s="59"/>
+      <c r="AM30" s="59"/>
+      <c r="AN30" s="59"/>
+      <c r="AO30" s="59"/>
+      <c r="AP30" s="59"/>
+      <c r="AQ30" s="59"/>
+      <c r="AR30" s="59"/>
+      <c r="AS30" s="59"/>
+      <c r="AT30" s="59"/>
+      <c r="AU30" s="59"/>
+      <c r="AV30" s="59"/>
     </row>
     <row r="31" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
@@ -17585,14 +17567,34 @@
       <c r="V31" s="8"/>
       <c r="W31" s="8"/>
       <c r="X31" s="8" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="Z31" s="4" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="AA31" s="5"/>
       <c r="AB31" s="6"/>
       <c r="AC31" s="9"/>
+      <c r="AE31" s="59" t="s">
+        <v>400</v>
+      </c>
+      <c r="AF31" s="59"/>
+      <c r="AG31" s="59"/>
+      <c r="AH31" s="59"/>
+      <c r="AI31" s="59"/>
+      <c r="AJ31" s="59"/>
+      <c r="AK31" s="59"/>
+      <c r="AL31" s="59"/>
+      <c r="AM31" s="59"/>
+      <c r="AN31" s="59"/>
+      <c r="AO31" s="59"/>
+      <c r="AP31" s="59"/>
+      <c r="AQ31" s="59"/>
+      <c r="AR31" s="59"/>
+      <c r="AS31" s="59"/>
+      <c r="AT31" s="59"/>
+      <c r="AU31" s="59"/>
+      <c r="AV31" s="59"/>
     </row>
     <row r="32" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
@@ -17602,7 +17604,7 @@
       <c r="E32" s="9"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
@@ -17612,7 +17614,7 @@
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
       <c r="P32" s="8" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
@@ -17637,14 +17639,14 @@
       <c r="E33" s="12"/>
       <c r="F33" s="8"/>
       <c r="G33" s="36" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="I33" s="8"/>
       <c r="J33" s="8" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
@@ -17652,12 +17654,12 @@
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
       <c r="P33" s="58" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="T33" s="8"/>
       <c r="U33" s="8"/>
@@ -17677,14 +17679,14 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="37" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="H34" s="8"/>
       <c r="I34" s="8" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
@@ -17728,7 +17730,7 @@
       <c r="S35" s="11"/>
       <c r="T35" s="11"/>
       <c r="U35" s="11" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="V35" s="11"/>
       <c r="W35" s="11"/>
@@ -17778,18 +17780,18 @@
       <c r="E38" s="6"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
       <c r="N38" s="8" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="O38" s="8"/>
       <c r="P38" s="8"/>
@@ -17832,10 +17834,10 @@
       <c r="V39" s="8"/>
       <c r="W39" s="8"/>
       <c r="X39" s="8" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="Z39" s="4" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="AA39" s="5"/>
       <c r="AB39" s="6"/>
@@ -17849,7 +17851,7 @@
       <c r="E40" s="9"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
@@ -17860,7 +17862,7 @@
       <c r="N40" s="8"/>
       <c r="O40" s="8"/>
       <c r="P40" s="8" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
@@ -17885,10 +17887,10 @@
       <c r="E41" s="12"/>
       <c r="F41" s="8"/>
       <c r="G41" s="36" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
@@ -17898,12 +17900,12 @@
       <c r="N41" s="8"/>
       <c r="O41" s="8"/>
       <c r="P41" s="58" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
       <c r="S41" s="8" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="T41" s="8"/>
       <c r="U41" s="8"/>
@@ -17923,11 +17925,11 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="37" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="H42" s="8"/>
       <c r="I42" s="8" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
@@ -18020,18 +18022,18 @@
       <c r="E46" s="6"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
       <c r="K46" s="8" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="L46" s="8"/>
       <c r="M46" s="8"/>
       <c r="N46" s="8" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="O46" s="8"/>
       <c r="P46" s="8"/>
@@ -18074,10 +18076,10 @@
       <c r="V47" s="8"/>
       <c r="W47" s="8"/>
       <c r="X47" s="8" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="Z47" s="4" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="AA47" s="5"/>
       <c r="AB47" s="6"/>
@@ -18091,7 +18093,7 @@
       <c r="E48" s="9"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
@@ -18102,7 +18104,7 @@
       <c r="N48" s="8"/>
       <c r="O48" s="8"/>
       <c r="P48" s="8" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="Q48" s="8"/>
       <c r="R48" s="8"/>
@@ -18127,14 +18129,14 @@
       <c r="E49" s="12"/>
       <c r="F49" s="8"/>
       <c r="G49" s="36" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="I49" s="8"/>
       <c r="J49" s="8" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
@@ -18142,12 +18144,12 @@
       <c r="N49" s="8"/>
       <c r="O49" s="8"/>
       <c r="P49" s="58" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="Q49" s="8"/>
       <c r="R49" s="8"/>
       <c r="S49" s="8" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="T49" s="8"/>
       <c r="U49" s="8"/>
@@ -18167,14 +18169,14 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="37" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="H50" s="8"/>
       <c r="I50" s="8" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="J50" s="8" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
@@ -18229,7 +18231,7 @@
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -18263,15 +18265,15 @@
     <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="8" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
       <c r="F54" s="8" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
@@ -18300,10 +18302,10 @@
     <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="8" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
@@ -18335,10 +18337,10 @@
     <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="8" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
@@ -18370,10 +18372,10 @@
     <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="19" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
@@ -18405,10 +18407,10 @@
     <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="19" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
@@ -18470,7 +18472,7 @@
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
@@ -18627,7 +18629,7 @@
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -18863,12 +18865,12 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
@@ -18878,7 +18880,7 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="2"/>
@@ -18888,7 +18890,7 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="2"/>

</xml_diff>

<commit_message>
perubahan table TRX dan BLNC
</commit_message>
<xml_diff>
--- a/document/spec.xlsx
+++ b/document/spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="7500" tabRatio="710" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="7500" tabRatio="710"/>
   </bookViews>
   <sheets>
     <sheet name="Agent Menu" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="480">
   <si>
     <t>Agent Register</t>
   </si>
@@ -1331,12 +1331,6 @@
     <t>Tamu</t>
   </si>
   <si>
-    <t>Konfirmasi Pembayaran</t>
-  </si>
-  <si>
-    <t>Biaya Pembatalan</t>
-  </si>
-  <si>
     <t>Total Pembayaran</t>
   </si>
   <si>
@@ -1358,9 +1352,6 @@
     <t>Detail Order</t>
   </si>
   <si>
-    <t>Alamat</t>
-  </si>
-  <si>
     <t>Hotel ABC</t>
   </si>
   <si>
@@ -1391,9 +1382,6 @@
     <t>Detail Booking</t>
   </si>
   <si>
-    <t>Kamar</t>
-  </si>
-  <si>
     <t>Rooms</t>
   </si>
   <si>
@@ -1440,6 +1428,39 @@
   </si>
   <si>
     <t>Remaining Deposit</t>
+  </si>
+  <si>
+    <t>Tanggal Pembayaran</t>
+  </si>
+  <si>
+    <t>bisa kosong semua</t>
+  </si>
+  <si>
+    <t>Room Only/Inc Breakfast (type)</t>
+  </si>
+  <si>
+    <t>Total Room</t>
+  </si>
+  <si>
+    <t>Room/IncBreakFast</t>
+  </si>
+  <si>
+    <t>dibuat tulisannya jd</t>
+  </si>
+  <si>
+    <t>Room Only / Include Breakfast</t>
+  </si>
+  <si>
+    <t>Part of Group</t>
+  </si>
+  <si>
+    <t>Group Name</t>
+  </si>
+  <si>
+    <t>Kalau part of grup dicentang</t>
+  </si>
+  <si>
+    <t>grup name harus diisi,klo ga sebaliknya</t>
   </si>
 </sst>
 </file>
@@ -1479,7 +1500,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1495,6 +1516,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1681,7 +1708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1754,6 +1781,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2212,10 +2246,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:BC141"/>
+  <dimension ref="B1:BC145"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="N115" sqref="N115"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="K135" sqref="K135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3544,7 +3578,7 @@
       <c r="B54" s="7"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
@@ -3618,7 +3652,7 @@
       <c r="C57" s="8"/>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="F57" s="8"/>
       <c r="G57" s="9"/>
@@ -3757,12 +3791,12 @@
       <c r="U62" s="11"/>
       <c r="V62" s="12"/>
     </row>
-    <row r="65" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B65" s="24" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="67" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>429</v>
       </c>
@@ -3772,7 +3806,12 @@
       <c r="L67" s="2"/>
       <c r="M67" s="3"/>
     </row>
-    <row r="69" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AD68" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="69" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>33</v>
       </c>
@@ -3790,7 +3829,7 @@
       <c r="X69" s="2"/>
       <c r="Y69" s="3"/>
     </row>
-    <row r="71" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>3</v>
       </c>
@@ -3809,7 +3848,7 @@
       <c r="W71" s="2"/>
       <c r="X71" s="3"/>
     </row>
-    <row r="73" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
         <v>431</v>
       </c>
@@ -3823,12 +3862,12 @@
         <v>432</v>
       </c>
     </row>
-    <row r="76" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C76" s="13" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="78" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C78" s="1" t="s">
         <v>434</v>
       </c>
@@ -3836,12 +3875,12 @@
       <c r="E78" s="2"/>
       <c r="F78" s="3"/>
       <c r="G78" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="H78" s="2"/>
       <c r="I78" s="3"/>
       <c r="J78" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="K78" s="2"/>
       <c r="L78" s="3"/>
@@ -3851,7 +3890,7 @@
       <c r="N78" s="2"/>
       <c r="O78" s="3"/>
       <c r="P78" s="1" t="s">
-        <v>436</v>
+        <v>469</v>
       </c>
       <c r="Q78" s="2"/>
       <c r="R78" s="2"/>
@@ -3860,31 +3899,23 @@
       <c r="U78" s="3"/>
       <c r="V78" s="1"/>
       <c r="W78" s="2" t="s">
-        <v>437</v>
+        <v>79</v>
       </c>
       <c r="X78" s="2"/>
-      <c r="Y78" s="2"/>
-      <c r="Z78" s="2"/>
-      <c r="AA78" s="3"/>
-      <c r="AB78" s="1"/>
-      <c r="AC78" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD78" s="2"/>
-      <c r="AE78" s="3"/>
-      <c r="AF78" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="AG78" s="2"/>
-      <c r="AH78" s="2"/>
-      <c r="AI78" s="2"/>
-      <c r="AJ78" s="3"/>
-      <c r="AK78" s="4"/>
-      <c r="AL78" s="5"/>
-      <c r="AM78" s="5"/>
-      <c r="AN78" s="3"/>
-    </row>
-    <row r="79" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="Y78" s="3"/>
+      <c r="Z78" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="AA78" s="2"/>
+      <c r="AB78" s="2"/>
+      <c r="AC78" s="2"/>
+      <c r="AD78" s="3"/>
+      <c r="AE78" s="4"/>
+      <c r="AF78" s="5"/>
+      <c r="AG78" s="5"/>
+      <c r="AH78" s="3"/>
+    </row>
+    <row r="79" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C79" s="7"/>
       <c r="D79" s="8"/>
       <c r="E79" s="8"/>
@@ -3907,26 +3938,20 @@
       <c r="V79" s="7"/>
       <c r="W79" s="8"/>
       <c r="X79" s="8"/>
-      <c r="Y79" s="8"/>
+      <c r="Y79" s="9"/>
       <c r="Z79" s="8"/>
-      <c r="AA79" s="9"/>
-      <c r="AB79" s="7"/>
+      <c r="AA79" s="8"/>
+      <c r="AB79" s="8"/>
       <c r="AC79" s="8"/>
-      <c r="AD79" s="8"/>
-      <c r="AE79" s="9"/>
-      <c r="AF79" s="8"/>
-      <c r="AG79" s="8"/>
-      <c r="AH79" s="8"/>
-      <c r="AI79" s="8"/>
-      <c r="AJ79" s="9"/>
-      <c r="AK79" s="30" t="s">
-        <v>442</v>
-      </c>
-      <c r="AL79" s="2"/>
-      <c r="AM79" s="3"/>
-      <c r="AN79" s="9"/>
-    </row>
-    <row r="80" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="AD79" s="9"/>
+      <c r="AE79" s="30" t="s">
+        <v>440</v>
+      </c>
+      <c r="AF79" s="2"/>
+      <c r="AG79" s="3"/>
+      <c r="AH79" s="9"/>
+    </row>
+    <row r="80" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C80" s="7"/>
       <c r="D80" s="8"/>
       <c r="E80" s="8"/>
@@ -3949,22 +3974,16 @@
       <c r="V80" s="7"/>
       <c r="W80" s="8"/>
       <c r="X80" s="8"/>
-      <c r="Y80" s="8"/>
+      <c r="Y80" s="9"/>
       <c r="Z80" s="8"/>
-      <c r="AA80" s="9"/>
-      <c r="AB80" s="7"/>
+      <c r="AA80" s="8"/>
+      <c r="AB80" s="8"/>
       <c r="AC80" s="8"/>
-      <c r="AD80" s="8"/>
-      <c r="AE80" s="9"/>
+      <c r="AD80" s="9"/>
+      <c r="AE80" s="7"/>
       <c r="AF80" s="8"/>
       <c r="AG80" s="8"/>
-      <c r="AH80" s="8"/>
-      <c r="AI80" s="8"/>
-      <c r="AJ80" s="9"/>
-      <c r="AK80" s="7"/>
-      <c r="AL80" s="8"/>
-      <c r="AM80" s="8"/>
-      <c r="AN80" s="9"/>
+      <c r="AH80" s="9"/>
     </row>
     <row r="81" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C81" s="7"/>
@@ -3989,24 +4008,18 @@
       <c r="V81" s="7"/>
       <c r="W81" s="8"/>
       <c r="X81" s="8"/>
-      <c r="Y81" s="8"/>
+      <c r="Y81" s="9"/>
       <c r="Z81" s="8"/>
-      <c r="AA81" s="9"/>
-      <c r="AB81" s="7"/>
+      <c r="AA81" s="8"/>
+      <c r="AB81" s="8"/>
       <c r="AC81" s="8"/>
-      <c r="AD81" s="8"/>
-      <c r="AE81" s="9"/>
-      <c r="AF81" s="8"/>
-      <c r="AG81" s="8"/>
-      <c r="AH81" s="8"/>
-      <c r="AI81" s="8"/>
-      <c r="AJ81" s="9"/>
-      <c r="AK81" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="AL81" s="2"/>
-      <c r="AM81" s="3"/>
-      <c r="AN81" s="9"/>
+      <c r="AD81" s="9"/>
+      <c r="AE81" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="AF81" s="2"/>
+      <c r="AG81" s="3"/>
+      <c r="AH81" s="9"/>
     </row>
     <row r="82" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C82" s="10"/>
@@ -4031,22 +4044,16 @@
       <c r="V82" s="10"/>
       <c r="W82" s="11"/>
       <c r="X82" s="11"/>
-      <c r="Y82" s="11"/>
+      <c r="Y82" s="12"/>
       <c r="Z82" s="11"/>
-      <c r="AA82" s="12"/>
-      <c r="AB82" s="10"/>
+      <c r="AA82" s="11"/>
+      <c r="AB82" s="11"/>
       <c r="AC82" s="11"/>
-      <c r="AD82" s="11"/>
-      <c r="AE82" s="12"/>
+      <c r="AD82" s="12"/>
+      <c r="AE82" s="10"/>
       <c r="AF82" s="11"/>
       <c r="AG82" s="11"/>
-      <c r="AH82" s="11"/>
-      <c r="AI82" s="11"/>
-      <c r="AJ82" s="12"/>
-      <c r="AK82" s="10"/>
-      <c r="AL82" s="11"/>
-      <c r="AM82" s="11"/>
-      <c r="AN82" s="12"/>
+      <c r="AH82" s="12"/>
     </row>
     <row r="83" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C83" s="7"/>
@@ -4071,22 +4078,16 @@
       <c r="V83" s="7"/>
       <c r="W83" s="8"/>
       <c r="X83" s="8"/>
-      <c r="Y83" s="8"/>
+      <c r="Y83" s="9"/>
       <c r="Z83" s="8"/>
-      <c r="AA83" s="9"/>
-      <c r="AB83" s="7"/>
+      <c r="AA83" s="8"/>
+      <c r="AB83" s="8"/>
       <c r="AC83" s="8"/>
-      <c r="AD83" s="8"/>
-      <c r="AE83" s="9"/>
+      <c r="AD83" s="9"/>
+      <c r="AE83" s="7"/>
       <c r="AF83" s="8"/>
       <c r="AG83" s="8"/>
-      <c r="AH83" s="8"/>
-      <c r="AI83" s="8"/>
-      <c r="AJ83" s="9"/>
-      <c r="AK83" s="7"/>
-      <c r="AL83" s="8"/>
-      <c r="AM83" s="8"/>
-      <c r="AN83" s="9"/>
+      <c r="AH83" s="9"/>
     </row>
     <row r="84" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C84" s="7"/>
@@ -4111,24 +4112,18 @@
       <c r="V84" s="7"/>
       <c r="W84" s="8"/>
       <c r="X84" s="8"/>
-      <c r="Y84" s="8"/>
+      <c r="Y84" s="9"/>
       <c r="Z84" s="8"/>
-      <c r="AA84" s="9"/>
-      <c r="AB84" s="7"/>
+      <c r="AA84" s="8"/>
+      <c r="AB84" s="8"/>
       <c r="AC84" s="8"/>
-      <c r="AD84" s="8"/>
-      <c r="AE84" s="9"/>
-      <c r="AF84" s="8"/>
-      <c r="AG84" s="8"/>
-      <c r="AH84" s="8"/>
-      <c r="AI84" s="8"/>
-      <c r="AJ84" s="9"/>
-      <c r="AK84" s="30" t="s">
-        <v>442</v>
-      </c>
-      <c r="AL84" s="2"/>
-      <c r="AM84" s="3"/>
-      <c r="AN84" s="9"/>
+      <c r="AD84" s="9"/>
+      <c r="AE84" s="30" t="s">
+        <v>440</v>
+      </c>
+      <c r="AF84" s="2"/>
+      <c r="AG84" s="3"/>
+      <c r="AH84" s="9"/>
     </row>
     <row r="85" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C85" s="7"/>
@@ -4153,22 +4148,16 @@
       <c r="V85" s="7"/>
       <c r="W85" s="8"/>
       <c r="X85" s="8"/>
-      <c r="Y85" s="8"/>
+      <c r="Y85" s="9"/>
       <c r="Z85" s="8"/>
-      <c r="AA85" s="9"/>
-      <c r="AB85" s="7"/>
+      <c r="AA85" s="8"/>
+      <c r="AB85" s="8"/>
       <c r="AC85" s="8"/>
-      <c r="AD85" s="8"/>
-      <c r="AE85" s="9"/>
+      <c r="AD85" s="9"/>
+      <c r="AE85" s="7"/>
       <c r="AF85" s="8"/>
       <c r="AG85" s="8"/>
-      <c r="AH85" s="8"/>
-      <c r="AI85" s="8"/>
-      <c r="AJ85" s="9"/>
-      <c r="AK85" s="7"/>
-      <c r="AL85" s="8"/>
-      <c r="AM85" s="8"/>
-      <c r="AN85" s="9"/>
+      <c r="AH85" s="9"/>
     </row>
     <row r="86" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C86" s="7"/>
@@ -4193,24 +4182,18 @@
       <c r="V86" s="7"/>
       <c r="W86" s="8"/>
       <c r="X86" s="8"/>
-      <c r="Y86" s="8"/>
+      <c r="Y86" s="9"/>
       <c r="Z86" s="8"/>
-      <c r="AA86" s="9"/>
-      <c r="AB86" s="7"/>
+      <c r="AA86" s="8"/>
+      <c r="AB86" s="8"/>
       <c r="AC86" s="8"/>
-      <c r="AD86" s="8"/>
-      <c r="AE86" s="9"/>
-      <c r="AF86" s="8"/>
-      <c r="AG86" s="8"/>
-      <c r="AH86" s="8"/>
-      <c r="AI86" s="8"/>
-      <c r="AJ86" s="9"/>
-      <c r="AK86" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="AL86" s="2"/>
-      <c r="AM86" s="3"/>
-      <c r="AN86" s="9"/>
+      <c r="AD86" s="9"/>
+      <c r="AE86" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="AF86" s="2"/>
+      <c r="AG86" s="3"/>
+      <c r="AH86" s="9"/>
     </row>
     <row r="87" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C87" s="10"/>
@@ -4235,22 +4218,16 @@
       <c r="V87" s="10"/>
       <c r="W87" s="11"/>
       <c r="X87" s="11"/>
-      <c r="Y87" s="11"/>
+      <c r="Y87" s="12"/>
       <c r="Z87" s="11"/>
-      <c r="AA87" s="12"/>
-      <c r="AB87" s="10"/>
+      <c r="AA87" s="11"/>
+      <c r="AB87" s="11"/>
       <c r="AC87" s="11"/>
-      <c r="AD87" s="11"/>
-      <c r="AE87" s="12"/>
+      <c r="AD87" s="12"/>
+      <c r="AE87" s="10"/>
       <c r="AF87" s="11"/>
       <c r="AG87" s="11"/>
-      <c r="AH87" s="11"/>
-      <c r="AI87" s="11"/>
-      <c r="AJ87" s="12"/>
-      <c r="AK87" s="10"/>
-      <c r="AL87" s="11"/>
-      <c r="AM87" s="11"/>
-      <c r="AN87" s="12"/>
+      <c r="AH87" s="12"/>
     </row>
     <row r="88" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C88" s="10"/>
@@ -4275,26 +4252,20 @@
       <c r="V88" s="10"/>
       <c r="W88" s="11"/>
       <c r="X88" s="11"/>
-      <c r="Y88" s="11"/>
+      <c r="Y88" s="12"/>
       <c r="Z88" s="11"/>
-      <c r="AA88" s="12"/>
-      <c r="AB88" s="10"/>
+      <c r="AA88" s="11"/>
+      <c r="AB88" s="11"/>
       <c r="AC88" s="11"/>
-      <c r="AD88" s="11"/>
-      <c r="AE88" s="12"/>
+      <c r="AD88" s="12"/>
+      <c r="AE88" s="10"/>
       <c r="AF88" s="11"/>
       <c r="AG88" s="11"/>
-      <c r="AH88" s="11"/>
-      <c r="AI88" s="11"/>
-      <c r="AJ88" s="12"/>
-      <c r="AK88" s="10"/>
-      <c r="AL88" s="11"/>
-      <c r="AM88" s="11"/>
-      <c r="AN88" s="12"/>
+      <c r="AH88" s="12"/>
     </row>
     <row r="91" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C91" s="24" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="92" spans="3:55" x14ac:dyDescent="0.25">
@@ -4352,7 +4323,7 @@
     </row>
     <row r="93" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C93" s="17" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D93" s="8"/>
       <c r="E93" s="8"/>
@@ -4381,7 +4352,7 @@
       <c r="AB93" s="8"/>
       <c r="AC93" s="9"/>
       <c r="AF93" s="7" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="AG93" s="8"/>
       <c r="AH93" s="8"/>
@@ -4456,7 +4427,7 @@
       <c r="AX94" s="11"/>
       <c r="AY94" s="11"/>
       <c r="AZ94" s="11" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="BA94" s="11"/>
       <c r="BB94" s="11"/>
@@ -4478,11 +4449,15 @@
       <c r="K95" s="8"/>
       <c r="L95" s="8"/>
       <c r="M95" s="8"/>
-      <c r="N95" s="8"/>
+      <c r="N95" s="8" t="s">
+        <v>451</v>
+      </c>
       <c r="O95" s="8"/>
       <c r="P95" s="8"/>
       <c r="Q95" s="8"/>
-      <c r="R95" s="8"/>
+      <c r="R95" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="S95" s="8"/>
       <c r="T95" s="8"/>
       <c r="U95" s="7"/>
@@ -4565,7 +4540,7 @@
       <c r="AO96" s="8"/>
       <c r="AP96" s="8"/>
       <c r="AQ96" s="8" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="AR96" s="8"/>
       <c r="AS96" s="8"/>
@@ -4600,11 +4575,15 @@
       <c r="K97" s="8"/>
       <c r="L97" s="8"/>
       <c r="M97" s="8"/>
-      <c r="N97" s="8"/>
+      <c r="N97" s="8" t="s">
+        <v>418</v>
+      </c>
       <c r="O97" s="8"/>
       <c r="P97" s="8"/>
       <c r="Q97" s="8"/>
-      <c r="R97" s="8"/>
+      <c r="R97" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="S97" s="8"/>
       <c r="T97" s="8"/>
       <c r="U97" s="7"/>
@@ -4670,7 +4649,7 @@
       <c r="AB98" s="8"/>
       <c r="AC98" s="9"/>
       <c r="AF98" s="7" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="AG98" s="8"/>
       <c r="AH98" s="8"/>
@@ -4697,10 +4676,14 @@
       <c r="AW98" s="8"/>
       <c r="AX98" s="8"/>
       <c r="AY98" s="8"/>
-      <c r="AZ98" s="8"/>
+      <c r="AZ98" s="8" t="s">
+        <v>418</v>
+      </c>
       <c r="BA98" s="8"/>
       <c r="BB98" s="8"/>
-      <c r="BC98" s="9"/>
+      <c r="BC98" s="9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="99" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C99" s="7" t="s">
@@ -4788,7 +4771,7 @@
       <c r="AB100" s="8"/>
       <c r="AC100" s="9"/>
       <c r="AF100" s="18" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="AG100" s="5"/>
       <c r="AH100" s="5"/>
@@ -4838,7 +4821,7 @@
       <c r="S101" s="8"/>
       <c r="T101" s="8"/>
       <c r="U101" s="15" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="V101" s="8"/>
       <c r="W101" s="8"/>
@@ -4928,7 +4911,7 @@
     </row>
     <row r="103" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C103" s="7" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D103" s="8"/>
       <c r="E103" s="8"/>
@@ -4950,7 +4933,7 @@
       <c r="S103" s="8"/>
       <c r="T103" s="8"/>
       <c r="U103" s="15" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="V103" s="8"/>
       <c r="W103" s="8"/>
@@ -5044,7 +5027,7 @@
     </row>
     <row r="105" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C105" s="7" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D105" s="8"/>
       <c r="E105" s="8"/>
@@ -5066,27 +5049,24 @@
       <c r="S105" s="8"/>
       <c r="T105" s="8"/>
       <c r="U105" s="8" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="V105" s="8"/>
       <c r="W105" s="8"/>
       <c r="X105" s="8" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="Y105" s="8"/>
       <c r="Z105" s="8"/>
       <c r="AA105" s="8" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="AB105" s="8"/>
       <c r="AC105" s="9"/>
       <c r="AF105" s="7" t="s">
-        <v>456</v>
-      </c>
-      <c r="AG105" s="8"/>
-      <c r="AH105" s="8"/>
-      <c r="AI105" s="8"/>
-      <c r="AJ105" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ105" t="s">
         <v>35</v>
       </c>
       <c r="AK105" s="8"/>
@@ -5138,10 +5118,6 @@
       <c r="AB106" s="8"/>
       <c r="AC106" s="9"/>
       <c r="AF106" s="7"/>
-      <c r="AG106" s="8"/>
-      <c r="AH106" s="8"/>
-      <c r="AI106" s="8"/>
-      <c r="AJ106" s="8"/>
       <c r="AK106" s="8"/>
       <c r="AL106" s="8"/>
       <c r="AM106" s="8"/>
@@ -5185,8 +5161,12 @@
       <c r="R107" s="8"/>
       <c r="S107" s="8"/>
       <c r="T107" s="8"/>
-      <c r="U107" s="8"/>
-      <c r="V107" s="8"/>
+      <c r="U107" s="8">
+        <v>2</v>
+      </c>
+      <c r="V107" s="8" t="s">
+        <v>213</v>
+      </c>
       <c r="W107" s="8"/>
       <c r="X107" s="8"/>
       <c r="Y107" s="8"/>
@@ -5195,7 +5175,7 @@
       <c r="AB107" s="8"/>
       <c r="AC107" s="9"/>
       <c r="AF107" s="7" t="s">
-        <v>445</v>
+        <v>143</v>
       </c>
       <c r="AG107" s="8"/>
       <c r="AH107" s="8"/>
@@ -5242,7 +5222,9 @@
       <c r="R108" s="8"/>
       <c r="S108" s="8"/>
       <c r="T108" s="8"/>
-      <c r="U108" s="8"/>
+      <c r="U108" s="8" t="s">
+        <v>471</v>
+      </c>
       <c r="V108" s="8"/>
       <c r="W108" s="8"/>
       <c r="X108" s="8"/>
@@ -5278,13 +5260,13 @@
     </row>
     <row r="109" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C109" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D109" s="2"/>
       <c r="E109" s="3"/>
       <c r="F109" s="8"/>
       <c r="G109" s="1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="H109" s="3"/>
       <c r="I109" s="2"/>
@@ -5309,33 +5291,11 @@
       <c r="AB109" s="8"/>
       <c r="AC109" s="9"/>
       <c r="AF109" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG109" s="8"/>
-      <c r="AH109" s="8"/>
-      <c r="AI109" s="8"/>
-      <c r="AJ109" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ109" t="s">
         <v>35</v>
       </c>
-      <c r="AK109" s="8"/>
-      <c r="AL109" s="8"/>
-      <c r="AM109" s="8"/>
-      <c r="AN109" s="8"/>
-      <c r="AO109" s="8"/>
-      <c r="AP109" s="8"/>
-      <c r="AQ109" s="8"/>
-      <c r="AR109" s="8"/>
-      <c r="AS109" s="8"/>
-      <c r="AT109" s="8"/>
-      <c r="AU109" s="8"/>
-      <c r="AV109" s="8"/>
-      <c r="AW109" s="8"/>
-      <c r="AX109" s="8"/>
-      <c r="AY109" s="8"/>
-      <c r="AZ109" s="8"/>
-      <c r="BA109" s="8"/>
-      <c r="BB109" s="8"/>
-      <c r="BC109" s="9"/>
     </row>
     <row r="110" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C110" s="7"/>
@@ -5366,29 +5326,6 @@
       <c r="AB110" s="8"/>
       <c r="AC110" s="9"/>
       <c r="AF110" s="7"/>
-      <c r="AG110" s="8"/>
-      <c r="AH110" s="8"/>
-      <c r="AI110" s="8"/>
-      <c r="AJ110" s="8"/>
-      <c r="AK110" s="8"/>
-      <c r="AL110" s="8"/>
-      <c r="AM110" s="8"/>
-      <c r="AN110" s="8"/>
-      <c r="AO110" s="8"/>
-      <c r="AP110" s="8"/>
-      <c r="AQ110" s="8"/>
-      <c r="AR110" s="8"/>
-      <c r="AS110" s="8"/>
-      <c r="AT110" s="8"/>
-      <c r="AU110" s="8"/>
-      <c r="AV110" s="8"/>
-      <c r="AW110" s="8"/>
-      <c r="AX110" s="8"/>
-      <c r="AY110" s="8"/>
-      <c r="AZ110" s="8"/>
-      <c r="BA110" s="8"/>
-      <c r="BB110" s="8"/>
-      <c r="BC110" s="9"/>
     </row>
     <row r="111" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C111" s="7"/>
@@ -5396,7 +5333,7 @@
       <c r="E111" s="8"/>
       <c r="F111" s="8"/>
       <c r="G111" s="1" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="H111" s="3"/>
       <c r="I111" s="2"/>
@@ -5421,7 +5358,7 @@
       <c r="AB111" s="8"/>
       <c r="AC111" s="9"/>
       <c r="AF111" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AG111" s="8"/>
       <c r="AH111" s="8"/>
@@ -5504,7 +5441,7 @@
     </row>
     <row r="113" spans="2:55" x14ac:dyDescent="0.25">
       <c r="AF113" s="7" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="AG113" s="8"/>
       <c r="AH113" s="8"/>
@@ -5560,7 +5497,7 @@
     </row>
     <row r="115" spans="2:55" x14ac:dyDescent="0.25">
       <c r="AF115" s="7" t="s">
-        <v>457</v>
+        <v>50</v>
       </c>
       <c r="AG115" s="8"/>
       <c r="AH115" s="8"/>
@@ -5640,7 +5577,7 @@
     </row>
     <row r="117" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B117" s="7" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
@@ -5666,7 +5603,7 @@
       <c r="X117" s="8"/>
       <c r="Y117" s="9"/>
       <c r="AF117" s="7" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="AG117" s="8"/>
       <c r="AH117" s="8"/>
@@ -5715,8 +5652,8 @@
       <c r="S118" s="11"/>
       <c r="T118" s="11"/>
       <c r="U118" s="11"/>
-      <c r="V118" s="11" t="s">
-        <v>441</v>
+      <c r="V118" s="74" t="s">
+        <v>439</v>
       </c>
       <c r="W118" s="11"/>
       <c r="X118" s="11"/>
@@ -5748,7 +5685,7 @@
     </row>
     <row r="119" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B119" s="18" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
@@ -5774,7 +5711,7 @@
       <c r="X119" s="5"/>
       <c r="Y119" s="6"/>
       <c r="AF119" s="7" t="s">
-        <v>312</v>
+        <v>454</v>
       </c>
       <c r="AG119" s="8"/>
       <c r="AH119" s="8"/>
@@ -5878,7 +5815,7 @@
       <c r="X121" s="8"/>
       <c r="Y121" s="9"/>
       <c r="AF121" s="7" t="s">
-        <v>213</v>
+        <v>312</v>
       </c>
       <c r="AG121" s="8"/>
       <c r="AH121" s="8"/>
@@ -5908,37 +5845,11 @@
     </row>
     <row r="122" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B122" s="7" t="s">
-        <v>462</v>
-      </c>
-      <c r="C122" s="8"/>
-      <c r="D122" s="8"/>
-      <c r="E122" s="8"/>
-      <c r="F122" s="8"/>
-      <c r="G122" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="G122" t="s">
         <v>35</v>
       </c>
-      <c r="H122" s="8"/>
-      <c r="I122" s="8"/>
-      <c r="J122" s="8"/>
-      <c r="K122" s="8"/>
-      <c r="L122" s="8"/>
-      <c r="M122" s="8"/>
-      <c r="N122" s="8" t="s">
-        <v>454</v>
-      </c>
-      <c r="O122" s="8"/>
-      <c r="P122" s="8"/>
-      <c r="Q122" s="8"/>
-      <c r="R122" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="S122" s="8"/>
-      <c r="T122" s="8"/>
-      <c r="U122" s="8"/>
-      <c r="V122" s="8"/>
-      <c r="W122" s="8"/>
-      <c r="X122" s="8"/>
-      <c r="Y122" s="9"/>
       <c r="AF122" s="7"/>
       <c r="AG122" s="8"/>
       <c r="AH122" s="8"/>
@@ -5966,34 +5877,15 @@
     </row>
     <row r="123" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B123" s="7"/>
-      <c r="C123" s="8"/>
-      <c r="D123" s="8"/>
-      <c r="E123" s="8"/>
-      <c r="F123" s="8"/>
-      <c r="G123" s="8"/>
-      <c r="H123" s="8"/>
-      <c r="I123" s="8"/>
-      <c r="J123" s="8"/>
-      <c r="K123" s="8"/>
-      <c r="L123" s="8"/>
-      <c r="M123" s="8"/>
-      <c r="N123" s="8"/>
-      <c r="O123" s="8"/>
-      <c r="P123" s="8"/>
-      <c r="Q123" s="8"/>
-      <c r="R123" s="8"/>
-      <c r="S123" s="8"/>
-      <c r="T123" s="8"/>
-      <c r="U123" s="8"/>
-      <c r="V123" s="8"/>
-      <c r="W123" s="8"/>
-      <c r="X123" s="8"/>
-      <c r="Y123" s="9"/>
-      <c r="AF123" s="7"/>
+      <c r="AF123" s="7" t="s">
+        <v>213</v>
+      </c>
       <c r="AG123" s="8"/>
       <c r="AH123" s="8"/>
       <c r="AI123" s="8"/>
-      <c r="AJ123" s="8"/>
+      <c r="AJ123" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="AK123" s="8"/>
       <c r="AL123" s="8"/>
       <c r="AM123" s="8"/>
@@ -6016,7 +5908,7 @@
     </row>
     <row r="124" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B124" s="7" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
@@ -6032,7 +5924,7 @@
       <c r="L124" s="8"/>
       <c r="M124" s="8"/>
       <c r="N124" s="8" t="s">
-        <v>311</v>
+        <v>451</v>
       </c>
       <c r="O124" s="8"/>
       <c r="P124" s="8"/>
@@ -6124,7 +6016,7 @@
     </row>
     <row r="126" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B126" s="7" t="s">
-        <v>77</v>
+        <v>459</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
@@ -6140,7 +6032,7 @@
       <c r="L126" s="8"/>
       <c r="M126" s="8"/>
       <c r="N126" s="8" t="s">
-        <v>466</v>
+        <v>311</v>
       </c>
       <c r="O126" s="8"/>
       <c r="P126" s="8"/>
@@ -6156,7 +6048,7 @@
       <c r="X126" s="8"/>
       <c r="Y126" s="9"/>
       <c r="AF126" s="4" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="AG126" s="5"/>
       <c r="AH126" s="5"/>
@@ -6234,7 +6126,7 @@
     </row>
     <row r="128" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B128" s="7" t="s">
-        <v>459</v>
+        <v>77</v>
       </c>
       <c r="C128" s="8"/>
       <c r="D128" s="8"/>
@@ -6250,7 +6142,7 @@
       <c r="L128" s="8"/>
       <c r="M128" s="8"/>
       <c r="N128" s="8" t="s">
-        <v>213</v>
+        <v>462</v>
       </c>
       <c r="O128" s="8"/>
       <c r="P128" s="8"/>
@@ -6341,35 +6233,31 @@
       <c r="BC129" s="9"/>
     </row>
     <row r="130" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B130" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="C130" s="2"/>
-      <c r="D130" s="2"/>
-      <c r="E130" s="3"/>
-      <c r="F130" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="G130" s="2"/>
-      <c r="H130" s="2"/>
-      <c r="I130" s="3"/>
-      <c r="J130" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K130" s="3"/>
-      <c r="L130" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="M130" s="3"/>
-      <c r="N130" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O130" s="3"/>
-      <c r="P130" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="Q130" s="3"/>
-      <c r="R130" s="8"/>
+      <c r="B130" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="C130" s="8"/>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8"/>
+      <c r="F130" s="8"/>
+      <c r="G130" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H130" s="8"/>
+      <c r="I130" s="8"/>
+      <c r="J130" s="8"/>
+      <c r="K130" s="8"/>
+      <c r="L130" s="8"/>
+      <c r="M130" s="8"/>
+      <c r="N130" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="O130" s="8"/>
+      <c r="P130" s="8"/>
+      <c r="Q130" s="8"/>
+      <c r="R130" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="S130" s="8"/>
       <c r="T130" s="8"/>
       <c r="U130" s="8"/>
@@ -6406,19 +6294,19 @@
       <c r="B131" s="7"/>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>
-      <c r="E131" s="9"/>
+      <c r="E131" s="8"/>
       <c r="F131" s="8"/>
       <c r="G131" s="8"/>
       <c r="H131" s="8"/>
       <c r="I131" s="8"/>
-      <c r="J131" s="7"/>
-      <c r="K131" s="9"/>
-      <c r="L131" s="7"/>
-      <c r="M131" s="9"/>
-      <c r="N131" s="7"/>
-      <c r="O131" s="9"/>
-      <c r="P131" s="7"/>
-      <c r="Q131" s="9"/>
+      <c r="J131" s="8"/>
+      <c r="K131" s="8"/>
+      <c r="L131" s="8"/>
+      <c r="M131" s="8"/>
+      <c r="N131" s="8"/>
+      <c r="O131" s="8"/>
+      <c r="P131" s="8"/>
+      <c r="Q131" s="8"/>
       <c r="R131" s="8"/>
       <c r="S131" s="8"/>
       <c r="T131" s="8"/>
@@ -6429,22 +6317,26 @@
       <c r="Y131" s="9"/>
     </row>
     <row r="132" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B132" s="7"/>
+      <c r="B132" s="7" t="s">
+        <v>472</v>
+      </c>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
-      <c r="E132" s="9"/>
+      <c r="E132" s="8"/>
       <c r="F132" s="8"/>
-      <c r="G132" s="8"/>
+      <c r="G132" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="H132" s="8"/>
       <c r="I132" s="8"/>
-      <c r="J132" s="7"/>
-      <c r="K132" s="9"/>
-      <c r="L132" s="7"/>
-      <c r="M132" s="9"/>
-      <c r="N132" s="7"/>
-      <c r="O132" s="9"/>
-      <c r="P132" s="7"/>
-      <c r="Q132" s="9"/>
+      <c r="J132" s="8"/>
+      <c r="K132" s="8"/>
+      <c r="L132" s="8"/>
+      <c r="M132" s="8"/>
+      <c r="N132" s="8"/>
+      <c r="O132" s="8"/>
+      <c r="P132" s="8"/>
+      <c r="Q132" s="8"/>
       <c r="R132" s="8"/>
       <c r="S132" s="8"/>
       <c r="T132" s="8"/>
@@ -6453,48 +6345,24 @@
       <c r="W132" s="8"/>
       <c r="X132" s="8"/>
       <c r="Y132" s="9"/>
-      <c r="AF132" s="8"/>
-      <c r="AG132" s="8"/>
-      <c r="AH132" s="8"/>
-      <c r="AI132" s="8"/>
-      <c r="AJ132" s="8"/>
-      <c r="AK132" s="8"/>
-      <c r="AL132" s="8"/>
-      <c r="AM132" s="8"/>
-      <c r="AN132" s="8"/>
-      <c r="AO132" s="8"/>
-      <c r="AP132" s="8"/>
-      <c r="AQ132" s="8"/>
-      <c r="AR132" s="8"/>
-      <c r="AS132" s="8"/>
-      <c r="AT132" s="8"/>
-      <c r="AU132" s="8"/>
-      <c r="AV132" s="8"/>
-      <c r="AW132" s="8"/>
-      <c r="AX132" s="8"/>
-      <c r="AY132" s="8"/>
-      <c r="AZ132" s="8"/>
-      <c r="BA132" s="8"/>
-      <c r="BB132" s="8"/>
-      <c r="BC132" s="8"/>
     </row>
     <row r="133" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B133" s="7"/>
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
-      <c r="E133" s="9"/>
+      <c r="E133" s="8"/>
       <c r="F133" s="8"/>
       <c r="G133" s="8"/>
       <c r="H133" s="8"/>
       <c r="I133" s="8"/>
-      <c r="J133" s="7"/>
-      <c r="K133" s="9"/>
-      <c r="L133" s="7"/>
-      <c r="M133" s="9"/>
-      <c r="N133" s="7"/>
-      <c r="O133" s="9"/>
-      <c r="P133" s="7"/>
-      <c r="Q133" s="9"/>
+      <c r="J133" s="8"/>
+      <c r="K133" s="8"/>
+      <c r="L133" s="8"/>
+      <c r="M133" s="8"/>
+      <c r="N133" s="8"/>
+      <c r="O133" s="8"/>
+      <c r="P133" s="8"/>
+      <c r="Q133" s="8"/>
       <c r="R133" s="8"/>
       <c r="S133" s="8"/>
       <c r="T133" s="8"/>
@@ -6505,23 +6373,35 @@
       <c r="Y133" s="9"/>
     </row>
     <row r="134" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B134" s="7"/>
-      <c r="C134" s="8"/>
-      <c r="D134" s="8"/>
-      <c r="E134" s="9"/>
-      <c r="F134" s="8"/>
-      <c r="G134" s="8"/>
-      <c r="H134" s="8"/>
-      <c r="I134" s="8"/>
-      <c r="J134" s="7"/>
-      <c r="K134" s="9"/>
-      <c r="L134" s="7"/>
-      <c r="M134" s="9"/>
-      <c r="N134" s="7"/>
-      <c r="O134" s="9"/>
-      <c r="P134" s="7"/>
-      <c r="Q134" s="9"/>
-      <c r="R134" s="8"/>
+      <c r="B134" s="22"/>
+      <c r="C134" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="D134" s="2"/>
+      <c r="E134" s="2"/>
+      <c r="F134" s="3"/>
+      <c r="G134" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="H134" s="2"/>
+      <c r="I134" s="2"/>
+      <c r="J134" s="3"/>
+      <c r="K134" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L134" s="3"/>
+      <c r="M134" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="N134" s="3"/>
+      <c r="O134" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P134" s="3"/>
+      <c r="Q134" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="R134" s="3"/>
       <c r="S134" s="8"/>
       <c r="T134" s="8"/>
       <c r="U134" s="8"/>
@@ -6531,23 +6411,23 @@
       <c r="Y134" s="9"/>
     </row>
     <row r="135" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B135" s="10"/>
-      <c r="C135" s="11"/>
-      <c r="D135" s="11"/>
-      <c r="E135" s="12"/>
-      <c r="F135" s="10"/>
-      <c r="G135" s="11"/>
-      <c r="H135" s="11"/>
-      <c r="I135" s="12"/>
-      <c r="J135" s="10"/>
-      <c r="K135" s="12"/>
-      <c r="L135" s="10"/>
-      <c r="M135" s="12"/>
-      <c r="N135" s="10"/>
-      <c r="O135" s="12"/>
-      <c r="P135" s="10"/>
-      <c r="Q135" s="12"/>
-      <c r="R135" s="8"/>
+      <c r="B135" s="22"/>
+      <c r="C135" s="7"/>
+      <c r="D135" s="8"/>
+      <c r="E135" s="8"/>
+      <c r="F135" s="9"/>
+      <c r="G135" s="8"/>
+      <c r="H135" s="8"/>
+      <c r="I135" s="8"/>
+      <c r="J135" s="8"/>
+      <c r="K135" s="7"/>
+      <c r="L135" s="9"/>
+      <c r="M135" s="7"/>
+      <c r="N135" s="9"/>
+      <c r="O135" s="7"/>
+      <c r="P135" s="9"/>
+      <c r="Q135" s="7"/>
+      <c r="R135" s="9"/>
       <c r="S135" s="8"/>
       <c r="T135" s="8"/>
       <c r="U135" s="8"/>
@@ -6557,23 +6437,23 @@
       <c r="Y135" s="9"/>
     </row>
     <row r="136" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B136" s="7"/>
-      <c r="C136" s="8"/>
+      <c r="B136" s="22"/>
+      <c r="C136" s="7"/>
       <c r="D136" s="8"/>
       <c r="E136" s="8"/>
-      <c r="F136" s="8"/>
+      <c r="F136" s="9"/>
       <c r="G136" s="8"/>
       <c r="H136" s="8"/>
       <c r="I136" s="8"/>
       <c r="J136" s="8"/>
-      <c r="K136" s="8"/>
-      <c r="L136" s="8"/>
-      <c r="M136" s="8"/>
-      <c r="N136" s="8"/>
-      <c r="O136" s="8"/>
-      <c r="P136" s="8"/>
-      <c r="Q136" s="8"/>
-      <c r="R136" s="8"/>
+      <c r="K136" s="7"/>
+      <c r="L136" s="9"/>
+      <c r="M136" s="7"/>
+      <c r="N136" s="9"/>
+      <c r="O136" s="7"/>
+      <c r="P136" s="9"/>
+      <c r="Q136" s="7"/>
+      <c r="R136" s="9"/>
       <c r="S136" s="8"/>
       <c r="T136" s="8"/>
       <c r="U136" s="8"/>
@@ -6583,27 +6463,23 @@
       <c r="Y136" s="9"/>
     </row>
     <row r="137" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B137" s="7" t="s">
-        <v>467</v>
-      </c>
-      <c r="C137" s="8"/>
+      <c r="B137" s="22"/>
+      <c r="C137" s="7"/>
       <c r="D137" s="8"/>
       <c r="E137" s="8"/>
-      <c r="F137" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="F137" s="9"/>
       <c r="G137" s="8"/>
       <c r="H137" s="8"/>
       <c r="I137" s="8"/>
       <c r="J137" s="8"/>
-      <c r="K137" s="8"/>
-      <c r="L137" s="8"/>
-      <c r="M137" s="8"/>
-      <c r="N137" s="8"/>
-      <c r="O137" s="8"/>
-      <c r="P137" s="8"/>
-      <c r="Q137" s="8"/>
-      <c r="R137" s="8"/>
+      <c r="K137" s="7"/>
+      <c r="L137" s="9"/>
+      <c r="M137" s="7"/>
+      <c r="N137" s="9"/>
+      <c r="O137" s="7"/>
+      <c r="P137" s="9"/>
+      <c r="Q137" s="7"/>
+      <c r="R137" s="9"/>
       <c r="S137" s="8"/>
       <c r="T137" s="8"/>
       <c r="U137" s="8"/>
@@ -6613,23 +6489,23 @@
       <c r="Y137" s="9"/>
     </row>
     <row r="138" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B138" s="7"/>
-      <c r="C138" s="8"/>
+      <c r="B138" s="22"/>
+      <c r="C138" s="7"/>
       <c r="D138" s="8"/>
       <c r="E138" s="8"/>
-      <c r="F138" s="8"/>
+      <c r="F138" s="9"/>
       <c r="G138" s="8"/>
       <c r="H138" s="8"/>
       <c r="I138" s="8"/>
       <c r="J138" s="8"/>
-      <c r="K138" s="8"/>
-      <c r="L138" s="8"/>
-      <c r="M138" s="8"/>
-      <c r="N138" s="8"/>
-      <c r="O138" s="8"/>
-      <c r="P138" s="8"/>
-      <c r="Q138" s="8"/>
-      <c r="R138" s="8"/>
+      <c r="K138" s="7"/>
+      <c r="L138" s="9"/>
+      <c r="M138" s="7"/>
+      <c r="N138" s="9"/>
+      <c r="O138" s="7"/>
+      <c r="P138" s="9"/>
+      <c r="Q138" s="7"/>
+      <c r="R138" s="9"/>
       <c r="S138" s="8"/>
       <c r="T138" s="8"/>
       <c r="U138" s="8"/>
@@ -6639,23 +6515,23 @@
       <c r="Y138" s="9"/>
     </row>
     <row r="139" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B139" s="7"/>
-      <c r="C139" s="8"/>
-      <c r="D139" s="8"/>
-      <c r="E139" s="8"/>
-      <c r="F139" s="8"/>
-      <c r="G139" s="8"/>
-      <c r="H139" s="8"/>
-      <c r="I139" s="8"/>
-      <c r="J139" s="8"/>
-      <c r="K139" s="8"/>
-      <c r="L139" s="8"/>
-      <c r="M139" s="8"/>
-      <c r="N139" s="8"/>
-      <c r="O139" s="8"/>
-      <c r="P139" s="8"/>
-      <c r="Q139" s="8"/>
-      <c r="R139" s="8"/>
+      <c r="B139" s="22"/>
+      <c r="C139" s="10"/>
+      <c r="D139" s="11"/>
+      <c r="E139" s="11"/>
+      <c r="F139" s="12"/>
+      <c r="G139" s="10"/>
+      <c r="H139" s="11"/>
+      <c r="I139" s="11"/>
+      <c r="J139" s="12"/>
+      <c r="K139" s="10"/>
+      <c r="L139" s="12"/>
+      <c r="M139" s="10"/>
+      <c r="N139" s="12"/>
+      <c r="O139" s="10"/>
+      <c r="P139" s="12"/>
+      <c r="Q139" s="10"/>
+      <c r="R139" s="12"/>
       <c r="S139" s="8"/>
       <c r="T139" s="8"/>
       <c r="U139" s="8"/>
@@ -6691,30 +6567,138 @@
       <c r="Y140" s="9"/>
     </row>
     <row r="141" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B141" s="10"/>
-      <c r="C141" s="11"/>
-      <c r="D141" s="11"/>
-      <c r="E141" s="11"/>
-      <c r="F141" s="11"/>
-      <c r="G141" s="11"/>
-      <c r="H141" s="11"/>
-      <c r="I141" s="11"/>
-      <c r="J141" s="11"/>
-      <c r="K141" s="11"/>
-      <c r="L141" s="11"/>
-      <c r="M141" s="11"/>
-      <c r="N141" s="11"/>
-      <c r="O141" s="11"/>
-      <c r="P141" s="11"/>
-      <c r="Q141" s="11"/>
-      <c r="R141" s="11"/>
-      <c r="S141" s="11"/>
-      <c r="T141" s="11"/>
-      <c r="U141" s="11"/>
-      <c r="V141" s="11"/>
-      <c r="W141" s="11"/>
-      <c r="X141" s="11"/>
-      <c r="Y141" s="12"/>
+      <c r="B141" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="C141" s="8"/>
+      <c r="D141" s="8"/>
+      <c r="E141" s="8"/>
+      <c r="F141" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G141" s="8"/>
+      <c r="H141" s="8"/>
+      <c r="I141" s="8"/>
+      <c r="J141" s="8"/>
+      <c r="K141" s="8"/>
+      <c r="L141" s="8"/>
+      <c r="M141" s="8"/>
+      <c r="N141" s="8"/>
+      <c r="O141" s="8"/>
+      <c r="P141" s="8"/>
+      <c r="Q141" s="8"/>
+      <c r="R141" s="8"/>
+      <c r="S141" s="8"/>
+      <c r="T141" s="8"/>
+      <c r="U141" s="8"/>
+      <c r="V141" s="8"/>
+      <c r="W141" s="8"/>
+      <c r="X141" s="8"/>
+      <c r="Y141" s="9"/>
+    </row>
+    <row r="142" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B142" s="7"/>
+      <c r="C142" s="8"/>
+      <c r="D142" s="8"/>
+      <c r="E142" s="8"/>
+      <c r="F142" s="8"/>
+      <c r="G142" s="8"/>
+      <c r="H142" s="8"/>
+      <c r="I142" s="8"/>
+      <c r="J142" s="8"/>
+      <c r="K142" s="8"/>
+      <c r="L142" s="8"/>
+      <c r="M142" s="8"/>
+      <c r="N142" s="8"/>
+      <c r="O142" s="8"/>
+      <c r="P142" s="8"/>
+      <c r="Q142" s="8"/>
+      <c r="R142" s="8"/>
+      <c r="S142" s="8"/>
+      <c r="T142" s="8"/>
+      <c r="U142" s="8"/>
+      <c r="V142" s="8"/>
+      <c r="W142" s="8"/>
+      <c r="X142" s="8"/>
+      <c r="Y142" s="9"/>
+    </row>
+    <row r="143" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B143" s="7"/>
+      <c r="C143" s="8"/>
+      <c r="D143" s="8"/>
+      <c r="E143" s="8"/>
+      <c r="F143" s="8"/>
+      <c r="G143" s="8"/>
+      <c r="H143" s="8"/>
+      <c r="I143" s="8"/>
+      <c r="J143" s="8"/>
+      <c r="K143" s="8"/>
+      <c r="L143" s="8"/>
+      <c r="M143" s="8"/>
+      <c r="N143" s="8"/>
+      <c r="O143" s="8"/>
+      <c r="P143" s="8"/>
+      <c r="Q143" s="8"/>
+      <c r="R143" s="8"/>
+      <c r="S143" s="8"/>
+      <c r="T143" s="8"/>
+      <c r="U143" s="8"/>
+      <c r="V143" s="8"/>
+      <c r="W143" s="8"/>
+      <c r="X143" s="8"/>
+      <c r="Y143" s="9"/>
+    </row>
+    <row r="144" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B144" s="7"/>
+      <c r="C144" s="8"/>
+      <c r="D144" s="8"/>
+      <c r="E144" s="8"/>
+      <c r="F144" s="8"/>
+      <c r="G144" s="8"/>
+      <c r="H144" s="8"/>
+      <c r="I144" s="8"/>
+      <c r="J144" s="8"/>
+      <c r="K144" s="8"/>
+      <c r="L144" s="8"/>
+      <c r="M144" s="8"/>
+      <c r="N144" s="8"/>
+      <c r="O144" s="8"/>
+      <c r="P144" s="8"/>
+      <c r="Q144" s="8"/>
+      <c r="R144" s="8"/>
+      <c r="S144" s="8"/>
+      <c r="T144" s="8"/>
+      <c r="U144" s="8"/>
+      <c r="V144" s="8"/>
+      <c r="W144" s="8"/>
+      <c r="X144" s="8"/>
+      <c r="Y144" s="9"/>
+    </row>
+    <row r="145" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B145" s="10"/>
+      <c r="C145" s="11"/>
+      <c r="D145" s="11"/>
+      <c r="E145" s="11"/>
+      <c r="F145" s="11"/>
+      <c r="G145" s="11"/>
+      <c r="H145" s="11"/>
+      <c r="I145" s="11"/>
+      <c r="J145" s="11"/>
+      <c r="K145" s="11"/>
+      <c r="L145" s="11"/>
+      <c r="M145" s="11"/>
+      <c r="N145" s="11"/>
+      <c r="O145" s="11"/>
+      <c r="P145" s="11"/>
+      <c r="Q145" s="11"/>
+      <c r="R145" s="11"/>
+      <c r="S145" s="11"/>
+      <c r="T145" s="11"/>
+      <c r="U145" s="11"/>
+      <c r="V145" s="11"/>
+      <c r="W145" s="11"/>
+      <c r="X145" s="11"/>
+      <c r="Y145" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8006,7 +7990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC94"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="AR44" sqref="AR44"/>
     </sheetView>
   </sheetViews>
@@ -10476,10 +10460,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:BE141"/>
+  <dimension ref="B2:BG141"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="AK102" sqref="AK102"/>
+    <sheetView topLeftCell="V89" workbookViewId="0">
+      <selection activeCell="AR81" sqref="AR81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12859,7 +12843,7 @@
       <c r="BB64" s="8"/>
       <c r="BC64" s="8"/>
     </row>
-    <row r="65" spans="2:55" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B65" s="7"/>
       <c r="C65" s="22"/>
       <c r="D65" s="7"/>
@@ -12913,7 +12897,7 @@
       <c r="BB65" s="8"/>
       <c r="BC65" s="8"/>
     </row>
-    <row r="66" spans="2:55" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B66" s="7"/>
       <c r="C66" s="23"/>
       <c r="D66" s="10"/>
@@ -12975,7 +12959,7 @@
       <c r="BB66" s="8"/>
       <c r="BC66" s="8"/>
     </row>
-    <row r="67" spans="2:55" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B67" s="7"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
@@ -13031,7 +13015,7 @@
       <c r="BB67" s="8"/>
       <c r="BC67" s="8"/>
     </row>
-    <row r="68" spans="2:55" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B68" s="7"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
@@ -13095,7 +13079,7 @@
       <c r="BB68" s="8"/>
       <c r="BC68" s="8"/>
     </row>
-    <row r="69" spans="2:55" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B69" s="10"/>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
@@ -13151,7 +13135,7 @@
       <c r="BB69" s="8"/>
       <c r="BC69" s="8"/>
     </row>
-    <row r="70" spans="2:55" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
@@ -13211,7 +13195,7 @@
       <c r="BB70" s="8"/>
       <c r="BC70" s="8"/>
     </row>
-    <row r="71" spans="2:55" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B71" s="8" t="s">
         <v>50</v>
       </c>
@@ -13269,7 +13253,7 @@
       <c r="BB71" s="8"/>
       <c r="BC71" s="8"/>
     </row>
-    <row r="72" spans="2:55" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B72" s="8">
         <v>1</v>
       </c>
@@ -13333,7 +13317,7 @@
       <c r="BB72" s="8"/>
       <c r="BC72" s="8"/>
     </row>
-    <row r="73" spans="2:55" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B73" s="8">
         <v>2</v>
       </c>
@@ -13395,7 +13379,7 @@
       <c r="BB73" s="8"/>
       <c r="BC73" s="8"/>
     </row>
-    <row r="74" spans="2:55" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B74" s="8"/>
       <c r="C74" s="8" t="s">
         <v>255</v>
@@ -13457,7 +13441,7 @@
       <c r="BB74" s="8"/>
       <c r="BC74" s="8"/>
     </row>
-    <row r="75" spans="2:55" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B75" s="8"/>
       <c r="C75" s="19" t="s">
         <v>256</v>
@@ -13515,7 +13499,7 @@
       <c r="BB75" s="8"/>
       <c r="BC75" s="8"/>
     </row>
-    <row r="76" spans="2:55" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B76" s="8"/>
       <c r="C76" s="32" t="s">
         <v>259</v>
@@ -13568,16 +13552,24 @@
       <c r="AS76" s="8"/>
       <c r="AT76" s="8"/>
       <c r="AU76" s="8"/>
-      <c r="AV76" s="8"/>
-      <c r="AW76" s="8"/>
-      <c r="AX76" s="8"/>
-      <c r="AY76" s="8"/>
-      <c r="AZ76" s="8"/>
-      <c r="BA76" s="8"/>
-      <c r="BB76" s="8"/>
-      <c r="BC76" s="8"/>
-    </row>
-    <row r="77" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="AV76" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW76" s="68"/>
+      <c r="AX76" s="69"/>
+      <c r="AY76" s="70"/>
+      <c r="AZ76" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA76" s="68"/>
+      <c r="BB76" s="68"/>
+      <c r="BC76" s="68"/>
+      <c r="BD76" s="71"/>
+      <c r="BE76" s="71"/>
+      <c r="BF76" s="71"/>
+      <c r="BG76" s="71"/>
+    </row>
+    <row r="77" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B77" s="8"/>
       <c r="C77" s="34" t="s">
         <v>260</v>
@@ -13628,16 +13620,22 @@
       <c r="AS77" s="8"/>
       <c r="AT77" s="8"/>
       <c r="AU77" s="8"/>
-      <c r="AV77" s="8"/>
-      <c r="AW77" s="8"/>
-      <c r="AX77" s="8"/>
-      <c r="AY77" s="8"/>
-      <c r="AZ77" s="8"/>
-      <c r="BA77" s="8"/>
-      <c r="BB77" s="8"/>
-      <c r="BC77" s="8"/>
-    </row>
-    <row r="78" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="AV77" s="68"/>
+      <c r="AW77" s="68"/>
+      <c r="AX77" s="68"/>
+      <c r="AY77" s="68"/>
+      <c r="AZ77" s="68" t="s">
+        <v>473</v>
+      </c>
+      <c r="BA77" s="68"/>
+      <c r="BB77" s="68"/>
+      <c r="BC77" s="68"/>
+      <c r="BD77" s="71"/>
+      <c r="BE77" s="71"/>
+      <c r="BF77" s="71"/>
+      <c r="BG77" s="71"/>
+    </row>
+    <row r="78" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
@@ -13666,32 +13664,40 @@
       <c r="AA78" s="8"/>
       <c r="AB78" s="8"/>
       <c r="AE78" s="7"/>
-      <c r="AF78" s="8"/>
-      <c r="AG78" s="8"/>
-      <c r="AH78" s="8"/>
-      <c r="AI78" s="8"/>
-      <c r="AJ78" s="8"/>
-      <c r="AK78" s="8"/>
-      <c r="AL78" s="8"/>
-      <c r="AM78" s="8"/>
-      <c r="AN78" s="8"/>
-      <c r="AO78" s="8"/>
-      <c r="AP78" s="8"/>
-      <c r="AQ78" s="8"/>
+      <c r="AF78" s="68" t="s">
+        <v>476</v>
+      </c>
+      <c r="AG78" s="68"/>
+      <c r="AH78" s="68"/>
+      <c r="AI78" s="68"/>
+      <c r="AJ78" s="68"/>
+      <c r="AK78" s="72"/>
+      <c r="AL78" s="68"/>
+      <c r="AM78" s="68"/>
+      <c r="AN78" s="68"/>
+      <c r="AO78" s="68"/>
+      <c r="AP78" s="68"/>
+      <c r="AQ78" s="68"/>
       <c r="AR78" s="8"/>
       <c r="AS78" s="8"/>
       <c r="AT78" s="8"/>
       <c r="AU78" s="8"/>
-      <c r="AV78" s="8"/>
-      <c r="AW78" s="8"/>
-      <c r="AX78" s="8"/>
-      <c r="AY78" s="8"/>
-      <c r="AZ78" s="8"/>
-      <c r="BA78" s="8"/>
-      <c r="BB78" s="8"/>
-      <c r="BC78" s="8"/>
-    </row>
-    <row r="79" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="AV78" s="68"/>
+      <c r="AW78" s="68"/>
+      <c r="AX78" s="68"/>
+      <c r="AY78" s="68"/>
+      <c r="AZ78" s="68" t="s">
+        <v>474</v>
+      </c>
+      <c r="BA78" s="68"/>
+      <c r="BB78" s="68"/>
+      <c r="BC78" s="68"/>
+      <c r="BD78" s="71"/>
+      <c r="BE78" s="71"/>
+      <c r="BF78" s="71"/>
+      <c r="BG78" s="71"/>
+    </row>
+    <row r="79" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B79" s="8"/>
       <c r="C79" s="19" t="s">
         <v>262</v>
@@ -13726,36 +13732,37 @@
       <c r="AA79" s="8"/>
       <c r="AB79" s="8"/>
       <c r="AE79" s="7"/>
-      <c r="AF79" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="AG79" s="8"/>
-      <c r="AH79" s="8"/>
-      <c r="AI79" s="8"/>
-      <c r="AJ79" s="8"/>
-      <c r="AK79" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="AL79" s="5"/>
-      <c r="AM79" s="5"/>
-      <c r="AN79" s="5"/>
-      <c r="AO79" s="5"/>
-      <c r="AP79" s="5"/>
-      <c r="AQ79" s="5"/>
-      <c r="AR79" s="5"/>
-      <c r="AS79" s="5"/>
-      <c r="AT79" s="5"/>
-      <c r="AU79" s="5"/>
-      <c r="AV79" s="5"/>
-      <c r="AW79" s="6"/>
-      <c r="AX79" s="8"/>
-      <c r="AY79" s="8"/>
-      <c r="AZ79" s="8"/>
-      <c r="BA79" s="8"/>
-      <c r="BB79" s="8"/>
-      <c r="BC79" s="8"/>
-    </row>
-    <row r="80" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="AF79" s="71"/>
+      <c r="AG79" s="71"/>
+      <c r="AH79" s="71"/>
+      <c r="AI79" s="71"/>
+      <c r="AJ79" s="71"/>
+      <c r="AK79" s="71"/>
+      <c r="AL79" s="71"/>
+      <c r="AM79" s="71"/>
+      <c r="AN79" s="71"/>
+      <c r="AO79" s="71"/>
+      <c r="AP79" s="71"/>
+      <c r="AQ79" s="71"/>
+      <c r="AR79" t="s">
+        <v>478</v>
+      </c>
+      <c r="AV79" s="71"/>
+      <c r="AW79" s="71"/>
+      <c r="AX79" s="71"/>
+      <c r="AY79" s="71"/>
+      <c r="AZ79" s="68" t="s">
+        <v>475</v>
+      </c>
+      <c r="BA79" s="71"/>
+      <c r="BB79" s="71"/>
+      <c r="BC79" s="71"/>
+      <c r="BD79" s="71"/>
+      <c r="BE79" s="71"/>
+      <c r="BF79" s="71"/>
+      <c r="BG79" s="71"/>
+    </row>
+    <row r="80" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
@@ -13788,30 +13795,23 @@
       <c r="AA80" s="8"/>
       <c r="AB80" s="8"/>
       <c r="AE80" s="7"/>
-      <c r="AF80" s="8"/>
-      <c r="AG80" s="8"/>
-      <c r="AH80" s="8"/>
-      <c r="AI80" s="8"/>
-      <c r="AJ80" s="8"/>
-      <c r="AK80" s="7"/>
-      <c r="AL80" s="8"/>
-      <c r="AM80" s="8"/>
-      <c r="AN80" s="8"/>
-      <c r="AO80" s="8"/>
-      <c r="AP80" s="8"/>
-      <c r="AQ80" s="8"/>
-      <c r="AR80" s="8"/>
-      <c r="AS80" s="8"/>
-      <c r="AT80" s="8"/>
-      <c r="AU80" s="8"/>
-      <c r="AV80" s="8"/>
-      <c r="AW80" s="9"/>
-      <c r="AX80" s="8"/>
-      <c r="AY80" s="8"/>
-      <c r="AZ80" s="8"/>
-      <c r="BA80" s="8"/>
-      <c r="BB80" s="8"/>
-      <c r="BC80" s="8"/>
+      <c r="AF80" s="71" t="s">
+        <v>477</v>
+      </c>
+      <c r="AG80" s="71"/>
+      <c r="AH80" s="71"/>
+      <c r="AI80" s="71"/>
+      <c r="AJ80" s="71"/>
+      <c r="AK80" s="69"/>
+      <c r="AL80" s="73"/>
+      <c r="AM80" s="73"/>
+      <c r="AN80" s="73"/>
+      <c r="AO80" s="73"/>
+      <c r="AP80" s="70"/>
+      <c r="AQ80" s="71"/>
+      <c r="AR80" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="81" spans="2:57" x14ac:dyDescent="0.25">
       <c r="B81" s="8"/>
@@ -13842,30 +13842,6 @@
       <c r="AA81" s="8"/>
       <c r="AB81" s="8"/>
       <c r="AE81" s="7"/>
-      <c r="AF81" s="8"/>
-      <c r="AG81" s="8"/>
-      <c r="AH81" s="8"/>
-      <c r="AI81" s="8"/>
-      <c r="AJ81" s="8"/>
-      <c r="AK81" s="10"/>
-      <c r="AL81" s="11"/>
-      <c r="AM81" s="11"/>
-      <c r="AN81" s="11"/>
-      <c r="AO81" s="11"/>
-      <c r="AP81" s="11"/>
-      <c r="AQ81" s="11"/>
-      <c r="AR81" s="11"/>
-      <c r="AS81" s="11"/>
-      <c r="AT81" s="11"/>
-      <c r="AU81" s="11"/>
-      <c r="AV81" s="11"/>
-      <c r="AW81" s="12"/>
-      <c r="AX81" s="8"/>
-      <c r="AY81" s="8"/>
-      <c r="AZ81" s="8"/>
-      <c r="BA81" s="8"/>
-      <c r="BB81" s="8"/>
-      <c r="BC81" s="8"/>
     </row>
     <row r="82" spans="2:57" x14ac:dyDescent="0.25">
       <c r="B82" s="8"/>
@@ -13898,27 +13874,30 @@
       <c r="AA82" s="8"/>
       <c r="AB82" s="8"/>
       <c r="AE82" s="7"/>
-      <c r="AF82" s="8"/>
+      <c r="AF82" s="8" t="s">
+        <v>244</v>
+      </c>
       <c r="AG82" s="8"/>
       <c r="AH82" s="8"/>
       <c r="AI82" s="8"/>
       <c r="AJ82" s="8"/>
-      <c r="AK82" s="8"/>
-      <c r="AL82" s="8"/>
-      <c r="AM82" s="8"/>
-      <c r="AN82" s="8"/>
-      <c r="AO82" s="8"/>
-      <c r="AP82" s="8"/>
-      <c r="AQ82" s="8"/>
-      <c r="AR82" s="8"/>
-      <c r="AS82" s="8"/>
-      <c r="AT82" s="8"/>
-      <c r="AU82" s="8"/>
-      <c r="AV82" s="8"/>
-      <c r="AW82" s="8"/>
+      <c r="AK82" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="AL82" s="5"/>
+      <c r="AM82" s="5"/>
+      <c r="AN82" s="5"/>
+      <c r="AO82" s="5"/>
+      <c r="AP82" s="5"/>
+      <c r="AQ82" s="5"/>
+      <c r="AR82" s="5"/>
+      <c r="AS82" s="5"/>
+      <c r="AT82" s="5"/>
+      <c r="AU82" s="5"/>
+      <c r="AV82" s="5"/>
+      <c r="AW82" s="6"/>
       <c r="AX82" s="8"/>
       <c r="AY82" s="8"/>
-      <c r="AZ82" s="8"/>
       <c r="BA82" s="8"/>
       <c r="BB82" s="8"/>
       <c r="BC82" s="8"/>
@@ -13954,28 +13933,26 @@
       <c r="AA83" s="8"/>
       <c r="AB83" s="8"/>
       <c r="AE83" s="7"/>
-      <c r="AF83" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="AG83" s="5"/>
-      <c r="AH83" s="5"/>
-      <c r="AI83" s="5"/>
-      <c r="AJ83" s="5"/>
-      <c r="AK83" s="5"/>
-      <c r="AL83" s="5"/>
-      <c r="AM83" s="5"/>
-      <c r="AN83" s="5"/>
-      <c r="AO83" s="5"/>
-      <c r="AP83" s="5"/>
-      <c r="AQ83" s="5"/>
-      <c r="AR83" s="5"/>
-      <c r="AS83" s="5"/>
-      <c r="AT83" s="5"/>
-      <c r="AU83" s="5"/>
-      <c r="AV83" s="5"/>
-      <c r="AW83" s="5"/>
-      <c r="AX83" s="5"/>
-      <c r="AY83" s="5"/>
+      <c r="AF83" s="8"/>
+      <c r="AG83" s="8"/>
+      <c r="AH83" s="8"/>
+      <c r="AI83" s="8"/>
+      <c r="AJ83" s="8"/>
+      <c r="AK83" s="7"/>
+      <c r="AL83" s="8"/>
+      <c r="AM83" s="8"/>
+      <c r="AN83" s="8"/>
+      <c r="AO83" s="8"/>
+      <c r="AP83" s="8"/>
+      <c r="AQ83" s="8"/>
+      <c r="AR83" s="8"/>
+      <c r="AS83" s="8"/>
+      <c r="AT83" s="8"/>
+      <c r="AU83" s="8"/>
+      <c r="AV83" s="8"/>
+      <c r="AW83" s="9"/>
+      <c r="AX83" s="8"/>
+      <c r="AY83" s="8"/>
       <c r="AZ83" s="8"/>
       <c r="BA83" s="8"/>
       <c r="BB83" s="8"/>
@@ -14012,26 +13989,24 @@
       <c r="AA84" s="8"/>
       <c r="AB84" s="8"/>
       <c r="AE84" s="7"/>
-      <c r="AF84" s="7"/>
+      <c r="AF84" s="8"/>
       <c r="AG84" s="8"/>
       <c r="AH84" s="8"/>
       <c r="AI84" s="8"/>
       <c r="AJ84" s="8"/>
-      <c r="AK84" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="AL84" s="8"/>
-      <c r="AM84" s="8"/>
-      <c r="AN84" s="8"/>
-      <c r="AO84" s="8"/>
-      <c r="AP84" s="8"/>
-      <c r="AQ84" s="8"/>
-      <c r="AR84" s="8"/>
-      <c r="AS84" s="8"/>
-      <c r="AT84" s="8"/>
-      <c r="AU84" s="8"/>
-      <c r="AV84" s="8"/>
-      <c r="AW84" s="8"/>
+      <c r="AK84" s="10"/>
+      <c r="AL84" s="11"/>
+      <c r="AM84" s="11"/>
+      <c r="AN84" s="11"/>
+      <c r="AO84" s="11"/>
+      <c r="AP84" s="11"/>
+      <c r="AQ84" s="11"/>
+      <c r="AR84" s="11"/>
+      <c r="AS84" s="11"/>
+      <c r="AT84" s="11"/>
+      <c r="AU84" s="11"/>
+      <c r="AV84" s="11"/>
+      <c r="AW84" s="12"/>
       <c r="AX84" s="8"/>
       <c r="AY84" s="8"/>
       <c r="AZ84" s="8"/>
@@ -14068,20 +14043,14 @@
       <c r="AA85" s="8"/>
       <c r="AB85" s="8"/>
       <c r="AE85" s="7"/>
-      <c r="AF85" s="7"/>
-      <c r="AG85" s="8" t="s">
-        <v>36</v>
-      </c>
+      <c r="AF85" s="8"/>
+      <c r="AG85" s="8"/>
       <c r="AH85" s="8"/>
       <c r="AI85" s="8"/>
       <c r="AJ85" s="8"/>
-      <c r="AK85" s="1"/>
-      <c r="AL85" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM85" s="8" t="s">
-        <v>216</v>
-      </c>
+      <c r="AK85" s="8"/>
+      <c r="AL85" s="8"/>
+      <c r="AM85" s="8"/>
       <c r="AN85" s="8"/>
       <c r="AO85" s="8"/>
       <c r="AP85" s="8"/>
@@ -14130,26 +14099,28 @@
       <c r="AA86" s="8"/>
       <c r="AB86" s="8"/>
       <c r="AE86" s="7"/>
-      <c r="AF86" s="7"/>
-      <c r="AG86" s="8"/>
-      <c r="AH86" s="8"/>
-      <c r="AI86" s="8"/>
-      <c r="AJ86" s="8"/>
-      <c r="AK86" s="8"/>
-      <c r="AL86" s="8"/>
-      <c r="AM86" s="8"/>
-      <c r="AN86" s="8"/>
-      <c r="AO86" s="8"/>
-      <c r="AP86" s="8"/>
-      <c r="AQ86" s="8"/>
-      <c r="AR86" s="8"/>
-      <c r="AS86" s="8"/>
-      <c r="AT86" s="8"/>
-      <c r="AU86" s="8"/>
-      <c r="AV86" s="8"/>
-      <c r="AW86" s="8"/>
-      <c r="AX86" s="8"/>
-      <c r="AY86" s="8"/>
+      <c r="AF86" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="AG86" s="5"/>
+      <c r="AH86" s="5"/>
+      <c r="AI86" s="5"/>
+      <c r="AJ86" s="5"/>
+      <c r="AK86" s="5"/>
+      <c r="AL86" s="5"/>
+      <c r="AM86" s="5"/>
+      <c r="AN86" s="5"/>
+      <c r="AO86" s="5"/>
+      <c r="AP86" s="5"/>
+      <c r="AQ86" s="5"/>
+      <c r="AR86" s="5"/>
+      <c r="AS86" s="5"/>
+      <c r="AT86" s="5"/>
+      <c r="AU86" s="5"/>
+      <c r="AV86" s="5"/>
+      <c r="AW86" s="5"/>
+      <c r="AX86" s="5"/>
+      <c r="AY86" s="5"/>
       <c r="AZ86" s="8"/>
       <c r="BA86" s="8"/>
       <c r="BB86" s="8"/>
@@ -14185,38 +14156,33 @@
       <c r="Z87" s="8"/>
       <c r="AA87" s="8"/>
       <c r="AB87" s="8"/>
-      <c r="AE87" s="22"/>
-      <c r="AG87" s="66" t="s">
-        <v>410</v>
-      </c>
-      <c r="AH87" s="66"/>
-      <c r="AI87" s="66"/>
-      <c r="AJ87" s="66"/>
-      <c r="AK87" s="61"/>
-      <c r="AL87" s="66" t="s">
-        <v>411</v>
-      </c>
-      <c r="AM87" s="66"/>
-      <c r="AN87" s="66"/>
-      <c r="AO87" s="66"/>
-      <c r="AP87" s="66" t="s">
-        <v>412</v>
-      </c>
-      <c r="AQ87" s="66"/>
-      <c r="AR87" s="66"/>
-      <c r="AS87" s="66"/>
-      <c r="AT87" s="66"/>
-      <c r="AU87" s="66"/>
-      <c r="AV87" s="66"/>
-      <c r="AW87" s="66"/>
-      <c r="AX87" s="66"/>
-      <c r="AY87" s="66"/>
-      <c r="AZ87" s="66"/>
-      <c r="BA87" s="66"/>
-      <c r="BB87" s="66"/>
-      <c r="BC87" s="66"/>
-      <c r="BD87" s="66"/>
-      <c r="BE87" s="66"/>
+      <c r="AE87" s="7"/>
+      <c r="AF87" s="7"/>
+      <c r="AG87" s="8"/>
+      <c r="AH87" s="8"/>
+      <c r="AI87" s="8"/>
+      <c r="AJ87" s="8"/>
+      <c r="AK87" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="AL87" s="8"/>
+      <c r="AM87" s="8"/>
+      <c r="AN87" s="8"/>
+      <c r="AO87" s="8"/>
+      <c r="AP87" s="8"/>
+      <c r="AQ87" s="8"/>
+      <c r="AR87" s="8"/>
+      <c r="AS87" s="8"/>
+      <c r="AT87" s="8"/>
+      <c r="AU87" s="8"/>
+      <c r="AV87" s="8"/>
+      <c r="AW87" s="8"/>
+      <c r="AX87" s="8"/>
+      <c r="AY87" s="8"/>
+      <c r="AZ87" s="8"/>
+      <c r="BA87" s="8"/>
+      <c r="BB87" s="8"/>
+      <c r="BC87" s="8"/>
     </row>
     <row r="88" spans="2:57" x14ac:dyDescent="0.25">
       <c r="B88" s="8"/>
@@ -14246,34 +14212,37 @@
       <c r="Z88" s="8"/>
       <c r="AA88" s="8"/>
       <c r="AB88" s="8"/>
-      <c r="AE88" s="22"/>
-      <c r="AG88" s="66"/>
-      <c r="AH88" s="66"/>
-      <c r="AI88" s="66"/>
-      <c r="AJ88" s="66"/>
-      <c r="AK88" s="66"/>
-      <c r="AL88" s="66"/>
-      <c r="AM88" s="66"/>
-      <c r="AN88" s="66"/>
-      <c r="AO88" s="66"/>
-      <c r="AP88" s="66" t="s">
-        <v>413</v>
-      </c>
-      <c r="AQ88" s="66"/>
-      <c r="AR88" s="66"/>
-      <c r="AS88" s="66"/>
-      <c r="AT88" s="66"/>
-      <c r="AU88" s="66"/>
-      <c r="AV88" s="66"/>
-      <c r="AW88" s="66"/>
-      <c r="AX88" s="66"/>
-      <c r="AY88" s="66"/>
-      <c r="AZ88" s="66"/>
-      <c r="BA88" s="66"/>
-      <c r="BB88" s="66"/>
-      <c r="BC88" s="66"/>
-      <c r="BD88" s="66"/>
-      <c r="BE88" s="66"/>
+      <c r="AE88" s="7"/>
+      <c r="AF88" s="7"/>
+      <c r="AG88" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH88" s="8"/>
+      <c r="AI88" s="8"/>
+      <c r="AJ88" s="8"/>
+      <c r="AK88" s="1"/>
+      <c r="AL88" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM88" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="AN88" s="8"/>
+      <c r="AO88" s="8"/>
+      <c r="AP88" s="8"/>
+      <c r="AQ88" s="8"/>
+      <c r="AR88" s="8"/>
+      <c r="AS88" s="8"/>
+      <c r="AT88" s="8"/>
+      <c r="AU88" s="8"/>
+      <c r="AV88" s="8"/>
+      <c r="AW88" s="8"/>
+      <c r="AX88" s="8"/>
+      <c r="AY88" s="8"/>
+      <c r="AZ88" s="8"/>
+      <c r="BA88" s="8"/>
+      <c r="BB88" s="8"/>
+      <c r="BC88" s="8"/>
     </row>
     <row r="89" spans="2:57" x14ac:dyDescent="0.25">
       <c r="B89" s="8">
@@ -14309,43 +14278,29 @@
       <c r="AB89" s="8"/>
       <c r="AE89" s="7"/>
       <c r="AF89" s="7"/>
-      <c r="AG89" s="60" t="s">
-        <v>407</v>
-      </c>
-      <c r="AH89" s="60"/>
-      <c r="AI89" s="60"/>
-      <c r="AJ89" s="60"/>
-      <c r="AK89" s="60"/>
-      <c r="AL89" s="60" t="s">
-        <v>202</v>
-      </c>
-      <c r="AM89" s="62" t="s">
-        <v>249</v>
-      </c>
-      <c r="AN89" s="63"/>
-      <c r="AO89" s="63"/>
-      <c r="AP89" s="64"/>
-      <c r="AQ89" s="60"/>
-      <c r="AR89" s="60"/>
-      <c r="AS89" s="60"/>
-      <c r="AT89" s="60" t="s">
-        <v>408</v>
-      </c>
-      <c r="AU89" s="60"/>
-      <c r="AV89" s="60"/>
-      <c r="AW89" s="60"/>
-      <c r="AX89" s="60"/>
-      <c r="AY89" s="60"/>
-      <c r="AZ89" s="60" t="s">
-        <v>202</v>
-      </c>
-      <c r="BA89" s="62" t="s">
-        <v>409</v>
-      </c>
-      <c r="BB89" s="63"/>
-      <c r="BC89" s="63"/>
-      <c r="BD89" s="64"/>
-      <c r="BE89" s="66"/>
+      <c r="AG89" s="8"/>
+      <c r="AH89" s="8"/>
+      <c r="AI89" s="8"/>
+      <c r="AJ89" s="8"/>
+      <c r="AK89" s="8"/>
+      <c r="AL89" s="8"/>
+      <c r="AM89" s="8"/>
+      <c r="AN89" s="8"/>
+      <c r="AO89" s="8"/>
+      <c r="AP89" s="8"/>
+      <c r="AQ89" s="8"/>
+      <c r="AR89" s="8"/>
+      <c r="AS89" s="8"/>
+      <c r="AT89" s="8"/>
+      <c r="AU89" s="8"/>
+      <c r="AV89" s="8"/>
+      <c r="AW89" s="8"/>
+      <c r="AX89" s="8"/>
+      <c r="AY89" s="8"/>
+      <c r="AZ89" s="8"/>
+      <c r="BA89" s="8"/>
+      <c r="BB89" s="8"/>
+      <c r="BC89" s="8"/>
     </row>
     <row r="90" spans="2:57" x14ac:dyDescent="0.25">
       <c r="B90" s="8"/>
@@ -14377,35 +14332,38 @@
       <c r="Z90" s="8"/>
       <c r="AA90" s="8"/>
       <c r="AB90" s="8"/>
-      <c r="AE90" s="7"/>
-      <c r="AF90" s="7"/>
-      <c r="AG90" s="8"/>
-      <c r="AH90" s="8"/>
-      <c r="AI90" s="8"/>
-      <c r="AJ90" s="8"/>
-      <c r="AK90" s="8"/>
-      <c r="AL90" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="AM90" s="8"/>
-      <c r="AN90" s="8"/>
-      <c r="AO90" s="8"/>
-      <c r="AP90" s="8"/>
-      <c r="AQ90" s="8"/>
-      <c r="AR90" s="8"/>
-      <c r="AS90" s="8"/>
-      <c r="AT90" s="8"/>
-      <c r="AU90" s="8"/>
-      <c r="AV90" s="8"/>
-      <c r="AW90" s="8"/>
-      <c r="AX90" s="8"/>
-      <c r="AY90" s="8"/>
-      <c r="AZ90" s="8"/>
-      <c r="BA90" s="8"/>
-      <c r="BB90" s="8"/>
-      <c r="BC90" s="8"/>
-      <c r="BD90" s="8"/>
-      <c r="BE90" s="8"/>
+      <c r="AE90" s="22"/>
+      <c r="AG90" s="66" t="s">
+        <v>410</v>
+      </c>
+      <c r="AH90" s="66"/>
+      <c r="AI90" s="66"/>
+      <c r="AJ90" s="66"/>
+      <c r="AK90" s="61"/>
+      <c r="AL90" s="66" t="s">
+        <v>411</v>
+      </c>
+      <c r="AM90" s="66"/>
+      <c r="AN90" s="66"/>
+      <c r="AO90" s="66"/>
+      <c r="AP90" s="66" t="s">
+        <v>412</v>
+      </c>
+      <c r="AQ90" s="66"/>
+      <c r="AR90" s="66"/>
+      <c r="AS90" s="66"/>
+      <c r="AT90" s="66"/>
+      <c r="AU90" s="66"/>
+      <c r="AV90" s="66"/>
+      <c r="AW90" s="66"/>
+      <c r="AX90" s="66"/>
+      <c r="AY90" s="66"/>
+      <c r="AZ90" s="66"/>
+      <c r="BA90" s="66"/>
+      <c r="BB90" s="66"/>
+      <c r="BC90" s="66"/>
+      <c r="BD90" s="66"/>
+      <c r="BE90" s="66"/>
     </row>
     <row r="91" spans="2:57" x14ac:dyDescent="0.25">
       <c r="B91" s="8"/>
@@ -14437,41 +14395,34 @@
       <c r="Z91" s="8"/>
       <c r="AA91" s="8"/>
       <c r="AB91" s="8"/>
-      <c r="AE91" s="7"/>
-      <c r="AF91" s="7"/>
-      <c r="AG91" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="AH91" s="8"/>
-      <c r="AI91" s="8"/>
-      <c r="AJ91" s="8"/>
-      <c r="AK91" s="8"/>
-      <c r="AL91" s="1"/>
-      <c r="AM91" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AN91" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="AO91" s="8"/>
-      <c r="AP91" s="8"/>
-      <c r="AQ91" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="AR91" s="8"/>
-      <c r="AS91" s="8"/>
-      <c r="AT91" s="8"/>
-      <c r="AU91" s="8"/>
-      <c r="AV91" s="8"/>
-      <c r="AW91" s="8"/>
-      <c r="AX91" s="8"/>
-      <c r="AY91" s="8"/>
-      <c r="AZ91" s="8"/>
-      <c r="BA91" s="8"/>
-      <c r="BB91" s="8"/>
-      <c r="BC91" s="8"/>
-      <c r="BD91" s="8"/>
-      <c r="BE91" s="8"/>
+      <c r="AE91" s="22"/>
+      <c r="AG91" s="66"/>
+      <c r="AH91" s="66"/>
+      <c r="AI91" s="66"/>
+      <c r="AJ91" s="66"/>
+      <c r="AK91" s="66"/>
+      <c r="AL91" s="66"/>
+      <c r="AM91" s="66"/>
+      <c r="AN91" s="66"/>
+      <c r="AO91" s="66"/>
+      <c r="AP91" s="66" t="s">
+        <v>413</v>
+      </c>
+      <c r="AQ91" s="66"/>
+      <c r="AR91" s="66"/>
+      <c r="AS91" s="66"/>
+      <c r="AT91" s="66"/>
+      <c r="AU91" s="66"/>
+      <c r="AV91" s="66"/>
+      <c r="AW91" s="66"/>
+      <c r="AX91" s="66"/>
+      <c r="AY91" s="66"/>
+      <c r="AZ91" s="66"/>
+      <c r="BA91" s="66"/>
+      <c r="BB91" s="66"/>
+      <c r="BC91" s="66"/>
+      <c r="BD91" s="66"/>
+      <c r="BE91" s="66"/>
     </row>
     <row r="92" spans="2:57" x14ac:dyDescent="0.25">
       <c r="B92" s="8"/>
@@ -14505,35 +14456,43 @@
       <c r="AB92" s="8"/>
       <c r="AE92" s="7"/>
       <c r="AF92" s="7"/>
-      <c r="AG92" s="8"/>
-      <c r="AH92" s="8"/>
-      <c r="AI92" s="8"/>
-      <c r="AJ92" s="8"/>
-      <c r="AK92" s="8"/>
-      <c r="AL92" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="AM92" s="8"/>
-      <c r="AN92" s="8"/>
-      <c r="AO92" s="8"/>
-      <c r="AP92" s="8"/>
-      <c r="AQ92" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="AR92" s="8"/>
-      <c r="AS92" s="8"/>
-      <c r="AT92" s="8"/>
-      <c r="AU92" s="8"/>
-      <c r="AV92" s="8"/>
-      <c r="AW92" s="8"/>
-      <c r="AX92" s="8"/>
-      <c r="AY92" s="8"/>
-      <c r="AZ92" s="8"/>
-      <c r="BA92" s="8"/>
-      <c r="BB92" s="8"/>
-      <c r="BC92" s="8"/>
-      <c r="BD92" s="8"/>
-      <c r="BE92" s="8"/>
+      <c r="AG92" s="60" t="s">
+        <v>407</v>
+      </c>
+      <c r="AH92" s="60"/>
+      <c r="AI92" s="60"/>
+      <c r="AJ92" s="60"/>
+      <c r="AK92" s="60"/>
+      <c r="AL92" s="60" t="s">
+        <v>202</v>
+      </c>
+      <c r="AM92" s="62" t="s">
+        <v>249</v>
+      </c>
+      <c r="AN92" s="63"/>
+      <c r="AO92" s="63"/>
+      <c r="AP92" s="64"/>
+      <c r="AQ92" s="60"/>
+      <c r="AR92" s="60"/>
+      <c r="AS92" s="60"/>
+      <c r="AT92" s="60" t="s">
+        <v>408</v>
+      </c>
+      <c r="AU92" s="60"/>
+      <c r="AV92" s="60"/>
+      <c r="AW92" s="60"/>
+      <c r="AX92" s="60"/>
+      <c r="AY92" s="60"/>
+      <c r="AZ92" s="60" t="s">
+        <v>202</v>
+      </c>
+      <c r="BA92" s="62" t="s">
+        <v>409</v>
+      </c>
+      <c r="BB92" s="63"/>
+      <c r="BC92" s="63"/>
+      <c r="BD92" s="64"/>
+      <c r="BE92" s="66"/>
     </row>
     <row r="93" spans="2:57" x14ac:dyDescent="0.25">
       <c r="B93" s="8"/>
@@ -14567,20 +14526,18 @@
       <c r="AB93" s="8"/>
       <c r="AE93" s="7"/>
       <c r="AF93" s="7"/>
-      <c r="AG93" s="8" t="s">
-        <v>220</v>
-      </c>
+      <c r="AG93" s="8"/>
       <c r="AH93" s="8"/>
       <c r="AI93" s="8"/>
       <c r="AJ93" s="8"/>
       <c r="AK93" s="8"/>
-      <c r="AL93" s="1"/>
-      <c r="AM93" s="3"/>
+      <c r="AL93" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM93" s="8"/>
       <c r="AN93" s="8"/>
       <c r="AO93" s="8"/>
-      <c r="AP93" s="8" t="s">
-        <v>222</v>
-      </c>
+      <c r="AP93" s="8"/>
       <c r="AQ93" s="8"/>
       <c r="AR93" s="8"/>
       <c r="AS93" s="8"/>
@@ -14629,19 +14586,25 @@
       <c r="AB94" s="8"/>
       <c r="AE94" s="7"/>
       <c r="AF94" s="7"/>
-      <c r="AG94" s="8"/>
+      <c r="AG94" s="8" t="s">
+        <v>218</v>
+      </c>
       <c r="AH94" s="8"/>
       <c r="AI94" s="8"/>
       <c r="AJ94" s="8"/>
       <c r="AK94" s="8"/>
-      <c r="AL94" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="AM94" s="8"/>
-      <c r="AN94" s="8"/>
+      <c r="AL94" s="1"/>
+      <c r="AM94" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN94" s="8" t="s">
+        <v>219</v>
+      </c>
       <c r="AO94" s="8"/>
       <c r="AP94" s="8"/>
-      <c r="AQ94" s="8"/>
+      <c r="AQ94" s="8" t="s">
+        <v>217</v>
+      </c>
       <c r="AR94" s="8"/>
       <c r="AS94" s="8"/>
       <c r="AT94" s="8"/>
@@ -14689,21 +14652,21 @@
       <c r="AB95" s="8"/>
       <c r="AE95" s="7"/>
       <c r="AF95" s="7"/>
-      <c r="AG95" s="8" t="s">
-        <v>221</v>
-      </c>
+      <c r="AG95" s="8"/>
       <c r="AH95" s="8"/>
       <c r="AI95" s="8"/>
       <c r="AJ95" s="8"/>
       <c r="AK95" s="8"/>
-      <c r="AL95" s="1"/>
-      <c r="AM95" s="3"/>
+      <c r="AL95" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="AM95" s="8"/>
       <c r="AN95" s="8"/>
       <c r="AO95" s="8"/>
-      <c r="AP95" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="AQ95" s="8"/>
+      <c r="AP95" s="8"/>
+      <c r="AQ95" s="8" t="s">
+        <v>223</v>
+      </c>
       <c r="AR95" s="8"/>
       <c r="AS95" s="8"/>
       <c r="AT95" s="8"/>
@@ -14751,16 +14714,20 @@
       <c r="AB96" s="8"/>
       <c r="AE96" s="7"/>
       <c r="AF96" s="7"/>
-      <c r="AG96" s="8"/>
+      <c r="AG96" s="8" t="s">
+        <v>220</v>
+      </c>
       <c r="AH96" s="8"/>
       <c r="AI96" s="8"/>
       <c r="AJ96" s="8"/>
       <c r="AK96" s="8"/>
-      <c r="AL96" s="8"/>
-      <c r="AM96" s="8"/>
+      <c r="AL96" s="1"/>
+      <c r="AM96" s="3"/>
       <c r="AN96" s="8"/>
       <c r="AO96" s="8"/>
-      <c r="AP96" s="8"/>
+      <c r="AP96" s="8" t="s">
+        <v>222</v>
+      </c>
       <c r="AQ96" s="8"/>
       <c r="AR96" s="8"/>
       <c r="AS96" s="8"/>
@@ -14809,27 +14776,25 @@
       <c r="AB97" s="8"/>
       <c r="AE97" s="7"/>
       <c r="AF97" s="7"/>
-      <c r="AG97" s="60" t="s">
-        <v>272</v>
-      </c>
-      <c r="AH97" s="60"/>
-      <c r="AI97" s="60"/>
-      <c r="AJ97" s="60"/>
-      <c r="AK97" s="60"/>
-      <c r="AL97" s="61"/>
-      <c r="AM97" s="60" t="s">
-        <v>275</v>
-      </c>
-      <c r="AN97" s="60"/>
-      <c r="AO97" s="60"/>
-      <c r="AP97" s="60"/>
-      <c r="AQ97" s="60"/>
-      <c r="AR97" s="60"/>
-      <c r="AS97" s="60"/>
-      <c r="AT97" s="60"/>
-      <c r="AU97" s="60"/>
-      <c r="AV97" s="60"/>
-      <c r="AW97" s="60"/>
+      <c r="AG97" s="8"/>
+      <c r="AH97" s="8"/>
+      <c r="AI97" s="8"/>
+      <c r="AJ97" s="8"/>
+      <c r="AK97" s="8"/>
+      <c r="AL97" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="AM97" s="8"/>
+      <c r="AN97" s="8"/>
+      <c r="AO97" s="8"/>
+      <c r="AP97" s="8"/>
+      <c r="AQ97" s="8"/>
+      <c r="AR97" s="8"/>
+      <c r="AS97" s="8"/>
+      <c r="AT97" s="8"/>
+      <c r="AU97" s="8"/>
+      <c r="AV97" s="8"/>
+      <c r="AW97" s="8"/>
       <c r="AX97" s="8"/>
       <c r="AY97" s="8"/>
       <c r="AZ97" s="8"/>
@@ -14873,23 +14838,27 @@
       <c r="AB98" s="8"/>
       <c r="AE98" s="7"/>
       <c r="AF98" s="7"/>
-      <c r="AG98" s="60"/>
-      <c r="AH98" s="60"/>
-      <c r="AI98" s="60"/>
-      <c r="AJ98" s="60"/>
-      <c r="AK98" s="60"/>
-      <c r="AL98" s="60"/>
-      <c r="AM98" s="60"/>
-      <c r="AN98" s="60"/>
-      <c r="AO98" s="60"/>
-      <c r="AP98" s="60"/>
-      <c r="AQ98" s="60"/>
-      <c r="AR98" s="60"/>
-      <c r="AS98" s="60"/>
-      <c r="AT98" s="60"/>
-      <c r="AU98" s="60"/>
-      <c r="AV98" s="60"/>
-      <c r="AW98" s="60"/>
+      <c r="AG98" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="AH98" s="8"/>
+      <c r="AI98" s="8"/>
+      <c r="AJ98" s="8"/>
+      <c r="AK98" s="8"/>
+      <c r="AL98" s="1"/>
+      <c r="AM98" s="3"/>
+      <c r="AN98" s="8"/>
+      <c r="AO98" s="8"/>
+      <c r="AP98" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="AQ98" s="8"/>
+      <c r="AR98" s="8"/>
+      <c r="AS98" s="8"/>
+      <c r="AT98" s="8"/>
+      <c r="AU98" s="8"/>
+      <c r="AV98" s="8"/>
+      <c r="AW98" s="8"/>
       <c r="AX98" s="8"/>
       <c r="AY98" s="8"/>
       <c r="AZ98" s="8"/>
@@ -14931,27 +14900,23 @@
       <c r="AB99" s="8"/>
       <c r="AE99" s="7"/>
       <c r="AF99" s="7"/>
-      <c r="AG99" s="60" t="s">
-        <v>273</v>
-      </c>
-      <c r="AH99" s="60"/>
-      <c r="AI99" s="60"/>
-      <c r="AJ99" s="60"/>
-      <c r="AK99" s="60"/>
-      <c r="AL99" s="62"/>
-      <c r="AM99" s="63"/>
-      <c r="AN99" s="64"/>
-      <c r="AO99" s="60"/>
-      <c r="AP99" s="60" t="s">
-        <v>274</v>
-      </c>
-      <c r="AQ99" s="60"/>
-      <c r="AR99" s="60"/>
-      <c r="AS99" s="60"/>
-      <c r="AT99" s="60"/>
-      <c r="AU99" s="60"/>
-      <c r="AV99" s="60"/>
-      <c r="AW99" s="60"/>
+      <c r="AG99" s="8"/>
+      <c r="AH99" s="8"/>
+      <c r="AI99" s="8"/>
+      <c r="AJ99" s="8"/>
+      <c r="AK99" s="8"/>
+      <c r="AL99" s="8"/>
+      <c r="AM99" s="8"/>
+      <c r="AN99" s="8"/>
+      <c r="AO99" s="8"/>
+      <c r="AP99" s="8"/>
+      <c r="AQ99" s="8"/>
+      <c r="AR99" s="8"/>
+      <c r="AS99" s="8"/>
+      <c r="AT99" s="8"/>
+      <c r="AU99" s="8"/>
+      <c r="AV99" s="8"/>
+      <c r="AW99" s="8"/>
       <c r="AX99" s="8"/>
       <c r="AY99" s="8"/>
       <c r="AZ99" s="8"/>
@@ -14992,28 +14957,30 @@
       <c r="AA100" s="39"/>
       <c r="AB100" s="8"/>
       <c r="AE100" s="7"/>
-      <c r="AF100" s="10"/>
-      <c r="AG100" s="65"/>
-      <c r="AH100" s="65"/>
-      <c r="AI100" s="65"/>
-      <c r="AJ100" s="65"/>
-      <c r="AK100" s="65"/>
-      <c r="AL100" s="65" t="s">
-        <v>276</v>
-      </c>
-      <c r="AM100" s="65"/>
-      <c r="AN100" s="65"/>
-      <c r="AO100" s="65"/>
-      <c r="AP100" s="65"/>
-      <c r="AQ100" s="65"/>
-      <c r="AR100" s="65"/>
-      <c r="AS100" s="65"/>
-      <c r="AT100" s="65"/>
-      <c r="AU100" s="65"/>
-      <c r="AV100" s="65"/>
-      <c r="AW100" s="65"/>
-      <c r="AX100" s="11"/>
-      <c r="AY100" s="11"/>
+      <c r="AF100" s="7"/>
+      <c r="AG100" s="60" t="s">
+        <v>272</v>
+      </c>
+      <c r="AH100" s="60"/>
+      <c r="AI100" s="60"/>
+      <c r="AJ100" s="60"/>
+      <c r="AK100" s="60"/>
+      <c r="AL100" s="61"/>
+      <c r="AM100" s="60" t="s">
+        <v>275</v>
+      </c>
+      <c r="AN100" s="60"/>
+      <c r="AO100" s="60"/>
+      <c r="AP100" s="60"/>
+      <c r="AQ100" s="60"/>
+      <c r="AR100" s="60"/>
+      <c r="AS100" s="60"/>
+      <c r="AT100" s="60"/>
+      <c r="AU100" s="60"/>
+      <c r="AV100" s="60"/>
+      <c r="AW100" s="60"/>
+      <c r="AX100" s="8"/>
+      <c r="AY100" s="8"/>
       <c r="AZ100" s="8"/>
       <c r="BA100" s="8"/>
       <c r="BB100" s="8"/>
@@ -15052,24 +15019,24 @@
       <c r="AA101" s="39"/>
       <c r="AB101" s="8"/>
       <c r="AE101" s="7"/>
-      <c r="AF101" s="8"/>
-      <c r="AG101" s="8"/>
-      <c r="AH101" s="8"/>
-      <c r="AI101" s="8"/>
-      <c r="AJ101" s="8"/>
-      <c r="AK101" s="8"/>
-      <c r="AL101" s="8"/>
-      <c r="AM101" s="8"/>
-      <c r="AN101" s="8"/>
-      <c r="AO101" s="8"/>
-      <c r="AP101" s="8"/>
-      <c r="AQ101" s="8"/>
-      <c r="AR101" s="8"/>
-      <c r="AS101" s="8"/>
-      <c r="AT101" s="8"/>
-      <c r="AU101" s="8"/>
-      <c r="AV101" s="8"/>
-      <c r="AW101" s="8"/>
+      <c r="AF101" s="7"/>
+      <c r="AG101" s="60"/>
+      <c r="AH101" s="60"/>
+      <c r="AI101" s="60"/>
+      <c r="AJ101" s="60"/>
+      <c r="AK101" s="60"/>
+      <c r="AL101" s="60"/>
+      <c r="AM101" s="60"/>
+      <c r="AN101" s="60"/>
+      <c r="AO101" s="60"/>
+      <c r="AP101" s="60"/>
+      <c r="AQ101" s="60"/>
+      <c r="AR101" s="60"/>
+      <c r="AS101" s="60"/>
+      <c r="AT101" s="60"/>
+      <c r="AU101" s="60"/>
+      <c r="AV101" s="60"/>
+      <c r="AW101" s="60"/>
       <c r="AX101" s="8"/>
       <c r="AY101" s="8"/>
       <c r="AZ101" s="8"/>
@@ -15115,26 +15082,28 @@
       <c r="AA102" s="8"/>
       <c r="AB102" s="8"/>
       <c r="AE102" s="7"/>
-      <c r="AF102" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="AG102" s="3"/>
-      <c r="AH102" s="8"/>
-      <c r="AI102" s="8"/>
-      <c r="AJ102" s="8"/>
-      <c r="AK102" s="8"/>
-      <c r="AL102" s="8"/>
-      <c r="AM102" s="8"/>
-      <c r="AN102" s="8"/>
-      <c r="AO102" s="8"/>
-      <c r="AP102" s="8"/>
-      <c r="AQ102" s="8"/>
-      <c r="AR102" s="8"/>
-      <c r="AS102" s="8"/>
-      <c r="AT102" s="8"/>
-      <c r="AU102" s="8"/>
-      <c r="AV102" s="8"/>
-      <c r="AW102" s="8"/>
+      <c r="AF102" s="7"/>
+      <c r="AG102" s="60" t="s">
+        <v>273</v>
+      </c>
+      <c r="AH102" s="60"/>
+      <c r="AI102" s="60"/>
+      <c r="AJ102" s="60"/>
+      <c r="AK102" s="60"/>
+      <c r="AL102" s="62"/>
+      <c r="AM102" s="63"/>
+      <c r="AN102" s="64"/>
+      <c r="AO102" s="60"/>
+      <c r="AP102" s="60" t="s">
+        <v>274</v>
+      </c>
+      <c r="AQ102" s="60"/>
+      <c r="AR102" s="60"/>
+      <c r="AS102" s="60"/>
+      <c r="AT102" s="60"/>
+      <c r="AU102" s="60"/>
+      <c r="AV102" s="60"/>
+      <c r="AW102" s="60"/>
       <c r="AX102" s="8"/>
       <c r="AY102" s="8"/>
       <c r="AZ102" s="8"/>
@@ -15145,25 +15114,27 @@
       <c r="BE102" s="8"/>
     </row>
     <row r="103" spans="2:57" x14ac:dyDescent="0.25">
-      <c r="AE103" s="10"/>
-      <c r="AF103" s="11"/>
-      <c r="AG103" s="11"/>
-      <c r="AH103" s="11"/>
-      <c r="AI103" s="11"/>
-      <c r="AJ103" s="11"/>
-      <c r="AK103" s="11"/>
-      <c r="AL103" s="11"/>
-      <c r="AM103" s="11"/>
-      <c r="AN103" s="11"/>
-      <c r="AO103" s="11"/>
-      <c r="AP103" s="11"/>
-      <c r="AQ103" s="11"/>
-      <c r="AR103" s="11"/>
-      <c r="AS103" s="11"/>
-      <c r="AT103" s="11"/>
-      <c r="AU103" s="11"/>
-      <c r="AV103" s="11"/>
-      <c r="AW103" s="11"/>
+      <c r="AE103" s="7"/>
+      <c r="AF103" s="10"/>
+      <c r="AG103" s="65"/>
+      <c r="AH103" s="65"/>
+      <c r="AI103" s="65"/>
+      <c r="AJ103" s="65"/>
+      <c r="AK103" s="65"/>
+      <c r="AL103" s="65" t="s">
+        <v>276</v>
+      </c>
+      <c r="AM103" s="65"/>
+      <c r="AN103" s="65"/>
+      <c r="AO103" s="65"/>
+      <c r="AP103" s="65"/>
+      <c r="AQ103" s="65"/>
+      <c r="AR103" s="65"/>
+      <c r="AS103" s="65"/>
+      <c r="AT103" s="65"/>
+      <c r="AU103" s="65"/>
+      <c r="AV103" s="65"/>
+      <c r="AW103" s="65"/>
       <c r="AX103" s="11"/>
       <c r="AY103" s="11"/>
       <c r="AZ103" s="8"/>
@@ -15205,7 +15176,7 @@
       <c r="Z104" s="66"/>
       <c r="AA104" s="66"/>
       <c r="AB104" s="66"/>
-      <c r="AE104" s="8"/>
+      <c r="AE104" s="7"/>
       <c r="AF104" s="8"/>
       <c r="AG104" s="8"/>
       <c r="AH104" s="8"/>
@@ -15263,9 +15234,11 @@
       <c r="Z105" s="66"/>
       <c r="AA105" s="66"/>
       <c r="AB105" s="66"/>
-      <c r="AE105" s="8"/>
-      <c r="AF105" s="8"/>
-      <c r="AG105" s="8"/>
+      <c r="AE105" s="7"/>
+      <c r="AF105" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AG105" s="3"/>
       <c r="AH105" s="8"/>
       <c r="AI105" s="8"/>
       <c r="AJ105" s="8"/>
@@ -15321,27 +15294,27 @@
       <c r="Z106" s="66"/>
       <c r="AA106" s="66"/>
       <c r="AB106" s="66"/>
-      <c r="AE106" s="8"/>
-      <c r="AF106" s="8"/>
-      <c r="AG106" s="8"/>
-      <c r="AH106" s="8"/>
-      <c r="AI106" s="8"/>
-      <c r="AJ106" s="8"/>
-      <c r="AK106" s="8"/>
-      <c r="AL106" s="8"/>
-      <c r="AM106" s="8"/>
-      <c r="AN106" s="8"/>
-      <c r="AO106" s="8"/>
-      <c r="AP106" s="8"/>
-      <c r="AQ106" s="8"/>
-      <c r="AR106" s="8"/>
-      <c r="AS106" s="8"/>
-      <c r="AT106" s="8"/>
-      <c r="AU106" s="8"/>
-      <c r="AV106" s="8"/>
-      <c r="AW106" s="8"/>
-      <c r="AX106" s="8"/>
-      <c r="AY106" s="8"/>
+      <c r="AE106" s="10"/>
+      <c r="AF106" s="11"/>
+      <c r="AG106" s="11"/>
+      <c r="AH106" s="11"/>
+      <c r="AI106" s="11"/>
+      <c r="AJ106" s="11"/>
+      <c r="AK106" s="11"/>
+      <c r="AL106" s="11"/>
+      <c r="AM106" s="11"/>
+      <c r="AN106" s="11"/>
+      <c r="AO106" s="11"/>
+      <c r="AP106" s="11"/>
+      <c r="AQ106" s="11"/>
+      <c r="AR106" s="11"/>
+      <c r="AS106" s="11"/>
+      <c r="AT106" s="11"/>
+      <c r="AU106" s="11"/>
+      <c r="AV106" s="11"/>
+      <c r="AW106" s="11"/>
+      <c r="AX106" s="11"/>
+      <c r="AY106" s="11"/>
       <c r="AZ106" s="8"/>
       <c r="BA106" s="8"/>
       <c r="BB106" s="8"/>
@@ -15379,6 +15352,33 @@
       <c r="Z107" s="66"/>
       <c r="AA107" s="66"/>
       <c r="AB107" s="66"/>
+      <c r="AE107" s="8"/>
+      <c r="AF107" s="8"/>
+      <c r="AG107" s="8"/>
+      <c r="AH107" s="8"/>
+      <c r="AI107" s="8"/>
+      <c r="AJ107" s="8"/>
+      <c r="AK107" s="8"/>
+      <c r="AL107" s="8"/>
+      <c r="AM107" s="8"/>
+      <c r="AN107" s="8"/>
+      <c r="AO107" s="8"/>
+      <c r="AP107" s="8"/>
+      <c r="AQ107" s="8"/>
+      <c r="AR107" s="8"/>
+      <c r="AS107" s="8"/>
+      <c r="AT107" s="8"/>
+      <c r="AU107" s="8"/>
+      <c r="AV107" s="8"/>
+      <c r="AW107" s="8"/>
+      <c r="AX107" s="8"/>
+      <c r="AY107" s="8"/>
+      <c r="AZ107" s="8"/>
+      <c r="BA107" s="8"/>
+      <c r="BB107" s="8"/>
+      <c r="BC107" s="8"/>
+      <c r="BD107" s="8"/>
+      <c r="BE107" s="8"/>
     </row>
     <row r="109" spans="2:57" x14ac:dyDescent="0.25">
       <c r="B109" s="1"/>
@@ -18221,7 +18221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BB73"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AO41" sqref="AO41"/>
     </sheetView>
   </sheetViews>
@@ -20792,7 +20792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AN81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="L75" sqref="L75"/>
     </sheetView>
   </sheetViews>
@@ -23471,7 +23471,7 @@
       <c r="D74" s="13"/>
       <c r="E74" s="8"/>
       <c r="F74" s="8" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
@@ -23479,7 +23479,7 @@
       <c r="J74" s="13"/>
       <c r="K74" s="8"/>
       <c r="L74" s="8" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="M74" s="8"/>
       <c r="N74" s="8"/>

</xml_diff>

<commit_message>
spec report dan query
</commit_message>
<xml_diff>
--- a/document/spec.xlsx
+++ b/document/spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="7500" tabRatio="710"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="7500" tabRatio="710" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Agent Menu" sheetId="2" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="Detail Hotel" sheetId="8" r:id="rId6"/>
     <sheet name="order hotel" sheetId="4" r:id="rId7"/>
     <sheet name="Cancel Booking" sheetId="9" r:id="rId8"/>
+    <sheet name="hotel report" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="483">
   <si>
     <t>Agent Register</t>
   </si>
@@ -1403,9 +1404,6 @@
     <t>Payment Date</t>
   </si>
   <si>
-    <t>Hotel Names</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -1461,6 +1459,18 @@
   </si>
   <si>
     <t>grup name harus diisi,klo ga sebaliknya</t>
+  </si>
+  <si>
+    <t>Report Booking Per periode</t>
+  </si>
+  <si>
+    <t>DI BLNC002 ada no_cof_order dikosongin, ntar diisi ma admin ada menu sendiri</t>
+  </si>
+  <si>
+    <t>status_payment = pending</t>
+  </si>
+  <si>
+    <t>Confirmation Number</t>
   </si>
 </sst>
 </file>
@@ -2246,10 +2256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:BC145"/>
+  <dimension ref="B1:BC148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="K135" sqref="K135"/>
+    <sheetView topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="P144" sqref="P144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3578,7 +3588,7 @@
       <c r="B54" s="7"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
@@ -3652,7 +3662,7 @@
       <c r="C57" s="8"/>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F57" s="8"/>
       <c r="G57" s="9"/>
@@ -3808,7 +3818,7 @@
     </row>
     <row r="68" spans="2:34" x14ac:dyDescent="0.25">
       <c r="AD68" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="69" spans="2:34" x14ac:dyDescent="0.25">
@@ -3890,7 +3900,7 @@
       <c r="N78" s="2"/>
       <c r="O78" s="3"/>
       <c r="P78" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q78" s="2"/>
       <c r="R78" s="2"/>
@@ -5223,7 +5233,7 @@
       <c r="S108" s="8"/>
       <c r="T108" s="8"/>
       <c r="U108" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="V108" s="8"/>
       <c r="W108" s="8"/>
@@ -5266,7 +5276,7 @@
       <c r="E109" s="3"/>
       <c r="F109" s="8"/>
       <c r="G109" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H109" s="3"/>
       <c r="I109" s="2"/>
@@ -5333,7 +5343,7 @@
       <c r="E111" s="8"/>
       <c r="F111" s="8"/>
       <c r="G111" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H111" s="3"/>
       <c r="I111" s="2"/>
@@ -5845,11 +5855,12 @@
     </row>
     <row r="122" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B122" s="7" t="s">
-        <v>418</v>
+        <v>141</v>
       </c>
       <c r="G122" t="s">
         <v>35</v>
       </c>
+      <c r="Y122" s="9"/>
       <c r="AF122" s="7"/>
       <c r="AG122" s="8"/>
       <c r="AH122" s="8"/>
@@ -5877,6 +5888,7 @@
     </row>
     <row r="123" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B123" s="7"/>
+      <c r="Y123" s="9"/>
       <c r="AF123" s="7" t="s">
         <v>213</v>
       </c>
@@ -5908,31 +5920,11 @@
     </row>
     <row r="124" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B124" s="7" t="s">
-        <v>458</v>
-      </c>
-      <c r="C124" s="8"/>
-      <c r="D124" s="8"/>
-      <c r="E124" s="8"/>
-      <c r="F124" s="8"/>
-      <c r="G124" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="G124" t="s">
         <v>35</v>
       </c>
-      <c r="H124" s="8"/>
-      <c r="I124" s="8"/>
-      <c r="J124" s="8"/>
-      <c r="K124" s="8"/>
-      <c r="L124" s="8"/>
-      <c r="M124" s="8"/>
-      <c r="N124" s="8" t="s">
-        <v>451</v>
-      </c>
-      <c r="O124" s="8"/>
-      <c r="P124" s="8"/>
-      <c r="Q124" s="8"/>
-      <c r="R124" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="S124" s="8"/>
       <c r="T124" s="8"/>
       <c r="U124" s="8"/>
       <c r="V124" s="8"/>
@@ -5966,23 +5958,6 @@
     </row>
     <row r="125" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B125" s="7"/>
-      <c r="C125" s="8"/>
-      <c r="D125" s="8"/>
-      <c r="E125" s="8"/>
-      <c r="F125" s="8"/>
-      <c r="G125" s="8"/>
-      <c r="H125" s="8"/>
-      <c r="I125" s="8"/>
-      <c r="J125" s="8"/>
-      <c r="K125" s="8"/>
-      <c r="L125" s="8"/>
-      <c r="M125" s="8"/>
-      <c r="N125" s="8"/>
-      <c r="O125" s="8"/>
-      <c r="P125" s="8"/>
-      <c r="Q125" s="8"/>
-      <c r="R125" s="8"/>
-      <c r="S125" s="8"/>
       <c r="T125" s="8"/>
       <c r="U125" s="8"/>
       <c r="V125" s="8"/>
@@ -6016,7 +5991,7 @@
     </row>
     <row r="126" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B126" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
@@ -6032,7 +6007,7 @@
       <c r="L126" s="8"/>
       <c r="M126" s="8"/>
       <c r="N126" s="8" t="s">
-        <v>311</v>
+        <v>451</v>
       </c>
       <c r="O126" s="8"/>
       <c r="P126" s="8"/>
@@ -6126,7 +6101,7 @@
     </row>
     <row r="128" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B128" s="7" t="s">
-        <v>77</v>
+        <v>459</v>
       </c>
       <c r="C128" s="8"/>
       <c r="D128" s="8"/>
@@ -6142,7 +6117,7 @@
       <c r="L128" s="8"/>
       <c r="M128" s="8"/>
       <c r="N128" s="8" t="s">
-        <v>462</v>
+        <v>311</v>
       </c>
       <c r="O128" s="8"/>
       <c r="P128" s="8"/>
@@ -6234,7 +6209,7 @@
     </row>
     <row r="130" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B130" s="7" t="s">
-        <v>455</v>
+        <v>77</v>
       </c>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
@@ -6250,7 +6225,7 @@
       <c r="L130" s="8"/>
       <c r="M130" s="8"/>
       <c r="N130" s="8" t="s">
-        <v>213</v>
+        <v>461</v>
       </c>
       <c r="O130" s="8"/>
       <c r="P130" s="8"/>
@@ -6318,7 +6293,7 @@
     </row>
     <row r="132" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B132" s="7" t="s">
-        <v>472</v>
+        <v>455</v>
       </c>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
@@ -6333,11 +6308,15 @@
       <c r="K132" s="8"/>
       <c r="L132" s="8"/>
       <c r="M132" s="8"/>
-      <c r="N132" s="8"/>
+      <c r="N132" s="8" t="s">
+        <v>213</v>
+      </c>
       <c r="O132" s="8"/>
       <c r="P132" s="8"/>
       <c r="Q132" s="8"/>
-      <c r="R132" s="8"/>
+      <c r="R132" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="S132" s="8"/>
       <c r="T132" s="8"/>
       <c r="U132" s="8"/>
@@ -6373,36 +6352,28 @@
       <c r="Y133" s="9"/>
     </row>
     <row r="134" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B134" s="22"/>
-      <c r="C134" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="D134" s="2"/>
-      <c r="E134" s="2"/>
-      <c r="F134" s="3"/>
-      <c r="G134" s="1" t="s">
+      <c r="B134" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="H134" s="2"/>
-      <c r="I134" s="2"/>
-      <c r="J134" s="3"/>
-      <c r="K134" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L134" s="3"/>
-      <c r="M134" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="N134" s="3"/>
-      <c r="O134" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P134" s="3"/>
-      <c r="Q134" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="R134" s="3"/>
-      <c r="S134" s="8"/>
+      <c r="G134" t="s">
+        <v>35</v>
+      </c>
+      <c r="H134" s="8"/>
+      <c r="I134" s="8"/>
+      <c r="J134" s="8"/>
+      <c r="K134" s="8"/>
+      <c r="L134" s="8"/>
+      <c r="M134" s="8"/>
+      <c r="N134" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="O134" s="8"/>
+      <c r="P134" s="8"/>
+      <c r="Q134" s="8"/>
+      <c r="R134" s="8"/>
+      <c r="S134" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="T134" s="8"/>
       <c r="U134" s="8"/>
       <c r="V134" s="8"/>
@@ -6411,49 +6382,27 @@
       <c r="Y134" s="9"/>
     </row>
     <row r="135" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B135" s="22"/>
-      <c r="C135" s="7"/>
-      <c r="D135" s="8"/>
-      <c r="E135" s="8"/>
-      <c r="F135" s="9"/>
-      <c r="G135" s="8"/>
-      <c r="H135" s="8"/>
-      <c r="I135" s="8"/>
-      <c r="J135" s="8"/>
-      <c r="K135" s="7"/>
-      <c r="L135" s="9"/>
-      <c r="M135" s="7"/>
-      <c r="N135" s="9"/>
-      <c r="O135" s="7"/>
-      <c r="P135" s="9"/>
-      <c r="Q135" s="7"/>
-      <c r="R135" s="9"/>
-      <c r="S135" s="8"/>
-      <c r="T135" s="8"/>
-      <c r="U135" s="8"/>
-      <c r="V135" s="8"/>
-      <c r="W135" s="8"/>
-      <c r="X135" s="8"/>
+      <c r="B135" s="7"/>
       <c r="Y135" s="9"/>
     </row>
     <row r="136" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B136" s="22"/>
-      <c r="C136" s="7"/>
+      <c r="B136" s="7"/>
+      <c r="C136" s="8"/>
       <c r="D136" s="8"/>
       <c r="E136" s="8"/>
-      <c r="F136" s="9"/>
+      <c r="F136" s="8"/>
       <c r="G136" s="8"/>
       <c r="H136" s="8"/>
       <c r="I136" s="8"/>
       <c r="J136" s="8"/>
-      <c r="K136" s="7"/>
-      <c r="L136" s="9"/>
-      <c r="M136" s="7"/>
-      <c r="N136" s="9"/>
-      <c r="O136" s="7"/>
-      <c r="P136" s="9"/>
-      <c r="Q136" s="7"/>
-      <c r="R136" s="9"/>
+      <c r="K136" s="8"/>
+      <c r="L136" s="8"/>
+      <c r="M136" s="8"/>
+      <c r="N136" s="8"/>
+      <c r="O136" s="8"/>
+      <c r="P136" s="8"/>
+      <c r="Q136" s="8"/>
+      <c r="R136" s="8"/>
       <c r="S136" s="8"/>
       <c r="T136" s="8"/>
       <c r="U136" s="8"/>
@@ -6464,22 +6413,18 @@
     </row>
     <row r="137" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B137" s="22"/>
-      <c r="C137" s="7"/>
-      <c r="D137" s="8"/>
-      <c r="E137" s="8"/>
-      <c r="F137" s="9"/>
-      <c r="G137" s="8"/>
-      <c r="H137" s="8"/>
-      <c r="I137" s="8"/>
-      <c r="J137" s="8"/>
-      <c r="K137" s="7"/>
-      <c r="L137" s="9"/>
-      <c r="M137" s="7"/>
-      <c r="N137" s="9"/>
-      <c r="O137" s="7"/>
-      <c r="P137" s="9"/>
-      <c r="Q137" s="7"/>
-      <c r="R137" s="9"/>
+      <c r="C137" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D137" s="3"/>
+      <c r="E137" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F137" s="3"/>
+      <c r="G137" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="H137" s="3"/>
       <c r="S137" s="8"/>
       <c r="T137" s="8"/>
       <c r="U137" s="8"/>
@@ -6491,21 +6436,11 @@
     <row r="138" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B138" s="22"/>
       <c r="C138" s="7"/>
-      <c r="D138" s="8"/>
-      <c r="E138" s="8"/>
+      <c r="D138" s="9"/>
+      <c r="E138" s="7"/>
       <c r="F138" s="9"/>
-      <c r="G138" s="8"/>
-      <c r="H138" s="8"/>
-      <c r="I138" s="8"/>
-      <c r="J138" s="8"/>
-      <c r="K138" s="7"/>
-      <c r="L138" s="9"/>
-      <c r="M138" s="7"/>
-      <c r="N138" s="9"/>
-      <c r="O138" s="7"/>
-      <c r="P138" s="9"/>
-      <c r="Q138" s="7"/>
-      <c r="R138" s="9"/>
+      <c r="G138" s="7"/>
+      <c r="H138" s="9"/>
       <c r="S138" s="8"/>
       <c r="T138" s="8"/>
       <c r="U138" s="8"/>
@@ -6516,22 +6451,12 @@
     </row>
     <row r="139" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B139" s="22"/>
-      <c r="C139" s="10"/>
-      <c r="D139" s="11"/>
-      <c r="E139" s="11"/>
-      <c r="F139" s="12"/>
-      <c r="G139" s="10"/>
-      <c r="H139" s="11"/>
-      <c r="I139" s="11"/>
-      <c r="J139" s="12"/>
-      <c r="K139" s="10"/>
-      <c r="L139" s="12"/>
-      <c r="M139" s="10"/>
-      <c r="N139" s="12"/>
-      <c r="O139" s="10"/>
-      <c r="P139" s="12"/>
-      <c r="Q139" s="10"/>
-      <c r="R139" s="12"/>
+      <c r="C139" s="7"/>
+      <c r="D139" s="9"/>
+      <c r="E139" s="7"/>
+      <c r="F139" s="9"/>
+      <c r="G139" s="7"/>
+      <c r="H139" s="9"/>
       <c r="S139" s="8"/>
       <c r="T139" s="8"/>
       <c r="U139" s="8"/>
@@ -6541,23 +6466,13 @@
       <c r="Y139" s="9"/>
     </row>
     <row r="140" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B140" s="7"/>
-      <c r="C140" s="8"/>
-      <c r="D140" s="8"/>
-      <c r="E140" s="8"/>
-      <c r="F140" s="8"/>
-      <c r="G140" s="8"/>
-      <c r="H140" s="8"/>
-      <c r="I140" s="8"/>
-      <c r="J140" s="8"/>
-      <c r="K140" s="8"/>
-      <c r="L140" s="8"/>
-      <c r="M140" s="8"/>
-      <c r="N140" s="8"/>
-      <c r="O140" s="8"/>
-      <c r="P140" s="8"/>
-      <c r="Q140" s="8"/>
-      <c r="R140" s="8"/>
+      <c r="B140" s="22"/>
+      <c r="C140" s="7"/>
+      <c r="D140" s="9"/>
+      <c r="E140" s="7"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="7"/>
+      <c r="H140" s="9"/>
       <c r="S140" s="8"/>
       <c r="T140" s="8"/>
       <c r="U140" s="8"/>
@@ -6567,27 +6482,13 @@
       <c r="Y140" s="9"/>
     </row>
     <row r="141" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B141" s="7" t="s">
-        <v>463</v>
-      </c>
-      <c r="C141" s="8"/>
-      <c r="D141" s="8"/>
-      <c r="E141" s="8"/>
-      <c r="F141" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G141" s="8"/>
-      <c r="H141" s="8"/>
-      <c r="I141" s="8"/>
-      <c r="J141" s="8"/>
-      <c r="K141" s="8"/>
-      <c r="L141" s="8"/>
-      <c r="M141" s="8"/>
-      <c r="N141" s="8"/>
-      <c r="O141" s="8"/>
-      <c r="P141" s="8"/>
-      <c r="Q141" s="8"/>
-      <c r="R141" s="8"/>
+      <c r="B141" s="22"/>
+      <c r="C141" s="7"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="7"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="7"/>
+      <c r="H141" s="9"/>
       <c r="S141" s="8"/>
       <c r="T141" s="8"/>
       <c r="U141" s="8"/>
@@ -6597,23 +6498,13 @@
       <c r="Y141" s="9"/>
     </row>
     <row r="142" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B142" s="7"/>
-      <c r="C142" s="8"/>
-      <c r="D142" s="8"/>
-      <c r="E142" s="8"/>
-      <c r="F142" s="8"/>
-      <c r="G142" s="8"/>
-      <c r="H142" s="8"/>
-      <c r="I142" s="8"/>
-      <c r="J142" s="8"/>
-      <c r="K142" s="8"/>
-      <c r="L142" s="8"/>
-      <c r="M142" s="8"/>
-      <c r="N142" s="8"/>
-      <c r="O142" s="8"/>
-      <c r="P142" s="8"/>
-      <c r="Q142" s="8"/>
-      <c r="R142" s="8"/>
+      <c r="B142" s="22"/>
+      <c r="C142" s="10"/>
+      <c r="D142" s="12"/>
+      <c r="E142" s="10"/>
+      <c r="F142" s="12"/>
+      <c r="G142" s="10"/>
+      <c r="H142" s="12"/>
       <c r="S142" s="8"/>
       <c r="T142" s="8"/>
       <c r="U142" s="8"/>
@@ -6649,11 +6540,15 @@
       <c r="Y143" s="9"/>
     </row>
     <row r="144" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B144" s="7"/>
+      <c r="B144" s="7" t="s">
+        <v>462</v>
+      </c>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
       <c r="E144" s="8"/>
-      <c r="F144" s="8"/>
+      <c r="F144" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="G144" s="8"/>
       <c r="H144" s="8"/>
       <c r="I144" s="8"/>
@@ -6675,30 +6570,108 @@
       <c r="Y144" s="9"/>
     </row>
     <row r="145" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B145" s="10"/>
-      <c r="C145" s="11"/>
-      <c r="D145" s="11"/>
-      <c r="E145" s="11"/>
-      <c r="F145" s="11"/>
-      <c r="G145" s="11"/>
-      <c r="H145" s="11"/>
-      <c r="I145" s="11"/>
-      <c r="J145" s="11"/>
-      <c r="K145" s="11"/>
-      <c r="L145" s="11"/>
-      <c r="M145" s="11"/>
-      <c r="N145" s="11"/>
-      <c r="O145" s="11"/>
-      <c r="P145" s="11"/>
-      <c r="Q145" s="11"/>
-      <c r="R145" s="11"/>
-      <c r="S145" s="11"/>
-      <c r="T145" s="11"/>
-      <c r="U145" s="11"/>
-      <c r="V145" s="11"/>
-      <c r="W145" s="11"/>
-      <c r="X145" s="11"/>
-      <c r="Y145" s="12"/>
+      <c r="B145" s="7"/>
+      <c r="C145" s="8"/>
+      <c r="D145" s="8"/>
+      <c r="E145" s="8"/>
+      <c r="F145" s="8"/>
+      <c r="G145" s="8"/>
+      <c r="H145" s="8"/>
+      <c r="I145" s="8"/>
+      <c r="J145" s="8"/>
+      <c r="K145" s="8"/>
+      <c r="L145" s="8"/>
+      <c r="M145" s="8"/>
+      <c r="N145" s="8"/>
+      <c r="O145" s="8"/>
+      <c r="P145" s="8"/>
+      <c r="Q145" s="8"/>
+      <c r="R145" s="8"/>
+      <c r="S145" s="8"/>
+      <c r="T145" s="8"/>
+      <c r="U145" s="8"/>
+      <c r="V145" s="8"/>
+      <c r="W145" s="8"/>
+      <c r="X145" s="8"/>
+      <c r="Y145" s="9"/>
+    </row>
+    <row r="146" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B146" s="7"/>
+      <c r="C146" s="8"/>
+      <c r="D146" s="8"/>
+      <c r="E146" s="8"/>
+      <c r="F146" s="8"/>
+      <c r="G146" s="8"/>
+      <c r="H146" s="8"/>
+      <c r="I146" s="8"/>
+      <c r="J146" s="8"/>
+      <c r="K146" s="8"/>
+      <c r="L146" s="8"/>
+      <c r="M146" s="8"/>
+      <c r="N146" s="8"/>
+      <c r="O146" s="8"/>
+      <c r="P146" s="8"/>
+      <c r="Q146" s="8"/>
+      <c r="R146" s="8"/>
+      <c r="S146" s="8"/>
+      <c r="T146" s="8"/>
+      <c r="U146" s="8"/>
+      <c r="V146" s="8"/>
+      <c r="W146" s="8"/>
+      <c r="X146" s="8"/>
+      <c r="Y146" s="9"/>
+    </row>
+    <row r="147" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B147" s="7"/>
+      <c r="C147" s="8"/>
+      <c r="D147" s="8"/>
+      <c r="E147" s="8"/>
+      <c r="F147" s="8"/>
+      <c r="G147" s="8"/>
+      <c r="H147" s="8"/>
+      <c r="I147" s="8"/>
+      <c r="J147" s="8"/>
+      <c r="K147" s="8"/>
+      <c r="L147" s="8"/>
+      <c r="M147" s="8"/>
+      <c r="N147" s="8"/>
+      <c r="O147" s="8"/>
+      <c r="P147" s="8"/>
+      <c r="Q147" s="8"/>
+      <c r="R147" s="8"/>
+      <c r="S147" s="8"/>
+      <c r="T147" s="8"/>
+      <c r="U147" s="8"/>
+      <c r="V147" s="8"/>
+      <c r="W147" s="8"/>
+      <c r="X147" s="8"/>
+      <c r="Y147" s="9"/>
+    </row>
+    <row r="148" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B148" s="10"/>
+      <c r="C148" s="11"/>
+      <c r="D148" s="11"/>
+      <c r="E148" s="11"/>
+      <c r="F148" s="11"/>
+      <c r="G148" s="11"/>
+      <c r="H148" s="11"/>
+      <c r="I148" s="11"/>
+      <c r="J148" s="11"/>
+      <c r="K148" s="11"/>
+      <c r="L148" s="11"/>
+      <c r="M148" s="11"/>
+      <c r="N148" s="11"/>
+      <c r="O148" s="11"/>
+      <c r="P148" s="11"/>
+      <c r="Q148" s="11"/>
+      <c r="R148" s="11"/>
+      <c r="S148" s="11"/>
+      <c r="T148" s="11"/>
+      <c r="U148" s="11"/>
+      <c r="V148" s="11"/>
+      <c r="W148" s="11"/>
+      <c r="X148" s="11"/>
+      <c r="Y148" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -13625,7 +13598,7 @@
       <c r="AX77" s="68"/>
       <c r="AY77" s="68"/>
       <c r="AZ77" s="68" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="BA77" s="68"/>
       <c r="BB77" s="68"/>
@@ -13665,7 +13638,7 @@
       <c r="AB78" s="8"/>
       <c r="AE78" s="7"/>
       <c r="AF78" s="68" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="AG78" s="68"/>
       <c r="AH78" s="68"/>
@@ -13687,7 +13660,7 @@
       <c r="AX78" s="68"/>
       <c r="AY78" s="68"/>
       <c r="AZ78" s="68" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="BA78" s="68"/>
       <c r="BB78" s="68"/>
@@ -13745,14 +13718,14 @@
       <c r="AP79" s="71"/>
       <c r="AQ79" s="71"/>
       <c r="AR79" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AV79" s="71"/>
       <c r="AW79" s="71"/>
       <c r="AX79" s="71"/>
       <c r="AY79" s="71"/>
       <c r="AZ79" s="68" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="BA79" s="71"/>
       <c r="BB79" s="71"/>
@@ -13796,7 +13769,7 @@
       <c r="AB80" s="8"/>
       <c r="AE80" s="7"/>
       <c r="AF80" s="71" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AG80" s="71"/>
       <c r="AH80" s="71"/>
@@ -13810,7 +13783,7 @@
       <c r="AP80" s="70"/>
       <c r="AQ80" s="71"/>
       <c r="AR80" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="81" spans="2:57" x14ac:dyDescent="0.25">
@@ -20792,8 +20765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AN81"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="L75" sqref="L75"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="W62" sqref="W62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23245,6 +23218,12 @@
       <c r="AB66" s="8"/>
       <c r="AC66" s="8"/>
       <c r="AD66" s="9"/>
+      <c r="AF66">
+        <v>10</v>
+      </c>
+      <c r="AG66" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="67" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B67" s="7"/>
@@ -23278,6 +23257,9 @@
       <c r="AB67" s="8"/>
       <c r="AC67" s="8"/>
       <c r="AD67" s="9"/>
+      <c r="AG67" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="68" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B68" s="7"/>
@@ -23471,7 +23453,7 @@
       <c r="D74" s="13"/>
       <c r="E74" s="8"/>
       <c r="F74" s="8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
@@ -23479,7 +23461,7 @@
       <c r="J74" s="13"/>
       <c r="K74" s="8"/>
       <c r="L74" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="M74" s="8"/>
       <c r="N74" s="8"/>
@@ -23878,4 +23860,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>482</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>310</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tambahan quey untuk report admin dan hotel
</commit_message>
<xml_diff>
--- a/document/spec.xlsx
+++ b/document/spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="7500" tabRatio="751" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="7500" tabRatio="790" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Agent Menu" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="618">
   <si>
     <t>Agent Register</t>
   </si>
@@ -1809,6 +1809,75 @@
   </si>
   <si>
     <t>update ke BLNC001, stts_pymnt</t>
+  </si>
+  <si>
+    <t>cancel booking</t>
+  </si>
+  <si>
+    <t>tgl check in</t>
+  </si>
+  <si>
+    <t>tgl check out</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>total payment</t>
+  </si>
+  <si>
+    <t>Cancel fee</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Status Pembayarn</t>
+  </si>
+  <si>
+    <t>pending/done/failed</t>
+  </si>
+  <si>
+    <t>Pending/Done/Cancel/failed</t>
+  </si>
+  <si>
+    <t>select * from BLNC001 a</t>
+  </si>
+  <si>
+    <t>inner join BLNC002 b on a.id = b.blnc001_id</t>
+  </si>
+  <si>
+    <t>inner join MST020 c on c.id = b.mst020_id</t>
+  </si>
+  <si>
+    <t>where a.order_no = :orderno</t>
+  </si>
+  <si>
+    <t>and a.no_conf_order =:orderconf</t>
+  </si>
+  <si>
+    <t>and b.check_in_date between :checkinfrom and :checkoutTo</t>
+  </si>
+  <si>
+    <t>and b.check_out_date between :checkoutfrom and :checkoutTo</t>
+  </si>
+  <si>
+    <t>and c.mst002_id = :countryID</t>
+  </si>
+  <si>
+    <t>and c.mst003_id = :cityId</t>
+  </si>
+  <si>
+    <t>and a.status_flg = :statusFlag</t>
+  </si>
+  <si>
+    <t>and a.status_pymnt = :statuspymtn</t>
+  </si>
+  <si>
+    <t>ini sama persis ma yang di agent menu cm tambahan filter mst001_id</t>
+  </si>
+  <si>
+    <t>Tgl Booking</t>
   </si>
 </sst>
 </file>
@@ -2737,8 +2806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BC148"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67:AH87"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="L90" sqref="L90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7164,10 +7233,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR51"/>
+  <dimension ref="A1:AR76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="AE39" sqref="AE39"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="AM65" sqref="AM65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8745,7 +8814,7 @@
       <c r="AB48" s="8"/>
       <c r="AC48" s="9"/>
     </row>
-    <row r="49" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
       <c r="C49" s="10"/>
       <c r="D49" s="12"/>
@@ -8775,7 +8844,7 @@
       <c r="AB49" s="8"/>
       <c r="AC49" s="9"/>
     </row>
-    <row r="50" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
@@ -8805,7 +8874,7 @@
       <c r="AB50" s="8"/>
       <c r="AC50" s="9"/>
     </row>
-    <row r="51" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B51" s="10"/>
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
@@ -8835,6 +8904,508 @@
       <c r="AB51" s="11"/>
       <c r="AC51" s="12"/>
     </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54" s="24" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C56" s="8" t="s">
+        <v>579</v>
+      </c>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
+      <c r="R56" s="8"/>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
+      <c r="M57" s="8"/>
+      <c r="N57" s="8"/>
+      <c r="O57" s="8"/>
+      <c r="P57" s="8"/>
+      <c r="Q57" s="8"/>
+      <c r="R57" s="8"/>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C58" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="8"/>
+      <c r="Q58" s="8"/>
+      <c r="R58" s="8"/>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>596</v>
+      </c>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="M60" s="8"/>
+      <c r="N60" s="13"/>
+      <c r="O60" s="13"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="3"/>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>597</v>
+      </c>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="M62" s="8"/>
+      <c r="N62" s="13"/>
+      <c r="O62" s="13"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="3"/>
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C64" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="3"/>
+    </row>
+    <row r="66" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="C66" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="D66" s="80"/>
+    </row>
+    <row r="68" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="C68" s="1"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="L68" s="5"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O68" s="6"/>
+      <c r="P68" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q68" s="6"/>
+      <c r="R68" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S68" s="5"/>
+      <c r="T68" s="5"/>
+      <c r="U68" s="6"/>
+      <c r="V68" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="W68" s="5"/>
+      <c r="X68" s="5"/>
+      <c r="Y68" s="6"/>
+      <c r="Z68" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="AA68" s="5"/>
+      <c r="AB68" s="6"/>
+      <c r="AC68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD68" s="6"/>
+      <c r="AE68" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="AF68" s="5"/>
+      <c r="AG68" s="5"/>
+      <c r="AH68" s="6"/>
+      <c r="AI68" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="AJ68" s="5"/>
+      <c r="AK68" s="6"/>
+      <c r="AL68" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="AM68" s="6"/>
+    </row>
+    <row r="69" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="C69" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="10"/>
+      <c r="L69" s="11"/>
+      <c r="M69" s="12"/>
+      <c r="N69" s="10"/>
+      <c r="O69" s="12"/>
+      <c r="P69" s="10"/>
+      <c r="Q69" s="12"/>
+      <c r="R69" s="10"/>
+      <c r="S69" s="11"/>
+      <c r="T69" s="11"/>
+      <c r="U69" s="12"/>
+      <c r="V69" s="10"/>
+      <c r="W69" s="11"/>
+      <c r="X69" s="11"/>
+      <c r="Y69" s="12"/>
+      <c r="Z69" s="10"/>
+      <c r="AA69" s="11"/>
+      <c r="AB69" s="12"/>
+      <c r="AC69" s="10"/>
+      <c r="AD69" s="12"/>
+      <c r="AE69" s="10"/>
+      <c r="AF69" s="11"/>
+      <c r="AG69" s="11"/>
+      <c r="AH69" s="12"/>
+      <c r="AI69" s="10"/>
+      <c r="AJ69" s="11"/>
+      <c r="AK69" s="12"/>
+      <c r="AL69" s="10"/>
+      <c r="AM69" s="12"/>
+    </row>
+    <row r="70" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="C70" s="7"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="7"/>
+      <c r="L70" s="8"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="6"/>
+      <c r="P70" s="7"/>
+      <c r="Q70" s="9"/>
+      <c r="R70" s="7"/>
+      <c r="S70" s="8"/>
+      <c r="T70" s="8"/>
+      <c r="U70" s="9"/>
+      <c r="V70" s="7"/>
+      <c r="W70" s="8"/>
+      <c r="X70" s="8"/>
+      <c r="Y70" s="9"/>
+      <c r="Z70" s="7"/>
+      <c r="AA70" s="8"/>
+      <c r="AB70" s="9"/>
+      <c r="AC70" s="7"/>
+      <c r="AD70" s="9"/>
+      <c r="AE70" s="7"/>
+      <c r="AF70" s="8"/>
+      <c r="AG70" s="8"/>
+      <c r="AH70" s="9"/>
+      <c r="AI70" s="7"/>
+      <c r="AJ70" s="8"/>
+      <c r="AK70" s="9"/>
+      <c r="AL70" s="7"/>
+      <c r="AM70" s="9"/>
+    </row>
+    <row r="71" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="C71" s="7"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="8"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="9"/>
+      <c r="P71" s="7"/>
+      <c r="Q71" s="9"/>
+      <c r="R71" s="7"/>
+      <c r="S71" s="8"/>
+      <c r="T71" s="8"/>
+      <c r="U71" s="9"/>
+      <c r="V71" s="7"/>
+      <c r="W71" s="8"/>
+      <c r="X71" s="8"/>
+      <c r="Y71" s="9"/>
+      <c r="Z71" s="7"/>
+      <c r="AA71" s="8"/>
+      <c r="AB71" s="9"/>
+      <c r="AC71" s="7"/>
+      <c r="AD71" s="9"/>
+      <c r="AE71" s="7"/>
+      <c r="AF71" s="8"/>
+      <c r="AG71" s="8"/>
+      <c r="AH71" s="9"/>
+      <c r="AI71" s="7"/>
+      <c r="AJ71" s="8"/>
+      <c r="AK71" s="9"/>
+      <c r="AL71" s="7"/>
+      <c r="AM71" s="9"/>
+    </row>
+    <row r="72" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="C72" s="7"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="7"/>
+      <c r="L72" s="8"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="7"/>
+      <c r="O72" s="9"/>
+      <c r="P72" s="7"/>
+      <c r="Q72" s="9"/>
+      <c r="R72" s="7"/>
+      <c r="S72" s="8"/>
+      <c r="T72" s="8"/>
+      <c r="U72" s="9"/>
+      <c r="V72" s="7"/>
+      <c r="W72" s="8"/>
+      <c r="X72" s="8"/>
+      <c r="Y72" s="9"/>
+      <c r="Z72" s="7"/>
+      <c r="AA72" s="8"/>
+      <c r="AB72" s="9"/>
+      <c r="AC72" s="7"/>
+      <c r="AD72" s="9"/>
+      <c r="AE72" s="7"/>
+      <c r="AF72" s="8"/>
+      <c r="AG72" s="8"/>
+      <c r="AH72" s="9"/>
+      <c r="AI72" s="7"/>
+      <c r="AJ72" s="8"/>
+      <c r="AK72" s="9"/>
+      <c r="AL72" s="7"/>
+      <c r="AM72" s="9"/>
+    </row>
+    <row r="73" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="C73" s="7"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="9"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="8"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="7"/>
+      <c r="O73" s="9"/>
+      <c r="P73" s="7"/>
+      <c r="Q73" s="9"/>
+      <c r="R73" s="7"/>
+      <c r="S73" s="8"/>
+      <c r="T73" s="8"/>
+      <c r="U73" s="9"/>
+      <c r="V73" s="7"/>
+      <c r="W73" s="8"/>
+      <c r="X73" s="8"/>
+      <c r="Y73" s="9"/>
+      <c r="Z73" s="7"/>
+      <c r="AA73" s="8"/>
+      <c r="AB73" s="9"/>
+      <c r="AC73" s="7"/>
+      <c r="AD73" s="9"/>
+      <c r="AE73" s="7"/>
+      <c r="AF73" s="8"/>
+      <c r="AG73" s="8"/>
+      <c r="AH73" s="9"/>
+      <c r="AI73" s="7"/>
+      <c r="AJ73" s="8"/>
+      <c r="AK73" s="9"/>
+      <c r="AL73" s="7"/>
+      <c r="AM73" s="9"/>
+    </row>
+    <row r="74" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="C74" s="7"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="9"/>
+      <c r="K74" s="7"/>
+      <c r="L74" s="8"/>
+      <c r="M74" s="9"/>
+      <c r="N74" s="7"/>
+      <c r="O74" s="9"/>
+      <c r="P74" s="7"/>
+      <c r="Q74" s="9"/>
+      <c r="R74" s="7"/>
+      <c r="S74" s="8"/>
+      <c r="T74" s="8"/>
+      <c r="U74" s="9"/>
+      <c r="V74" s="7"/>
+      <c r="W74" s="8"/>
+      <c r="X74" s="8"/>
+      <c r="Y74" s="9"/>
+      <c r="Z74" s="7"/>
+      <c r="AA74" s="8"/>
+      <c r="AB74" s="9"/>
+      <c r="AC74" s="7"/>
+      <c r="AD74" s="9"/>
+      <c r="AE74" s="7"/>
+      <c r="AF74" s="8"/>
+      <c r="AG74" s="8"/>
+      <c r="AH74" s="9"/>
+      <c r="AI74" s="7"/>
+      <c r="AJ74" s="8"/>
+      <c r="AK74" s="9"/>
+      <c r="AL74" s="7"/>
+      <c r="AM74" s="9"/>
+    </row>
+    <row r="75" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="C75" s="7"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="9"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="8"/>
+      <c r="M75" s="9"/>
+      <c r="N75" s="7"/>
+      <c r="O75" s="9"/>
+      <c r="P75" s="7"/>
+      <c r="Q75" s="9"/>
+      <c r="R75" s="7"/>
+      <c r="S75" s="8"/>
+      <c r="T75" s="8"/>
+      <c r="U75" s="9"/>
+      <c r="V75" s="7"/>
+      <c r="W75" s="8"/>
+      <c r="X75" s="8"/>
+      <c r="Y75" s="9"/>
+      <c r="Z75" s="7"/>
+      <c r="AA75" s="8"/>
+      <c r="AB75" s="9"/>
+      <c r="AC75" s="7"/>
+      <c r="AD75" s="9"/>
+      <c r="AE75" s="7"/>
+      <c r="AF75" s="8"/>
+      <c r="AG75" s="8"/>
+      <c r="AH75" s="9"/>
+      <c r="AI75" s="7"/>
+      <c r="AJ75" s="8"/>
+      <c r="AK75" s="9"/>
+      <c r="AL75" s="7"/>
+      <c r="AM75" s="9"/>
+    </row>
+    <row r="76" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="C76" s="10"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="11"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="10"/>
+      <c r="L76" s="11"/>
+      <c r="M76" s="12"/>
+      <c r="N76" s="10"/>
+      <c r="O76" s="12"/>
+      <c r="P76" s="10"/>
+      <c r="Q76" s="12"/>
+      <c r="R76" s="10"/>
+      <c r="S76" s="11"/>
+      <c r="T76" s="11"/>
+      <c r="U76" s="12"/>
+      <c r="V76" s="10"/>
+      <c r="W76" s="11"/>
+      <c r="X76" s="11"/>
+      <c r="Y76" s="12"/>
+      <c r="Z76" s="10"/>
+      <c r="AA76" s="11"/>
+      <c r="AB76" s="12"/>
+      <c r="AC76" s="10"/>
+      <c r="AD76" s="12"/>
+      <c r="AE76" s="10"/>
+      <c r="AF76" s="11"/>
+      <c r="AG76" s="11"/>
+      <c r="AH76" s="12"/>
+      <c r="AI76" s="10"/>
+      <c r="AJ76" s="11"/>
+      <c r="AK76" s="12"/>
+      <c r="AL76" s="10"/>
+      <c r="AM76" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8843,20 +9414,20 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO22"/>
+  <dimension ref="A1:AR33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>439</v>
       </c>
@@ -8866,7 +9437,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>281</v>
       </c>
@@ -8882,7 +9453,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>440</v>
       </c>
@@ -8898,7 +9469,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>3</v>
       </c>
@@ -8917,7 +9488,7 @@
       <c r="S9" s="2"/>
       <c r="T9" s="3"/>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>441</v>
       </c>
@@ -8931,7 +9502,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="C13" s="13" t="s">
         <v>392</v>
       </c>
@@ -8943,12 +9514,12 @@
         <v>446</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>444</v>
       </c>
@@ -8956,58 +9527,63 @@
       <c r="E16" s="2"/>
       <c r="F16" s="3"/>
       <c r="G16" s="1" t="s">
-        <v>58</v>
+        <v>617</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="3"/>
       <c r="J16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
       <c r="N16" s="2"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="1" t="s">
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="2" t="s">
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="2" t="s">
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AA16" s="2"/>
-      <c r="AB16" s="2"/>
-      <c r="AC16" s="3"/>
-      <c r="AD16" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD16" s="2"/>
       <c r="AE16" s="2"/>
       <c r="AF16" s="3"/>
-      <c r="AG16" s="1"/>
-      <c r="AH16" s="2" t="s">
-        <v>74</v>
-      </c>
+      <c r="AG16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH16" s="2"/>
       <c r="AI16" s="3"/>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL16" s="3"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="AL16" s="2"/>
-      <c r="AM16" s="2"/>
-      <c r="AN16" s="2"/>
-      <c r="AO16" s="3"/>
-    </row>
-    <row r="17" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AO16" s="2"/>
+      <c r="AP16" s="2"/>
+      <c r="AQ16" s="2"/>
+      <c r="AR16" s="3"/>
+    </row>
+    <row r="17" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -9017,25 +9593,25 @@
       <c r="I17" s="9"/>
       <c r="J17" s="7"/>
       <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="7"/>
       <c r="N17" s="8"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="7"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="7"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="8"/>
       <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="7"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
       <c r="Z17" s="8"/>
-      <c r="AA17" s="8"/>
-      <c r="AB17" s="8"/>
-      <c r="AC17" s="9"/>
-      <c r="AD17" s="7"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="8"/>
+      <c r="AD17" s="8"/>
       <c r="AE17" s="8"/>
       <c r="AF17" s="9"/>
       <c r="AG17" s="7"/>
@@ -9043,12 +9619,15 @@
       <c r="AI17" s="9"/>
       <c r="AJ17" s="7"/>
       <c r="AK17" s="8"/>
-      <c r="AL17" s="8"/>
-      <c r="AM17" s="8"/>
+      <c r="AL17" s="9"/>
+      <c r="AM17" s="7"/>
       <c r="AN17" s="8"/>
-      <c r="AO17" s="9"/>
-    </row>
-    <row r="18" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AO17" s="8"/>
+      <c r="AP17" s="8"/>
+      <c r="AQ17" s="8"/>
+      <c r="AR17" s="9"/>
+    </row>
+    <row r="18" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -9058,25 +9637,25 @@
       <c r="I18" s="9"/>
       <c r="J18" s="7"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="7"/>
       <c r="N18" s="8"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="7"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="7"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="8"/>
       <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="9"/>
-      <c r="Y18" s="7"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="8"/>
       <c r="Z18" s="8"/>
-      <c r="AA18" s="8"/>
-      <c r="AB18" s="8"/>
-      <c r="AC18" s="9"/>
-      <c r="AD18" s="7"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="8"/>
+      <c r="AD18" s="8"/>
       <c r="AE18" s="8"/>
       <c r="AF18" s="9"/>
       <c r="AG18" s="7"/>
@@ -9084,12 +9663,15 @@
       <c r="AI18" s="9"/>
       <c r="AJ18" s="7"/>
       <c r="AK18" s="8"/>
-      <c r="AL18" s="8"/>
-      <c r="AM18" s="8"/>
+      <c r="AL18" s="9"/>
+      <c r="AM18" s="7"/>
       <c r="AN18" s="8"/>
-      <c r="AO18" s="9"/>
-    </row>
-    <row r="19" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AO18" s="8"/>
+      <c r="AP18" s="8"/>
+      <c r="AQ18" s="8"/>
+      <c r="AR18" s="9"/>
+    </row>
+    <row r="19" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -9099,25 +9681,25 @@
       <c r="I19" s="9"/>
       <c r="J19" s="7"/>
       <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="7"/>
       <c r="N19" s="8"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="7"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="7"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="8"/>
       <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="7"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
-      <c r="AA19" s="8"/>
-      <c r="AB19" s="8"/>
-      <c r="AC19" s="9"/>
-      <c r="AD19" s="7"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="7"/>
+      <c r="AC19" s="8"/>
+      <c r="AD19" s="8"/>
       <c r="AE19" s="8"/>
       <c r="AF19" s="9"/>
       <c r="AG19" s="7"/>
@@ -9125,12 +9707,15 @@
       <c r="AI19" s="9"/>
       <c r="AJ19" s="7"/>
       <c r="AK19" s="8"/>
-      <c r="AL19" s="8"/>
-      <c r="AM19" s="8"/>
+      <c r="AL19" s="9"/>
+      <c r="AM19" s="7"/>
       <c r="AN19" s="8"/>
-      <c r="AO19" s="9"/>
-    </row>
-    <row r="20" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AO19" s="8"/>
+      <c r="AP19" s="8"/>
+      <c r="AQ19" s="8"/>
+      <c r="AR19" s="9"/>
+    </row>
+    <row r="20" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -9140,25 +9725,25 @@
       <c r="I20" s="9"/>
       <c r="J20" s="7"/>
       <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="7"/>
       <c r="N20" s="8"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="7"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="7"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="8"/>
       <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="7"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
       <c r="Z20" s="8"/>
-      <c r="AA20" s="8"/>
-      <c r="AB20" s="8"/>
-      <c r="AC20" s="9"/>
-      <c r="AD20" s="7"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="8"/>
+      <c r="AD20" s="8"/>
       <c r="AE20" s="8"/>
       <c r="AF20" s="9"/>
       <c r="AG20" s="7"/>
@@ -9166,12 +9751,15 @@
       <c r="AI20" s="9"/>
       <c r="AJ20" s="7"/>
       <c r="AK20" s="8"/>
-      <c r="AL20" s="8"/>
-      <c r="AM20" s="8"/>
+      <c r="AL20" s="9"/>
+      <c r="AM20" s="7"/>
       <c r="AN20" s="8"/>
-      <c r="AO20" s="9"/>
-    </row>
-    <row r="21" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AO20" s="8"/>
+      <c r="AP20" s="8"/>
+      <c r="AQ20" s="8"/>
+      <c r="AR20" s="9"/>
+    </row>
+    <row r="21" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -9181,25 +9769,25 @@
       <c r="I21" s="9"/>
       <c r="J21" s="7"/>
       <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="7"/>
       <c r="N21" s="8"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="7"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="7"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="8"/>
       <c r="U21" s="8"/>
-      <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="7"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="8"/>
       <c r="Z21" s="8"/>
-      <c r="AA21" s="8"/>
-      <c r="AB21" s="8"/>
-      <c r="AC21" s="9"/>
-      <c r="AD21" s="7"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="7"/>
+      <c r="AC21" s="8"/>
+      <c r="AD21" s="8"/>
       <c r="AE21" s="8"/>
       <c r="AF21" s="9"/>
       <c r="AG21" s="7"/>
@@ -9207,12 +9795,15 @@
       <c r="AI21" s="9"/>
       <c r="AJ21" s="7"/>
       <c r="AK21" s="8"/>
-      <c r="AL21" s="8"/>
-      <c r="AM21" s="8"/>
+      <c r="AL21" s="9"/>
+      <c r="AM21" s="7"/>
       <c r="AN21" s="8"/>
-      <c r="AO21" s="9"/>
-    </row>
-    <row r="22" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AO21" s="8"/>
+      <c r="AP21" s="8"/>
+      <c r="AQ21" s="8"/>
+      <c r="AR21" s="9"/>
+    </row>
+    <row r="22" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
@@ -9222,25 +9813,25 @@
       <c r="I22" s="12"/>
       <c r="J22" s="10"/>
       <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="10"/>
       <c r="N22" s="11"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="10"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="12"/>
-      <c r="T22" s="10"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="11"/>
       <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="10"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
       <c r="Z22" s="11"/>
-      <c r="AA22" s="11"/>
-      <c r="AB22" s="11"/>
-      <c r="AC22" s="12"/>
-      <c r="AD22" s="10"/>
+      <c r="AA22" s="12"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="11"/>
+      <c r="AD22" s="11"/>
       <c r="AE22" s="11"/>
       <c r="AF22" s="12"/>
       <c r="AG22" s="10"/>
@@ -9248,10 +9839,63 @@
       <c r="AI22" s="12"/>
       <c r="AJ22" s="10"/>
       <c r="AK22" s="11"/>
-      <c r="AL22" s="11"/>
-      <c r="AM22" s="11"/>
+      <c r="AL22" s="12"/>
+      <c r="AM22" s="10"/>
       <c r="AN22" s="11"/>
-      <c r="AO22" s="12"/>
+      <c r="AO22" s="11"/>
+      <c r="AP22" s="11"/>
+      <c r="AQ22" s="11"/>
+      <c r="AR22" s="12"/>
+    </row>
+    <row r="24" spans="3:44" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="25" spans="3:44" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="26" spans="3:44" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="27" spans="3:44" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="28" spans="3:44" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="29" spans="3:44" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="30" spans="3:44" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="31" spans="3:44" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="32" spans="3:44" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>614</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28874,15 +29518,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ47"/>
+  <dimension ref="A1:AV58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" s="15">
         <v>1</v>
       </c>
@@ -28925,7 +29569,7 @@
       <c r="AJ1" s="8"/>
       <c r="AK1" s="8"/>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -28964,7 +29608,7 @@
       <c r="AJ2" s="8"/>
       <c r="AK2" s="8"/>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" t="s">
         <v>32</v>
@@ -28986,10 +29630,10 @@
       <c r="AC3" s="2"/>
       <c r="AD3" s="3"/>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" t="s">
         <v>281</v>
@@ -29006,10 +29650,10 @@
       <c r="R5" s="1"/>
       <c r="S5" s="3"/>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" t="s">
         <v>440</v>
@@ -29026,10 +29670,10 @@
       <c r="R7" s="1"/>
       <c r="S7" s="3"/>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" t="s">
         <v>3</v>
@@ -29049,10 +29693,10 @@
       <c r="R9" s="2"/>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" t="s">
         <v>441</v>
@@ -29064,13 +29708,26 @@
       <c r="K11" s="2"/>
       <c r="L11" s="3"/>
       <c r="M11" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+        <v>604</v>
+      </c>
+      <c r="S11" t="s">
+        <v>585</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="13" t="s">
         <v>392</v>
@@ -29083,16 +29740,16 @@
         <v>446</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="G14" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="1" t="s">
         <v>32</v>
@@ -29148,16 +29805,23 @@
         <v>74</v>
       </c>
       <c r="AK16" s="3"/>
-      <c r="AL16" s="1"/>
-      <c r="AM16" s="2" t="s">
-        <v>395</v>
-      </c>
+      <c r="AL16" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
       <c r="AO16" s="2"/>
-      <c r="AP16" s="2"/>
-      <c r="AQ16" s="3"/>
-    </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AP16" s="3"/>
+      <c r="AQ16" s="1"/>
+      <c r="AR16" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="AS16" s="2"/>
+      <c r="AT16" s="2"/>
+      <c r="AU16" s="2"/>
+      <c r="AV16" s="3"/>
+    </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -29199,10 +29863,15 @@
       <c r="AM17" s="8"/>
       <c r="AN17" s="8"/>
       <c r="AO17" s="8"/>
-      <c r="AP17" s="8"/>
-      <c r="AQ17" s="9"/>
-    </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AP17" s="9"/>
+      <c r="AQ17" s="7"/>
+      <c r="AR17" s="8"/>
+      <c r="AS17" s="8"/>
+      <c r="AT17" s="8"/>
+      <c r="AU17" s="8"/>
+      <c r="AV17" s="9"/>
+    </row>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -29244,10 +29913,15 @@
       <c r="AM18" s="8"/>
       <c r="AN18" s="8"/>
       <c r="AO18" s="8"/>
-      <c r="AP18" s="8"/>
-      <c r="AQ18" s="9"/>
-    </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AP18" s="9"/>
+      <c r="AQ18" s="7"/>
+      <c r="AR18" s="8"/>
+      <c r="AS18" s="8"/>
+      <c r="AT18" s="8"/>
+      <c r="AU18" s="8"/>
+      <c r="AV18" s="9"/>
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
@@ -29289,10 +29963,15 @@
       <c r="AM19" s="8"/>
       <c r="AN19" s="8"/>
       <c r="AO19" s="8"/>
-      <c r="AP19" s="8"/>
-      <c r="AQ19" s="9"/>
-    </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AP19" s="9"/>
+      <c r="AQ19" s="7"/>
+      <c r="AR19" s="8"/>
+      <c r="AS19" s="8"/>
+      <c r="AT19" s="8"/>
+      <c r="AU19" s="8"/>
+      <c r="AV19" s="9"/>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="9"/>
@@ -29333,10 +30012,15 @@
       <c r="AM20" s="8"/>
       <c r="AN20" s="8"/>
       <c r="AO20" s="8"/>
-      <c r="AP20" s="8"/>
-      <c r="AQ20" s="9"/>
-    </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AP20" s="9"/>
+      <c r="AQ20" s="7"/>
+      <c r="AR20" s="8"/>
+      <c r="AS20" s="8"/>
+      <c r="AT20" s="8"/>
+      <c r="AU20" s="8"/>
+      <c r="AV20" s="9"/>
+    </row>
+    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
@@ -29377,10 +30061,15 @@
       <c r="AM21" s="8"/>
       <c r="AN21" s="8"/>
       <c r="AO21" s="8"/>
-      <c r="AP21" s="8"/>
-      <c r="AQ21" s="9"/>
-    </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AP21" s="9"/>
+      <c r="AQ21" s="7"/>
+      <c r="AR21" s="8"/>
+      <c r="AS21" s="8"/>
+      <c r="AT21" s="8"/>
+      <c r="AU21" s="8"/>
+      <c r="AV21" s="9"/>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="12"/>
@@ -29421,491 +30110,554 @@
       <c r="AM22" s="11"/>
       <c r="AN22" s="11"/>
       <c r="AO22" s="11"/>
-      <c r="AP22" s="11"/>
-      <c r="AQ22" s="12"/>
-    </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A26" s="24">
+      <c r="AP22" s="12"/>
+      <c r="AQ22" s="10"/>
+      <c r="AR22" s="11"/>
+      <c r="AS22" s="11"/>
+      <c r="AT22" s="11"/>
+      <c r="AU22" s="11"/>
+      <c r="AV22" s="12"/>
+    </row>
+    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A37" s="24">
         <v>2</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B37" s="24" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>507</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="3"/>
-      <c r="O27" t="s">
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="3"/>
+      <c r="O38" t="s">
         <v>388</v>
       </c>
-      <c r="T27" s="1"/>
-      <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
-      <c r="X27" s="3"/>
-    </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AC28" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>33</v>
-      </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="3"/>
-      <c r="O29" t="s">
-        <v>34</v>
-      </c>
-      <c r="T29" s="1"/>
-      <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
-      <c r="X29" s="3"/>
-    </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I31" s="2"/>
-      <c r="J31" s="3"/>
-      <c r="O31" t="s">
-        <v>389</v>
-      </c>
-      <c r="T31" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="3"/>
-    </row>
-    <row r="33" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>390</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="3"/>
-      <c r="L33" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="36" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B36" s="13" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="38" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="J38" s="2"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="M38" s="2"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="S38" s="2"/>
-      <c r="T38" s="2"/>
+      <c r="T38" s="1"/>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
-      <c r="W38" s="3"/>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="2" t="s">
+      <c r="W38" s="2"/>
+      <c r="X38" s="3"/>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC39" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="3"/>
+      <c r="O40" t="s">
+        <v>34</v>
+      </c>
+      <c r="T40" s="1"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="3"/>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="3"/>
+      <c r="O42" t="s">
+        <v>389</v>
+      </c>
+      <c r="T42" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="3"/>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>390</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="3"/>
+      <c r="L44" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B47" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="E47" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="49" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="J49" s="2"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="M49" s="2"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
+      <c r="V49" s="2"/>
+      <c r="W49" s="3"/>
+      <c r="X49" s="1"/>
+      <c r="Y49" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Z38" s="2"/>
-      <c r="AA38" s="3"/>
-      <c r="AB38" s="2" t="s">
+      <c r="Z49" s="2"/>
+      <c r="AA49" s="3"/>
+      <c r="AB49" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="AC38" s="2"/>
-      <c r="AD38" s="2"/>
-      <c r="AE38" s="2"/>
-      <c r="AF38" s="3"/>
-      <c r="AG38" s="4"/>
-      <c r="AH38" s="5"/>
-      <c r="AI38" s="5"/>
-      <c r="AJ38" s="3"/>
-    </row>
-    <row r="39" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B39" s="7"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="7"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="9"/>
-      <c r="R39" s="7"/>
-      <c r="S39" s="8"/>
-      <c r="T39" s="8"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="8"/>
-      <c r="W39" s="9"/>
-      <c r="X39" s="7"/>
-      <c r="Y39" s="8"/>
-      <c r="Z39" s="8"/>
-      <c r="AA39" s="9"/>
-      <c r="AB39" s="8"/>
-      <c r="AC39" s="8"/>
-      <c r="AD39" s="8"/>
-      <c r="AE39" s="8"/>
-      <c r="AF39" s="9"/>
-      <c r="AG39" s="30" t="s">
+      <c r="AC49" s="2"/>
+      <c r="AD49" s="2"/>
+      <c r="AE49" s="2"/>
+      <c r="AF49" s="3"/>
+      <c r="AG49" s="4"/>
+      <c r="AH49" s="5"/>
+      <c r="AI49" s="5"/>
+      <c r="AJ49" s="3"/>
+    </row>
+    <row r="50" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B50" s="7"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="8"/>
+      <c r="T50" s="8"/>
+      <c r="U50" s="8"/>
+      <c r="V50" s="8"/>
+      <c r="W50" s="9"/>
+      <c r="X50" s="7"/>
+      <c r="Y50" s="8"/>
+      <c r="Z50" s="8"/>
+      <c r="AA50" s="9"/>
+      <c r="AB50" s="8"/>
+      <c r="AC50" s="8"/>
+      <c r="AD50" s="8"/>
+      <c r="AE50" s="8"/>
+      <c r="AF50" s="9"/>
+      <c r="AG50" s="30" t="s">
         <v>399</v>
       </c>
-      <c r="AH39" s="2"/>
-      <c r="AI39" s="3"/>
-      <c r="AJ39" s="9"/>
-    </row>
-    <row r="40" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="9"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="9"/>
-      <c r="R40" s="7"/>
-      <c r="S40" s="8"/>
-      <c r="T40" s="8"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="8"/>
-      <c r="W40" s="9"/>
-      <c r="X40" s="7"/>
-      <c r="Y40" s="8"/>
-      <c r="Z40" s="8"/>
-      <c r="AA40" s="9"/>
-      <c r="AB40" s="8"/>
-      <c r="AC40" s="8"/>
-      <c r="AD40" s="8"/>
-      <c r="AE40" s="8"/>
-      <c r="AF40" s="9"/>
-      <c r="AG40" s="7"/>
-      <c r="AH40" s="8"/>
-      <c r="AI40" s="8"/>
-      <c r="AJ40" s="9"/>
-    </row>
-    <row r="41" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B41" s="7"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="7"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="9"/>
-      <c r="R41" s="7"/>
-      <c r="S41" s="8"/>
-      <c r="T41" s="8"/>
-      <c r="U41" s="8"/>
-      <c r="V41" s="8"/>
-      <c r="W41" s="9"/>
-      <c r="X41" s="7"/>
-      <c r="Y41" s="8"/>
-      <c r="Z41" s="8"/>
-      <c r="AA41" s="9"/>
-      <c r="AB41" s="8"/>
-      <c r="AC41" s="8"/>
-      <c r="AD41" s="8"/>
-      <c r="AE41" s="8"/>
-      <c r="AF41" s="9"/>
-      <c r="AG41" s="1" t="s">
+      <c r="AH50" s="2"/>
+      <c r="AI50" s="3"/>
+      <c r="AJ50" s="9"/>
+    </row>
+    <row r="51" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B51" s="7"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="9"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="8"/>
+      <c r="Q51" s="9"/>
+      <c r="R51" s="7"/>
+      <c r="S51" s="8"/>
+      <c r="T51" s="8"/>
+      <c r="U51" s="8"/>
+      <c r="V51" s="8"/>
+      <c r="W51" s="9"/>
+      <c r="X51" s="7"/>
+      <c r="Y51" s="8"/>
+      <c r="Z51" s="8"/>
+      <c r="AA51" s="9"/>
+      <c r="AB51" s="8"/>
+      <c r="AC51" s="8"/>
+      <c r="AD51" s="8"/>
+      <c r="AE51" s="8"/>
+      <c r="AF51" s="9"/>
+      <c r="AG51" s="7"/>
+      <c r="AH51" s="8"/>
+      <c r="AI51" s="8"/>
+      <c r="AJ51" s="9"/>
+    </row>
+    <row r="52" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B52" s="7"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="9"/>
+      <c r="O52" s="7"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="9"/>
+      <c r="R52" s="7"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
+      <c r="V52" s="8"/>
+      <c r="W52" s="9"/>
+      <c r="X52" s="7"/>
+      <c r="Y52" s="8"/>
+      <c r="Z52" s="8"/>
+      <c r="AA52" s="9"/>
+      <c r="AB52" s="8"/>
+      <c r="AC52" s="8"/>
+      <c r="AD52" s="8"/>
+      <c r="AE52" s="8"/>
+      <c r="AF52" s="9"/>
+      <c r="AG52" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="AH41" s="2"/>
-      <c r="AI41" s="3"/>
-      <c r="AJ41" s="9"/>
-    </row>
-    <row r="42" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B42" s="10"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="12"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="12"/>
-      <c r="R42" s="10"/>
-      <c r="S42" s="11"/>
-      <c r="T42" s="11"/>
-      <c r="U42" s="11"/>
-      <c r="V42" s="11"/>
-      <c r="W42" s="12"/>
-      <c r="X42" s="10"/>
-      <c r="Y42" s="11"/>
-      <c r="Z42" s="11"/>
-      <c r="AA42" s="12"/>
-      <c r="AB42" s="11"/>
-      <c r="AC42" s="11"/>
-      <c r="AD42" s="11"/>
-      <c r="AE42" s="11"/>
-      <c r="AF42" s="12"/>
-      <c r="AG42" s="10"/>
-      <c r="AH42" s="11"/>
-      <c r="AI42" s="11"/>
-      <c r="AJ42" s="12"/>
-    </row>
-    <row r="43" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B43" s="7"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="7"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="9"/>
-      <c r="R43" s="7"/>
-      <c r="S43" s="8"/>
-      <c r="T43" s="8"/>
-      <c r="U43" s="8"/>
-      <c r="V43" s="8"/>
-      <c r="W43" s="9"/>
-      <c r="X43" s="7"/>
-      <c r="Y43" s="8"/>
-      <c r="Z43" s="8"/>
-      <c r="AA43" s="9"/>
-      <c r="AB43" s="8"/>
-      <c r="AC43" s="8"/>
-      <c r="AD43" s="8"/>
-      <c r="AE43" s="8"/>
-      <c r="AF43" s="9"/>
-      <c r="AG43" s="7"/>
-      <c r="AH43" s="8"/>
-      <c r="AI43" s="8"/>
-      <c r="AJ43" s="9"/>
-    </row>
-    <row r="44" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B44" s="7"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="7"/>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="9"/>
-      <c r="R44" s="7"/>
-      <c r="S44" s="8"/>
-      <c r="T44" s="8"/>
-      <c r="U44" s="8"/>
-      <c r="V44" s="8"/>
-      <c r="W44" s="9"/>
-      <c r="X44" s="7"/>
-      <c r="Y44" s="8"/>
-      <c r="Z44" s="8"/>
-      <c r="AA44" s="9"/>
-      <c r="AB44" s="8"/>
-      <c r="AC44" s="8"/>
-      <c r="AD44" s="8"/>
-      <c r="AE44" s="8"/>
-      <c r="AF44" s="9"/>
-      <c r="AG44" s="30" t="s">
+      <c r="AH52" s="2"/>
+      <c r="AI52" s="3"/>
+      <c r="AJ52" s="9"/>
+    </row>
+    <row r="53" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B53" s="10"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="12"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="12"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="11"/>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="10"/>
+      <c r="S53" s="11"/>
+      <c r="T53" s="11"/>
+      <c r="U53" s="11"/>
+      <c r="V53" s="11"/>
+      <c r="W53" s="12"/>
+      <c r="X53" s="10"/>
+      <c r="Y53" s="11"/>
+      <c r="Z53" s="11"/>
+      <c r="AA53" s="12"/>
+      <c r="AB53" s="11"/>
+      <c r="AC53" s="11"/>
+      <c r="AD53" s="11"/>
+      <c r="AE53" s="11"/>
+      <c r="AF53" s="12"/>
+      <c r="AG53" s="10"/>
+      <c r="AH53" s="11"/>
+      <c r="AI53" s="11"/>
+      <c r="AJ53" s="12"/>
+    </row>
+    <row r="54" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B54" s="7"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="8"/>
+      <c r="N54" s="9"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="8"/>
+      <c r="Q54" s="9"/>
+      <c r="R54" s="7"/>
+      <c r="S54" s="8"/>
+      <c r="T54" s="8"/>
+      <c r="U54" s="8"/>
+      <c r="V54" s="8"/>
+      <c r="W54" s="9"/>
+      <c r="X54" s="7"/>
+      <c r="Y54" s="8"/>
+      <c r="Z54" s="8"/>
+      <c r="AA54" s="9"/>
+      <c r="AB54" s="8"/>
+      <c r="AC54" s="8"/>
+      <c r="AD54" s="8"/>
+      <c r="AE54" s="8"/>
+      <c r="AF54" s="9"/>
+      <c r="AG54" s="7"/>
+      <c r="AH54" s="8"/>
+      <c r="AI54" s="8"/>
+      <c r="AJ54" s="9"/>
+    </row>
+    <row r="55" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B55" s="7"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="9"/>
+      <c r="O55" s="7"/>
+      <c r="P55" s="8"/>
+      <c r="Q55" s="9"/>
+      <c r="R55" s="7"/>
+      <c r="S55" s="8"/>
+      <c r="T55" s="8"/>
+      <c r="U55" s="8"/>
+      <c r="V55" s="8"/>
+      <c r="W55" s="9"/>
+      <c r="X55" s="7"/>
+      <c r="Y55" s="8"/>
+      <c r="Z55" s="8"/>
+      <c r="AA55" s="9"/>
+      <c r="AB55" s="8"/>
+      <c r="AC55" s="8"/>
+      <c r="AD55" s="8"/>
+      <c r="AE55" s="8"/>
+      <c r="AF55" s="9"/>
+      <c r="AG55" s="30" t="s">
         <v>399</v>
       </c>
-      <c r="AH44" s="2"/>
-      <c r="AI44" s="3"/>
-      <c r="AJ44" s="9"/>
-    </row>
-    <row r="45" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B45" s="7"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="9"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="9"/>
-      <c r="O45" s="7"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="9"/>
-      <c r="R45" s="7"/>
-      <c r="S45" s="8"/>
-      <c r="T45" s="8"/>
-      <c r="U45" s="8"/>
-      <c r="V45" s="8"/>
-      <c r="W45" s="9"/>
-      <c r="X45" s="7"/>
-      <c r="Y45" s="8"/>
-      <c r="Z45" s="8"/>
-      <c r="AA45" s="9"/>
-      <c r="AB45" s="8"/>
-      <c r="AC45" s="8"/>
-      <c r="AD45" s="8"/>
-      <c r="AE45" s="8"/>
-      <c r="AF45" s="9"/>
-      <c r="AG45" s="7"/>
-      <c r="AH45" s="8"/>
-      <c r="AI45" s="8"/>
-      <c r="AJ45" s="9"/>
-    </row>
-    <row r="46" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B46" s="7"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="7"/>
-      <c r="P46" s="8"/>
-      <c r="Q46" s="9"/>
-      <c r="R46" s="7"/>
-      <c r="S46" s="8"/>
-      <c r="T46" s="8"/>
-      <c r="U46" s="8"/>
-      <c r="V46" s="8"/>
-      <c r="W46" s="9"/>
-      <c r="X46" s="7"/>
-      <c r="Y46" s="8"/>
-      <c r="Z46" s="8"/>
-      <c r="AA46" s="9"/>
-      <c r="AB46" s="8"/>
-      <c r="AC46" s="8"/>
-      <c r="AD46" s="8"/>
-      <c r="AE46" s="8"/>
-      <c r="AF46" s="9"/>
-      <c r="AG46" s="1" t="s">
+      <c r="AH55" s="2"/>
+      <c r="AI55" s="3"/>
+      <c r="AJ55" s="9"/>
+    </row>
+    <row r="56" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B56" s="7"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="9"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="9"/>
+      <c r="R56" s="7"/>
+      <c r="S56" s="8"/>
+      <c r="T56" s="8"/>
+      <c r="U56" s="8"/>
+      <c r="V56" s="8"/>
+      <c r="W56" s="9"/>
+      <c r="X56" s="7"/>
+      <c r="Y56" s="8"/>
+      <c r="Z56" s="8"/>
+      <c r="AA56" s="9"/>
+      <c r="AB56" s="8"/>
+      <c r="AC56" s="8"/>
+      <c r="AD56" s="8"/>
+      <c r="AE56" s="8"/>
+      <c r="AF56" s="9"/>
+      <c r="AG56" s="7"/>
+      <c r="AH56" s="8"/>
+      <c r="AI56" s="8"/>
+      <c r="AJ56" s="9"/>
+    </row>
+    <row r="57" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B57" s="7"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="8"/>
+      <c r="N57" s="9"/>
+      <c r="O57" s="7"/>
+      <c r="P57" s="8"/>
+      <c r="Q57" s="9"/>
+      <c r="R57" s="7"/>
+      <c r="S57" s="8"/>
+      <c r="T57" s="8"/>
+      <c r="U57" s="8"/>
+      <c r="V57" s="8"/>
+      <c r="W57" s="9"/>
+      <c r="X57" s="7"/>
+      <c r="Y57" s="8"/>
+      <c r="Z57" s="8"/>
+      <c r="AA57" s="9"/>
+      <c r="AB57" s="8"/>
+      <c r="AC57" s="8"/>
+      <c r="AD57" s="8"/>
+      <c r="AE57" s="8"/>
+      <c r="AF57" s="9"/>
+      <c r="AG57" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="AH46" s="2"/>
-      <c r="AI46" s="3"/>
-      <c r="AJ46" s="9"/>
-    </row>
-    <row r="47" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B47" s="10"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="12"/>
-      <c r="L47" s="10"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="12"/>
-      <c r="O47" s="10"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="12"/>
-      <c r="R47" s="10"/>
-      <c r="S47" s="11"/>
-      <c r="T47" s="11"/>
-      <c r="U47" s="11"/>
-      <c r="V47" s="11"/>
-      <c r="W47" s="12"/>
-      <c r="X47" s="10"/>
-      <c r="Y47" s="11"/>
-      <c r="Z47" s="11"/>
-      <c r="AA47" s="12"/>
-      <c r="AB47" s="11"/>
-      <c r="AC47" s="11"/>
-      <c r="AD47" s="11"/>
-      <c r="AE47" s="11"/>
-      <c r="AF47" s="12"/>
-      <c r="AG47" s="10"/>
-      <c r="AH47" s="11"/>
-      <c r="AI47" s="11"/>
-      <c r="AJ47" s="12"/>
+      <c r="AH57" s="2"/>
+      <c r="AI57" s="3"/>
+      <c r="AJ57" s="9"/>
+    </row>
+    <row r="58" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B58" s="10"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="10"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="12"/>
+      <c r="O58" s="10"/>
+      <c r="P58" s="11"/>
+      <c r="Q58" s="12"/>
+      <c r="R58" s="10"/>
+      <c r="S58" s="11"/>
+      <c r="T58" s="11"/>
+      <c r="U58" s="11"/>
+      <c r="V58" s="11"/>
+      <c r="W58" s="12"/>
+      <c r="X58" s="10"/>
+      <c r="Y58" s="11"/>
+      <c r="Z58" s="11"/>
+      <c r="AA58" s="12"/>
+      <c r="AB58" s="11"/>
+      <c r="AC58" s="11"/>
+      <c r="AD58" s="11"/>
+      <c r="AE58" s="11"/>
+      <c r="AF58" s="12"/>
+      <c r="AG58" s="10"/>
+      <c r="AH58" s="11"/>
+      <c r="AI58" s="11"/>
+      <c r="AJ58" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
spec halaman konfirmasi pembyaran
</commit_message>
<xml_diff>
--- a/document/spec.xlsx
+++ b/document/spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="7500" tabRatio="790" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="7500" tabRatio="790" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Agent Menu" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="687">
   <si>
     <t>Agent Register</t>
   </si>
@@ -1742,24 +1742,6 @@
     <t>update ke BLNC001, stts_pymnt</t>
   </si>
   <si>
-    <t>cancel booking</t>
-  </si>
-  <si>
-    <t>tgl check in</t>
-  </si>
-  <si>
-    <t>tgl check out</t>
-  </si>
-  <si>
-    <t>Order</t>
-  </si>
-  <si>
-    <t>total payment</t>
-  </si>
-  <si>
-    <t>Cancel fee</t>
-  </si>
-  <si>
     <t>Cancel</t>
   </si>
   <si>
@@ -1835,54 +1817,12 @@
     <t>combonya status payment</t>
   </si>
   <si>
-    <t xml:space="preserve">query </t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
-    <t>select a.order_no,a.order_date,c.comp_name,e.city_name,d.hotel_name,</t>
-  </si>
-  <si>
-    <t>inner join BLNC002 b on b.blnc001_id = a.id</t>
-  </si>
-  <si>
-    <t>inner join MST010 c on c.mst001_id = a.mst001_id</t>
-  </si>
-  <si>
-    <t>inner join MST020 d on d.id = b.mst020_id</t>
-  </si>
-  <si>
-    <t>inner join MST003 e on e.id = d.mst003_id</t>
-  </si>
-  <si>
-    <t>where a.order_no =</t>
-  </si>
-  <si>
-    <t xml:space="preserve">and  a.mst001_id = </t>
-  </si>
-  <si>
-    <t>and b.check_in_date &gt;= :fromdate and b.check_in_date &lt;= enddate</t>
-  </si>
-  <si>
-    <t>and b.check_out_date &gt;= :fromdate and b.check_out_date &lt;= enddate</t>
-  </si>
-  <si>
-    <t>and a.status_pymnt = :statusPymnt</t>
-  </si>
-  <si>
-    <t>and a.status_flg &lt;&gt; 'Cancel'</t>
-  </si>
-  <si>
     <t>cancel_fee_value</t>
   </si>
   <si>
-    <t>b.check_in_date,b.check_out_date,b.room_num,b.room_name,b.night,a.tot_payment,</t>
-  </si>
-  <si>
-    <t>from BLNC001 a</t>
-  </si>
-  <si>
     <t>tax_base_price + tax_value</t>
   </si>
   <si>
@@ -1931,30 +1871,12 @@
     <t>Klik confirm bakal kirm email ke hotel kalau status payment = done</t>
   </si>
   <si>
-    <t>case when ABS(DATEDIFF(CURDATE(), b.check_in_date)) = b.cut_off  AND b.cancel_fee_flag = 'Yes' THEN a.tot_payment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">when ABS(DATEDIFF(CURDATE(), b.check_in_date)) &lt; b.cut_off and b.cancel_fee_flag = 'Yes'  THEN b.cancel_fee_val ELSE 0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">when cancel_fee_flag = 'No' THEN a.tot_payment </t>
-  </si>
-  <si>
-    <t xml:space="preserve">when cancel_fee_flag = 'Yes' and ABS(DATEDIFF(CURDATE(), b.check_in_date)) &gt; b.cut_off THEN 0 </t>
-  </si>
-  <si>
-    <t>when status_payment &lt;&gt; 'Done' THEN 0 END as cancel_fee</t>
-  </si>
-  <si>
     <t>validasi, kalau nomor konfirmasi diisi statusnya harus confirmed</t>
   </si>
   <si>
     <t>kalau ga diisi ga blh confirmed</t>
   </si>
   <si>
-    <t>update ke BLNC001, status_flag = cancel</t>
-  </si>
-  <si>
     <t>Payment Later</t>
   </si>
   <si>
@@ -2103,6 +2025,66 @@
   </si>
   <si>
     <t>sesuai sama BLNC004nya, trus ksh minus untuk used allotmentnya soalnya ga jd dipakai</t>
+  </si>
+  <si>
+    <t>failed/done</t>
+  </si>
+  <si>
+    <t>Display Konfirmasi Pembayaran</t>
+  </si>
+  <si>
+    <t>Tanggal Konfirmasi Pembayaran</t>
+  </si>
+  <si>
+    <t>Nomor Order</t>
+  </si>
+  <si>
+    <t>Tanggal order</t>
+  </si>
+  <si>
+    <t>tanggal Order</t>
+  </si>
+  <si>
+    <t>nilai pembyaran</t>
+  </si>
+  <si>
+    <t>tanggal transfer</t>
+  </si>
+  <si>
+    <t>bank transfer</t>
+  </si>
+  <si>
+    <t>account transfer</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Status Booking</t>
+  </si>
+  <si>
+    <t>Status Payment</t>
+  </si>
+  <si>
+    <t>select a.order_no,a.order_date,a.payment_val,a.transfer_date,a.bank_transfer,a.account_transfer,a.name,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b.status_flag,b.status_pymnt from TRX001 a </t>
+  </si>
+  <si>
+    <t>inner join BLNC001 b on a.order_no = b.order_no</t>
+  </si>
+  <si>
+    <t>and a.order_date = b.order_date</t>
+  </si>
+  <si>
+    <t>where a.transfer_date between ptransferdatefrom and ptransferdateto</t>
+  </si>
+  <si>
+    <t>and a.order_no = porderno</t>
+  </si>
+  <si>
+    <t>and a.order_date between porderdatefrom and porderdaterto</t>
   </si>
 </sst>
 </file>
@@ -4777,7 +4759,7 @@
       <c r="W78" s="2"/>
       <c r="X78" s="2"/>
       <c r="Y78" s="1" t="s">
-        <v>687</v>
+        <v>661</v>
       </c>
       <c r="Z78" s="2"/>
       <c r="AA78" s="2"/>
@@ -5005,13 +4987,13 @@
       <c r="AJ83" s="8"/>
       <c r="AK83" s="8"/>
       <c r="AL83" s="1" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="AM83" s="2"/>
       <c r="AN83" s="3"/>
       <c r="AO83" s="9"/>
       <c r="AR83" t="s">
-        <v>648</v>
+        <v>622</v>
       </c>
     </row>
     <row r="84" spans="3:44" x14ac:dyDescent="0.25">
@@ -5098,7 +5080,7 @@
       <c r="AN85" s="3"/>
       <c r="AO85" s="9"/>
       <c r="AR85" s="74" t="s">
-        <v>686</v>
+        <v>660</v>
       </c>
     </row>
     <row r="86" spans="3:44" x14ac:dyDescent="0.25">
@@ -5142,7 +5124,7 @@
       <c r="AN86" s="11"/>
       <c r="AO86" s="12"/>
       <c r="AR86" s="74" t="s">
-        <v>646</v>
+        <v>620</v>
       </c>
     </row>
     <row r="87" spans="3:44" x14ac:dyDescent="0.25">
@@ -5391,7 +5373,7 @@
       <c r="AJ92" s="8"/>
       <c r="AK92" s="8"/>
       <c r="AL92" s="1" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="AM92" s="2"/>
       <c r="AN92" s="3"/>
@@ -5513,7 +5495,7 @@
         <v>1</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="E96" s="8"/>
       <c r="F96" s="8"/>
@@ -5549,10 +5531,10 @@
     <row r="97" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C97" s="8"/>
       <c r="D97" s="8" t="s">
-        <v>647</v>
+        <v>621</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>655</v>
+        <v>629</v>
       </c>
       <c r="F97" s="8"/>
       <c r="G97" s="8"/>
@@ -5587,10 +5569,10 @@
     <row r="98" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C98" s="8"/>
       <c r="D98" s="8" t="s">
-        <v>650</v>
+        <v>624</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>656</v>
+        <v>630</v>
       </c>
       <c r="F98" s="8"/>
       <c r="G98" s="8"/>
@@ -5625,10 +5607,10 @@
     <row r="99" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C99" s="8"/>
       <c r="D99" s="8" t="s">
-        <v>658</v>
+        <v>632</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>649</v>
+        <v>623</v>
       </c>
       <c r="F99" s="8"/>
       <c r="G99" s="8"/>
@@ -5663,10 +5645,10 @@
     <row r="100" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C100" s="8"/>
       <c r="D100" s="8" t="s">
-        <v>657</v>
+        <v>631</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>651</v>
+        <v>625</v>
       </c>
       <c r="F100" s="8"/>
       <c r="G100" s="8"/>
@@ -5702,7 +5684,7 @@
       <c r="C101" s="8"/>
       <c r="D101" s="19"/>
       <c r="E101" s="8" t="s">
-        <v>652</v>
+        <v>626</v>
       </c>
       <c r="F101" s="8"/>
       <c r="G101" s="8"/>
@@ -5738,7 +5720,7 @@
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
       <c r="E102" s="19" t="s">
-        <v>653</v>
+        <v>627</v>
       </c>
       <c r="F102" s="8"/>
       <c r="G102" s="8"/>
@@ -5774,7 +5756,7 @@
       <c r="C103" s="8"/>
       <c r="D103" s="8"/>
       <c r="E103" s="19" t="s">
-        <v>654</v>
+        <v>628</v>
       </c>
       <c r="F103" s="8"/>
       <c r="G103" s="8"/>
@@ -5881,10 +5863,10 @@
     <row r="106" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C106" s="8"/>
       <c r="D106" s="8" t="s">
-        <v>647</v>
+        <v>621</v>
       </c>
       <c r="E106" s="19" t="s">
-        <v>659</v>
+        <v>633</v>
       </c>
       <c r="F106" s="8"/>
       <c r="G106" s="8"/>
@@ -5956,7 +5938,7 @@
       <c r="E108" s="8"/>
       <c r="F108" s="13"/>
       <c r="G108" s="8" t="s">
-        <v>661</v>
+        <v>635</v>
       </c>
       <c r="H108" s="8"/>
       <c r="I108" s="8"/>
@@ -5969,7 +5951,7 @@
       <c r="P108" s="8"/>
       <c r="Q108" s="13"/>
       <c r="R108" s="8" t="s">
-        <v>660</v>
+        <v>634</v>
       </c>
       <c r="U108" s="8"/>
       <c r="V108" s="8"/>
@@ -6197,7 +6179,7 @@
     <row r="115" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C115" s="8"/>
       <c r="D115" s="8" t="s">
-        <v>650</v>
+        <v>624</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>64</v>
@@ -6236,7 +6218,7 @@
       <c r="C116" s="8"/>
       <c r="D116" s="8"/>
       <c r="E116" s="8" t="s">
-        <v>662</v>
+        <v>636</v>
       </c>
       <c r="F116" s="8"/>
       <c r="G116" s="8"/>
@@ -6272,7 +6254,7 @@
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
       <c r="E117" s="8" t="s">
-        <v>663</v>
+        <v>637</v>
       </c>
       <c r="F117" s="8"/>
       <c r="G117" s="8"/>
@@ -6309,7 +6291,7 @@
       <c r="D118" s="8"/>
       <c r="E118" s="8"/>
       <c r="F118" s="8" t="s">
-        <v>664</v>
+        <v>638</v>
       </c>
       <c r="G118" s="8"/>
       <c r="H118" s="8"/>
@@ -6345,7 +6327,7 @@
       <c r="D119" s="8"/>
       <c r="E119" s="8"/>
       <c r="F119" s="8" t="s">
-        <v>666</v>
+        <v>640</v>
       </c>
       <c r="G119" s="8"/>
       <c r="H119" s="8"/>
@@ -6381,7 +6363,7 @@
       <c r="D120" s="8"/>
       <c r="E120" s="8"/>
       <c r="F120" s="8" t="s">
-        <v>681</v>
+        <v>655</v>
       </c>
       <c r="G120" s="8"/>
       <c r="H120" s="8"/>
@@ -6416,7 +6398,7 @@
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
       <c r="E121" s="19" t="s">
-        <v>667</v>
+        <v>641</v>
       </c>
       <c r="F121" s="8"/>
       <c r="G121" s="8"/>
@@ -6453,7 +6435,7 @@
       <c r="D122" s="8"/>
       <c r="E122" s="19"/>
       <c r="F122" s="8" t="s">
-        <v>668</v>
+        <v>642</v>
       </c>
       <c r="G122" s="8"/>
       <c r="H122" s="8"/>
@@ -6488,7 +6470,7 @@
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
       <c r="E123" s="19" t="s">
-        <v>665</v>
+        <v>639</v>
       </c>
       <c r="F123" s="8"/>
       <c r="G123" s="8"/>
@@ -6525,7 +6507,7 @@
       <c r="D124" s="8"/>
       <c r="E124" s="19"/>
       <c r="F124" s="19" t="s">
-        <v>669</v>
+        <v>643</v>
       </c>
       <c r="G124" s="8"/>
       <c r="H124" s="8"/>
@@ -6560,7 +6542,7 @@
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
       <c r="E125" s="19" t="s">
-        <v>670</v>
+        <v>644</v>
       </c>
       <c r="F125" s="8"/>
       <c r="G125" s="8"/>
@@ -9072,10 +9054,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR135"/>
+  <dimension ref="A1:AR80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="AF50" sqref="AF50"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9949,7 +9931,7 @@
         <v>4</v>
       </c>
       <c r="AC20" s="74" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="AD20" s="74"/>
       <c r="AE20" s="74"/>
@@ -9979,7 +9961,7 @@
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B22" s="74" t="s">
-        <v>674</v>
+        <v>648</v>
       </c>
       <c r="C22" s="74"/>
       <c r="D22" s="74"/>
@@ -10003,7 +9985,7 @@
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B23" s="74"/>
       <c r="C23" s="74" t="s">
-        <v>680</v>
+        <v>654</v>
       </c>
       <c r="D23" s="74"/>
       <c r="E23" s="74"/>
@@ -10026,7 +10008,7 @@
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B24" s="74"/>
       <c r="C24" s="74" t="s">
-        <v>675</v>
+        <v>649</v>
       </c>
       <c r="D24" s="74"/>
       <c r="E24" s="74"/>
@@ -10049,7 +10031,7 @@
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B25" s="74"/>
       <c r="C25" s="74" t="s">
-        <v>676</v>
+        <v>650</v>
       </c>
       <c r="D25" s="74"/>
       <c r="E25" s="74"/>
@@ -10072,7 +10054,7 @@
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B26" s="74"/>
       <c r="C26" s="74" t="s">
-        <v>677</v>
+        <v>651</v>
       </c>
       <c r="D26" s="74"/>
       <c r="E26" s="74"/>
@@ -10080,7 +10062,7 @@
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B27" s="74"/>
       <c r="C27" s="74" t="s">
-        <v>679</v>
+        <v>653</v>
       </c>
       <c r="D27" s="74"/>
       <c r="E27" s="74"/>
@@ -10088,7 +10070,7 @@
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B28" s="74"/>
       <c r="C28" s="74" t="s">
-        <v>678</v>
+        <v>652</v>
       </c>
       <c r="D28" s="74"/>
       <c r="E28" s="74"/>
@@ -10098,7 +10080,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -10394,7 +10376,7 @@
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
       <c r="O37" s="8" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="P37" s="8"/>
       <c r="Q37" s="8"/>
@@ -10452,7 +10434,7 @@
     <row r="39" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B39" s="7"/>
       <c r="C39" s="8" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
@@ -10578,7 +10560,7 @@
         <v>3</v>
       </c>
       <c r="AF42" t="s">
-        <v>689</v>
+        <v>663</v>
       </c>
     </row>
     <row r="43" spans="2:33" x14ac:dyDescent="0.25">
@@ -10623,7 +10605,7 @@
       <c r="AB43" s="8"/>
       <c r="AC43" s="9"/>
       <c r="AF43" t="s">
-        <v>595</v>
+        <v>667</v>
       </c>
     </row>
     <row r="44" spans="2:33" x14ac:dyDescent="0.25">
@@ -10695,7 +10677,7 @@
         <v>4</v>
       </c>
       <c r="AF45" s="74" t="s">
-        <v>690</v>
+        <v>664</v>
       </c>
       <c r="AG45" s="74"/>
     </row>
@@ -10730,7 +10712,7 @@
       <c r="AC46" s="9"/>
       <c r="AE46" s="74"/>
       <c r="AF46" s="74" t="s">
-        <v>691</v>
+        <v>665</v>
       </c>
       <c r="AG46" s="74"/>
     </row>
@@ -10765,7 +10747,7 @@
       <c r="AC47" s="9"/>
       <c r="AE47" s="74"/>
       <c r="AF47" s="74" t="s">
-        <v>692</v>
+        <v>666</v>
       </c>
       <c r="AG47" s="74"/>
     </row>
@@ -10954,7 +10936,7 @@
         <v>3</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -11256,7 +11238,7 @@
       <c r="M64" s="8"/>
       <c r="N64" s="8"/>
       <c r="O64" s="8" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="P64" s="8"/>
       <c r="Q64" s="8"/>
@@ -11308,13 +11290,13 @@
         <v>2</v>
       </c>
       <c r="AL65" t="s">
-        <v>621</v>
+        <v>601</v>
       </c>
     </row>
     <row r="66" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B66" s="7"/>
       <c r="C66" s="8" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
@@ -11440,7 +11422,7 @@
         <v>3</v>
       </c>
       <c r="AL69" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
     </row>
     <row r="70" spans="2:38" x14ac:dyDescent="0.25">
@@ -11483,7 +11465,7 @@
       <c r="Z70" s="5"/>
       <c r="AA70" s="6"/>
       <c r="AB70" s="4" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="AC70" s="5"/>
       <c r="AD70" s="5"/>
@@ -11491,7 +11473,7 @@
       <c r="AF70" s="6"/>
       <c r="AI70" s="9"/>
       <c r="AL70" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
     </row>
     <row r="71" spans="2:38" x14ac:dyDescent="0.25">
@@ -11571,7 +11553,7 @@
         <v>4</v>
       </c>
       <c r="AL72" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="73" spans="2:38" x14ac:dyDescent="0.25">
@@ -11608,7 +11590,7 @@
       <c r="AF73" s="9"/>
       <c r="AI73" s="9"/>
       <c r="AL73" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
     </row>
     <row r="74" spans="2:38" x14ac:dyDescent="0.25">
@@ -11682,7 +11664,7 @@
         <v>5</v>
       </c>
       <c r="AL75" t="s">
-        <v>640</v>
+        <v>615</v>
       </c>
     </row>
     <row r="76" spans="2:38" x14ac:dyDescent="0.25">
@@ -11719,7 +11701,7 @@
       <c r="AF76" s="9"/>
       <c r="AI76" s="9"/>
       <c r="AL76" t="s">
-        <v>641</v>
+        <v>616</v>
       </c>
     </row>
     <row r="77" spans="2:38" x14ac:dyDescent="0.25">
@@ -11862,1281 +11844,6 @@
       <c r="AH80" s="11"/>
       <c r="AI80" s="12"/>
     </row>
-    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>3</v>
-      </c>
-      <c r="B85" s="24" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="B86" s="4"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5"/>
-      <c r="G86" s="5"/>
-      <c r="H86" s="5"/>
-      <c r="I86" s="5"/>
-      <c r="J86" s="5"/>
-      <c r="K86" s="5"/>
-      <c r="L86" s="5"/>
-      <c r="M86" s="5"/>
-      <c r="N86" s="5"/>
-      <c r="O86" s="5"/>
-      <c r="P86" s="5"/>
-      <c r="Q86" s="5"/>
-      <c r="R86" s="5"/>
-      <c r="S86" s="5"/>
-      <c r="T86" s="5"/>
-      <c r="U86" s="5"/>
-      <c r="V86" s="5"/>
-      <c r="W86" s="5"/>
-      <c r="X86" s="5"/>
-      <c r="Y86" s="5"/>
-      <c r="Z86" s="5"/>
-      <c r="AA86" s="5"/>
-      <c r="AB86" s="5"/>
-      <c r="AC86" s="5"/>
-      <c r="AD86" s="5"/>
-      <c r="AE86" s="5"/>
-      <c r="AF86" s="5"/>
-      <c r="AG86" s="5"/>
-      <c r="AH86" s="5"/>
-      <c r="AI86" s="5"/>
-      <c r="AJ86" s="5"/>
-      <c r="AK86" s="5"/>
-      <c r="AL86" s="5"/>
-      <c r="AM86" s="5"/>
-      <c r="AN86" s="5"/>
-      <c r="AO86" s="5"/>
-      <c r="AP86" s="6"/>
-    </row>
-    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="B87" s="7"/>
-      <c r="C87" s="8" t="s">
-        <v>556</v>
-      </c>
-      <c r="D87" s="8"/>
-      <c r="E87" s="8"/>
-      <c r="F87" s="8"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="2"/>
-      <c r="K87" s="2"/>
-      <c r="L87" s="2"/>
-      <c r="M87" s="3"/>
-      <c r="N87" s="8"/>
-      <c r="O87" s="8"/>
-      <c r="P87" s="8"/>
-      <c r="Q87" s="8"/>
-      <c r="R87" s="8"/>
-      <c r="S87" s="8"/>
-      <c r="T87" s="8"/>
-      <c r="U87" s="8"/>
-      <c r="V87" s="8"/>
-      <c r="W87" s="8"/>
-      <c r="X87" s="8"/>
-      <c r="Y87" s="8"/>
-      <c r="Z87" s="8"/>
-      <c r="AA87" s="8"/>
-      <c r="AB87" s="8"/>
-      <c r="AC87" s="8"/>
-      <c r="AD87" s="8"/>
-      <c r="AE87" s="8"/>
-      <c r="AF87" s="8"/>
-      <c r="AG87" s="8"/>
-      <c r="AH87" s="8"/>
-      <c r="AI87" s="8"/>
-      <c r="AJ87" s="8"/>
-      <c r="AK87" s="8"/>
-      <c r="AL87" s="8"/>
-      <c r="AM87" s="8"/>
-      <c r="AN87" s="8"/>
-      <c r="AO87" s="8"/>
-      <c r="AP87" s="9"/>
-    </row>
-    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="B88" s="7"/>
-      <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8"/>
-      <c r="F88" s="8"/>
-      <c r="I88" s="8"/>
-      <c r="J88" s="8"/>
-      <c r="K88" s="8"/>
-      <c r="L88" s="8"/>
-      <c r="M88" s="8"/>
-      <c r="N88" s="8"/>
-      <c r="O88" s="8"/>
-      <c r="P88" s="8"/>
-      <c r="Q88" s="8"/>
-      <c r="R88" s="8"/>
-      <c r="S88" s="8"/>
-      <c r="T88" s="8"/>
-      <c r="U88" s="8"/>
-      <c r="V88" s="8"/>
-      <c r="W88" s="8"/>
-      <c r="X88" s="8"/>
-      <c r="Y88" s="8"/>
-      <c r="Z88" s="8"/>
-      <c r="AA88" s="8"/>
-      <c r="AB88" s="8"/>
-      <c r="AC88" s="8"/>
-      <c r="AD88" s="8"/>
-      <c r="AE88" s="8"/>
-      <c r="AF88" s="8"/>
-      <c r="AG88" s="8"/>
-      <c r="AH88" s="8"/>
-      <c r="AI88" s="8"/>
-      <c r="AJ88" s="8"/>
-      <c r="AK88" s="8"/>
-      <c r="AL88" s="8"/>
-      <c r="AM88" s="8"/>
-      <c r="AN88" s="8"/>
-      <c r="AO88" s="8"/>
-      <c r="AP88" s="9"/>
-    </row>
-    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="B89" s="7"/>
-      <c r="C89" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8"/>
-      <c r="F89" s="8"/>
-      <c r="I89" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J89" s="2"/>
-      <c r="K89" s="2"/>
-      <c r="L89" s="2"/>
-      <c r="M89" s="3"/>
-      <c r="N89" s="8"/>
-      <c r="O89" s="8"/>
-      <c r="P89" s="8"/>
-      <c r="Q89" s="8"/>
-      <c r="R89" s="8"/>
-      <c r="S89" s="8"/>
-      <c r="T89" s="8"/>
-      <c r="U89" s="8"/>
-      <c r="V89" s="8"/>
-      <c r="W89" s="8"/>
-      <c r="X89" s="8"/>
-      <c r="Y89" s="8"/>
-      <c r="Z89" s="8"/>
-      <c r="AA89" s="8"/>
-      <c r="AB89" s="8"/>
-      <c r="AC89" s="8"/>
-      <c r="AD89" s="8"/>
-      <c r="AE89" s="8"/>
-      <c r="AF89" s="8"/>
-      <c r="AG89" s="8"/>
-      <c r="AH89" s="8"/>
-      <c r="AI89" s="8"/>
-      <c r="AJ89" s="8"/>
-      <c r="AK89" s="8"/>
-      <c r="AL89" s="8"/>
-      <c r="AM89" s="8"/>
-      <c r="AN89" s="8"/>
-      <c r="AO89" s="8"/>
-      <c r="AP89" s="9"/>
-    </row>
-    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="B90" s="7"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="8"/>
-      <c r="F90" s="8"/>
-      <c r="I90" s="8"/>
-      <c r="J90" s="8"/>
-      <c r="K90" s="8"/>
-      <c r="L90" s="8"/>
-      <c r="M90" s="8"/>
-      <c r="N90" s="8"/>
-      <c r="O90" s="8"/>
-      <c r="P90" s="8"/>
-      <c r="Q90" s="8"/>
-      <c r="R90" s="8"/>
-      <c r="S90" s="8"/>
-      <c r="T90" s="8"/>
-      <c r="U90" s="8"/>
-      <c r="V90" s="8"/>
-      <c r="W90" s="8"/>
-      <c r="X90" s="8"/>
-      <c r="Y90" s="8"/>
-      <c r="Z90" s="8"/>
-      <c r="AA90" s="8"/>
-      <c r="AB90" s="8"/>
-      <c r="AC90" s="8"/>
-      <c r="AD90" s="8"/>
-      <c r="AE90" s="8"/>
-      <c r="AF90" s="8"/>
-      <c r="AG90" s="8"/>
-      <c r="AH90" s="8"/>
-      <c r="AI90" s="8"/>
-      <c r="AJ90" s="8"/>
-      <c r="AK90" s="8"/>
-      <c r="AL90" s="8"/>
-      <c r="AM90" s="8"/>
-      <c r="AN90" s="8"/>
-      <c r="AO90" s="8"/>
-      <c r="AP90" s="9"/>
-    </row>
-    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="B91" s="7"/>
-      <c r="C91" s="8" t="s">
-        <v>573</v>
-      </c>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="8"/>
-      <c r="I91" s="13"/>
-      <c r="J91" s="13"/>
-      <c r="K91" s="1"/>
-      <c r="L91" s="3"/>
-      <c r="M91" s="8"/>
-      <c r="N91" s="8" t="s">
-        <v>558</v>
-      </c>
-      <c r="O91" s="8"/>
-      <c r="P91" s="13"/>
-      <c r="Q91" s="13"/>
-      <c r="R91" s="1"/>
-      <c r="S91" s="3"/>
-      <c r="T91" s="8"/>
-      <c r="U91" s="8"/>
-      <c r="V91" s="8"/>
-      <c r="W91" s="8"/>
-      <c r="X91" s="8"/>
-      <c r="Y91" s="8"/>
-      <c r="Z91" s="8"/>
-      <c r="AA91" s="8"/>
-      <c r="AB91" s="8"/>
-      <c r="AC91" s="8"/>
-      <c r="AD91" s="8"/>
-      <c r="AE91" s="8"/>
-      <c r="AF91" s="8"/>
-      <c r="AG91" s="8"/>
-      <c r="AH91" s="8"/>
-      <c r="AI91" s="8"/>
-      <c r="AJ91" s="8"/>
-      <c r="AK91" s="8"/>
-      <c r="AL91" s="8"/>
-      <c r="AM91" s="8"/>
-      <c r="AN91" s="8"/>
-      <c r="AO91" s="8"/>
-      <c r="AP91" s="9"/>
-    </row>
-    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="B92" s="7"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="8"/>
-      <c r="I92" s="8"/>
-      <c r="J92" s="8"/>
-      <c r="K92" s="8"/>
-      <c r="L92" s="8"/>
-      <c r="M92" s="8"/>
-      <c r="N92" s="8"/>
-      <c r="O92" s="8"/>
-      <c r="P92" s="8"/>
-      <c r="Q92" s="8"/>
-      <c r="R92" s="8"/>
-      <c r="S92" s="8"/>
-      <c r="T92" s="8"/>
-      <c r="U92" s="8"/>
-      <c r="V92" s="8"/>
-      <c r="W92" s="8"/>
-      <c r="X92" s="8"/>
-      <c r="Y92" s="8"/>
-      <c r="Z92" s="8"/>
-      <c r="AA92" s="8"/>
-      <c r="AB92" s="8"/>
-      <c r="AC92" s="8"/>
-      <c r="AD92" s="8"/>
-      <c r="AE92" s="8"/>
-      <c r="AF92" s="8"/>
-      <c r="AG92" s="8"/>
-      <c r="AH92" s="8"/>
-      <c r="AI92" s="8"/>
-      <c r="AJ92" s="8"/>
-      <c r="AK92" s="8"/>
-      <c r="AL92" s="8"/>
-      <c r="AM92" s="8"/>
-      <c r="AN92" s="8"/>
-      <c r="AO92" s="8"/>
-      <c r="AP92" s="9"/>
-    </row>
-    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="B93" s="7"/>
-      <c r="C93" s="8" t="s">
-        <v>574</v>
-      </c>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="8"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="13"/>
-      <c r="K93" s="1"/>
-      <c r="L93" s="3"/>
-      <c r="M93" s="8"/>
-      <c r="N93" s="8" t="s">
-        <v>558</v>
-      </c>
-      <c r="O93" s="8"/>
-      <c r="P93" s="13"/>
-      <c r="Q93" s="13"/>
-      <c r="R93" s="1"/>
-      <c r="S93" s="3"/>
-      <c r="T93" s="8"/>
-      <c r="U93" s="8"/>
-      <c r="V93" s="8"/>
-      <c r="W93" s="8"/>
-      <c r="X93" s="8"/>
-      <c r="Y93" s="8"/>
-      <c r="Z93" s="8"/>
-      <c r="AA93" s="8"/>
-      <c r="AB93" s="8"/>
-      <c r="AC93" s="8"/>
-      <c r="AD93" s="8"/>
-      <c r="AE93" s="8"/>
-      <c r="AF93" s="8"/>
-      <c r="AG93" s="8"/>
-      <c r="AH93" s="8"/>
-      <c r="AI93" s="8"/>
-      <c r="AJ93" s="8"/>
-      <c r="AK93" s="8"/>
-      <c r="AL93" s="8"/>
-      <c r="AM93" s="8"/>
-      <c r="AN93" s="8"/>
-      <c r="AO93" s="8"/>
-      <c r="AP93" s="9"/>
-    </row>
-    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="B94" s="7"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="8"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
-      <c r="I94" s="8"/>
-      <c r="J94" s="8"/>
-      <c r="K94" s="8"/>
-      <c r="L94" s="8"/>
-      <c r="M94" s="8"/>
-      <c r="N94" s="8"/>
-      <c r="O94" s="8"/>
-      <c r="P94" s="8"/>
-      <c r="Q94" s="8"/>
-      <c r="R94" s="8"/>
-      <c r="S94" s="8"/>
-      <c r="T94" s="8"/>
-      <c r="U94" s="8"/>
-      <c r="V94" s="8"/>
-      <c r="W94" s="8"/>
-      <c r="X94" s="8"/>
-      <c r="Y94" s="8"/>
-      <c r="Z94" s="8"/>
-      <c r="AA94" s="8"/>
-      <c r="AB94" s="8"/>
-      <c r="AC94" s="8"/>
-      <c r="AD94" s="8"/>
-      <c r="AE94" s="8"/>
-      <c r="AF94" s="8"/>
-      <c r="AG94" s="8"/>
-      <c r="AH94" s="8"/>
-      <c r="AI94" s="8"/>
-      <c r="AJ94" s="8"/>
-      <c r="AK94" s="8"/>
-      <c r="AL94" s="8"/>
-      <c r="AM94" s="8"/>
-      <c r="AN94" s="8"/>
-      <c r="AO94" s="8"/>
-      <c r="AP94" s="9"/>
-    </row>
-    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="B95" s="7"/>
-      <c r="C95" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="8"/>
-      <c r="I95" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J95" s="2"/>
-      <c r="K95" s="2"/>
-      <c r="L95" s="2"/>
-      <c r="M95" s="3"/>
-      <c r="N95" s="8"/>
-      <c r="O95" s="8"/>
-      <c r="P95" s="8"/>
-      <c r="Q95" s="8"/>
-      <c r="R95" s="8"/>
-      <c r="S95" s="8"/>
-      <c r="T95" s="8"/>
-      <c r="U95" s="8"/>
-      <c r="V95" s="8"/>
-      <c r="W95" s="8"/>
-      <c r="X95" s="8"/>
-      <c r="Y95" s="8"/>
-      <c r="Z95" s="8"/>
-      <c r="AA95" s="8"/>
-      <c r="AB95" s="8"/>
-      <c r="AC95" s="8"/>
-      <c r="AD95" s="8"/>
-      <c r="AE95" s="8"/>
-      <c r="AF95" s="8"/>
-      <c r="AG95" s="8"/>
-      <c r="AH95" s="8"/>
-      <c r="AI95" s="8"/>
-      <c r="AJ95" s="8"/>
-      <c r="AK95" s="8"/>
-      <c r="AL95" s="8"/>
-      <c r="AM95" s="8"/>
-      <c r="AN95" s="8"/>
-      <c r="AO95" s="8"/>
-      <c r="AP95" s="9"/>
-    </row>
-    <row r="96" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="B96" s="7"/>
-      <c r="C96" s="8"/>
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
-      <c r="F96" s="8"/>
-      <c r="G96" s="8"/>
-      <c r="H96" s="8"/>
-      <c r="I96" s="8"/>
-      <c r="J96" s="8"/>
-      <c r="K96" s="8"/>
-      <c r="L96" s="8"/>
-      <c r="M96" s="8"/>
-      <c r="N96" s="8"/>
-      <c r="O96" s="8"/>
-      <c r="P96" s="8"/>
-      <c r="Q96" s="8"/>
-      <c r="R96" s="8"/>
-      <c r="S96" s="8"/>
-      <c r="T96" s="8"/>
-      <c r="U96" s="8"/>
-      <c r="V96" s="8"/>
-      <c r="W96" s="8"/>
-      <c r="X96" s="8"/>
-      <c r="Y96" s="8"/>
-      <c r="Z96" s="8"/>
-      <c r="AA96" s="8"/>
-      <c r="AB96" s="8"/>
-      <c r="AC96" s="8"/>
-      <c r="AD96" s="8"/>
-      <c r="AE96" s="8"/>
-      <c r="AF96" s="8"/>
-      <c r="AG96" s="8"/>
-      <c r="AH96" s="8"/>
-      <c r="AI96" s="8"/>
-      <c r="AJ96" s="8"/>
-      <c r="AK96" s="8"/>
-      <c r="AL96" s="8"/>
-      <c r="AM96" s="8"/>
-      <c r="AN96" s="8"/>
-      <c r="AO96" s="8"/>
-      <c r="AP96" s="9"/>
-    </row>
-    <row r="97" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B97" s="7"/>
-      <c r="C97" s="8" t="s">
-        <v>562</v>
-      </c>
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
-      <c r="F97" s="8"/>
-      <c r="G97" s="8"/>
-      <c r="H97" s="8"/>
-      <c r="I97" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J97" s="2"/>
-      <c r="K97" s="2"/>
-      <c r="L97" s="2"/>
-      <c r="M97" s="3"/>
-      <c r="N97" s="8"/>
-      <c r="O97" s="8"/>
-      <c r="P97" t="s">
-        <v>595</v>
-      </c>
-      <c r="Q97" s="8"/>
-      <c r="R97" s="8"/>
-      <c r="S97" s="8"/>
-      <c r="T97" s="8"/>
-      <c r="U97" s="8"/>
-      <c r="V97" s="8"/>
-      <c r="W97" s="8"/>
-      <c r="X97" s="8"/>
-      <c r="Y97" s="8"/>
-      <c r="Z97" s="8"/>
-      <c r="AA97" s="8"/>
-      <c r="AB97" s="8"/>
-      <c r="AC97" s="8"/>
-      <c r="AD97" s="8"/>
-      <c r="AE97" s="8"/>
-      <c r="AF97" s="8"/>
-      <c r="AG97" s="8"/>
-      <c r="AH97" s="8"/>
-      <c r="AI97" s="8"/>
-      <c r="AJ97" s="8"/>
-      <c r="AK97" s="8"/>
-      <c r="AL97" s="8"/>
-      <c r="AM97" s="8"/>
-      <c r="AN97" s="8"/>
-      <c r="AO97" s="8"/>
-      <c r="AP97" s="9"/>
-    </row>
-    <row r="98" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B98" s="7"/>
-      <c r="C98" s="8"/>
-      <c r="D98" s="8"/>
-      <c r="E98" s="8"/>
-      <c r="F98" s="8"/>
-      <c r="G98" s="8"/>
-      <c r="H98" s="8"/>
-      <c r="I98" s="8"/>
-      <c r="J98" s="8"/>
-      <c r="K98" s="8"/>
-      <c r="L98" s="8"/>
-      <c r="M98" s="8"/>
-      <c r="N98" s="8"/>
-      <c r="O98" s="8"/>
-      <c r="P98" s="8"/>
-      <c r="Q98" s="8"/>
-      <c r="R98" s="8"/>
-      <c r="S98" s="8"/>
-      <c r="T98" s="8"/>
-      <c r="U98" s="8"/>
-      <c r="V98" s="8"/>
-      <c r="W98" s="8"/>
-      <c r="X98" s="8"/>
-      <c r="Y98" s="8"/>
-      <c r="Z98" s="8"/>
-      <c r="AA98" s="8"/>
-      <c r="AB98" s="8"/>
-      <c r="AC98" s="8"/>
-      <c r="AD98" s="8"/>
-      <c r="AE98" s="8"/>
-      <c r="AF98" s="8"/>
-      <c r="AG98" s="8"/>
-      <c r="AH98" s="8"/>
-      <c r="AI98" s="8"/>
-      <c r="AJ98" s="8"/>
-      <c r="AK98" s="8"/>
-      <c r="AL98" s="8"/>
-      <c r="AM98" s="8"/>
-      <c r="AN98" s="8"/>
-      <c r="AO98" s="8"/>
-      <c r="AP98" s="9"/>
-    </row>
-    <row r="99" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B99" s="7"/>
-      <c r="C99" s="14" t="s">
-        <v>391</v>
-      </c>
-      <c r="D99" s="75"/>
-      <c r="E99" s="8"/>
-      <c r="F99" s="8"/>
-      <c r="G99" s="8"/>
-      <c r="H99" s="8"/>
-      <c r="I99" s="8"/>
-      <c r="J99" s="8"/>
-      <c r="K99" s="8"/>
-      <c r="L99" s="8"/>
-      <c r="M99" s="8"/>
-      <c r="N99" s="8"/>
-      <c r="O99" s="8"/>
-      <c r="P99" s="8"/>
-      <c r="Q99" s="8"/>
-      <c r="R99" s="8"/>
-      <c r="S99" s="8"/>
-      <c r="T99" s="8"/>
-      <c r="U99" s="8"/>
-      <c r="V99" s="8"/>
-      <c r="W99" s="8"/>
-      <c r="X99" s="8"/>
-      <c r="Y99" s="8"/>
-      <c r="Z99" s="8"/>
-      <c r="AA99" s="8"/>
-      <c r="AB99" s="8"/>
-      <c r="AC99" s="8"/>
-      <c r="AD99" s="8"/>
-      <c r="AE99" s="8"/>
-      <c r="AF99" s="8"/>
-      <c r="AG99" s="8"/>
-      <c r="AH99" s="8"/>
-      <c r="AI99" s="8"/>
-      <c r="AJ99" s="8"/>
-      <c r="AK99" s="8"/>
-      <c r="AL99" s="8"/>
-      <c r="AM99" s="8"/>
-      <c r="AN99" s="8"/>
-      <c r="AO99" s="8"/>
-      <c r="AP99" s="9"/>
-    </row>
-    <row r="100" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B100" s="7"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
-      <c r="F100" s="8"/>
-      <c r="G100" s="8"/>
-      <c r="H100" s="8"/>
-      <c r="I100" s="8"/>
-      <c r="J100" s="8"/>
-      <c r="K100" s="8"/>
-      <c r="L100" s="8"/>
-      <c r="M100" s="8"/>
-      <c r="N100" s="8"/>
-      <c r="O100" s="8"/>
-      <c r="P100" s="8"/>
-      <c r="Q100" s="8"/>
-      <c r="R100" s="8"/>
-      <c r="S100" s="8"/>
-      <c r="T100" s="8"/>
-      <c r="U100" s="8"/>
-      <c r="V100" s="8"/>
-      <c r="W100" s="8"/>
-      <c r="X100" s="8"/>
-      <c r="Y100" s="8"/>
-      <c r="Z100" s="8"/>
-      <c r="AA100" s="8"/>
-      <c r="AB100" s="8"/>
-      <c r="AC100" s="8"/>
-      <c r="AD100" s="8"/>
-      <c r="AE100" s="8"/>
-      <c r="AF100" s="8"/>
-      <c r="AG100" s="8"/>
-      <c r="AH100" s="8"/>
-      <c r="AI100" s="8"/>
-      <c r="AJ100" s="8"/>
-      <c r="AK100" s="8"/>
-      <c r="AL100" s="8"/>
-      <c r="AM100" s="8"/>
-      <c r="AN100" s="8"/>
-      <c r="AO100" s="8"/>
-      <c r="AP100" s="9"/>
-    </row>
-    <row r="101" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B101" s="7"/>
-      <c r="C101" s="8"/>
-      <c r="D101" s="4" t="s">
-        <v>578</v>
-      </c>
-      <c r="E101" s="6"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="I101" s="2"/>
-      <c r="J101" s="2"/>
-      <c r="K101" s="2"/>
-      <c r="L101" s="2"/>
-      <c r="M101" s="3"/>
-      <c r="N101" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="O101" s="5"/>
-      <c r="P101" s="6"/>
-      <c r="Q101" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="R101" s="6"/>
-      <c r="S101" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="T101" s="6"/>
-      <c r="U101" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="V101" s="5"/>
-      <c r="W101" s="5"/>
-      <c r="X101" s="6"/>
-      <c r="Y101" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z101" s="5"/>
-      <c r="AA101" s="5"/>
-      <c r="AB101" s="6"/>
-      <c r="AC101" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="AD101" s="5"/>
-      <c r="AE101" s="6"/>
-      <c r="AF101" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="AG101" s="6"/>
-      <c r="AH101" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI101" s="6"/>
-      <c r="AJ101" s="4" t="s">
-        <v>576</v>
-      </c>
-      <c r="AK101" s="5"/>
-      <c r="AL101" s="5"/>
-      <c r="AM101" s="6"/>
-      <c r="AN101" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="AO101" s="5"/>
-      <c r="AP101" s="6"/>
-    </row>
-    <row r="102" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B102" s="7"/>
-      <c r="C102" s="8"/>
-      <c r="D102" s="10"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="3"/>
-      <c r="J102" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="K102" s="2"/>
-      <c r="L102" s="2"/>
-      <c r="M102" s="3"/>
-      <c r="N102" s="10"/>
-      <c r="O102" s="11"/>
-      <c r="P102" s="12"/>
-      <c r="Q102" s="10"/>
-      <c r="R102" s="12"/>
-      <c r="S102" s="10"/>
-      <c r="T102" s="12"/>
-      <c r="U102" s="10"/>
-      <c r="V102" s="11"/>
-      <c r="W102" s="11"/>
-      <c r="X102" s="12"/>
-      <c r="Y102" s="10"/>
-      <c r="Z102" s="11"/>
-      <c r="AA102" s="11"/>
-      <c r="AB102" s="12"/>
-      <c r="AC102" s="10" t="s">
-        <v>604</v>
-      </c>
-      <c r="AD102" s="11"/>
-      <c r="AE102" s="11"/>
-      <c r="AF102" s="10"/>
-      <c r="AG102" s="12"/>
-      <c r="AH102" s="11"/>
-      <c r="AI102" s="12"/>
-      <c r="AJ102" s="10"/>
-      <c r="AK102" s="11"/>
-      <c r="AL102" s="11"/>
-      <c r="AM102" s="12"/>
-      <c r="AN102" s="10"/>
-      <c r="AO102" s="11"/>
-      <c r="AP102" s="12"/>
-    </row>
-    <row r="103" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B103" s="7"/>
-      <c r="C103" s="8"/>
-      <c r="D103" s="1"/>
-      <c r="E103" s="3"/>
-      <c r="F103" s="7"/>
-      <c r="G103" s="8"/>
-      <c r="H103" s="8"/>
-      <c r="I103" s="9"/>
-      <c r="J103" s="8"/>
-      <c r="K103" s="8"/>
-      <c r="L103" s="8"/>
-      <c r="M103" s="9"/>
-      <c r="N103" s="7"/>
-      <c r="O103" s="8"/>
-      <c r="P103" s="9"/>
-      <c r="Q103" s="4"/>
-      <c r="R103" s="6"/>
-      <c r="S103" s="7"/>
-      <c r="T103" s="9"/>
-      <c r="U103" s="7"/>
-      <c r="V103" s="8"/>
-      <c r="W103" s="8"/>
-      <c r="X103" s="9"/>
-      <c r="Y103" s="7"/>
-      <c r="Z103" s="8"/>
-      <c r="AA103" s="8"/>
-      <c r="AB103" s="9"/>
-      <c r="AC103" s="7"/>
-      <c r="AD103" s="8"/>
-      <c r="AE103" s="9"/>
-      <c r="AF103" s="7"/>
-      <c r="AG103" s="9"/>
-      <c r="AH103" s="7"/>
-      <c r="AI103" s="9"/>
-      <c r="AJ103" s="7"/>
-      <c r="AK103" s="8"/>
-      <c r="AL103" s="8"/>
-      <c r="AM103" s="9"/>
-      <c r="AN103" s="7"/>
-      <c r="AO103" s="8"/>
-      <c r="AP103" s="9"/>
-    </row>
-    <row r="104" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B104" s="7"/>
-      <c r="C104" s="8"/>
-      <c r="D104" s="7"/>
-      <c r="E104" s="9"/>
-      <c r="F104" s="7"/>
-      <c r="G104" s="8"/>
-      <c r="H104" s="8"/>
-      <c r="I104" s="9"/>
-      <c r="J104" s="8"/>
-      <c r="K104" s="8"/>
-      <c r="L104" s="8"/>
-      <c r="M104" s="9"/>
-      <c r="N104" s="7"/>
-      <c r="O104" s="8"/>
-      <c r="P104" s="9"/>
-      <c r="Q104" s="7"/>
-      <c r="R104" s="9"/>
-      <c r="S104" s="7"/>
-      <c r="T104" s="9"/>
-      <c r="U104" s="7"/>
-      <c r="V104" s="8"/>
-      <c r="W104" s="8"/>
-      <c r="X104" s="9"/>
-      <c r="Y104" s="7"/>
-      <c r="Z104" s="8"/>
-      <c r="AA104" s="8"/>
-      <c r="AB104" s="9"/>
-      <c r="AC104" s="7"/>
-      <c r="AD104" s="8"/>
-      <c r="AE104" s="9"/>
-      <c r="AF104" s="7"/>
-      <c r="AG104" s="9"/>
-      <c r="AH104" s="7"/>
-      <c r="AI104" s="9"/>
-      <c r="AJ104" s="7"/>
-      <c r="AK104" s="8"/>
-      <c r="AL104" s="8"/>
-      <c r="AM104" s="9"/>
-      <c r="AN104" s="7"/>
-      <c r="AO104" s="8"/>
-      <c r="AP104" s="9"/>
-    </row>
-    <row r="105" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B105" s="7"/>
-      <c r="C105" s="8"/>
-      <c r="D105" s="7"/>
-      <c r="E105" s="9"/>
-      <c r="F105" s="7"/>
-      <c r="G105" s="8"/>
-      <c r="H105" s="8"/>
-      <c r="I105" s="9"/>
-      <c r="J105" s="8"/>
-      <c r="K105" s="8"/>
-      <c r="L105" s="8"/>
-      <c r="M105" s="9"/>
-      <c r="N105" s="7"/>
-      <c r="O105" s="8"/>
-      <c r="P105" s="9"/>
-      <c r="Q105" s="7"/>
-      <c r="R105" s="9"/>
-      <c r="S105" s="7"/>
-      <c r="T105" s="9"/>
-      <c r="U105" s="7"/>
-      <c r="V105" s="8"/>
-      <c r="W105" s="8"/>
-      <c r="X105" s="9"/>
-      <c r="Y105" s="7"/>
-      <c r="Z105" s="8"/>
-      <c r="AA105" s="8"/>
-      <c r="AB105" s="9"/>
-      <c r="AC105" s="7"/>
-      <c r="AD105" s="8"/>
-      <c r="AE105" s="9"/>
-      <c r="AF105" s="7"/>
-      <c r="AG105" s="9"/>
-      <c r="AH105" s="7"/>
-      <c r="AI105" s="9"/>
-      <c r="AJ105" s="7"/>
-      <c r="AK105" s="8"/>
-      <c r="AL105" s="8"/>
-      <c r="AM105" s="9"/>
-      <c r="AN105" s="7"/>
-      <c r="AO105" s="8"/>
-      <c r="AP105" s="9"/>
-    </row>
-    <row r="106" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B106" s="7"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="7"/>
-      <c r="E106" s="9"/>
-      <c r="F106" s="7"/>
-      <c r="G106" s="8"/>
-      <c r="H106" s="8"/>
-      <c r="I106" s="9"/>
-      <c r="J106" s="8"/>
-      <c r="K106" s="8"/>
-      <c r="L106" s="8"/>
-      <c r="M106" s="9"/>
-      <c r="N106" s="7"/>
-      <c r="O106" s="8"/>
-      <c r="P106" s="9"/>
-      <c r="Q106" s="7"/>
-      <c r="R106" s="9"/>
-      <c r="S106" s="7"/>
-      <c r="T106" s="9"/>
-      <c r="U106" s="7"/>
-      <c r="V106" s="8"/>
-      <c r="W106" s="8"/>
-      <c r="X106" s="9"/>
-      <c r="Y106" s="7"/>
-      <c r="Z106" s="8"/>
-      <c r="AA106" s="8"/>
-      <c r="AB106" s="9"/>
-      <c r="AC106" s="7"/>
-      <c r="AD106" s="8"/>
-      <c r="AE106" s="9"/>
-      <c r="AF106" s="7"/>
-      <c r="AG106" s="9"/>
-      <c r="AH106" s="7"/>
-      <c r="AI106" s="9"/>
-      <c r="AJ106" s="7"/>
-      <c r="AK106" s="8"/>
-      <c r="AL106" s="8"/>
-      <c r="AM106" s="9"/>
-      <c r="AN106" s="7"/>
-      <c r="AO106" s="8"/>
-      <c r="AP106" s="9"/>
-    </row>
-    <row r="107" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B107" s="7"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="7"/>
-      <c r="E107" s="9"/>
-      <c r="F107" s="7"/>
-      <c r="G107" s="8"/>
-      <c r="H107" s="8"/>
-      <c r="I107" s="9"/>
-      <c r="J107" s="8"/>
-      <c r="K107" s="8"/>
-      <c r="L107" s="8"/>
-      <c r="M107" s="9"/>
-      <c r="N107" s="7"/>
-      <c r="O107" s="8"/>
-      <c r="P107" s="9"/>
-      <c r="Q107" s="7"/>
-      <c r="R107" s="9"/>
-      <c r="S107" s="7"/>
-      <c r="T107" s="9"/>
-      <c r="U107" s="7"/>
-      <c r="V107" s="8"/>
-      <c r="W107" s="8"/>
-      <c r="X107" s="9"/>
-      <c r="Y107" s="7"/>
-      <c r="Z107" s="8"/>
-      <c r="AA107" s="8"/>
-      <c r="AB107" s="9"/>
-      <c r="AC107" s="7"/>
-      <c r="AD107" s="8"/>
-      <c r="AE107" s="9"/>
-      <c r="AF107" s="7"/>
-      <c r="AG107" s="9"/>
-      <c r="AH107" s="7"/>
-      <c r="AI107" s="9"/>
-      <c r="AJ107" s="7"/>
-      <c r="AK107" s="8"/>
-      <c r="AL107" s="8"/>
-      <c r="AM107" s="9"/>
-      <c r="AN107" s="7"/>
-      <c r="AO107" s="8"/>
-      <c r="AP107" s="9"/>
-    </row>
-    <row r="108" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B108" s="7"/>
-      <c r="C108" s="8"/>
-      <c r="D108" s="7"/>
-      <c r="E108" s="9"/>
-      <c r="F108" s="7"/>
-      <c r="G108" s="8"/>
-      <c r="H108" s="8"/>
-      <c r="I108" s="9"/>
-      <c r="J108" s="8"/>
-      <c r="K108" s="8"/>
-      <c r="L108" s="8"/>
-      <c r="M108" s="9"/>
-      <c r="N108" s="7"/>
-      <c r="O108" s="8"/>
-      <c r="P108" s="9"/>
-      <c r="Q108" s="7"/>
-      <c r="R108" s="9"/>
-      <c r="S108" s="7"/>
-      <c r="T108" s="9"/>
-      <c r="U108" s="7"/>
-      <c r="V108" s="8"/>
-      <c r="W108" s="8"/>
-      <c r="X108" s="9"/>
-      <c r="Y108" s="7"/>
-      <c r="Z108" s="8"/>
-      <c r="AA108" s="8"/>
-      <c r="AB108" s="9"/>
-      <c r="AC108" s="7"/>
-      <c r="AD108" s="8"/>
-      <c r="AE108" s="9"/>
-      <c r="AF108" s="7"/>
-      <c r="AG108" s="9"/>
-      <c r="AH108" s="7"/>
-      <c r="AI108" s="9"/>
-      <c r="AJ108" s="7"/>
-      <c r="AK108" s="8"/>
-      <c r="AL108" s="8"/>
-      <c r="AM108" s="9"/>
-      <c r="AN108" s="7"/>
-      <c r="AO108" s="8"/>
-      <c r="AP108" s="9"/>
-    </row>
-    <row r="109" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B109" s="7"/>
-      <c r="C109" s="8"/>
-      <c r="D109" s="10"/>
-      <c r="E109" s="12"/>
-      <c r="F109" s="10"/>
-      <c r="G109" s="11"/>
-      <c r="H109" s="11"/>
-      <c r="I109" s="12"/>
-      <c r="J109" s="11"/>
-      <c r="K109" s="11"/>
-      <c r="L109" s="11"/>
-      <c r="M109" s="12"/>
-      <c r="N109" s="10"/>
-      <c r="O109" s="11"/>
-      <c r="P109" s="12"/>
-      <c r="Q109" s="10"/>
-      <c r="R109" s="12"/>
-      <c r="S109" s="10"/>
-      <c r="T109" s="12"/>
-      <c r="U109" s="10"/>
-      <c r="V109" s="11"/>
-      <c r="W109" s="11"/>
-      <c r="X109" s="12"/>
-      <c r="Y109" s="10"/>
-      <c r="Z109" s="11"/>
-      <c r="AA109" s="11"/>
-      <c r="AB109" s="12"/>
-      <c r="AC109" s="10"/>
-      <c r="AD109" s="11"/>
-      <c r="AE109" s="12"/>
-      <c r="AF109" s="10"/>
-      <c r="AG109" s="12"/>
-      <c r="AH109" s="10"/>
-      <c r="AI109" s="12"/>
-      <c r="AJ109" s="10"/>
-      <c r="AK109" s="11"/>
-      <c r="AL109" s="11"/>
-      <c r="AM109" s="12"/>
-      <c r="AN109" s="10"/>
-      <c r="AO109" s="11"/>
-      <c r="AP109" s="12"/>
-    </row>
-    <row r="110" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B110" s="7"/>
-      <c r="C110" s="8"/>
-      <c r="D110" s="8"/>
-      <c r="E110" s="8"/>
-      <c r="F110" s="8"/>
-      <c r="G110" s="8"/>
-      <c r="H110" s="8"/>
-      <c r="I110" s="8"/>
-      <c r="J110" s="8"/>
-      <c r="K110" s="8"/>
-      <c r="L110" s="8"/>
-      <c r="M110" s="8"/>
-      <c r="N110" s="8"/>
-      <c r="O110" s="8"/>
-      <c r="P110" s="8"/>
-      <c r="Q110" s="8"/>
-      <c r="R110" s="8"/>
-      <c r="S110" s="8"/>
-      <c r="T110" s="8"/>
-      <c r="U110" s="8"/>
-      <c r="V110" s="8"/>
-      <c r="W110" s="8"/>
-      <c r="X110" s="8"/>
-      <c r="Y110" s="8"/>
-      <c r="Z110" s="8"/>
-      <c r="AA110" s="8"/>
-      <c r="AB110" s="8"/>
-      <c r="AC110" s="8"/>
-      <c r="AD110" s="8"/>
-      <c r="AE110" s="8"/>
-      <c r="AF110" s="8"/>
-      <c r="AG110" s="8"/>
-      <c r="AH110" s="8"/>
-      <c r="AI110" s="8"/>
-      <c r="AJ110" s="8"/>
-      <c r="AK110" s="8"/>
-      <c r="AL110" s="8"/>
-      <c r="AM110" s="8"/>
-      <c r="AN110" s="8"/>
-      <c r="AO110" s="8"/>
-      <c r="AP110" s="9"/>
-    </row>
-    <row r="111" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B111" s="10"/>
-      <c r="C111" s="11"/>
-      <c r="D111" s="11"/>
-      <c r="E111" s="11"/>
-      <c r="F111" s="11"/>
-      <c r="G111" s="11"/>
-      <c r="H111" s="11"/>
-      <c r="I111" s="11"/>
-      <c r="J111" s="11"/>
-      <c r="K111" s="11"/>
-      <c r="L111" s="11"/>
-      <c r="M111" s="11"/>
-      <c r="N111" s="11"/>
-      <c r="O111" s="11"/>
-      <c r="P111" s="11"/>
-      <c r="Q111" s="11"/>
-      <c r="R111" s="11"/>
-      <c r="S111" s="11"/>
-      <c r="T111" s="11"/>
-      <c r="U111" s="11"/>
-      <c r="V111" s="11"/>
-      <c r="W111" s="11"/>
-      <c r="X111" s="11"/>
-      <c r="Y111" s="11"/>
-      <c r="Z111" s="11"/>
-      <c r="AA111" s="11"/>
-      <c r="AB111" s="11"/>
-      <c r="AC111" s="11"/>
-      <c r="AD111" s="11"/>
-      <c r="AE111" s="11"/>
-      <c r="AF111" s="11"/>
-      <c r="AG111" s="11"/>
-      <c r="AH111" s="11"/>
-      <c r="AI111" s="11"/>
-      <c r="AJ111" s="11"/>
-      <c r="AK111" s="11"/>
-      <c r="AL111" s="11"/>
-      <c r="AM111" s="11"/>
-      <c r="AN111" s="11"/>
-      <c r="AO111" s="11"/>
-      <c r="AP111" s="12"/>
-    </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B113">
-        <v>1</v>
-      </c>
-      <c r="C113" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C114" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C115" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C116" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C117" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C118" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C119" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C120" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C121" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C122" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C123" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C124" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C125" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C126" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C127" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C128" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C129" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C130" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C131" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B133">
-        <v>2</v>
-      </c>
-      <c r="C133" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B135">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13258,7 +11965,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="3"/>
       <c r="G16" s="1" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="3"/>
@@ -13580,52 +12287,52 @@
     </row>
     <row r="24" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
     </row>
     <row r="25" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
     </row>
     <row r="26" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
     </row>
     <row r="27" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
     </row>
     <row r="28" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
     </row>
     <row r="29" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
     </row>
     <row r="30" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
     </row>
     <row r="31" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
     </row>
     <row r="32" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
     </row>
   </sheetData>
@@ -13760,7 +12467,7 @@
       <c r="X5" s="8"/>
       <c r="Y5" s="9"/>
       <c r="AA5" t="s">
-        <v>671</v>
+        <v>645</v>
       </c>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.25">
@@ -13849,7 +12556,7 @@
       <c r="X8" s="8"/>
       <c r="Y8" s="9"/>
       <c r="AA8" s="74" t="s">
-        <v>633</v>
+        <v>613</v>
       </c>
       <c r="AB8" s="74"/>
       <c r="AC8" s="74"/>
@@ -13881,7 +12588,7 @@
       <c r="X9" s="8"/>
       <c r="Y9" s="9"/>
       <c r="AA9" s="74" t="s">
-        <v>631</v>
+        <v>611</v>
       </c>
       <c r="AB9" s="74"/>
       <c r="AC9" s="74"/>
@@ -13917,7 +12624,7 @@
       <c r="X10" s="8"/>
       <c r="Y10" s="9"/>
       <c r="AA10" s="74" t="s">
-        <v>632</v>
+        <v>612</v>
       </c>
       <c r="AB10" s="74"/>
       <c r="AC10" s="74"/>
@@ -13977,7 +12684,7 @@
       <c r="X12" s="8"/>
       <c r="Y12" s="9"/>
       <c r="AA12" s="74" t="s">
-        <v>688</v>
+        <v>662</v>
       </c>
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.25">
@@ -15537,25 +14244,25 @@
       <c r="N43" s="3"/>
       <c r="O43" s="8"/>
       <c r="P43" s="74" t="s">
-        <v>682</v>
+        <v>656</v>
       </c>
       <c r="Q43" s="74"/>
       <c r="R43" s="41" t="s">
-        <v>683</v>
+        <v>657</v>
       </c>
       <c r="S43" s="43"/>
       <c r="T43" s="43"/>
       <c r="U43" s="42"/>
       <c r="V43" s="39"/>
       <c r="W43" s="39" t="s">
-        <v>684</v>
+        <v>658</v>
       </c>
       <c r="X43" s="39"/>
       <c r="Y43" s="39"/>
       <c r="Z43" s="40"/>
       <c r="AA43" s="74"/>
       <c r="AB43" s="74" t="s">
-        <v>685</v>
+        <v>659</v>
       </c>
       <c r="AC43" s="74"/>
       <c r="AD43" s="74"/>
@@ -21477,7 +20184,7 @@
       <c r="AS100" s="19"/>
       <c r="AT100" s="19"/>
       <c r="AU100" s="19" t="s">
-        <v>673</v>
+        <v>647</v>
       </c>
       <c r="AV100" s="19"/>
       <c r="AW100" s="19"/>
@@ -27416,7 +26123,7 @@
       <c r="AB60" s="8"/>
       <c r="AC60" s="9"/>
       <c r="AG60" t="s">
-        <v>634</v>
+        <v>614</v>
       </c>
     </row>
     <row r="61" spans="1:56" x14ac:dyDescent="0.25">
@@ -28880,7 +27587,7 @@
         <v>35</v>
       </c>
       <c r="AL24" t="s">
-        <v>629</v>
+        <v>609</v>
       </c>
     </row>
     <row r="25" spans="2:44" x14ac:dyDescent="0.25">
@@ -28923,7 +27630,7 @@
         <v>35</v>
       </c>
       <c r="AL25" t="s">
-        <v>628</v>
+        <v>608</v>
       </c>
     </row>
     <row r="26" spans="2:44" x14ac:dyDescent="0.25">
@@ -28966,7 +27673,7 @@
         <v>35</v>
       </c>
       <c r="AL26" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
     </row>
     <row r="27" spans="2:44" x14ac:dyDescent="0.25">
@@ -29007,7 +27714,7 @@
         <v>35</v>
       </c>
       <c r="AL27" t="s">
-        <v>626</v>
+        <v>606</v>
       </c>
     </row>
     <row r="28" spans="2:44" x14ac:dyDescent="0.25">
@@ -29048,7 +27755,7 @@
         <v>35</v>
       </c>
       <c r="AL28" t="s">
-        <v>625</v>
+        <v>605</v>
       </c>
     </row>
     <row r="29" spans="2:44" x14ac:dyDescent="0.25">
@@ -29127,7 +27834,7 @@
       <c r="AB30" s="8"/>
       <c r="AC30" s="9"/>
       <c r="AE30" s="54" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="AF30" s="54"/>
       <c r="AG30" s="54"/>
@@ -29138,7 +27845,7 @@
         <v>35</v>
       </c>
       <c r="AL30" s="54" t="s">
-        <v>624</v>
+        <v>604</v>
       </c>
       <c r="AM30" s="54"/>
       <c r="AN30" s="54"/>
@@ -29192,7 +27899,7 @@
         <v>35</v>
       </c>
       <c r="AL31" s="54" t="s">
-        <v>623</v>
+        <v>603</v>
       </c>
       <c r="AM31" s="54"/>
       <c r="AN31" s="54"/>
@@ -29265,7 +27972,7 @@
       <c r="AB33" s="8"/>
       <c r="AC33" s="9"/>
       <c r="AE33" s="24" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
     </row>
     <row r="34" spans="2:40" x14ac:dyDescent="0.25">
@@ -29691,7 +28398,7 @@
         <v>35</v>
       </c>
       <c r="AK43" t="s">
-        <v>619</v>
+        <v>599</v>
       </c>
     </row>
     <row r="44" spans="2:40" x14ac:dyDescent="0.25">
@@ -29874,7 +28581,7 @@
       <c r="AB48" s="8"/>
       <c r="AC48" s="9"/>
       <c r="AE48" t="s">
-        <v>672</v>
+        <v>646</v>
       </c>
     </row>
     <row r="49" spans="3:29" x14ac:dyDescent="0.25">
@@ -30887,7 +29594,7 @@
         <v>35</v>
       </c>
       <c r="AJ23" t="s">
-        <v>629</v>
+        <v>609</v>
       </c>
     </row>
     <row r="24" spans="1:49" x14ac:dyDescent="0.25">
@@ -30929,7 +29636,7 @@
         <v>35</v>
       </c>
       <c r="AJ24" t="s">
-        <v>628</v>
+        <v>608</v>
       </c>
     </row>
     <row r="25" spans="1:49" x14ac:dyDescent="0.25">
@@ -30971,7 +29678,7 @@
         <v>35</v>
       </c>
       <c r="AJ25" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
     </row>
     <row r="26" spans="1:49" x14ac:dyDescent="0.25">
@@ -31011,7 +29718,7 @@
         <v>35</v>
       </c>
       <c r="AJ26" t="s">
-        <v>626</v>
+        <v>606</v>
       </c>
     </row>
     <row r="27" spans="1:49" x14ac:dyDescent="0.25">
@@ -31051,7 +29758,7 @@
         <v>35</v>
       </c>
       <c r="AJ27" t="s">
-        <v>625</v>
+        <v>605</v>
       </c>
     </row>
     <row r="28" spans="1:49" x14ac:dyDescent="0.25">
@@ -31128,7 +29835,7 @@
       <c r="Z29" s="8"/>
       <c r="AA29" s="9"/>
       <c r="AC29" s="54" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="AD29" s="54"/>
       <c r="AE29" s="54"/>
@@ -31139,7 +29846,7 @@
         <v>35</v>
       </c>
       <c r="AJ29" s="54" t="s">
-        <v>624</v>
+        <v>604</v>
       </c>
       <c r="AK29" s="54"/>
     </row>
@@ -31187,7 +29894,7 @@
         <v>35</v>
       </c>
       <c r="AJ30" s="54" t="s">
-        <v>623</v>
+        <v>603</v>
       </c>
       <c r="AK30" s="54"/>
       <c r="AL30" s="54"/>
@@ -31389,7 +30096,7 @@
       <c r="Z35" s="8"/>
       <c r="AA35" s="9"/>
       <c r="AC35" s="24" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.25">
@@ -31799,7 +30506,7 @@
         <v>35</v>
       </c>
       <c r="AI45" t="s">
-        <v>619</v>
+        <v>599</v>
       </c>
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.25">
@@ -32604,7 +31311,7 @@
         <v>5</v>
       </c>
       <c r="AG68" t="s">
-        <v>630</v>
+        <v>610</v>
       </c>
     </row>
     <row r="69" spans="2:42" x14ac:dyDescent="0.25">
@@ -33046,7 +31753,7 @@
         <v>11</v>
       </c>
       <c r="AG79" s="54" t="s">
-        <v>644</v>
+        <v>618</v>
       </c>
       <c r="AH79" s="54"/>
       <c r="AI79" s="54"/>
@@ -33063,7 +31770,7 @@
       <c r="C80" s="8"/>
       <c r="D80" s="66"/>
       <c r="F80" s="19" t="s">
-        <v>643</v>
+        <v>617</v>
       </c>
       <c r="I80" s="19"/>
       <c r="J80" s="19"/>
@@ -33318,7 +32025,7 @@
     </row>
     <row r="91" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B91" s="54" t="s">
-        <v>645</v>
+        <v>619</v>
       </c>
       <c r="C91" s="54"/>
       <c r="D91" s="54"/>
@@ -33714,10 +32421,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV58"/>
+  <dimension ref="A1:AV93"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33917,7 +32624,7 @@
       <c r="AC11" s="2"/>
       <c r="AD11" s="3"/>
       <c r="AE11" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.25">
@@ -34002,7 +32709,7 @@
       </c>
       <c r="AK16" s="3"/>
       <c r="AL16" s="1" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
@@ -34316,57 +33023,57 @@
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
     </row>
     <row r="27" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
@@ -34458,10 +33165,10 @@
         <v>391</v>
       </c>
       <c r="E47" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="49" spans="2:36" x14ac:dyDescent="0.25">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>73</v>
       </c>
@@ -34514,7 +33221,7 @@
       <c r="AI49" s="5"/>
       <c r="AJ49" s="3"/>
     </row>
-    <row r="50" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
       <c r="D50" s="9"/>
@@ -34553,7 +33260,7 @@
       <c r="AI50" s="3"/>
       <c r="AJ50" s="9"/>
     </row>
-    <row r="51" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B51" s="7"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
@@ -34590,7 +33297,7 @@
       <c r="AI51" s="8"/>
       <c r="AJ51" s="9"/>
     </row>
-    <row r="52" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
       <c r="C52" s="8"/>
       <c r="D52" s="9"/>
@@ -34629,7 +33336,7 @@
       <c r="AI52" s="3"/>
       <c r="AJ52" s="9"/>
     </row>
-    <row r="53" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B53" s="10"/>
       <c r="C53" s="11"/>
       <c r="D53" s="12"/>
@@ -34666,7 +33373,7 @@
       <c r="AI53" s="11"/>
       <c r="AJ53" s="12"/>
     </row>
-    <row r="54" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
       <c r="C54" s="8"/>
       <c r="D54" s="9"/>
@@ -34703,7 +33410,7 @@
       <c r="AI54" s="8"/>
       <c r="AJ54" s="9"/>
     </row>
-    <row r="55" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B55" s="7"/>
       <c r="C55" s="8"/>
       <c r="D55" s="9"/>
@@ -34742,7 +33449,7 @@
       <c r="AI55" s="3"/>
       <c r="AJ55" s="9"/>
     </row>
-    <row r="56" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
       <c r="C56" s="8"/>
       <c r="D56" s="9"/>
@@ -34779,7 +33486,7 @@
       <c r="AI56" s="8"/>
       <c r="AJ56" s="9"/>
     </row>
-    <row r="57" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B57" s="7"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
@@ -34818,7 +33525,7 @@
       <c r="AI57" s="3"/>
       <c r="AJ57" s="9"/>
     </row>
-    <row r="58" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B58" s="10"/>
       <c r="C58" s="11"/>
       <c r="D58" s="12"/>
@@ -34855,6 +33562,1136 @@
       <c r="AI58" s="11"/>
       <c r="AJ58" s="12"/>
     </row>
+    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A62" s="74">
+        <v>3</v>
+      </c>
+      <c r="B62" s="74" t="s">
+        <v>668</v>
+      </c>
+      <c r="C62" s="74"/>
+      <c r="D62" s="74"/>
+      <c r="E62" s="74"/>
+      <c r="F62" s="74"/>
+      <c r="G62" s="74"/>
+      <c r="H62" s="74"/>
+      <c r="I62" s="74"/>
+    </row>
+    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B63" s="4"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5"/>
+      <c r="O63" s="5"/>
+      <c r="P63" s="5"/>
+      <c r="Q63" s="5"/>
+      <c r="R63" s="5"/>
+      <c r="S63" s="5"/>
+      <c r="T63" s="5"/>
+      <c r="U63" s="5"/>
+      <c r="V63" s="5"/>
+      <c r="W63" s="5"/>
+      <c r="X63" s="5"/>
+      <c r="Y63" s="5"/>
+      <c r="Z63" s="5"/>
+      <c r="AA63" s="5"/>
+      <c r="AB63" s="5"/>
+      <c r="AC63" s="5"/>
+      <c r="AD63" s="5"/>
+      <c r="AE63" s="5"/>
+      <c r="AF63" s="5"/>
+      <c r="AG63" s="5"/>
+      <c r="AH63" s="5"/>
+      <c r="AI63" s="5"/>
+      <c r="AJ63" s="5"/>
+      <c r="AK63" s="5"/>
+      <c r="AL63" s="5"/>
+      <c r="AM63" s="5"/>
+      <c r="AN63" s="5"/>
+      <c r="AO63" s="5"/>
+      <c r="AP63" s="5"/>
+      <c r="AQ63" s="6"/>
+    </row>
+    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B64" s="7"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="8"/>
+      <c r="K64" s="8"/>
+      <c r="L64" s="8"/>
+      <c r="M64" s="8"/>
+      <c r="N64" s="8"/>
+      <c r="O64" s="8"/>
+      <c r="P64" s="8"/>
+      <c r="Q64" s="8"/>
+      <c r="R64" s="8"/>
+      <c r="S64" s="8"/>
+      <c r="T64" s="8"/>
+      <c r="U64" s="8"/>
+      <c r="V64" s="8"/>
+      <c r="W64" s="8"/>
+      <c r="X64" s="8"/>
+      <c r="Y64" s="8"/>
+      <c r="Z64" s="8"/>
+      <c r="AA64" s="8"/>
+      <c r="AB64" s="8"/>
+      <c r="AC64" s="8"/>
+      <c r="AD64" s="8"/>
+      <c r="AE64" s="8"/>
+      <c r="AF64" s="8"/>
+      <c r="AG64" s="8"/>
+      <c r="AH64" s="8"/>
+      <c r="AI64" s="8"/>
+      <c r="AJ64" s="8"/>
+      <c r="AK64" s="8"/>
+      <c r="AL64" s="8"/>
+      <c r="AM64" s="8"/>
+      <c r="AN64" s="8"/>
+      <c r="AO64" s="8"/>
+      <c r="AP64" s="8"/>
+      <c r="AQ64" s="9"/>
+    </row>
+    <row r="65" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B65" s="7"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8" t="s">
+        <v>669</v>
+      </c>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="8"/>
+      <c r="K65" s="8"/>
+      <c r="L65" s="8"/>
+      <c r="M65" s="8"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="2"/>
+      <c r="P65" s="2"/>
+      <c r="Q65" s="2"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="8"/>
+      <c r="T65" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="U65" s="8"/>
+      <c r="V65" s="8"/>
+      <c r="W65" s="1"/>
+      <c r="X65" s="2"/>
+      <c r="Y65" s="2"/>
+      <c r="Z65" s="2"/>
+      <c r="AA65" s="3"/>
+      <c r="AB65" s="8"/>
+      <c r="AC65" s="8"/>
+      <c r="AD65" s="8"/>
+      <c r="AE65" s="8"/>
+      <c r="AF65" s="8"/>
+      <c r="AG65" s="8"/>
+      <c r="AH65" s="8"/>
+      <c r="AI65" s="8"/>
+      <c r="AJ65" s="8"/>
+      <c r="AK65" s="8"/>
+      <c r="AL65" s="8"/>
+      <c r="AM65" s="8"/>
+      <c r="AN65" s="8"/>
+      <c r="AO65" s="8"/>
+      <c r="AP65" s="8"/>
+      <c r="AQ65" s="9"/>
+    </row>
+    <row r="66" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B66" s="7"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="8"/>
+      <c r="I66" s="8"/>
+      <c r="J66" s="8"/>
+      <c r="K66" s="8"/>
+      <c r="L66" s="8"/>
+      <c r="M66" s="8"/>
+      <c r="N66" s="8"/>
+      <c r="O66" s="8"/>
+      <c r="P66" s="8"/>
+      <c r="Q66" s="8"/>
+      <c r="R66" s="8"/>
+      <c r="S66" s="8"/>
+      <c r="T66" s="8"/>
+      <c r="U66" s="8"/>
+      <c r="V66" s="8"/>
+      <c r="W66" s="8"/>
+      <c r="X66" s="8"/>
+      <c r="Y66" s="8"/>
+      <c r="Z66" s="8"/>
+      <c r="AA66" s="8"/>
+      <c r="AB66" s="8"/>
+      <c r="AC66" s="8"/>
+      <c r="AD66" s="8"/>
+      <c r="AE66" s="8"/>
+      <c r="AF66" s="8"/>
+      <c r="AG66" s="8"/>
+      <c r="AH66" s="8"/>
+      <c r="AI66" s="8"/>
+      <c r="AJ66" s="8"/>
+      <c r="AK66" s="8"/>
+      <c r="AL66" s="8"/>
+      <c r="AM66" s="8"/>
+      <c r="AN66" s="8"/>
+      <c r="AO66" s="8"/>
+      <c r="AP66" s="8"/>
+      <c r="AQ66" s="9"/>
+    </row>
+    <row r="67" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B67" s="7"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8" t="s">
+        <v>670</v>
+      </c>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="8"/>
+      <c r="K67" s="8"/>
+      <c r="L67" s="8"/>
+      <c r="M67" s="8"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="2"/>
+      <c r="P67" s="2"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="8"/>
+      <c r="S67" s="8"/>
+      <c r="T67" s="8"/>
+      <c r="U67" s="8"/>
+      <c r="V67" s="8"/>
+      <c r="W67" s="8"/>
+      <c r="X67" s="8"/>
+      <c r="Y67" s="8"/>
+      <c r="Z67" s="8"/>
+      <c r="AA67" s="8"/>
+      <c r="AB67" s="8"/>
+      <c r="AC67" s="8"/>
+      <c r="AD67" s="8"/>
+      <c r="AE67" s="8"/>
+      <c r="AF67" s="8"/>
+      <c r="AG67" s="8"/>
+      <c r="AH67" s="8"/>
+      <c r="AI67" s="8"/>
+      <c r="AJ67" s="8"/>
+      <c r="AK67" s="8"/>
+      <c r="AL67" s="8"/>
+      <c r="AM67" s="8"/>
+      <c r="AN67" s="8"/>
+      <c r="AO67" s="8"/>
+      <c r="AP67" s="8"/>
+      <c r="AQ67" s="9"/>
+    </row>
+    <row r="68" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B68" s="7"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+      <c r="K68" s="8"/>
+      <c r="L68" s="8"/>
+      <c r="M68" s="8"/>
+      <c r="N68" s="8"/>
+      <c r="O68" s="8"/>
+      <c r="P68" s="8"/>
+      <c r="Q68" s="8"/>
+      <c r="R68" s="8"/>
+      <c r="S68" s="8"/>
+      <c r="T68" s="8"/>
+      <c r="U68" s="8"/>
+      <c r="V68" s="8"/>
+      <c r="W68" s="8"/>
+      <c r="X68" s="8"/>
+      <c r="Y68" s="8"/>
+      <c r="Z68" s="8"/>
+      <c r="AA68" s="8"/>
+      <c r="AB68" s="8"/>
+      <c r="AC68" s="8"/>
+      <c r="AD68" s="8"/>
+      <c r="AE68" s="8"/>
+      <c r="AF68" s="8"/>
+      <c r="AG68" s="8"/>
+      <c r="AH68" s="8"/>
+      <c r="AI68" s="8"/>
+      <c r="AJ68" s="8"/>
+      <c r="AK68" s="8"/>
+      <c r="AL68" s="8"/>
+      <c r="AM68" s="8"/>
+      <c r="AN68" s="8"/>
+      <c r="AO68" s="8"/>
+      <c r="AP68" s="8"/>
+      <c r="AQ68" s="9"/>
+    </row>
+    <row r="69" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B69" s="7"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8" t="s">
+        <v>671</v>
+      </c>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="8"/>
+      <c r="K69" s="8"/>
+      <c r="L69" s="8"/>
+      <c r="M69" s="8"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="2"/>
+      <c r="P69" s="2"/>
+      <c r="Q69" s="3"/>
+      <c r="R69" s="8" t="s">
+        <v>558</v>
+      </c>
+      <c r="S69" s="1"/>
+      <c r="T69" s="2"/>
+      <c r="U69" s="2"/>
+      <c r="V69" s="3"/>
+      <c r="W69" s="8"/>
+      <c r="X69" s="8"/>
+      <c r="Y69" s="8"/>
+      <c r="Z69" s="8"/>
+      <c r="AA69" s="8"/>
+      <c r="AB69" s="8"/>
+      <c r="AC69" s="8"/>
+      <c r="AD69" s="8"/>
+      <c r="AE69" s="8"/>
+      <c r="AF69" s="8"/>
+      <c r="AG69" s="8"/>
+      <c r="AH69" s="8"/>
+      <c r="AI69" s="8"/>
+      <c r="AJ69" s="8"/>
+      <c r="AK69" s="8"/>
+      <c r="AL69" s="8"/>
+      <c r="AM69" s="8"/>
+      <c r="AN69" s="8"/>
+      <c r="AO69" s="8"/>
+      <c r="AP69" s="8"/>
+      <c r="AQ69" s="9"/>
+    </row>
+    <row r="70" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B70" s="7"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
+      <c r="J70" s="8"/>
+      <c r="K70" s="8"/>
+      <c r="L70" s="8"/>
+      <c r="M70" s="8"/>
+      <c r="N70" s="8"/>
+      <c r="O70" s="8"/>
+      <c r="P70" s="8"/>
+      <c r="Q70" s="8"/>
+      <c r="R70" s="8"/>
+      <c r="S70" s="8"/>
+      <c r="T70" s="8"/>
+      <c r="U70" s="8"/>
+      <c r="V70" s="8"/>
+      <c r="W70" s="8"/>
+      <c r="X70" s="8"/>
+      <c r="Y70" s="8"/>
+      <c r="Z70" s="8"/>
+      <c r="AA70" s="8"/>
+      <c r="AB70" s="8"/>
+      <c r="AC70" s="8"/>
+      <c r="AD70" s="8"/>
+      <c r="AE70" s="8"/>
+      <c r="AF70" s="8"/>
+      <c r="AG70" s="8"/>
+      <c r="AH70" s="8"/>
+      <c r="AI70" s="8"/>
+      <c r="AJ70" s="8"/>
+      <c r="AK70" s="8"/>
+      <c r="AL70" s="8"/>
+      <c r="AM70" s="8"/>
+      <c r="AN70" s="8"/>
+      <c r="AO70" s="8"/>
+      <c r="AP70" s="8"/>
+      <c r="AQ70" s="9"/>
+    </row>
+    <row r="71" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B71" s="7"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="13" t="s">
+        <v>391</v>
+      </c>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="8"/>
+      <c r="K71" s="8"/>
+      <c r="L71" s="8"/>
+      <c r="M71" s="8"/>
+      <c r="N71" s="8"/>
+      <c r="O71" s="8"/>
+      <c r="P71" s="8"/>
+      <c r="Q71" s="8"/>
+      <c r="R71" s="8"/>
+      <c r="S71" s="8"/>
+      <c r="T71" s="8"/>
+      <c r="U71" s="8"/>
+      <c r="V71" s="8"/>
+      <c r="W71" s="8"/>
+      <c r="X71" s="8"/>
+      <c r="Y71" s="8"/>
+      <c r="Z71" s="8"/>
+      <c r="AA71" s="8"/>
+      <c r="AB71" s="8"/>
+      <c r="AC71" s="8"/>
+      <c r="AD71" s="8"/>
+      <c r="AE71" s="8"/>
+      <c r="AF71" s="8"/>
+      <c r="AG71" s="8"/>
+      <c r="AH71" s="8"/>
+      <c r="AI71" s="8"/>
+      <c r="AJ71" s="8"/>
+      <c r="AK71" s="8"/>
+      <c r="AL71" s="8"/>
+      <c r="AM71" s="8"/>
+      <c r="AN71" s="8"/>
+      <c r="AO71" s="8"/>
+      <c r="AP71" s="8"/>
+      <c r="AQ71" s="9"/>
+    </row>
+    <row r="72" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B72" s="7"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="8"/>
+      <c r="K72" s="8"/>
+      <c r="L72" s="8"/>
+      <c r="M72" s="8"/>
+      <c r="N72" s="8"/>
+      <c r="O72" s="8"/>
+      <c r="P72" s="8"/>
+      <c r="Q72" s="8"/>
+      <c r="R72" s="8"/>
+      <c r="S72" s="8"/>
+      <c r="T72" s="8"/>
+      <c r="U72" s="8"/>
+      <c r="V72" s="8"/>
+      <c r="W72" s="8"/>
+      <c r="X72" s="8"/>
+      <c r="Y72" s="8"/>
+      <c r="Z72" s="8"/>
+      <c r="AA72" s="8"/>
+      <c r="AB72" s="8"/>
+      <c r="AC72" s="8"/>
+      <c r="AD72" s="8"/>
+      <c r="AE72" s="8"/>
+      <c r="AF72" s="8"/>
+      <c r="AG72" s="8"/>
+      <c r="AH72" s="8"/>
+      <c r="AI72" s="8"/>
+      <c r="AJ72" s="8"/>
+      <c r="AK72" s="8"/>
+      <c r="AL72" s="8"/>
+      <c r="AM72" s="8"/>
+      <c r="AN72" s="8"/>
+      <c r="AO72" s="8"/>
+      <c r="AP72" s="8"/>
+      <c r="AQ72" s="9"/>
+    </row>
+    <row r="73" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B73" s="7"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="N73" s="2"/>
+      <c r="O73" s="2"/>
+      <c r="P73" s="3"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="S73" s="2"/>
+      <c r="T73" s="2"/>
+      <c r="U73" s="3"/>
+      <c r="V73" s="1"/>
+      <c r="W73" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="X73" s="2"/>
+      <c r="Y73" s="2"/>
+      <c r="Z73" s="3"/>
+      <c r="AA73" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="AB73" s="2"/>
+      <c r="AC73" s="2"/>
+      <c r="AD73" s="3"/>
+      <c r="AE73" s="1"/>
+      <c r="AF73" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AG73" s="3"/>
+      <c r="AH73" s="2"/>
+      <c r="AI73" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="AJ73" s="2"/>
+      <c r="AK73" s="3"/>
+      <c r="AL73" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="AM73" s="2"/>
+      <c r="AN73" s="2"/>
+      <c r="AO73" s="3"/>
+      <c r="AP73" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="AQ73" s="3"/>
+      <c r="AR73" s="2"/>
+      <c r="AS73" s="2"/>
+      <c r="AT73" s="3"/>
+    </row>
+    <row r="74" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B74" s="7"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="8"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="7"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="8"/>
+      <c r="K74" s="9"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="8"/>
+      <c r="N74" s="8"/>
+      <c r="O74" s="8"/>
+      <c r="P74" s="9"/>
+      <c r="Q74" s="7"/>
+      <c r="R74" s="8"/>
+      <c r="S74" s="8"/>
+      <c r="T74" s="8"/>
+      <c r="U74" s="9"/>
+      <c r="V74" s="7"/>
+      <c r="W74" s="8"/>
+      <c r="X74" s="8"/>
+      <c r="Y74" s="8"/>
+      <c r="Z74" s="9"/>
+      <c r="AA74" s="7"/>
+      <c r="AB74" s="8"/>
+      <c r="AC74" s="8"/>
+      <c r="AD74" s="9"/>
+      <c r="AE74" s="7"/>
+      <c r="AF74" s="8"/>
+      <c r="AG74" s="9"/>
+      <c r="AH74" s="8"/>
+      <c r="AI74" s="8"/>
+      <c r="AJ74" s="8"/>
+      <c r="AK74" s="9"/>
+      <c r="AL74" s="7"/>
+      <c r="AM74" s="8"/>
+      <c r="AN74" s="8"/>
+      <c r="AO74" s="9"/>
+      <c r="AP74" s="7"/>
+      <c r="AQ74" s="9"/>
+      <c r="AR74" s="8"/>
+      <c r="AS74" s="8"/>
+      <c r="AT74" s="9"/>
+    </row>
+    <row r="75" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B75" s="7"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="7"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="8"/>
+      <c r="K75" s="9"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="8"/>
+      <c r="N75" s="8"/>
+      <c r="O75" s="8"/>
+      <c r="P75" s="9"/>
+      <c r="Q75" s="7"/>
+      <c r="R75" s="8"/>
+      <c r="S75" s="8"/>
+      <c r="T75" s="8"/>
+      <c r="U75" s="9"/>
+      <c r="V75" s="7"/>
+      <c r="W75" s="8"/>
+      <c r="X75" s="8"/>
+      <c r="Y75" s="8"/>
+      <c r="Z75" s="9"/>
+      <c r="AA75" s="7"/>
+      <c r="AB75" s="8"/>
+      <c r="AC75" s="8"/>
+      <c r="AD75" s="9"/>
+      <c r="AE75" s="7"/>
+      <c r="AF75" s="8"/>
+      <c r="AG75" s="9"/>
+      <c r="AH75" s="8"/>
+      <c r="AI75" s="8"/>
+      <c r="AJ75" s="8"/>
+      <c r="AK75" s="9"/>
+      <c r="AL75" s="7"/>
+      <c r="AM75" s="8"/>
+      <c r="AN75" s="8"/>
+      <c r="AO75" s="9"/>
+      <c r="AP75" s="7"/>
+      <c r="AQ75" s="9"/>
+      <c r="AR75" s="8"/>
+      <c r="AS75" s="8"/>
+      <c r="AT75" s="9"/>
+    </row>
+    <row r="76" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B76" s="7"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="8"/>
+      <c r="J76" s="8"/>
+      <c r="K76" s="9"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="8"/>
+      <c r="N76" s="8"/>
+      <c r="O76" s="8"/>
+      <c r="P76" s="9"/>
+      <c r="Q76" s="7"/>
+      <c r="R76" s="8"/>
+      <c r="S76" s="8"/>
+      <c r="T76" s="8"/>
+      <c r="U76" s="9"/>
+      <c r="V76" s="7"/>
+      <c r="W76" s="8"/>
+      <c r="X76" s="8"/>
+      <c r="Y76" s="8"/>
+      <c r="Z76" s="9"/>
+      <c r="AA76" s="7"/>
+      <c r="AB76" s="8"/>
+      <c r="AC76" s="8"/>
+      <c r="AD76" s="9"/>
+      <c r="AE76" s="7"/>
+      <c r="AF76" s="8"/>
+      <c r="AG76" s="9"/>
+      <c r="AH76" s="8"/>
+      <c r="AI76" s="8"/>
+      <c r="AJ76" s="8"/>
+      <c r="AK76" s="9"/>
+      <c r="AL76" s="7"/>
+      <c r="AM76" s="8"/>
+      <c r="AN76" s="8"/>
+      <c r="AO76" s="9"/>
+      <c r="AP76" s="7"/>
+      <c r="AQ76" s="9"/>
+      <c r="AR76" s="8"/>
+      <c r="AS76" s="8"/>
+      <c r="AT76" s="9"/>
+    </row>
+    <row r="77" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B77" s="7"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="8"/>
+      <c r="J77" s="8"/>
+      <c r="K77" s="9"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="8"/>
+      <c r="N77" s="8"/>
+      <c r="O77" s="8"/>
+      <c r="P77" s="9"/>
+      <c r="Q77" s="7"/>
+      <c r="R77" s="8"/>
+      <c r="S77" s="8"/>
+      <c r="T77" s="8"/>
+      <c r="U77" s="9"/>
+      <c r="V77" s="7"/>
+      <c r="W77" s="8"/>
+      <c r="X77" s="8"/>
+      <c r="Y77" s="8"/>
+      <c r="Z77" s="9"/>
+      <c r="AA77" s="7"/>
+      <c r="AB77" s="8"/>
+      <c r="AC77" s="8"/>
+      <c r="AD77" s="9"/>
+      <c r="AE77" s="7"/>
+      <c r="AF77" s="8"/>
+      <c r="AG77" s="9"/>
+      <c r="AH77" s="8"/>
+      <c r="AI77" s="8"/>
+      <c r="AJ77" s="8"/>
+      <c r="AK77" s="9"/>
+      <c r="AL77" s="7"/>
+      <c r="AM77" s="8"/>
+      <c r="AN77" s="8"/>
+      <c r="AO77" s="9"/>
+      <c r="AP77" s="7"/>
+      <c r="AQ77" s="9"/>
+      <c r="AR77" s="8"/>
+      <c r="AS77" s="8"/>
+      <c r="AT77" s="9"/>
+    </row>
+    <row r="78" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B78" s="7"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="7"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="8"/>
+      <c r="K78" s="9"/>
+      <c r="L78" s="7"/>
+      <c r="M78" s="8"/>
+      <c r="N78" s="8"/>
+      <c r="O78" s="8"/>
+      <c r="P78" s="9"/>
+      <c r="Q78" s="7"/>
+      <c r="R78" s="8"/>
+      <c r="S78" s="8"/>
+      <c r="T78" s="8"/>
+      <c r="U78" s="9"/>
+      <c r="V78" s="7"/>
+      <c r="W78" s="8"/>
+      <c r="X78" s="8"/>
+      <c r="Y78" s="8"/>
+      <c r="Z78" s="9"/>
+      <c r="AA78" s="7"/>
+      <c r="AB78" s="8"/>
+      <c r="AC78" s="8"/>
+      <c r="AD78" s="9"/>
+      <c r="AE78" s="7"/>
+      <c r="AF78" s="8"/>
+      <c r="AG78" s="9"/>
+      <c r="AH78" s="8"/>
+      <c r="AI78" s="8"/>
+      <c r="AJ78" s="8"/>
+      <c r="AK78" s="9"/>
+      <c r="AL78" s="7"/>
+      <c r="AM78" s="8"/>
+      <c r="AN78" s="8"/>
+      <c r="AO78" s="9"/>
+      <c r="AP78" s="7"/>
+      <c r="AQ78" s="9"/>
+      <c r="AR78" s="8"/>
+      <c r="AS78" s="8"/>
+      <c r="AT78" s="9"/>
+    </row>
+    <row r="79" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B79" s="7"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="7"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="8"/>
+      <c r="K79" s="9"/>
+      <c r="L79" s="7"/>
+      <c r="M79" s="8"/>
+      <c r="N79" s="8"/>
+      <c r="O79" s="8"/>
+      <c r="P79" s="9"/>
+      <c r="Q79" s="7"/>
+      <c r="R79" s="8"/>
+      <c r="S79" s="8"/>
+      <c r="T79" s="8"/>
+      <c r="U79" s="9"/>
+      <c r="V79" s="7"/>
+      <c r="W79" s="8"/>
+      <c r="X79" s="8"/>
+      <c r="Y79" s="8"/>
+      <c r="Z79" s="9"/>
+      <c r="AA79" s="7"/>
+      <c r="AB79" s="8"/>
+      <c r="AC79" s="8"/>
+      <c r="AD79" s="9"/>
+      <c r="AE79" s="7"/>
+      <c r="AF79" s="8"/>
+      <c r="AG79" s="9"/>
+      <c r="AH79" s="8"/>
+      <c r="AI79" s="8"/>
+      <c r="AJ79" s="8"/>
+      <c r="AK79" s="9"/>
+      <c r="AL79" s="7"/>
+      <c r="AM79" s="8"/>
+      <c r="AN79" s="8"/>
+      <c r="AO79" s="9"/>
+      <c r="AP79" s="7"/>
+      <c r="AQ79" s="9"/>
+      <c r="AR79" s="8"/>
+      <c r="AS79" s="8"/>
+      <c r="AT79" s="9"/>
+    </row>
+    <row r="80" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B80" s="7"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="7"/>
+      <c r="I80" s="8"/>
+      <c r="J80" s="8"/>
+      <c r="K80" s="9"/>
+      <c r="L80" s="7"/>
+      <c r="M80" s="8"/>
+      <c r="N80" s="8"/>
+      <c r="O80" s="8"/>
+      <c r="P80" s="9"/>
+      <c r="Q80" s="7"/>
+      <c r="R80" s="8"/>
+      <c r="S80" s="8"/>
+      <c r="T80" s="8"/>
+      <c r="U80" s="9"/>
+      <c r="V80" s="7"/>
+      <c r="W80" s="8"/>
+      <c r="X80" s="8"/>
+      <c r="Y80" s="8"/>
+      <c r="Z80" s="9"/>
+      <c r="AA80" s="7"/>
+      <c r="AB80" s="8"/>
+      <c r="AC80" s="8"/>
+      <c r="AD80" s="9"/>
+      <c r="AE80" s="7"/>
+      <c r="AF80" s="8"/>
+      <c r="AG80" s="9"/>
+      <c r="AH80" s="8"/>
+      <c r="AI80" s="8"/>
+      <c r="AJ80" s="8"/>
+      <c r="AK80" s="9"/>
+      <c r="AL80" s="7"/>
+      <c r="AM80" s="8"/>
+      <c r="AN80" s="8"/>
+      <c r="AO80" s="9"/>
+      <c r="AP80" s="7"/>
+      <c r="AQ80" s="9"/>
+      <c r="AR80" s="8"/>
+      <c r="AS80" s="8"/>
+      <c r="AT80" s="9"/>
+    </row>
+    <row r="81" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B81" s="7"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="8"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="8"/>
+      <c r="J81" s="8"/>
+      <c r="K81" s="9"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="8"/>
+      <c r="N81" s="8"/>
+      <c r="O81" s="8"/>
+      <c r="P81" s="9"/>
+      <c r="Q81" s="7"/>
+      <c r="R81" s="8"/>
+      <c r="S81" s="8"/>
+      <c r="T81" s="8"/>
+      <c r="U81" s="9"/>
+      <c r="V81" s="7"/>
+      <c r="W81" s="8"/>
+      <c r="X81" s="8"/>
+      <c r="Y81" s="8"/>
+      <c r="Z81" s="9"/>
+      <c r="AA81" s="7"/>
+      <c r="AB81" s="8"/>
+      <c r="AC81" s="8"/>
+      <c r="AD81" s="9"/>
+      <c r="AE81" s="7"/>
+      <c r="AF81" s="8"/>
+      <c r="AG81" s="9"/>
+      <c r="AH81" s="8"/>
+      <c r="AI81" s="8"/>
+      <c r="AJ81" s="8"/>
+      <c r="AK81" s="9"/>
+      <c r="AL81" s="7"/>
+      <c r="AM81" s="8"/>
+      <c r="AN81" s="8"/>
+      <c r="AO81" s="9"/>
+      <c r="AP81" s="7"/>
+      <c r="AQ81" s="9"/>
+      <c r="AR81" s="8"/>
+      <c r="AS81" s="8"/>
+      <c r="AT81" s="9"/>
+    </row>
+    <row r="82" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B82" s="7"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="7"/>
+      <c r="I82" s="8"/>
+      <c r="J82" s="8"/>
+      <c r="K82" s="9"/>
+      <c r="L82" s="7"/>
+      <c r="M82" s="8"/>
+      <c r="N82" s="8"/>
+      <c r="O82" s="8"/>
+      <c r="P82" s="9"/>
+      <c r="Q82" s="7"/>
+      <c r="R82" s="8"/>
+      <c r="S82" s="8"/>
+      <c r="T82" s="8"/>
+      <c r="U82" s="9"/>
+      <c r="V82" s="7"/>
+      <c r="W82" s="8"/>
+      <c r="X82" s="8"/>
+      <c r="Y82" s="8"/>
+      <c r="Z82" s="9"/>
+      <c r="AA82" s="7"/>
+      <c r="AB82" s="8"/>
+      <c r="AC82" s="8"/>
+      <c r="AD82" s="9"/>
+      <c r="AE82" s="7"/>
+      <c r="AF82" s="8"/>
+      <c r="AG82" s="9"/>
+      <c r="AH82" s="8"/>
+      <c r="AI82" s="8"/>
+      <c r="AJ82" s="8"/>
+      <c r="AK82" s="9"/>
+      <c r="AL82" s="7"/>
+      <c r="AM82" s="8"/>
+      <c r="AN82" s="8"/>
+      <c r="AO82" s="9"/>
+      <c r="AP82" s="7"/>
+      <c r="AQ82" s="9"/>
+      <c r="AR82" s="8"/>
+      <c r="AS82" s="8"/>
+      <c r="AT82" s="9"/>
+    </row>
+    <row r="83" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B83" s="7"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="12"/>
+      <c r="H83" s="10"/>
+      <c r="I83" s="11"/>
+      <c r="J83" s="11"/>
+      <c r="K83" s="12"/>
+      <c r="L83" s="10"/>
+      <c r="M83" s="11"/>
+      <c r="N83" s="11"/>
+      <c r="O83" s="11"/>
+      <c r="P83" s="12"/>
+      <c r="Q83" s="10"/>
+      <c r="R83" s="11"/>
+      <c r="S83" s="11"/>
+      <c r="T83" s="11"/>
+      <c r="U83" s="12"/>
+      <c r="V83" s="10"/>
+      <c r="W83" s="11"/>
+      <c r="X83" s="11"/>
+      <c r="Y83" s="11"/>
+      <c r="Z83" s="12"/>
+      <c r="AA83" s="10"/>
+      <c r="AB83" s="11"/>
+      <c r="AC83" s="11"/>
+      <c r="AD83" s="12"/>
+      <c r="AE83" s="10"/>
+      <c r="AF83" s="11"/>
+      <c r="AG83" s="12"/>
+      <c r="AH83" s="11"/>
+      <c r="AI83" s="11"/>
+      <c r="AJ83" s="11"/>
+      <c r="AK83" s="12"/>
+      <c r="AL83" s="10"/>
+      <c r="AM83" s="11"/>
+      <c r="AN83" s="11"/>
+      <c r="AO83" s="12"/>
+      <c r="AP83" s="10"/>
+      <c r="AQ83" s="12"/>
+      <c r="AR83" s="11"/>
+      <c r="AS83" s="11"/>
+      <c r="AT83" s="12"/>
+    </row>
+    <row r="84" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B84" s="7"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="8"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
+      <c r="I84" s="8"/>
+      <c r="J84" s="8"/>
+      <c r="K84" s="8"/>
+      <c r="L84" s="8"/>
+      <c r="M84" s="8"/>
+      <c r="N84" s="8"/>
+      <c r="O84" s="8"/>
+      <c r="P84" s="8"/>
+      <c r="Q84" s="8"/>
+      <c r="R84" s="8"/>
+      <c r="S84" s="8"/>
+      <c r="T84" s="8"/>
+      <c r="U84" s="8"/>
+      <c r="V84" s="8"/>
+      <c r="W84" s="8"/>
+      <c r="X84" s="8"/>
+      <c r="Y84" s="8"/>
+      <c r="Z84" s="8"/>
+      <c r="AA84" s="8"/>
+      <c r="AB84" s="8"/>
+      <c r="AC84" s="8"/>
+      <c r="AD84" s="8"/>
+      <c r="AE84" s="8"/>
+      <c r="AF84" s="8"/>
+      <c r="AG84" s="8"/>
+      <c r="AH84" s="8"/>
+      <c r="AI84" s="8"/>
+      <c r="AJ84" s="8"/>
+      <c r="AK84" s="8"/>
+      <c r="AL84" s="8"/>
+      <c r="AM84" s="8"/>
+      <c r="AN84" s="8"/>
+      <c r="AO84" s="8"/>
+      <c r="AP84" s="8"/>
+      <c r="AQ84" s="9"/>
+    </row>
+    <row r="85" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B85" s="10"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="11"/>
+      <c r="I85" s="11"/>
+      <c r="J85" s="11"/>
+      <c r="K85" s="11"/>
+      <c r="L85" s="11"/>
+      <c r="M85" s="11"/>
+      <c r="N85" s="11"/>
+      <c r="O85" s="11"/>
+      <c r="P85" s="11"/>
+      <c r="Q85" s="11"/>
+      <c r="R85" s="11"/>
+      <c r="S85" s="11"/>
+      <c r="T85" s="11"/>
+      <c r="U85" s="11"/>
+      <c r="V85" s="11"/>
+      <c r="W85" s="11"/>
+      <c r="X85" s="11"/>
+      <c r="Y85" s="11"/>
+      <c r="Z85" s="11"/>
+      <c r="AA85" s="11"/>
+      <c r="AB85" s="11"/>
+      <c r="AC85" s="11"/>
+      <c r="AD85" s="11"/>
+      <c r="AE85" s="11"/>
+      <c r="AF85" s="11"/>
+      <c r="AG85" s="11"/>
+      <c r="AH85" s="11"/>
+      <c r="AI85" s="11"/>
+      <c r="AJ85" s="11"/>
+      <c r="AK85" s="11"/>
+      <c r="AL85" s="11"/>
+      <c r="AM85" s="11"/>
+      <c r="AN85" s="11"/>
+      <c r="AO85" s="11"/>
+      <c r="AP85" s="11"/>
+      <c r="AQ85" s="12"/>
+    </row>
+    <row r="87" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="88" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="89" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="90" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="91" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="92" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="93" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>686</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>